<commit_message>
runtime update (2025-10-27 20:30:04)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -500,7 +500,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -555,14 +555,14 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:35.017765</t>
+          <t>2025-10-27T20:28:22.871346</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -617,14 +617,14 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:36.874223</t>
+          <t>2025-10-27T20:28:26.453559</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -679,14 +679,14 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:36.874242</t>
+          <t>2025-10-27T20:28:26.453586</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -741,14 +741,14 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:36.874250</t>
+          <t>2025-10-27T20:28:26.453604</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -803,14 +803,14 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:36.874258</t>
+          <t>2025-10-27T20:28:26.453621</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -865,14 +865,14 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:36.874266</t>
+          <t>2025-10-27T20:28:26.453637</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -927,14 +927,14 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:38.680985</t>
+          <t>2025-10-27T20:28:35.815926</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -989,14 +989,14 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:38.681002</t>
+          <t>2025-10-27T20:28:35.815955</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1051,14 +1051,14 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:40.461134</t>
+          <t>2025-10-27T20:28:38.716488</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1113,14 +1113,14 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:42.465548</t>
+          <t>2025-10-27T20:28:41.253774</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1175,14 +1175,14 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:42.465575</t>
+          <t>2025-10-27T20:28:41.253803</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1237,14 +1237,14 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:44.624983</t>
+          <t>2025-10-27T20:28:43.845087</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1299,14 +1299,14 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:44.625009</t>
+          <t>2025-10-27T20:28:43.845114</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1361,14 +1361,14 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:44.625028</t>
+          <t>2025-10-27T20:28:43.845132</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1423,14 +1423,14 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:44.625045</t>
+          <t>2025-10-27T20:28:43.845150</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1485,14 +1485,14 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:56.226615</t>
+          <t>2025-10-27T20:28:52.142197</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1547,14 +1547,14 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2025-10-26T18:34:58.475213</t>
+          <t>2025-10-27T20:28:55.082295</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1609,14 +1609,14 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:00.364774</t>
+          <t>2025-10-27T20:28:57.625787</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1671,14 +1671,14 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:02.170146</t>
+          <t>2025-10-27T20:29:00.125266</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1733,14 +1733,14 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:02.170186</t>
+          <t>2025-10-27T20:29:00.125294</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1795,14 +1795,14 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:03.947205</t>
+          <t>2025-10-27T20:29:03.018397</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1857,14 +1857,14 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:03.947237</t>
+          <t>2025-10-27T20:29:03.018423</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1919,14 +1919,14 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:03.947262</t>
+          <t>2025-10-27T20:29:03.018439</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1981,14 +1981,14 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:03.947281</t>
+          <t>2025-10-27T20:29:03.018456</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2043,14 +2043,14 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:03.947299</t>
+          <t>2025-10-27T20:29:03.018472</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2105,14 +2105,14 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:05.831846</t>
+          <t>2025-10-27T20:29:05.483522</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2167,14 +2167,14 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:10.123028</t>
+          <t>2025-10-27T20:29:10.743538</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2229,14 +2229,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:10.123058</t>
+          <t>2025-10-27T20:29:10.743562</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2256,27 +2256,27 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Уткин Дмитрий А</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>15</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>35195</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СОЧ_уткиндмитрийа</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2291,54 +2291,54 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:10.123088</t>
+          <t>2025-10-27T20:29:10.743579</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>30</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2348,44 +2348,44 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:12.212189</t>
+          <t>2025-10-27T20:29:10.743595</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>24</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2395,12 +2395,12 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2410,19 +2410,19 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:14.328959</t>
+          <t>2025-10-27T20:29:13.263160</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2442,12 +2442,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>61</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -2457,12 +2457,12 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2477,14 +2477,14 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:14.328987</t>
+          <t>2025-10-27T20:29:15.799036</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2504,27 +2504,27 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>83</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2539,14 +2539,14 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:14.329004</t>
+          <t>2025-10-27T20:29:15.799060</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2566,27 +2566,27 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>52</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -2601,14 +2601,14 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:14.329021</t>
+          <t>2025-10-27T20:29:15.799076</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2628,12 +2628,12 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Набиев Артём</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>17</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -2643,12 +2643,12 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>41187</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_набиевартем</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -2663,14 +2663,14 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:14.329037</t>
+          <t>2025-10-27T20:29:15.799092</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2690,12 +2690,12 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Пименов Артём</t>
+          <t>Набиев Артём</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>79</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -2705,12 +2705,12 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>21205</t>
+          <t>41187</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_пименовартем</t>
+          <t>1369_СЮЛ_набиевартем</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2725,14 +2725,14 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:14.329053</t>
+          <t>2025-10-27T20:29:15.799107</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2752,27 +2752,27 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Стюарт Дин</t>
+          <t>Пименов Артём</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>68</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>43791</t>
+          <t>21205</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_стюартдин</t>
+          <t>1369_СЮЛ_пименовартем</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -2787,14 +2787,14 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:14.329068</t>
+          <t>2025-10-27T20:29:15.799124</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2849,14 +2849,14 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:14.329084</t>
+          <t>2025-10-27T20:29:15.799140</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2911,14 +2911,14 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:14.329100</t>
+          <t>2025-10-27T20:29:15.799156</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2973,14 +2973,14 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:14.329115</t>
+          <t>2025-10-27T20:29:15.799169</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3035,14 +3035,14 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:16.973396</t>
+          <t>2025-10-27T20:29:18.255366</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3097,14 +3097,14 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:16.973428</t>
+          <t>2025-10-27T20:29:18.255391</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3159,14 +3159,14 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:21.649148</t>
+          <t>2025-10-27T20:29:23.772661</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3221,14 +3221,14 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:23.800522</t>
+          <t>2025-10-27T20:29:26.244275</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3283,14 +3283,14 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:23.800556</t>
+          <t>2025-10-27T20:29:26.244300</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3345,14 +3345,14 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:23.800576</t>
+          <t>2025-10-27T20:29:26.244317</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>по состоянию на 26 октября 2025</t>
+          <t>по состоянию на 27 октября 2025</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3407,7 +3407,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2025-10-26T18:35:23.800594</t>
+          <t>2025-10-27T20:29:26.244332</t>
         </is>
       </c>
     </row>
@@ -3422,7 +3422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3459,6 +3459,38 @@
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>changed_at</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>СЮЛ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Салават Юлаев</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Стюарт Дин</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_СЮЛ_стюартдин</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-10-27T20:29:26.849817</t>
         </is>
       </c>
     </row>
@@ -3473,7 +3505,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3513,6 +3545,38 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>СОЧ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Уткин Дмитрий А</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_СОЧ_уткиндмитрийа</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-10-27T20:29:26.853860</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
runtime update (2025-10-27 21:57:09)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,60 +438,55 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>date_snapshot</t>
+          <t>team_abbr</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>team_abbr</t>
+          <t>team_name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>team_name</t>
+          <t>team_slug</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>team_slug</t>
+          <t>player_name</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>player_name</t>
+          <t>number</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>position</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>position</t>
+          <t>player_id_khl</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>player_id_khl</t>
+          <t>player_uid</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>player_uid</t>
+          <t>status</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>status</t>
+          <t>source_url</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>source_url</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>scraped_at</t>
         </is>
@@ -500,2914 +495,2736 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>АВГ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>АВГ</t>
+          <t>Авангард</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Авангард</t>
+          <t>avangard</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>avangard</t>
+          <t>Якупов Наиль</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Якупов Наиль</t>
+          <t>65</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>16391</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>16391</t>
+          <t>1369_АВГ_якуповнаиль</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1369_АВГ_якуповнаиль</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/avangard/team/</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/avangard/team/</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:22.871346</t>
+          <t>2025-10-27T13:54:49.897523+00:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>АВТ</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>Автомобилист</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>avtomobilist</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>avtomobilist</t>
+          <t>Буше Рид</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Буше Рид</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>39158</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>39158</t>
+          <t>1369_АВТ_бушерид</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1369_АВТ_бушерид</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:26.453559</t>
+          <t>2025-10-27T13:54:52.038991+00:00</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>АВТ</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>Автомобилист</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>avtomobilist</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>avtomobilist</t>
+          <t>Зборовский Сергей</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Зборовский Сергей</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>20989</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>20989</t>
+          <t>1369_АВТ_зборовскийсергей</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1369_АВТ_зборовскийсергей</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:26.453586</t>
+          <t>2025-10-27T13:54:52.039008+00:00</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>АВТ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>Автомобилист</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>avtomobilist</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>avtomobilist</t>
+          <t>Кизимов Семён</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Кизимов Семён</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>25697</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>25697</t>
+          <t>1369_АВТ_кизимовсемен</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1369_АВТ_кизимовсемен</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:26.453604</t>
+          <t>2025-10-27T13:54:52.039016+00:00</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>АВТ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>Автомобилист</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>avtomobilist</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>avtomobilist</t>
+          <t>Осипов Максим И</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Осипов Максим И</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>17459</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>17459</t>
+          <t>1369_АВТ_осиповмаксими</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1369_АВТ_осиповмаксими</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:26.453621</t>
+          <t>2025-10-27T13:54:52.039024+00:00</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>АВТ</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>Автомобилист</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>avtomobilist</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>avtomobilist</t>
+          <t>Трямкин Никита</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Трямкин Никита</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>17594</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>17594</t>
+          <t>1369_АВТ_трямкинникита</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1369_АВТ_трямкинникита</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:26.453637</t>
+          <t>2025-10-27T13:54:52.039031+00:00</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>admiral</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>admiral</t>
+          <t>Грман Марио</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Грман Марио</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>31232</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>31232</t>
+          <t>1369_АДМ_грманмарио</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1369_АДМ_грманмарио</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/admiral/team/</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/admiral/team/</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:35.815926</t>
+          <t>2025-10-27T13:54:54.576491+00:00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>admiral</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>admiral</t>
+          <t>Шепелев Александр</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Шепелев Александр</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>23447</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>23447</t>
+          <t>1369_АДМ_шепелевалександр</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1369_АДМ_шепелевалександр</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/admiral/team/</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/admiral/team/</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:35.815955</t>
+          <t>2025-10-27T13:54:54.576505+00:00</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>АКБ</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>АКБ</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>ak_bars</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ak_bars</t>
+          <t>Яруллин Альберт</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Яруллин Альберт</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>16365</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>16365</t>
+          <t>1369_АКБ_яруллинальберт</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1369_АКБ_яруллинальберт</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:38.716488</t>
+          <t>2025-10-27T13:54:56.703608+00:00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>amur</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>Абросимов Роман</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Абросимов Роман</t>
+          <t>94</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>17968</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>17968</t>
+          <t>1369_АМР_абросимовроман</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1369_АМР_абросимовроман</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:41.253774</t>
+          <t>2025-10-27T13:54:59.177773+00:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>amur</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>Гиздатуллин Артур</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Гиздатуллин Артур</t>
+          <t>87</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>22208</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>22208</t>
+          <t>1369_АМР_гиздатуллинартур</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>1369_АМР_гиздатуллинартур</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:41.253803</t>
+          <t>2025-10-27T13:54:59.177790+00:00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>Асетов Алихан</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Асетов Алихан</t>
+          <t>96</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>20852</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>20852</t>
+          <t>1369_БАР_асетовалихан</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>1369_БАР_асетовалихан</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:43.845087</t>
+          <t>2025-10-27T13:55:01.332931+00:00</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>28244</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>28244</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:43.845114</t>
+          <t>2025-10-27T13:55:01.332946+00:00</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>Галимов Эмиль</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Галимов Эмиль</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>15997</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>15997</t>
+          <t>1369_БАР_галимовэмиль</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>1369_БАР_галимовэмиль</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:43.845132</t>
+          <t>2025-10-27T13:55:01.332954+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>Мухаметов Максим</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Мухаметов Максим</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>25207</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>25207</t>
+          <t>1369_БАР_мухаметовмаксим</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1369_БАР_мухаметовмаксим</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:43.845150</t>
+          <t>2025-10-27T13:55:01.332961+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:52.142197</t>
+          <t>2025-10-27T13:55:08.534704+00:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:55.082295</t>
+          <t>2025-10-27T13:55:10.626197+00:00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:28:57.625787</t>
+          <t>2025-10-27T13:55:12.844001+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:00.125266</t>
+          <t>2025-10-27T13:55:15.420348+00:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>Попугаев Никита О</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>22683</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>22683</t>
+          <t>1369_НХК_попугаевникитао</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:00.125294</t>
+          <t>2025-10-27T13:55:15.420364+00:00</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>Ващенко Григорий</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Ващенко Григорий</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>14155</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>14155</t>
+          <t>1369_СЕВ_ващенкогригорий</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>1369_СЕВ_ващенкогригорий</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:03.018397</t>
+          <t>2025-10-27T13:55:18.125208+00:00</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>Грудинин Владимир</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Грудинин Владимир</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>35064</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>35064</t>
+          <t>1369_СЕВ_грудининвладимир</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>1369_СЕВ_грудининвладимир</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:03.018423</t>
+          <t>2025-10-27T13:55:18.125223+00:00</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>Лишка Адам</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Лишка Адам</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>25514</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>25514</t>
+          <t>1369_СЕВ_лишкаадам</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>1369_СЕВ_лишкаадам</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:03.018439</t>
+          <t>2025-10-27T13:55:18.125232+00:00</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>Танков Кирилл</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Танков Кирилл</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>32981</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>32981</t>
+          <t>1369_СЕВ_танковкирилл</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>1369_СЕВ_танковкирилл</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:03.018456</t>
+          <t>2025-10-27T13:55:18.125240+00:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:03.018472</t>
+          <t>2025-10-27T13:55:18.125248+00:00</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>Фарранс Дэвид</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Фарранс Дэвид</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>45062</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>45062</t>
+          <t>1369_СИБ_фаррансдэвид</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>1369_СИБ_фаррансдэвид</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:05.483522</t>
+          <t>2025-10-27T13:55:20.678743+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>Гараев Амир</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Гараев Амир</t>
+          <t>67</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>28624</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>28624</t>
+          <t>1369_СОЧ_гараевамир</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гараевамир</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:10.743538</t>
+          <t>2025-10-27T13:55:25.449571+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:10.743562</t>
+          <t>2025-10-27T13:55:25.449585+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>Уткин Дмитрий А</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Уткин Дмитрий А</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>35195</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>35195</t>
+          <t>1369_СОЧ_уткиндмитрийа</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>1369_СОЧ_уткиндмитрийа</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:10.743579</t>
+          <t>2025-10-27T13:55:25.449593+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:10.743595</t>
+          <t>2025-10-27T13:55:25.449600+00:00</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:13.263160</t>
+          <t>2025-10-27T13:55:27.573273+00:00</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:15.799036</t>
+          <t>2025-10-27T13:55:27.573291+00:00</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:15.799060</t>
+          <t>2025-10-27T13:55:29.674791+00:00</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:15.799076</t>
+          <t>2025-10-27T13:55:29.674807+00:00</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:15.799092</t>
+          <t>2025-10-27T13:55:29.674814+00:00</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Набиев Артём</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>41187</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_набиевартем</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:15.799107</t>
+          <t>2025-10-27T13:55:29.674821+00:00</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>Набиев Артём</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Пименов Артём</t>
+          <t>79</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>41187</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>21205</t>
+          <t>1369_СЮЛ_набиевартем</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_пименовартем</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:15.799124</t>
+          <t>2025-10-27T13:55:29.674828+00:00</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>Пименов Артём</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>68</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>21205</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>1369_СЮЛ_пименовартем</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:15.799140</t>
+          <t>2025-10-27T13:55:29.674836+00:00</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Хохряков Пётр</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>15413</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хохряковпетр</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
-        </is>
-      </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:15.799156</t>
+          <t>2025-10-27T13:55:29.674843+00:00</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>Хохряков Пётр</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>15413</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>1369_СЮЛ_хохряковпетр</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
-        </is>
-      </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:15.799169</t>
+          <t>2025-10-27T13:55:29.674850+00:00</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:18.255366</t>
+          <t>2025-10-27T13:55:29.674857+00:00</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:18.255391</t>
+          <t>2025-10-27T13:55:32.291435+00:00</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:23.772661</t>
+          <t>2025-10-27T13:55:32.291449+00:00</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:26.244275</t>
+          <t>2025-10-27T13:55:36.573911+00:00</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Попугаев Никита А</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>22684</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>1369_ШДР_попугаевникитаа</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:26.244300</t>
+          <t>2025-10-27T13:55:38.701074+00:00</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>Попугаев Никита А</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Саттер Райли</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>22684</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>45491</t>
+          <t>1369_ШДР_попугаевникитаа</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>1369_ШДР_саттеррайли</t>
+          <t>injured_active</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>injured_active</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:26.244317</t>
+          <t>2025-10-27T13:55:38.701114+00:00</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>по состоянию на 27 октября 2025</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Саттер Райли</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>45491</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>1369_ШДР_саттеррайли</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>2025-10-27T13:55:38.701121+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
           <t>ШДР</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="B49" t="inlineStr">
         <is>
           <t>Драконы</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>kunlun</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>Фу Спенсер</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="F49" t="inlineStr">
         <is>
           <t>нападающий</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr">
+      <c r="G49" t="inlineStr">
         <is>
           <t>34934</t>
         </is>
       </c>
-      <c r="I48" t="inlineStr">
+      <c r="H49" t="inlineStr">
         <is>
           <t>1369_ШДР_фуспенсер</t>
         </is>
       </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
         <is>
           <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:26.244332</t>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>2025-10-27T13:55:38.701128+00:00</t>
         </is>
       </c>
     </row>
@@ -3422,7 +3239,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3461,36 +3278,9 @@
           <t>changed_at</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>СЮЛ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Салават Юлаев</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Стюарт Дин</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_СЮЛ_стюартдин</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:29:26.849817</t>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>changed_day</t>
         </is>
       </c>
     </row>
@@ -3505,7 +3295,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3544,26 +3334,31 @@
           <t>changed_at</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>changed_day</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Уткин Дмитрий А</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_СОЧ_уткиндмитрийа</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -3573,7 +3368,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-10-27T20:29:26.853860</t>
+          <t>2025-10-27T21:55:39.207982+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-10-27</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
runtime update (2025-10-28 00:14:41)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-27T13:54:49.897523+00:00</t>
+          <t>2025-10-27T16:01:47.137976+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-27T13:54:52.038991+00:00</t>
+          <t>2025-10-27T16:01:49.181182+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-27T13:54:52.039008+00:00</t>
+          <t>2025-10-27T16:01:49.181200+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-27T13:54:52.039016+00:00</t>
+          <t>2025-10-27T16:01:49.181210+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-27T13:54:52.039024+00:00</t>
+          <t>2025-10-27T16:01:49.181217+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-27T13:54:52.039031+00:00</t>
+          <t>2025-10-27T16:01:49.181225+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-27T13:54:54.576491+00:00</t>
+          <t>2025-10-27T16:01:51.248645+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-27T13:54:54.576505+00:00</t>
+          <t>2025-10-27T16:01:51.248662+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-27T13:54:56.703608+00:00</t>
+          <t>2025-10-27T16:01:53.298973+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-27T13:54:59.177773+00:00</t>
+          <t>2025-10-27T16:01:56.107801+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-27T13:54:59.177790+00:00</t>
+          <t>2025-10-27T16:01:56.107832+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:01.332931+00:00</t>
+          <t>2025-10-27T16:01:58.461119+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:01.332946+00:00</t>
+          <t>2025-10-27T16:01:58.461148+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:01.332954+00:00</t>
+          <t>2025-10-27T16:01:58.461165+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:01.332961+00:00</t>
+          <t>2025-10-27T16:01:58.461183+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:08.534704+00:00</t>
+          <t>2025-10-27T16:02:06.214093+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:10.626197+00:00</t>
+          <t>2025-10-27T16:02:08.531195+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:12.844001+00:00</t>
+          <t>2025-10-27T16:02:10.872977+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:15.420348+00:00</t>
+          <t>2025-10-27T16:02:13.251352+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:15.420364+00:00</t>
+          <t>2025-10-27T16:02:13.251381+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:18.125208+00:00</t>
+          <t>2025-10-27T16:02:15.767660+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:18.125223+00:00</t>
+          <t>2025-10-27T16:02:15.767693+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:18.125232+00:00</t>
+          <t>2025-10-27T16:02:15.767712+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:18.125240+00:00</t>
+          <t>2025-10-27T16:02:15.767729+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:18.125248+00:00</t>
+          <t>2025-10-27T16:02:15.767746+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:20.678743+00:00</t>
+          <t>2025-10-27T16:02:18.136923+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:25.449571+00:00</t>
+          <t>2025-10-27T16:02:22.915619+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:25.449585+00:00</t>
+          <t>2025-10-27T16:02:22.915647+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:25.449593+00:00</t>
+          <t>2025-10-27T16:02:22.915666+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:25.449600+00:00</t>
+          <t>2025-10-27T16:02:22.915683+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:27.573273+00:00</t>
+          <t>2025-10-27T16:02:25.247979+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:27.573291+00:00</t>
+          <t>2025-10-27T16:02:25.248008+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:29.674791+00:00</t>
+          <t>2025-10-27T16:02:27.611081+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:29.674807+00:00</t>
+          <t>2025-10-27T16:02:27.611113+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:29.674814+00:00</t>
+          <t>2025-10-27T16:02:27.611132+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:29.674821+00:00</t>
+          <t>2025-10-27T16:02:27.611149+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:29.674828+00:00</t>
+          <t>2025-10-27T16:02:27.611167+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:29.674836+00:00</t>
+          <t>2025-10-27T16:02:27.611184+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:29.674843+00:00</t>
+          <t>2025-10-27T16:02:27.611204+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:29.674850+00:00</t>
+          <t>2025-10-27T16:02:27.611222+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:29.674857+00:00</t>
+          <t>2025-10-27T16:02:27.611237+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:32.291435+00:00</t>
+          <t>2025-10-27T16:02:30.478161+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:32.291449+00:00</t>
+          <t>2025-10-27T16:02:30.478189+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:36.573911+00:00</t>
+          <t>2025-10-27T16:02:35.778418+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:38.701074+00:00</t>
+          <t>2025-10-27T16:02:38.116630+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:38.701114+00:00</t>
+          <t>2025-10-27T16:02:38.116659+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:38.701121+00:00</t>
+          <t>2025-10-27T16:02:38.116676+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-10-27T13:55:38.701128+00:00</t>
+          <t>2025-10-27T16:02:38.116692+00:00</t>
         </is>
       </c>
     </row>
@@ -3295,7 +3295,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3340,43 +3340,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>СПР</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Спартак</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Воробьёв Иван В</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_СПР_воробьевиванв</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-10-27T21:55:39.207982+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-10-27</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
runtime update (2025-10-28 00:27:33)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:47.137976+00:00</t>
+          <t>2025-10-27T16:21:29.502651+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:49.181182+00:00</t>
+          <t>2025-10-27T16:21:31.587520+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:49.181200+00:00</t>
+          <t>2025-10-27T16:21:31.587540+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:49.181210+00:00</t>
+          <t>2025-10-27T16:21:31.587550+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:49.181217+00:00</t>
+          <t>2025-10-27T16:21:31.587558+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:49.181225+00:00</t>
+          <t>2025-10-27T16:21:31.587566+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:51.248645+00:00</t>
+          <t>2025-10-27T16:21:33.679237+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:51.248662+00:00</t>
+          <t>2025-10-27T16:21:33.679255+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:53.298973+00:00</t>
+          <t>2025-10-27T16:21:35.685236+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:56.107801+00:00</t>
+          <t>2025-10-27T16:21:38.537677+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:56.107832+00:00</t>
+          <t>2025-10-27T16:21:38.537693+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:58.461119+00:00</t>
+          <t>2025-10-27T16:21:40.700179+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:58.461148+00:00</t>
+          <t>2025-10-27T16:21:40.700196+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:58.461165+00:00</t>
+          <t>2025-10-27T16:21:40.700204+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-27T16:01:58.461183+00:00</t>
+          <t>2025-10-27T16:21:40.700212+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:06.214093+00:00</t>
+          <t>2025-10-27T16:21:47.143774+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:08.531195+00:00</t>
+          <t>2025-10-27T16:21:49.185950+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:10.872977+00:00</t>
+          <t>2025-10-27T16:21:51.176975+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:13.251352+00:00</t>
+          <t>2025-10-27T16:21:53.231308+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:13.251381+00:00</t>
+          <t>2025-10-27T16:21:53.231327+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:15.767660+00:00</t>
+          <t>2025-10-27T16:21:55.667200+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:15.767693+00:00</t>
+          <t>2025-10-27T16:21:55.667226+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:15.767712+00:00</t>
+          <t>2025-10-27T16:21:55.667234+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:15.767729+00:00</t>
+          <t>2025-10-27T16:21:55.667241+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:15.767746+00:00</t>
+          <t>2025-10-27T16:21:55.667249+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:18.136923+00:00</t>
+          <t>2025-10-27T16:21:58.082418+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:22.915619+00:00</t>
+          <t>2025-10-27T16:22:02.551092+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:22.915647+00:00</t>
+          <t>2025-10-27T16:22:02.551110+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:22.915666+00:00</t>
+          <t>2025-10-27T16:22:02.551117+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:22.915683+00:00</t>
+          <t>2025-10-27T16:22:02.551125+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:25.247979+00:00</t>
+          <t>2025-10-27T16:22:04.585314+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:25.248008+00:00</t>
+          <t>2025-10-27T16:22:04.585331+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:27.611081+00:00</t>
+          <t>2025-10-27T16:22:06.506160+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:27.611113+00:00</t>
+          <t>2025-10-27T16:22:06.506177+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:27.611132+00:00</t>
+          <t>2025-10-27T16:22:06.506184+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:27.611149+00:00</t>
+          <t>2025-10-27T16:22:06.506191+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:27.611167+00:00</t>
+          <t>2025-10-27T16:22:06.506198+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:27.611184+00:00</t>
+          <t>2025-10-27T16:22:06.506206+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:27.611204+00:00</t>
+          <t>2025-10-27T16:22:06.506213+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:27.611222+00:00</t>
+          <t>2025-10-27T16:22:06.506220+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:27.611237+00:00</t>
+          <t>2025-10-27T16:22:06.506226+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:30.478161+00:00</t>
+          <t>2025-10-27T16:22:08.584087+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:30.478189+00:00</t>
+          <t>2025-10-27T16:22:08.584104+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:35.778418+00:00</t>
+          <t>2025-10-27T16:22:13.103979+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:38.116630+00:00</t>
+          <t>2025-10-27T16:22:15.101542+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:38.116659+00:00</t>
+          <t>2025-10-27T16:22:15.101559+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:38.116676+00:00</t>
+          <t>2025-10-27T16:22:15.101567+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-10-27T16:02:38.116692+00:00</t>
+          <t>2025-10-27T16:22:15.101574+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
runtime update (2025-10-28 01:40:06)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:29.502651+00:00</t>
+          <t>2025-10-27T17:33:38.569685+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:31.587520+00:00</t>
+          <t>2025-10-27T17:33:41.097216+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:31.587540+00:00</t>
+          <t>2025-10-27T17:33:41.097234+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:31.587550+00:00</t>
+          <t>2025-10-27T17:33:41.097242+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:31.587558+00:00</t>
+          <t>2025-10-27T17:33:41.097250+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:31.587566+00:00</t>
+          <t>2025-10-27T17:33:41.097258+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:33.679237+00:00</t>
+          <t>2025-10-27T17:33:43.089918+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:33.679255+00:00</t>
+          <t>2025-10-27T17:33:43.089934+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:35.685236+00:00</t>
+          <t>2025-10-27T17:33:45.609861+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:38.537677+00:00</t>
+          <t>2025-10-27T17:33:47.587329+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:38.537693+00:00</t>
+          <t>2025-10-27T17:33:47.587345+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:40.700179+00:00</t>
+          <t>2025-10-27T17:33:49.710467+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:40.700196+00:00</t>
+          <t>2025-10-27T17:33:49.710483+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:40.700204+00:00</t>
+          <t>2025-10-27T17:33:49.710490+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:40.700212+00:00</t>
+          <t>2025-10-27T17:33:49.710497+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:47.143774+00:00</t>
+          <t>2025-10-27T17:33:56.981246+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:49.185950+00:00</t>
+          <t>2025-10-27T17:33:59.438920+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:51.176975+00:00</t>
+          <t>2025-10-27T17:34:01.924318+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:53.231308+00:00</t>
+          <t>2025-10-27T17:34:03.921896+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:53.231327+00:00</t>
+          <t>2025-10-27T17:34:03.921914+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:55.667200+00:00</t>
+          <t>2025-10-27T17:34:06.356864+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:55.667226+00:00</t>
+          <t>2025-10-27T17:34:06.356881+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:55.667234+00:00</t>
+          <t>2025-10-27T17:34:06.356888+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:55.667241+00:00</t>
+          <t>2025-10-27T17:34:06.356895+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:55.667249+00:00</t>
+          <t>2025-10-27T17:34:06.356902+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-27T16:21:58.082418+00:00</t>
+          <t>2025-10-27T17:34:08.853921+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:02.551092+00:00</t>
+          <t>2025-10-27T17:34:13.305781+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:02.551110+00:00</t>
+          <t>2025-10-27T17:34:13.305799+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:02.551117+00:00</t>
+          <t>2025-10-27T17:34:13.305808+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:02.551125+00:00</t>
+          <t>2025-10-27T17:34:13.305815+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:04.585314+00:00</t>
+          <t>2025-10-27T17:34:15.271455+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:04.585331+00:00</t>
+          <t>2025-10-27T17:34:15.271472+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:06.506160+00:00</t>
+          <t>2025-10-27T17:34:17.256009+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:06.506177+00:00</t>
+          <t>2025-10-27T17:34:17.256028+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:06.506184+00:00</t>
+          <t>2025-10-27T17:34:17.256036+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:06.506191+00:00</t>
+          <t>2025-10-27T17:34:17.256043+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:06.506198+00:00</t>
+          <t>2025-10-27T17:34:17.256050+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:06.506206+00:00</t>
+          <t>2025-10-27T17:34:17.256057+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:06.506213+00:00</t>
+          <t>2025-10-27T17:34:17.256064+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:06.506220+00:00</t>
+          <t>2025-10-27T17:34:17.256071+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:06.506226+00:00</t>
+          <t>2025-10-27T17:34:17.256078+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:08.584087+00:00</t>
+          <t>2025-10-27T17:34:19.263200+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:08.584104+00:00</t>
+          <t>2025-10-27T17:34:19.263219+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:13.103979+00:00</t>
+          <t>2025-10-27T17:34:23.293443+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:15.101542+00:00</t>
+          <t>2025-10-27T17:34:25.274086+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:15.101559+00:00</t>
+          <t>2025-10-27T17:34:25.274103+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:15.101567+00:00</t>
+          <t>2025-10-27T17:34:25.274111+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-10-27T16:22:15.101574+00:00</t>
+          <t>2025-10-27T17:34:25.274118+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
runtime update (2025-10-28 11:08:25)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:38.569685+00:00</t>
+          <t>2025-10-28T03:01:35.696706+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:41.097216+00:00</t>
+          <t>2025-10-28T03:01:38.406631+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:41.097234+00:00</t>
+          <t>2025-10-28T03:01:38.406661+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:41.097242+00:00</t>
+          <t>2025-10-28T03:01:38.406680+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:41.097250+00:00</t>
+          <t>2025-10-28T03:01:38.406698+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:41.097258+00:00</t>
+          <t>2025-10-28T03:01:38.406714+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:43.089918+00:00</t>
+          <t>2025-10-28T03:01:40.783084+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:43.089934+00:00</t>
+          <t>2025-10-28T03:01:40.783117+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:45.609861+00:00</t>
+          <t>2025-10-28T03:01:43.497716+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:47.587329+00:00</t>
+          <t>2025-10-28T03:01:45.862860+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:47.587345+00:00</t>
+          <t>2025-10-28T03:01:45.862890+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:49.710467+00:00</t>
+          <t>2025-10-28T03:01:48.695365+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:49.710483+00:00</t>
+          <t>2025-10-28T03:01:48.695393+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:49.710490+00:00</t>
+          <t>2025-10-28T03:01:48.695411+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:49.710497+00:00</t>
+          <t>2025-10-28T03:01:48.695427+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:56.981246+00:00</t>
+          <t>2025-10-28T03:01:56.921274+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-27T17:33:59.438920+00:00</t>
+          <t>2025-10-28T03:01:59.722973+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:01.924318+00:00</t>
+          <t>2025-10-28T03:02:02.097136+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:03.921896+00:00</t>
+          <t>2025-10-28T03:02:04.388043+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:03.921914+00:00</t>
+          <t>2025-10-28T03:02:04.388071+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:06.356864+00:00</t>
+          <t>2025-10-28T03:02:07.165817+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:06.356881+00:00</t>
+          <t>2025-10-28T03:02:07.165847+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:06.356888+00:00</t>
+          <t>2025-10-28T03:02:07.165865+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:06.356895+00:00</t>
+          <t>2025-10-28T03:02:07.165881+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:06.356902+00:00</t>
+          <t>2025-10-28T03:02:07.165897+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:08.853921+00:00</t>
+          <t>2025-10-28T03:02:09.518310+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:13.305781+00:00</t>
+          <t>2025-10-28T03:02:14.603208+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:13.305799+00:00</t>
+          <t>2025-10-28T03:02:14.603239+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:13.305808+00:00</t>
+          <t>2025-10-28T03:02:14.603257+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:13.305815+00:00</t>
+          <t>2025-10-28T03:02:14.603274+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:15.271455+00:00</t>
+          <t>2025-10-28T03:02:17.388868+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:15.271472+00:00</t>
+          <t>2025-10-28T03:02:17.388899+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:17.256009+00:00</t>
+          <t>2025-10-28T03:02:19.724444+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:17.256028+00:00</t>
+          <t>2025-10-28T03:02:19.724472+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:17.256036+00:00</t>
+          <t>2025-10-28T03:02:19.724492+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:17.256043+00:00</t>
+          <t>2025-10-28T03:02:19.724508+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:17.256050+00:00</t>
+          <t>2025-10-28T03:02:19.724524+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:17.256057+00:00</t>
+          <t>2025-10-28T03:02:19.724544+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:17.256064+00:00</t>
+          <t>2025-10-28T03:02:19.724560+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:17.256071+00:00</t>
+          <t>2025-10-28T03:02:19.724575+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:17.256078+00:00</t>
+          <t>2025-10-28T03:02:19.724589+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:19.263200+00:00</t>
+          <t>2025-10-28T03:02:22.062228+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:19.263219+00:00</t>
+          <t>2025-10-28T03:02:22.062257+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:23.293443+00:00</t>
+          <t>2025-10-28T03:02:27.534599+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:25.274086+00:00</t>
+          <t>2025-10-28T03:02:30.242140+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:25.274103+00:00</t>
+          <t>2025-10-28T03:02:30.242169+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:25.274111+00:00</t>
+          <t>2025-10-28T03:02:30.242185+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-10-27T17:34:25.274118+00:00</t>
+          <t>2025-10-28T03:02:30.242204+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
runtime update (2025-10-28 15:09:46)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:35.696706+00:00</t>
+          <t>2025-10-28T07:02:58.814490+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:38.406631+00:00</t>
+          <t>2025-10-28T07:03:01.138963+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:38.406661+00:00</t>
+          <t>2025-10-28T07:03:01.138992+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:38.406680+00:00</t>
+          <t>2025-10-28T07:03:01.139011+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:38.406698+00:00</t>
+          <t>2025-10-28T07:03:01.139028+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:38.406714+00:00</t>
+          <t>2025-10-28T07:03:01.139044+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:40.783084+00:00</t>
+          <t>2025-10-28T07:03:03.978942+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:40.783117+00:00</t>
+          <t>2025-10-28T07:03:03.978970+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:43.497716+00:00</t>
+          <t>2025-10-28T07:03:06.720279+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:45.862860+00:00</t>
+          <t>2025-10-28T07:03:09.038582+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:45.862890+00:00</t>
+          <t>2025-10-28T07:03:09.038609+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:48.695365+00:00</t>
+          <t>2025-10-28T07:03:11.373338+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:48.695393+00:00</t>
+          <t>2025-10-28T07:03:11.373366+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:48.695411+00:00</t>
+          <t>2025-10-28T07:03:11.373384+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:48.695427+00:00</t>
+          <t>2025-10-28T07:03:11.373401+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:56.921274+00:00</t>
+          <t>2025-10-28T07:03:19.695236+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-28T03:01:59.722973+00:00</t>
+          <t>2025-10-28T07:03:22.512244+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:02.097136+00:00</t>
+          <t>2025-10-28T07:03:25.538223+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:04.388043+00:00</t>
+          <t>2025-10-28T07:03:28.375744+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:04.388071+00:00</t>
+          <t>2025-10-28T07:03:28.375773+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:07.165817+00:00</t>
+          <t>2025-10-28T07:03:30.712171+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:07.165847+00:00</t>
+          <t>2025-10-28T07:03:30.712199+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:07.165865+00:00</t>
+          <t>2025-10-28T07:03:30.712216+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:07.165881+00:00</t>
+          <t>2025-10-28T07:03:30.712232+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:07.165897+00:00</t>
+          <t>2025-10-28T07:03:30.712248+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:09.518310+00:00</t>
+          <t>2025-10-28T07:03:33.402475+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:14.603208+00:00</t>
+          <t>2025-10-28T07:03:38.413015+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:14.603239+00:00</t>
+          <t>2025-10-28T07:03:38.413042+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:14.603257+00:00</t>
+          <t>2025-10-28T07:03:38.413061+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:14.603274+00:00</t>
+          <t>2025-10-28T07:03:38.413077+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:17.388868+00:00</t>
+          <t>2025-10-28T07:03:40.715210+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:17.388899+00:00</t>
+          <t>2025-10-28T07:03:40.715237+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:19.724444+00:00</t>
+          <t>2025-10-28T07:03:42.996572+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:19.724472+00:00</t>
+          <t>2025-10-28T07:03:42.996600+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:19.724492+00:00</t>
+          <t>2025-10-28T07:03:42.996617+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:19.724508+00:00</t>
+          <t>2025-10-28T07:03:42.996633+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:19.724524+00:00</t>
+          <t>2025-10-28T07:03:42.996649+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:19.724544+00:00</t>
+          <t>2025-10-28T07:03:42.996667+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:19.724560+00:00</t>
+          <t>2025-10-28T07:03:42.996682+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:19.724575+00:00</t>
+          <t>2025-10-28T07:03:42.996697+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:19.724589+00:00</t>
+          <t>2025-10-28T07:03:42.996711+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:22.062228+00:00</t>
+          <t>2025-10-28T07:03:45.358137+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:22.062257+00:00</t>
+          <t>2025-10-28T07:03:45.358166+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:27.534599+00:00</t>
+          <t>2025-10-28T07:03:49.880029+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:30.242140+00:00</t>
+          <t>2025-10-28T07:03:52.123924+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:30.242169+00:00</t>
+          <t>2025-10-28T07:03:52.123955+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:30.242185+00:00</t>
+          <t>2025-10-28T07:03:52.123973+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-10-28T03:02:30.242204+00:00</t>
+          <t>2025-10-28T07:03:52.123989+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
runtime update (2025-10-28 21:12:57)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-28T07:02:58.814490+00:00</t>
+          <t>2025-10-28T13:06:33.727615+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:01.138963+00:00</t>
+          <t>2025-10-28T13:06:35.795830+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:01.138992+00:00</t>
+          <t>2025-10-28T13:06:35.795847+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:01.139011+00:00</t>
+          <t>2025-10-28T13:06:35.795855+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:01.139028+00:00</t>
+          <t>2025-10-28T13:06:35.795863+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:01.139044+00:00</t>
+          <t>2025-10-28T13:06:35.795870+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:03.978942+00:00</t>
+          <t>2025-10-28T13:06:38.040824+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:03.978970+00:00</t>
+          <t>2025-10-28T13:06:38.040840+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:06.720279+00:00</t>
+          <t>2025-10-28T13:06:40.166925+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:09.038582+00:00</t>
+          <t>2025-10-28T13:06:42.930049+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:09.038609+00:00</t>
+          <t>2025-10-28T13:06:42.930078+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:11.373338+00:00</t>
+          <t>2025-10-28T13:06:45.947213+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:11.373366+00:00</t>
+          <t>2025-10-28T13:06:45.947242+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:11.373384+00:00</t>
+          <t>2025-10-28T13:06:45.947260+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:11.373401+00:00</t>
+          <t>2025-10-28T13:06:45.947278+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:19.695236+00:00</t>
+          <t>2025-10-28T13:06:53.916643+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:22.512244+00:00</t>
+          <t>2025-10-28T13:06:56.705517+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:25.538223+00:00</t>
+          <t>2025-10-28T13:06:59.022961+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:28.375744+00:00</t>
+          <t>2025-10-28T13:07:01.338159+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:28.375773+00:00</t>
+          <t>2025-10-28T13:07:01.338189+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:30.712171+00:00</t>
+          <t>2025-10-28T13:07:03.607644+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:30.712199+00:00</t>
+          <t>2025-10-28T13:07:03.607678+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:30.712216+00:00</t>
+          <t>2025-10-28T13:07:03.607696+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:30.712232+00:00</t>
+          <t>2025-10-28T13:07:03.607714+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:30.712248+00:00</t>
+          <t>2025-10-28T13:07:03.607731+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:33.402475+00:00</t>
+          <t>2025-10-28T13:07:05.982882+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:38.413015+00:00</t>
+          <t>2025-10-28T13:07:10.984358+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:38.413042+00:00</t>
+          <t>2025-10-28T13:07:10.984388+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:38.413061+00:00</t>
+          <t>2025-10-28T13:07:10.984407+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:38.413077+00:00</t>
+          <t>2025-10-28T13:07:10.984423+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:40.715210+00:00</t>
+          <t>2025-10-28T13:07:13.802919+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,34 +2312,34 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:40.715237+00:00</t>
+          <t>2025-10-28T13:07:13.802946+00:00</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2349,12 +2349,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2364,12 +2364,12 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:42.996572+00:00</t>
+          <t>2025-10-28T13:07:13.802963+00:00</t>
         </is>
       </c>
     </row>
@@ -2391,12 +2391,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2406,12 +2406,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:42.996600+00:00</t>
+          <t>2025-10-28T13:07:16.242499+00:00</t>
         </is>
       </c>
     </row>
@@ -2448,27 +2448,27 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:42.996617+00:00</t>
+          <t>2025-10-28T13:07:16.242527+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,27 +2505,27 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:42.996633+00:00</t>
+          <t>2025-10-28T13:07:16.242544+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,12 +2562,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Набиев Артём</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>41187</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_набиевартем</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:42.996649+00:00</t>
+          <t>2025-10-28T13:07:16.242559+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,12 +2619,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Пименов Артём</t>
+          <t>Набиев Артём</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>79</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2634,12 +2634,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>21205</t>
+          <t>41187</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_пименовартем</t>
+          <t>1369_СЮЛ_набиевартем</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:42.996667+00:00</t>
+          <t>2025-10-28T13:07:16.242577+00:00</t>
         </is>
       </c>
     </row>
@@ -2676,12 +2676,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Пименов Артём</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>68</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2691,12 +2691,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>21205</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_пименовартем</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:42.996682+00:00</t>
+          <t>2025-10-28T13:07:16.242592+00:00</t>
         </is>
       </c>
     </row>
@@ -2733,12 +2733,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Хохряков Пётр</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2748,12 +2748,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>15413</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хохряковпетр</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:42.996697+00:00</t>
+          <t>2025-10-28T13:07:16.242607+00:00</t>
         </is>
       </c>
     </row>
@@ -2790,12 +2790,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Хохряков Пётр</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2805,12 +2805,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>15413</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_СЮЛ_хохряковпетр</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2825,49 +2825,49 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:42.996711+00:00</t>
+          <t>2025-10-28T13:07:16.242621+00:00</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2877,12 +2877,12 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:45.358137+00:00</t>
+          <t>2025-10-28T13:07:16.242636+00:00</t>
         </is>
       </c>
     </row>
@@ -2904,27 +2904,27 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2939,34 +2939,34 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:45.358166+00:00</t>
+          <t>2025-10-28T13:07:18.675266+00:00</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2976,12 +2976,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2991,54 +2991,54 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:49.880029+00:00</t>
+          <t>2025-10-28T13:07:18.675293+00:00</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3048,12 +3048,12 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:52.123924+00:00</t>
+          <t>2025-10-28T13:07:23.522488+00:00</t>
         </is>
       </c>
     </row>
@@ -3075,27 +3075,27 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Попугаев Никита А</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>22684</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>1369_ШДР_попугаевникитаа</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:52.123955+00:00</t>
+          <t>2025-10-28T13:07:25.897226+00:00</t>
         </is>
       </c>
     </row>
@@ -3132,12 +3132,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Саттер Райли</t>
+          <t>Попугаев Никита А</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -3147,12 +3147,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>45491</t>
+          <t>22684</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1369_ШДР_саттеррайли</t>
+          <t>1369_ШДР_попугаевникитаа</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-28T07:03:52.123973+00:00</t>
+          <t>2025-10-28T13:07:25.897256+00:00</t>
         </is>
       </c>
     </row>
@@ -3189,42 +3189,99 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
+          <t>Саттер Райли</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>45491</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>1369_ШДР_саттеррайли</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>2025-10-28T13:07:25.897274+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
           <t>Фу Спенсер</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="F50" t="inlineStr">
         <is>
           <t>нападающий</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="G50" t="inlineStr">
         <is>
           <t>34934</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr">
+      <c r="H50" t="inlineStr">
         <is>
           <t>1369_ШДР_фуспенсер</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
         <is>
           <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>2025-10-28T07:03:52.123989+00:00</t>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>2025-10-28T13:07:25.897291+00:00</t>
         </is>
       </c>
     </row>
@@ -3295,7 +3352,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3340,6 +3397,43 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>СПР</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Спартак</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Рубцов Герман</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_СПР_рубцовгерман</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-10-28T21:07:26.410868+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-10-28</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
runtime update (2025-10-29 15:08:10)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:33.727615+00:00</t>
+          <t>2025-10-29T07:01:45.823026+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:35.795830+00:00</t>
+          <t>2025-10-29T07:01:48.522227+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:35.795847+00:00</t>
+          <t>2025-10-29T07:01:48.522259+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:35.795855+00:00</t>
+          <t>2025-10-29T07:01:48.522279+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:35.795863+00:00</t>
+          <t>2025-10-29T07:01:48.522298+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:35.795870+00:00</t>
+          <t>2025-10-29T07:01:48.522315+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:38.040824+00:00</t>
+          <t>2025-10-29T07:01:51.192646+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:38.040840+00:00</t>
+          <t>2025-10-29T07:01:51.192678+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:40.166925+00:00</t>
+          <t>2025-10-29T07:01:53.355958+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:42.930049+00:00</t>
+          <t>2025-10-29T07:01:55.488430+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:42.930078+00:00</t>
+          <t>2025-10-29T07:01:55.488459+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:45.947213+00:00</t>
+          <t>2025-10-29T07:01:57.743348+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:45.947242+00:00</t>
+          <t>2025-10-29T07:01:57.743378+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:45.947260+00:00</t>
+          <t>2025-10-29T07:01:57.743396+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:45.947278+00:00</t>
+          <t>2025-10-29T07:01:57.743414+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:53.916643+00:00</t>
+          <t>2025-10-29T07:02:05.714970+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:56.705517+00:00</t>
+          <t>2025-10-29T07:02:07.979092+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-28T13:06:59.022961+00:00</t>
+          <t>2025-10-29T07:02:10.197347+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:01.338159+00:00</t>
+          <t>2025-10-29T07:02:12.909016+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,34 +1628,34 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:01.338189+00:00</t>
+          <t>2025-10-29T07:02:12.909048+00:00</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Ващенко Григорий</t>
+          <t>Профака Лука</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1665,12 +1665,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>14155</t>
+          <t>43943</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СЕВ_ващенкогригорий</t>
+          <t>1369_НХК_профакалука</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1680,12 +1680,12 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:03.607644+00:00</t>
+          <t>2025-10-29T07:02:12.909066+00:00</t>
         </is>
       </c>
     </row>
@@ -1707,12 +1707,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Грудинин Владимир</t>
+          <t>Ващенко Григорий</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1722,12 +1722,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>35064</t>
+          <t>14155</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СЕВ_грудининвладимир</t>
+          <t>1369_СЕВ_ващенкогригорий</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:03.607678+00:00</t>
+          <t>2025-10-29T07:02:15.324653+00:00</t>
         </is>
       </c>
     </row>
@@ -1764,27 +1764,27 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Лишка Адам</t>
+          <t>Грудинин Владимир</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>25514</t>
+          <t>35064</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СЕВ_лишкаадам</t>
+          <t>1369_СЕВ_грудининвладимир</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:03.607696+00:00</t>
+          <t>2025-10-29T07:02:15.324680+00:00</t>
         </is>
       </c>
     </row>
@@ -1821,12 +1821,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Танков Кирилл</t>
+          <t>Лишка Адам</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1836,12 +1836,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>32981</t>
+          <t>25514</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СЕВ_танковкирилл</t>
+          <t>1369_СЕВ_лишкаадам</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:03.607714+00:00</t>
+          <t>2025-10-29T07:02:15.324697+00:00</t>
         </is>
       </c>
     </row>
@@ -1878,12 +1878,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Танков Кирилл</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>32981</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СЕВ_танковкирилл</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1913,49 +1913,49 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:03.607731+00:00</t>
+          <t>2025-10-29T07:02:15.324712+00:00</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Фарранс Дэвид</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>45062</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СИБ_фаррансдэвид</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1965,54 +1965,54 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:05.982882+00:00</t>
+          <t>2025-10-29T07:02:15.324728+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Гараев Амир</t>
+          <t>Фарранс Дэвид</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>28624</t>
+          <t>45062</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гараевамир</t>
+          <t>1369_СИБ_фаррансдэвид</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,12 +2022,12 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:10.984358+00:00</t>
+          <t>2025-10-29T07:02:17.791427+00:00</t>
         </is>
       </c>
     </row>
@@ -2049,27 +2049,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Гараев Амир</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>67</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>28624</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СОЧ_гараевамир</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:10.984388+00:00</t>
+          <t>2025-10-29T07:02:22.757749+00:00</t>
         </is>
       </c>
     </row>
@@ -2106,27 +2106,27 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Уткин Дмитрий А</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>35195</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СОЧ_уткиндмитрийа</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:10.984407+00:00</t>
+          <t>2025-10-29T07:02:22.757777+00:00</t>
         </is>
       </c>
     </row>
@@ -2163,27 +2163,27 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Уткин Дмитрий А</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>35195</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СОЧ_уткиндмитрийа</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2198,49 +2198,49 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:10.984423+00:00</t>
+          <t>2025-10-29T07:02:22.757795+00:00</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2250,12 +2250,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:13.802919+00:00</t>
+          <t>2025-10-29T07:02:22.757811+00:00</t>
         </is>
       </c>
     </row>
@@ -2277,12 +2277,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2292,12 +2292,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:13.802946+00:00</t>
+          <t>2025-10-29T07:02:25.100333+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,12 +2334,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2349,12 +2349,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,34 +2369,34 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:13.802963+00:00</t>
+          <t>2025-10-29T07:02:25.100362+00:00</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2406,12 +2406,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2421,12 +2421,12 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:16.242499+00:00</t>
+          <t>2025-10-29T07:02:25.100380+00:00</t>
         </is>
       </c>
     </row>
@@ -2448,12 +2448,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2463,12 +2463,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:16.242527+00:00</t>
+          <t>2025-10-29T07:02:27.483134+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,27 +2505,27 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:16.242544+00:00</t>
+          <t>2025-10-29T07:02:27.483161+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,27 +2562,27 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:16.242559+00:00</t>
+          <t>2025-10-29T07:02:27.483178+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,12 +2619,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Набиев Артём</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2634,12 +2634,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>41187</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_набиевартем</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:16.242577+00:00</t>
+          <t>2025-10-29T07:02:27.483193+00:00</t>
         </is>
       </c>
     </row>
@@ -2676,12 +2676,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Пименов Артём</t>
+          <t>Набиев Артём</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>79</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2691,12 +2691,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>21205</t>
+          <t>41187</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_пименовартем</t>
+          <t>1369_СЮЛ_набиевартем</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:16.242592+00:00</t>
+          <t>2025-10-29T07:02:27.483208+00:00</t>
         </is>
       </c>
     </row>
@@ -2733,12 +2733,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Пименов Артём</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>68</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2748,12 +2748,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>21205</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_пименовартем</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:16.242607+00:00</t>
+          <t>2025-10-29T07:02:27.483228+00:00</t>
         </is>
       </c>
     </row>
@@ -2790,12 +2790,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Хохряков Пётр</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2805,12 +2805,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>15413</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хохряковпетр</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:16.242621+00:00</t>
+          <t>2025-10-29T07:02:27.483243+00:00</t>
         </is>
       </c>
     </row>
@@ -2847,12 +2847,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Хохряков Пётр</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2862,12 +2862,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>15413</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_СЮЛ_хохряковпетр</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2882,49 +2882,49 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:16.242636+00:00</t>
+          <t>2025-10-29T07:02:27.483259+00:00</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2934,12 +2934,12 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:18.675266+00:00</t>
+          <t>2025-10-29T07:02:27.483273+00:00</t>
         </is>
       </c>
     </row>
@@ -2961,27 +2961,27 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2996,34 +2996,34 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:18.675293+00:00</t>
+          <t>2025-10-29T07:02:30.202990+00:00</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3033,12 +3033,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3048,54 +3048,54 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:23.522488+00:00</t>
+          <t>2025-10-29T07:02:30.203019+00:00</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -3105,12 +3105,12 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:25.897226+00:00</t>
+          <t>2025-10-29T07:02:35.342781+00:00</t>
         </is>
       </c>
     </row>
@@ -3132,27 +3132,27 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Попугаев Никита А</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>22684</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1369_ШДР_попугаевникитаа</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:25.897256+00:00</t>
+          <t>2025-10-29T07:02:38.047713+00:00</t>
         </is>
       </c>
     </row>
@@ -3189,12 +3189,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Саттер Райли</t>
+          <t>Попугаев Никита А</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -3204,12 +3204,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>45491</t>
+          <t>22684</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>1369_ШДР_саттеррайли</t>
+          <t>1369_ШДР_попугаевникитаа</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-10-28T13:07:25.897274+00:00</t>
+          <t>2025-10-29T07:02:38.047742+00:00</t>
         </is>
       </c>
     </row>
@@ -3246,42 +3246,99 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
+          <t>Саттер Райли</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>45491</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>1369_ШДР_саттеррайли</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>2025-10-29T07:02:38.047761+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
           <t>Фу Спенсер</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="F51" t="inlineStr">
         <is>
           <t>нападающий</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr">
+      <c r="G51" t="inlineStr">
         <is>
           <t>34934</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr">
+      <c r="H51" t="inlineStr">
         <is>
           <t>1369_ШДР_фуспенсер</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
         <is>
           <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>2025-10-28T13:07:25.897291+00:00</t>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>2025-10-29T07:02:38.047777+00:00</t>
         </is>
       </c>
     </row>
@@ -3400,22 +3457,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Профака Лука</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_НХК_профакалука</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -3425,12 +3482,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-10-28T21:07:26.410868+08:00</t>
+          <t>2025-10-29T15:02:38.553086+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
runtime update (2025-10-29 21:09:22)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:45.823026+00:00</t>
+          <t>2025-10-29T13:08:08.426764+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:48.522227+00:00</t>
+          <t>2025-10-29T13:08:10.467424+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:48.522259+00:00</t>
+          <t>2025-10-29T13:08:10.467441+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:48.522279+00:00</t>
+          <t>2025-10-29T13:08:10.467450+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:48.522298+00:00</t>
+          <t>2025-10-29T13:08:10.467458+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:48.522315+00:00</t>
+          <t>2025-10-29T13:08:10.467465+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:51.192646+00:00</t>
+          <t>2025-10-29T13:08:12.568705+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:51.192678+00:00</t>
+          <t>2025-10-29T13:08:12.568721+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:53.355958+00:00</t>
+          <t>2025-10-29T13:08:14.598217+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:55.488430+00:00</t>
+          <t>2025-10-29T13:08:16.577779+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:55.488459+00:00</t>
+          <t>2025-10-29T13:08:16.577795+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:57.743348+00:00</t>
+          <t>2025-10-29T13:08:18.800987+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:57.743378+00:00</t>
+          <t>2025-10-29T13:08:18.801002+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:57.743396+00:00</t>
+          <t>2025-10-29T13:08:18.801010+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-29T07:01:57.743414+00:00</t>
+          <t>2025-10-29T13:08:18.801017+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:05.714970+00:00</t>
+          <t>2025-10-29T13:08:24.982635+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:07.979092+00:00</t>
+          <t>2025-10-29T13:08:26.960682+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:10.197347+00:00</t>
+          <t>2025-10-29T13:08:29.006311+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:12.909016+00:00</t>
+          <t>2025-10-29T13:08:30.989093+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:12.909048+00:00</t>
+          <t>2025-10-29T13:08:30.989110+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:12.909066+00:00</t>
+          <t>2025-10-29T13:08:30.989118+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:15.324653+00:00</t>
+          <t>2025-10-29T13:08:33.448093+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:15.324680+00:00</t>
+          <t>2025-10-29T13:08:33.448109+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:15.324697+00:00</t>
+          <t>2025-10-29T13:08:33.448116+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:15.324712+00:00</t>
+          <t>2025-10-29T13:08:33.448123+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,49 +1970,49 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:15.324728+00:00</t>
+          <t>2025-10-29T13:08:33.448131+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Фарранс Дэвид</t>
+          <t>Гараев Амир</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>67</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>45062</t>
+          <t>28624</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СИБ_фаррансдэвид</t>
+          <t>1369_СОЧ_гараевамир</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,12 +2022,12 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:17.791427+00:00</t>
+          <t>2025-10-29T13:08:40.431219+00:00</t>
         </is>
       </c>
     </row>
@@ -2049,27 +2049,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Гараев Амир</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>28624</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гараевамир</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:22.757749+00:00</t>
+          <t>2025-10-29T13:08:40.431235+00:00</t>
         </is>
       </c>
     </row>
@@ -2106,27 +2106,27 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Уткин Дмитрий А</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>35195</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СОЧ_уткиндмитрийа</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:22.757777+00:00</t>
+          <t>2025-10-29T13:08:40.431243+00:00</t>
         </is>
       </c>
     </row>
@@ -2163,27 +2163,27 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Уткин Дмитрий А</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>35195</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СОЧ_уткиндмитрийа</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2198,49 +2198,49 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:22.757795+00:00</t>
+          <t>2025-10-29T13:08:40.431251+00:00</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2250,12 +2250,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:22.757811+00:00</t>
+          <t>2025-10-29T13:08:42.383583+00:00</t>
         </is>
       </c>
     </row>
@@ -2277,12 +2277,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2292,12 +2292,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:25.100333+00:00</t>
+          <t>2025-10-29T13:08:42.383600+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,12 +2334,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2349,12 +2349,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,34 +2369,34 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:25.100362+00:00</t>
+          <t>2025-10-29T13:08:42.383608+00:00</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2406,12 +2406,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2421,12 +2421,12 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:25.100380+00:00</t>
+          <t>2025-10-29T13:08:44.394858+00:00</t>
         </is>
       </c>
     </row>
@@ -2448,12 +2448,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2463,12 +2463,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:27.483134+00:00</t>
+          <t>2025-10-29T13:08:44.394877+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,27 +2505,27 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:27.483161+00:00</t>
+          <t>2025-10-29T13:08:44.394885+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,27 +2562,27 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:27.483178+00:00</t>
+          <t>2025-10-29T13:08:44.394892+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,12 +2619,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Набиев Артём</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>79</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2634,12 +2634,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>41187</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_набиевартем</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:27.483193+00:00</t>
+          <t>2025-10-29T13:08:44.394903+00:00</t>
         </is>
       </c>
     </row>
@@ -2676,12 +2676,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Набиев Артём</t>
+          <t>Пименов Артём</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>68</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2691,12 +2691,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>41187</t>
+          <t>21205</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_набиевартем</t>
+          <t>1369_СЮЛ_пименовартем</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:27.483208+00:00</t>
+          <t>2025-10-29T13:08:44.394910+00:00</t>
         </is>
       </c>
     </row>
@@ -2733,12 +2733,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Пименов Артём</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2748,12 +2748,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>21205</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_пименовартем</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:27.483228+00:00</t>
+          <t>2025-10-29T13:08:44.394919+00:00</t>
         </is>
       </c>
     </row>
@@ -2790,12 +2790,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Хохряков Пётр</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2805,12 +2805,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>15413</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_хохряковпетр</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:27.483243+00:00</t>
+          <t>2025-10-29T13:08:44.394927+00:00</t>
         </is>
       </c>
     </row>
@@ -2847,12 +2847,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Хохряков Пётр</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2862,12 +2862,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>15413</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хохряковпетр</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2882,49 +2882,49 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:27.483259+00:00</t>
+          <t>2025-10-29T13:08:44.394934+00:00</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2934,12 +2934,12 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:27.483273+00:00</t>
+          <t>2025-10-29T13:08:46.383149+00:00</t>
         </is>
       </c>
     </row>
@@ -2961,27 +2961,27 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2996,34 +2996,34 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:30.202990+00:00</t>
+          <t>2025-10-29T13:08:46.383167+00:00</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3033,12 +3033,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3048,54 +3048,54 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:30.203019+00:00</t>
+          <t>2025-10-29T13:08:50.456984+00:00</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -3105,12 +3105,12 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:35.342781+00:00</t>
+          <t>2025-10-29T13:08:52.858587+00:00</t>
         </is>
       </c>
     </row>
@@ -3132,27 +3132,27 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Попугаев Никита А</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>22684</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ШДР_попугаевникитаа</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:38.047713+00:00</t>
+          <t>2025-10-29T13:08:52.858603+00:00</t>
         </is>
       </c>
     </row>
@@ -3189,12 +3189,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Попугаев Никита А</t>
+          <t>Саттер Райли</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -3204,12 +3204,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>22684</t>
+          <t>45491</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>1369_ШДР_попугаевникитаа</t>
+          <t>1369_ШДР_саттеррайли</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:38.047742+00:00</t>
+          <t>2025-10-29T13:08:52.858610+00:00</t>
         </is>
       </c>
     </row>
@@ -3246,12 +3246,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Саттер Райли</t>
+          <t>Фу Спенсер</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -3261,12 +3261,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>45491</t>
+          <t>34934</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>1369_ШДР_саттеррайли</t>
+          <t>1369_ШДР_фуспенсер</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -3281,64 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-10-29T07:02:38.047761+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Фу Спенсер</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>34934</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>1369_ШДР_фуспенсер</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>2025-10-29T07:02:38.047777+00:00</t>
+          <t>2025-10-29T13:08:52.858617+00:00</t>
         </is>
       </c>
     </row>
@@ -3348,6 +3291,99 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>team_abbr</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>team_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>player_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>player_uid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>changed_at</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>changed_day</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>СИБ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Фарранс Дэвид</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_СИБ_фаррансдэвид</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-10-29T21:08:53.360093+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-10-29</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3401,97 +3437,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>team_abbr</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>team_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>player_name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>player_uid</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>changed_at</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>changed_day</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>НХК</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Нефтехимик</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Профака Лука</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_НХК_профакалука</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-10-29T15:02:38.553086+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-10-29</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
runtime update (2025-10-29 21:15:25)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:08.426764+00:00</t>
+          <t>2025-10-29T13:14:08.772524+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:10.467424+00:00</t>
+          <t>2025-10-29T13:14:11.387724+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:10.467441+00:00</t>
+          <t>2025-10-29T13:14:11.387741+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:10.467450+00:00</t>
+          <t>2025-10-29T13:14:11.387749+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:10.467458+00:00</t>
+          <t>2025-10-29T13:14:11.387757+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:10.467465+00:00</t>
+          <t>2025-10-29T13:14:11.387765+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:12.568705+00:00</t>
+          <t>2025-10-29T13:14:13.474366+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:12.568721+00:00</t>
+          <t>2025-10-29T13:14:13.474387+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:14.598217+00:00</t>
+          <t>2025-10-29T13:14:15.942585+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:16.577779+00:00</t>
+          <t>2025-10-29T13:14:18.408390+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:16.577795+00:00</t>
+          <t>2025-10-29T13:14:18.408406+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:18.800987+00:00</t>
+          <t>2025-10-29T13:14:20.502856+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:18.801002+00:00</t>
+          <t>2025-10-29T13:14:20.502872+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:18.801010+00:00</t>
+          <t>2025-10-29T13:14:20.502880+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:18.801017+00:00</t>
+          <t>2025-10-29T13:14:20.502887+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:24.982635+00:00</t>
+          <t>2025-10-29T13:14:27.107801+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:26.960682+00:00</t>
+          <t>2025-10-29T13:14:29.151993+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:29.006311+00:00</t>
+          <t>2025-10-29T13:14:31.281310+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:30.989093+00:00</t>
+          <t>2025-10-29T13:14:33.679217+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:30.989110+00:00</t>
+          <t>2025-10-29T13:14:33.679236+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:30.989118+00:00</t>
+          <t>2025-10-29T13:14:33.679244+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:33.448093+00:00</t>
+          <t>2025-10-29T13:14:35.717396+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:33.448109+00:00</t>
+          <t>2025-10-29T13:14:35.717412+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:33.448116+00:00</t>
+          <t>2025-10-29T13:14:35.717420+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:33.448123+00:00</t>
+          <t>2025-10-29T13:14:35.717427+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:33.448131+00:00</t>
+          <t>2025-10-29T13:14:35.717434+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:40.431219+00:00</t>
+          <t>2025-10-29T13:14:42.714248+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:40.431235+00:00</t>
+          <t>2025-10-29T13:14:42.714282+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:40.431243+00:00</t>
+          <t>2025-10-29T13:14:42.714302+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:40.431251+00:00</t>
+          <t>2025-10-29T13:14:42.714319+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:42.383583+00:00</t>
+          <t>2025-10-29T13:14:45.016888+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:42.383600+00:00</t>
+          <t>2025-10-29T13:14:45.016918+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:42.383608+00:00</t>
+          <t>2025-10-29T13:14:45.016936+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:44.394858+00:00</t>
+          <t>2025-10-29T13:14:47.420790+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:44.394877+00:00</t>
+          <t>2025-10-29T13:14:47.420816+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:44.394885+00:00</t>
+          <t>2025-10-29T13:14:47.420833+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:44.394892+00:00</t>
+          <t>2025-10-29T13:14:47.420848+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:44.394903+00:00</t>
+          <t>2025-10-29T13:14:47.420865+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:44.394910+00:00</t>
+          <t>2025-10-29T13:14:47.420880+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:44.394919+00:00</t>
+          <t>2025-10-29T13:14:47.420897+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:44.394927+00:00</t>
+          <t>2025-10-29T13:14:47.420912+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:44.394934+00:00</t>
+          <t>2025-10-29T13:14:47.420926+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:46.383149+00:00</t>
+          <t>2025-10-29T13:14:49.719519+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:46.383167+00:00</t>
+          <t>2025-10-29T13:14:49.719547+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:50.456984+00:00</t>
+          <t>2025-10-29T13:14:54.799374+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:52.858587+00:00</t>
+          <t>2025-10-29T13:14:57.509386+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:52.858603+00:00</t>
+          <t>2025-10-29T13:14:57.509414+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:52.858610+00:00</t>
+          <t>2025-10-29T13:14:57.509431+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-10-29T13:08:52.858617+00:00</t>
+          <t>2025-10-29T13:14:57.509447+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
runtime update (2025-10-30 11:03:20)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:08.772524+00:00</t>
+          <t>2025-10-30T03:01:40.962534+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:11.387724+00:00</t>
+          <t>2025-10-30T03:01:43.761920+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:11.387741+00:00</t>
+          <t>2025-10-30T03:01:43.761950+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:11.387749+00:00</t>
+          <t>2025-10-30T03:01:43.761969+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:11.387757+00:00</t>
+          <t>2025-10-30T03:01:43.761986+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:11.387765+00:00</t>
+          <t>2025-10-30T03:01:43.762002+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:13.474366+00:00</t>
+          <t>2025-10-30T03:01:46.084856+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:13.474387+00:00</t>
+          <t>2025-10-30T03:01:46.084884+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:15.942585+00:00</t>
+          <t>2025-10-30T03:01:48.843727+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:18.408390+00:00</t>
+          <t>2025-10-30T03:01:51.634871+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:18.408406+00:00</t>
+          <t>2025-10-30T03:01:51.634904+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:20.502856+00:00</t>
+          <t>2025-10-30T03:01:53.926844+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:20.502872+00:00</t>
+          <t>2025-10-30T03:01:53.926875+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:20.502880+00:00</t>
+          <t>2025-10-30T03:01:53.926891+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:20.502887+00:00</t>
+          <t>2025-10-30T03:01:53.926907+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:27.107801+00:00</t>
+          <t>2025-10-30T03:02:01.663220+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:29.151993+00:00</t>
+          <t>2025-10-30T03:02:04.428959+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:31.281310+00:00</t>
+          <t>2025-10-30T03:02:07.293863+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:33.679217+00:00</t>
+          <t>2025-10-30T03:02:10.076586+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:33.679236+00:00</t>
+          <t>2025-10-30T03:02:10.076625+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:33.679244+00:00</t>
+          <t>2025-10-30T03:02:10.076647+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:35.717396+00:00</t>
+          <t>2025-10-30T03:02:12.760114+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:35.717412+00:00</t>
+          <t>2025-10-30T03:02:12.760141+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:35.717420+00:00</t>
+          <t>2025-10-30T03:02:12.760158+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:35.717427+00:00</t>
+          <t>2025-10-30T03:02:12.760173+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:35.717434+00:00</t>
+          <t>2025-10-30T03:02:12.760189+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:42.714248+00:00</t>
+          <t>2025-10-30T03:02:20.817076+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:42.714282+00:00</t>
+          <t>2025-10-30T03:02:20.817114+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:42.714302+00:00</t>
+          <t>2025-10-30T03:02:20.817138+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:42.714319+00:00</t>
+          <t>2025-10-30T03:02:20.817159+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:45.016888+00:00</t>
+          <t>2025-10-30T03:02:23.436599+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:45.016918+00:00</t>
+          <t>2025-10-30T03:02:23.436627+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:45.016936+00:00</t>
+          <t>2025-10-30T03:02:23.436645+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:47.420790+00:00</t>
+          <t>2025-10-30T03:02:25.644733+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:47.420816+00:00</t>
+          <t>2025-10-30T03:02:25.644761+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:47.420833+00:00</t>
+          <t>2025-10-30T03:02:25.644778+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:47.420848+00:00</t>
+          <t>2025-10-30T03:02:25.644793+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:47.420865+00:00</t>
+          <t>2025-10-30T03:02:25.644808+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:47.420880+00:00</t>
+          <t>2025-10-30T03:02:25.644822+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:47.420897+00:00</t>
+          <t>2025-10-30T03:02:25.644837+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:47.420912+00:00</t>
+          <t>2025-10-30T03:02:25.644857+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:47.420926+00:00</t>
+          <t>2025-10-30T03:02:25.644871+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:49.719519+00:00</t>
+          <t>2025-10-30T03:02:28.430295+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:49.719547+00:00</t>
+          <t>2025-10-30T03:02:28.430372+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:54.799374+00:00</t>
+          <t>2025-10-30T03:02:33.979146+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:57.509386+00:00</t>
+          <t>2025-10-30T03:02:36.779689+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:57.509414+00:00</t>
+          <t>2025-10-30T03:02:36.779717+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:57.509431+00:00</t>
+          <t>2025-10-30T03:02:36.779734+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-10-29T13:14:57.509447+00:00</t>
+          <t>2025-10-30T03:02:36.779750+00:00</t>
         </is>
       </c>
     </row>
@@ -3296,7 +3296,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3338,43 +3338,6 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>changed_day</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>СИБ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Сибирь</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Фарранс Дэвид</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_СИБ_фаррансдэвид</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-10-29T21:08:53.360093+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-10-29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
runtime update (2025-10-30 11:39:31)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:40.962534+00:00</t>
+          <t>2025-10-30T03:38:27.802493+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:43.761920+00:00</t>
+          <t>2025-10-30T03:38:29.736682+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:43.761950+00:00</t>
+          <t>2025-10-30T03:38:29.736698+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:43.761969+00:00</t>
+          <t>2025-10-30T03:38:29.736707+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:43.761986+00:00</t>
+          <t>2025-10-30T03:38:29.736715+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:43.762002+00:00</t>
+          <t>2025-10-30T03:38:29.736722+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:46.084856+00:00</t>
+          <t>2025-10-30T03:38:31.706255+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:46.084884+00:00</t>
+          <t>2025-10-30T03:38:31.706271+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:48.843727+00:00</t>
+          <t>2025-10-30T03:38:33.678259+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:51.634871+00:00</t>
+          <t>2025-10-30T03:38:35.653629+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:51.634904+00:00</t>
+          <t>2025-10-30T03:38:35.653645+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:53.926844+00:00</t>
+          <t>2025-10-30T03:38:38.110253+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:53.926875+00:00</t>
+          <t>2025-10-30T03:38:38.110269+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:53.926891+00:00</t>
+          <t>2025-10-30T03:38:38.110276+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-30T03:01:53.926907+00:00</t>
+          <t>2025-10-30T03:38:38.110284+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:01.663220+00:00</t>
+          <t>2025-10-30T03:38:45.519642+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:04.428959+00:00</t>
+          <t>2025-10-30T03:38:47.573574+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:07.293863+00:00</t>
+          <t>2025-10-30T03:38:49.522526+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:10.076586+00:00</t>
+          <t>2025-10-30T03:38:51.937235+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:10.076625+00:00</t>
+          <t>2025-10-30T03:38:51.937251+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:10.076647+00:00</t>
+          <t>2025-10-30T03:38:51.937259+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:12.760114+00:00</t>
+          <t>2025-10-30T03:38:54.307093+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:12.760141+00:00</t>
+          <t>2025-10-30T03:38:54.307109+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:12.760158+00:00</t>
+          <t>2025-10-30T03:38:54.307116+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:12.760173+00:00</t>
+          <t>2025-10-30T03:38:54.307124+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:12.760189+00:00</t>
+          <t>2025-10-30T03:38:54.307131+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:20.817076+00:00</t>
+          <t>2025-10-30T03:39:01.507967+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:20.817114+00:00</t>
+          <t>2025-10-30T03:39:01.507984+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:20.817138+00:00</t>
+          <t>2025-10-30T03:39:01.507993+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:20.817159+00:00</t>
+          <t>2025-10-30T03:39:01.508001+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:23.436599+00:00</t>
+          <t>2025-10-30T03:39:03.978508+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:23.436627+00:00</t>
+          <t>2025-10-30T03:39:03.978525+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:23.436645+00:00</t>
+          <t>2025-10-30T03:39:03.978532+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:25.644733+00:00</t>
+          <t>2025-10-30T03:39:06.146788+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:25.644761+00:00</t>
+          <t>2025-10-30T03:39:06.146806+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:25.644778+00:00</t>
+          <t>2025-10-30T03:39:06.146813+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:25.644793+00:00</t>
+          <t>2025-10-30T03:39:06.146820+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:25.644808+00:00</t>
+          <t>2025-10-30T03:39:06.146827+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:25.644822+00:00</t>
+          <t>2025-10-30T03:39:06.146833+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:25.644837+00:00</t>
+          <t>2025-10-30T03:39:06.146840+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:25.644857+00:00</t>
+          <t>2025-10-30T03:39:06.146850+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:25.644871+00:00</t>
+          <t>2025-10-30T03:39:06.146856+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:28.430295+00:00</t>
+          <t>2025-10-30T03:39:08.154979+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:28.430372+00:00</t>
+          <t>2025-10-30T03:39:08.154995+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:33.979146+00:00</t>
+          <t>2025-10-30T03:39:12.579182+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:36.779689+00:00</t>
+          <t>2025-10-30T03:39:14.567908+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:36.779717+00:00</t>
+          <t>2025-10-30T03:39:14.567923+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:36.779734+00:00</t>
+          <t>2025-10-30T03:39:14.567931+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-10-30T03:02:36.779750+00:00</t>
+          <t>2025-10-30T03:39:14.567937+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-10-30 12:27:33)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:27.802493+00:00</t>
+          <t>2025-10-30T04:26:24.051260+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:29.736682+00:00</t>
+          <t>2025-10-30T04:26:26.082601+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:29.736698+00:00</t>
+          <t>2025-10-30T04:26:26.082617+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:29.736707+00:00</t>
+          <t>2025-10-30T04:26:26.082625+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:29.736715+00:00</t>
+          <t>2025-10-30T04:26:26.082633+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:29.736722+00:00</t>
+          <t>2025-10-30T04:26:26.082640+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:31.706255+00:00</t>
+          <t>2025-10-30T04:26:28.007987+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:31.706271+00:00</t>
+          <t>2025-10-30T04:26:28.008019+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:33.678259+00:00</t>
+          <t>2025-10-30T04:26:30.035558+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:35.653629+00:00</t>
+          <t>2025-10-30T04:26:32.770902+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:35.653645+00:00</t>
+          <t>2025-10-30T04:26:32.770931+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:38.110253+00:00</t>
+          <t>2025-10-30T04:26:35.098490+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:38.110269+00:00</t>
+          <t>2025-10-30T04:26:35.098518+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:38.110276+00:00</t>
+          <t>2025-10-30T04:26:35.098536+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:38.110284+00:00</t>
+          <t>2025-10-30T04:26:35.098552+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:45.519642+00:00</t>
+          <t>2025-10-30T04:26:43.201049+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:47.573574+00:00</t>
+          <t>2025-10-30T04:26:45.956182+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:49.522526+00:00</t>
+          <t>2025-10-30T04:26:48.261303+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:51.937235+00:00</t>
+          <t>2025-10-30T04:26:50.985374+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:51.937251+00:00</t>
+          <t>2025-10-30T04:26:50.985406+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:51.937259+00:00</t>
+          <t>2025-10-30T04:26:50.985424+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:54.307093+00:00</t>
+          <t>2025-10-30T04:26:53.331844+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:54.307109+00:00</t>
+          <t>2025-10-30T04:26:53.331880+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:54.307116+00:00</t>
+          <t>2025-10-30T04:26:53.331900+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:54.307124+00:00</t>
+          <t>2025-10-30T04:26:53.331918+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-30T03:38:54.307131+00:00</t>
+          <t>2025-10-30T04:26:53.331937+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:01.507967+00:00</t>
+          <t>2025-10-30T04:27:00.303160+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:01.507984+00:00</t>
+          <t>2025-10-30T04:27:00.303190+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:01.507993+00:00</t>
+          <t>2025-10-30T04:27:00.303209+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:01.508001+00:00</t>
+          <t>2025-10-30T04:27:00.303227+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:03.978508+00:00</t>
+          <t>2025-10-30T04:27:03.114542+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:03.978525+00:00</t>
+          <t>2025-10-30T04:27:03.114573+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:03.978532+00:00</t>
+          <t>2025-10-30T04:27:03.114592+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:06.146788+00:00</t>
+          <t>2025-10-30T04:27:05.491739+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:06.146806+00:00</t>
+          <t>2025-10-30T04:27:05.491769+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:06.146813+00:00</t>
+          <t>2025-10-30T04:27:05.491788+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:06.146820+00:00</t>
+          <t>2025-10-30T04:27:05.491805+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:06.146827+00:00</t>
+          <t>2025-10-30T04:27:05.491822+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:06.146833+00:00</t>
+          <t>2025-10-30T04:27:05.491838+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:06.146840+00:00</t>
+          <t>2025-10-30T04:27:05.491855+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:06.146850+00:00</t>
+          <t>2025-10-30T04:27:05.491875+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:06.146856+00:00</t>
+          <t>2025-10-30T04:27:05.491891+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:08.154979+00:00</t>
+          <t>2025-10-30T04:27:07.764916+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:08.154995+00:00</t>
+          <t>2025-10-30T04:27:07.764946+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:12.579182+00:00</t>
+          <t>2025-10-30T04:27:12.799825+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:14.567908+00:00</t>
+          <t>2025-10-30T04:27:15.472434+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:14.567923+00:00</t>
+          <t>2025-10-30T04:27:15.472462+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:14.567931+00:00</t>
+          <t>2025-10-30T04:27:15.472479+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-10-30T03:39:14.567937+00:00</t>
+          <t>2025-10-30T04:27:15.472494+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-10-30 15:03:09)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:24.051260+00:00</t>
+          <t>2025-10-30T07:01:42.353576+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:26.082601+00:00</t>
+          <t>2025-10-30T07:01:44.631832+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:26.082617+00:00</t>
+          <t>2025-10-30T07:01:44.631894+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:26.082625+00:00</t>
+          <t>2025-10-30T07:01:44.631922+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:26.082633+00:00</t>
+          <t>2025-10-30T07:01:44.631943+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:26.082640+00:00</t>
+          <t>2025-10-30T07:01:44.631962+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:28.007987+00:00</t>
+          <t>2025-10-30T07:01:47.365292+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:28.008019+00:00</t>
+          <t>2025-10-30T07:01:47.365324+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:30.035558+00:00</t>
+          <t>2025-10-30T07:01:50.218952+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:32.770902+00:00</t>
+          <t>2025-10-30T07:01:52.535673+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:32.770931+00:00</t>
+          <t>2025-10-30T07:01:52.535706+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:35.098490+00:00</t>
+          <t>2025-10-30T07:01:54.998708+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:35.098518+00:00</t>
+          <t>2025-10-30T07:01:54.998740+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:35.098536+00:00</t>
+          <t>2025-10-30T07:01:54.998758+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:35.098552+00:00</t>
+          <t>2025-10-30T07:01:54.998776+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:43.201049+00:00</t>
+          <t>2025-10-30T07:02:02.330791+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:45.956182+00:00</t>
+          <t>2025-10-30T07:02:05.183984+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:48.261303+00:00</t>
+          <t>2025-10-30T07:02:07.866335+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:50.985374+00:00</t>
+          <t>2025-10-30T07:02:10.535743+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:50.985406+00:00</t>
+          <t>2025-10-30T07:02:10.535775+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:50.985424+00:00</t>
+          <t>2025-10-30T07:02:10.535793+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:53.331844+00:00</t>
+          <t>2025-10-30T07:02:12.875695+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:53.331880+00:00</t>
+          <t>2025-10-30T07:02:12.875725+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:53.331900+00:00</t>
+          <t>2025-10-30T07:02:12.875743+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:53.331918+00:00</t>
+          <t>2025-10-30T07:02:12.875759+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-30T04:26:53.331937+00:00</t>
+          <t>2025-10-30T07:02:12.875776+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:00.303160+00:00</t>
+          <t>2025-10-30T07:02:20.579502+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:00.303190+00:00</t>
+          <t>2025-10-30T07:02:20.579533+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:00.303209+00:00</t>
+          <t>2025-10-30T07:02:20.579552+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:00.303227+00:00</t>
+          <t>2025-10-30T07:02:20.579570+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:03.114542+00:00</t>
+          <t>2025-10-30T07:02:23.251964+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:03.114573+00:00</t>
+          <t>2025-10-30T07:02:23.251995+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:03.114592+00:00</t>
+          <t>2025-10-30T07:02:23.252014+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:05.491739+00:00</t>
+          <t>2025-10-30T07:02:25.478586+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:05.491769+00:00</t>
+          <t>2025-10-30T07:02:25.478617+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:05.491788+00:00</t>
+          <t>2025-10-30T07:02:25.478635+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:05.491805+00:00</t>
+          <t>2025-10-30T07:02:25.478652+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:05.491822+00:00</t>
+          <t>2025-10-30T07:02:25.478669+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:05.491838+00:00</t>
+          <t>2025-10-30T07:02:25.478685+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:05.491855+00:00</t>
+          <t>2025-10-30T07:02:25.478701+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:05.491875+00:00</t>
+          <t>2025-10-30T07:02:25.478723+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:05.491891+00:00</t>
+          <t>2025-10-30T07:02:25.478739+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:07.764916+00:00</t>
+          <t>2025-10-30T07:02:27.669444+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:07.764946+00:00</t>
+          <t>2025-10-30T07:02:27.669476+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:12.799825+00:00</t>
+          <t>2025-10-30T07:02:32.479432+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:15.472434+00:00</t>
+          <t>2025-10-30T07:02:34.715968+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:15.472462+00:00</t>
+          <t>2025-10-30T07:02:34.716007+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:15.472479+00:00</t>
+          <t>2025-10-30T07:02:34.716029+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-10-30T04:27:15.472494+00:00</t>
+          <t>2025-10-30T07:02:34.716048+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-10-31 11:03:20)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:42.353576+00:00</t>
+          <t>2025-10-31T03:01:38.129996+00:00</t>
         </is>
       </c>
     </row>
@@ -567,27 +567,27 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Буше Рид</t>
+          <t>Зборовский Сергей</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>39158</t>
+          <t>20989</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1369_АВТ_бушерид</t>
+          <t>1369_АВТ_зборовскийсергей</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:44.631832+00:00</t>
+          <t>2025-10-31T03:01:41.103331+00:00</t>
         </is>
       </c>
     </row>
@@ -624,27 +624,27 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Зборовский Сергей</t>
+          <t>Кизимов Семён</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>20989</t>
+          <t>25697</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1369_АВТ_зборовскийсергей</t>
+          <t>1369_АВТ_кизимовсемен</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:44.631894+00:00</t>
+          <t>2025-10-31T03:01:41.103365+00:00</t>
         </is>
       </c>
     </row>
@@ -681,27 +681,27 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Кизимов Семён</t>
+          <t>Осипов Максим И</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>25697</t>
+          <t>17459</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1369_АВТ_кизимовсемен</t>
+          <t>1369_АВТ_осиповмаксими</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:44.631922+00:00</t>
+          <t>2025-10-31T03:01:41.103386+00:00</t>
         </is>
       </c>
     </row>
@@ -738,12 +738,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Осипов Максим И</t>
+          <t>Трямкин Никита</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -753,12 +753,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>17459</t>
+          <t>17594</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1369_АВТ_осиповмаксими</t>
+          <t>1369_АВТ_трямкинникита</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -773,34 +773,34 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:44.631943+00:00</t>
+          <t>2025-10-31T03:01:41.103403+00:00</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>avtomobilist</t>
+          <t>admiral</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Трямкин Никита</t>
+          <t>Грман Марио</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -810,12 +810,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>17594</t>
+          <t>31232</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1369_АВТ_трямкинникита</t>
+          <t>1369_АДМ_грманмарио</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -825,12 +825,12 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
+          <t>https://www.khl.ru/clubs/admiral/team/</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:44.631962+00:00</t>
+          <t>2025-10-31T03:01:44.010179+00:00</t>
         </is>
       </c>
     </row>
@@ -852,12 +852,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Грман Марио</t>
+          <t>Шепелев Александр</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -867,12 +867,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>31232</t>
+          <t>23447</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1369_АДМ_грманмарио</t>
+          <t>1369_АДМ_шепелевалександр</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -887,34 +887,34 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:47.365292+00:00</t>
+          <t>2025-10-31T03:01:44.010209+00:00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>АКБ</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>admiral</t>
+          <t>ak_bars</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Шепелев Александр</t>
+          <t>Яруллин Альберт</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -924,12 +924,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>23447</t>
+          <t>16365</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1369_АДМ_шепелевалександр</t>
+          <t>1369_АКБ_яруллинальберт</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -939,39 +939,39 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/admiral/team/</t>
+          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:47.365324+00:00</t>
+          <t>2025-10-31T03:01:46.747654+00:00</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>АКБ</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ak_bars</t>
+          <t>amur</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Яруллин Альберт</t>
+          <t>Абросимов Роман</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>94</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -981,12 +981,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>16365</t>
+          <t>17968</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1369_АКБ_яруллинальберт</t>
+          <t>1369_АМР_абросимовроман</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -996,12 +996,12 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:50.218952+00:00</t>
+          <t>2025-10-31T03:01:49.607666+00:00</t>
         </is>
       </c>
     </row>
@@ -1023,27 +1023,27 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Абросимов Роман</t>
+          <t>Гиздатуллин Артур</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>87</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>17968</t>
+          <t>22208</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1369_АМР_абросимовроман</t>
+          <t>1369_АМР_гиздатуллинартур</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1058,49 +1058,49 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:52.535673+00:00</t>
+          <t>2025-10-31T03:01:49.607694+00:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Гиздатуллин Артур</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>22208</t>
+          <t>28244</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_АМР_гиздатуллинартур</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1110,12 +1110,12 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:52.535706+00:00</t>
+          <t>2025-10-31T03:01:52.580310+00:00</t>
         </is>
       </c>
     </row>
@@ -1137,12 +1137,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Асетов Алихан</t>
+          <t>Галимов Эмиль</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>20852</t>
+          <t>15997</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_БАР_асетовалихан</t>
+          <t>1369_БАР_галимовэмиль</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:54.998708+00:00</t>
+          <t>2025-10-31T03:01:52.580338+00:00</t>
         </is>
       </c>
     </row>
@@ -1194,27 +1194,27 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Мухаметов Максим</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>28244</t>
+          <t>25207</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_БАР_мухаметовмаксим</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1229,34 +1229,34 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:54.998740+00:00</t>
+          <t>2025-10-31T03:01:52.580356+00:00</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Галимов Эмиль</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1266,12 +1266,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>15997</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_БАР_галимовэмиль</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1281,54 +1281,54 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:54.998758+00:00</t>
+          <t>2025-10-31T03:02:01.047836+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Мухаметов Максим</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>25207</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_БАР_мухаметовмаксим</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,39 +1338,39 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-30T07:01:54.998776+00:00</t>
+          <t>2025-10-31T03:02:03.969604+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1380,12 +1380,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,54 +1395,54 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:02.330791+00:00</t>
+          <t>2025-10-31T03:02:06.872066+00:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1452,39 +1452,39 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:05.183984+00:00</t>
+          <t>2025-10-31T03:02:09.574861+00:00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Попугаев Никита О</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1494,12 +1494,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>22683</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_НХК_попугаевникитао</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1509,12 +1509,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:07.866335+00:00</t>
+          <t>2025-10-31T03:02:09.574895+00:00</t>
         </is>
       </c>
     </row>
@@ -1536,27 +1536,27 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Профака Лука</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>43943</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_НХК_профакалука</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1571,49 +1571,49 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:10.535743+00:00</t>
+          <t>2025-10-31T03:02:09.574914+00:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>Ващенко Григорий</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>22683</t>
+          <t>14155</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>1369_СЕВ_ващенкогригорий</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1623,39 +1623,39 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:10.535775+00:00</t>
+          <t>2025-10-31T03:02:11.870583+00:00</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Профака Лука</t>
+          <t>Грудинин Владимир</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1665,12 +1665,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>43943</t>
+          <t>35064</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_НХК_профакалука</t>
+          <t>1369_СЕВ_грудининвладимир</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1680,12 +1680,12 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:10.535793+00:00</t>
+          <t>2025-10-31T03:02:11.870613+00:00</t>
         </is>
       </c>
     </row>
@@ -1707,27 +1707,27 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Ващенко Григорий</t>
+          <t>Лишка Адам</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>14155</t>
+          <t>25514</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СЕВ_ващенкогригорий</t>
+          <t>1369_СЕВ_лишкаадам</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:12.875695+00:00</t>
+          <t>2025-10-31T03:02:11.870632+00:00</t>
         </is>
       </c>
     </row>
@@ -1764,27 +1764,27 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Грудинин Владимир</t>
+          <t>Танков Кирилл</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>35064</t>
+          <t>32981</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СЕВ_грудининвладимир</t>
+          <t>1369_СЕВ_танковкирилл</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:12.875725+00:00</t>
+          <t>2025-10-31T03:02:11.870650+00:00</t>
         </is>
       </c>
     </row>
@@ -1821,12 +1821,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Лишка Адам</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1836,12 +1836,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>25514</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СЕВ_лишкаадам</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1856,34 +1856,34 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:12.875743+00:00</t>
+          <t>2025-10-31T03:02:11.870667+00:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Танков Кирилл</t>
+          <t>Гараев Амир</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>67</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>32981</t>
+          <t>28624</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СЕВ_танковкирилл</t>
+          <t>1369_СОЧ_гараевамир</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1908,54 +1908,54 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:12.875759+00:00</t>
+          <t>2025-10-31T03:02:20.368802+00:00</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1965,12 +1965,12 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:12.875776+00:00</t>
+          <t>2025-10-31T03:02:20.368829+00:00</t>
         </is>
       </c>
     </row>
@@ -1992,12 +1992,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Гараев Амир</t>
+          <t>Уткин Дмитрий А</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2007,12 +2007,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>28624</t>
+          <t>35195</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гараевамир</t>
+          <t>1369_СОЧ_уткиндмитрийа</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:20.579502+00:00</t>
+          <t>2025-10-31T03:02:20.368847+00:00</t>
         </is>
       </c>
     </row>
@@ -2049,27 +2049,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2084,34 +2084,34 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:20.579533+00:00</t>
+          <t>2025-10-31T03:02:20.368864+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Уткин Дмитрий А</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2121,12 +2121,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>35195</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СОЧ_уткиндмитрийа</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2136,54 +2136,54 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:20.579552+00:00</t>
+          <t>2025-10-31T03:02:23.142240+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,12 +2193,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:20.579570+00:00</t>
+          <t>2025-10-31T03:02:23.142268+00:00</t>
         </is>
       </c>
     </row>
@@ -2220,12 +2220,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2235,12 +2235,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2255,34 +2255,34 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:23.251964+00:00</t>
+          <t>2025-10-31T03:02:23.142286+00:00</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2292,12 +2292,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2307,39 +2307,39 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:23.251995+00:00</t>
+          <t>2025-10-31T03:02:25.440004+00:00</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2349,12 +2349,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2364,12 +2364,12 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:23.252014+00:00</t>
+          <t>2025-10-31T03:02:25.440033+00:00</t>
         </is>
       </c>
     </row>
@@ -2391,27 +2391,27 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:25.478586+00:00</t>
+          <t>2025-10-31T03:02:25.440052+00:00</t>
         </is>
       </c>
     </row>
@@ -2448,12 +2448,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2463,12 +2463,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:25.478617+00:00</t>
+          <t>2025-10-31T03:02:25.440069+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,27 +2505,27 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Набиев Артём</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>79</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>41187</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_набиевартем</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:25.478635+00:00</t>
+          <t>2025-10-31T03:02:25.440085+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,12 +2562,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Пименов Артём</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>68</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>21205</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_пименовартем</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:25.478652+00:00</t>
+          <t>2025-10-31T03:02:25.440101+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,12 +2619,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Набиев Артём</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2634,12 +2634,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>41187</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_набиевартем</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:25.478669+00:00</t>
+          <t>2025-10-31T03:02:25.440121+00:00</t>
         </is>
       </c>
     </row>
@@ -2676,12 +2676,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Пименов Артём</t>
+          <t>Хохряков Пётр</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2691,12 +2691,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>21205</t>
+          <t>15413</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_пименовартем</t>
+          <t>1369_СЮЛ_хохряковпетр</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:25.478685+00:00</t>
+          <t>2025-10-31T03:02:25.440137+00:00</t>
         </is>
       </c>
     </row>
@@ -2733,12 +2733,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2748,12 +2748,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2768,49 +2768,49 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:25.478701+00:00</t>
+          <t>2025-10-31T03:02:25.440151+00:00</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Хохряков Пётр</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>15413</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хохряковпетр</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2820,39 +2820,39 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:25.478723+00:00</t>
+          <t>2025-10-31T03:02:28.297301+00:00</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2862,12 +2862,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2877,54 +2877,54 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:25.478739+00:00</t>
+          <t>2025-10-31T03:02:28.297333+00:00</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2934,54 +2934,54 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:27.669444+00:00</t>
+          <t>2025-10-31T03:02:33.361056+00:00</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2991,39 +2991,39 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:27.669476+00:00</t>
+          <t>2025-10-31T03:02:36.062893+00:00</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Попугаев Никита А</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3033,12 +3033,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>22684</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ШДР_попугаевникитаа</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3048,12 +3048,12 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:32.479432+00:00</t>
+          <t>2025-10-31T03:02:36.062925+00:00</t>
         </is>
       </c>
     </row>
@@ -3075,27 +3075,27 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Саттер Райли</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>45491</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ШДР_саттеррайли</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:34.715968+00:00</t>
+          <t>2025-10-31T03:02:36.062944+00:00</t>
         </is>
       </c>
     </row>
@@ -3132,12 +3132,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Попугаев Никита А</t>
+          <t>Фу Спенсер</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -3147,12 +3147,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>22684</t>
+          <t>34934</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1369_ШДР_попугаевникитаа</t>
+          <t>1369_ШДР_фуспенсер</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3167,121 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-30T07:02:34.716007+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Саттер Райли</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>45491</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>1369_ШДР_саттеррайли</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>2025-10-30T07:02:34.716029+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Фу Спенсер</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>34934</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>1369_ШДР_фуспенсер</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>2025-10-30T07:02:34.716048+00:00</t>
+          <t>2025-10-31T03:02:36.062960+00:00</t>
         </is>
       </c>
     </row>
@@ -3296,7 +3182,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3338,6 +3224,80 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>changed_day</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>АВТ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Автомобилист</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Буше Рид</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_АВТ_бушерид</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-10-31T11:02:36.570189+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>БАР</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Барыс</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Асетов Алихан</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1369_БАР_асетовалихан</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-10-31T11:02:36.570189+08:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-10-31 15:03:18)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-31T03:01:38.129996+00:00</t>
+          <t>2025-10-31T07:01:50.533873+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-31T03:01:41.103331+00:00</t>
+          <t>2025-10-31T07:01:53.208599+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-31T03:01:41.103365+00:00</t>
+          <t>2025-10-31T07:01:53.208630+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-31T03:01:41.103386+00:00</t>
+          <t>2025-10-31T07:01:53.208650+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-31T03:01:41.103403+00:00</t>
+          <t>2025-10-31T07:01:53.208667+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-31T03:01:44.010179+00:00</t>
+          <t>2025-10-31T07:01:55.564044+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-31T03:01:44.010209+00:00</t>
+          <t>2025-10-31T07:01:55.564076+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-31T03:01:46.747654+00:00</t>
+          <t>2025-10-31T07:01:57.864150+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-31T03:01:49.607666+00:00</t>
+          <t>2025-10-31T07:02:00.644788+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-31T03:01:49.607694+00:00</t>
+          <t>2025-10-31T07:02:00.644817+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-31T03:01:52.580310+00:00</t>
+          <t>2025-10-31T07:02:03.507666+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-31T03:01:52.580338+00:00</t>
+          <t>2025-10-31T07:02:03.507694+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-31T03:01:52.580356+00:00</t>
+          <t>2025-10-31T07:02:03.507713+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:01.047836+00:00</t>
+          <t>2025-10-31T07:02:11.051218+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:03.969604+00:00</t>
+          <t>2025-10-31T07:02:13.408140+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:06.872066+00:00</t>
+          <t>2025-10-31T07:02:15.752756+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:09.574861+00:00</t>
+          <t>2025-10-31T07:02:18.050314+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:09.574895+00:00</t>
+          <t>2025-10-31T07:02:18.050344+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:09.574914+00:00</t>
+          <t>2025-10-31T07:02:18.050362+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:11.870583+00:00</t>
+          <t>2025-10-31T07:02:20.433948+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:11.870613+00:00</t>
+          <t>2025-10-31T07:02:20.433977+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:11.870632+00:00</t>
+          <t>2025-10-31T07:02:20.433995+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:11.870650+00:00</t>
+          <t>2025-10-31T07:02:20.434011+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:11.870667+00:00</t>
+          <t>2025-10-31T07:02:20.434028+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:20.368802+00:00</t>
+          <t>2025-10-31T07:02:28.316231+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:20.368829+00:00</t>
+          <t>2025-10-31T07:02:28.316262+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:20.368847+00:00</t>
+          <t>2025-10-31T07:02:28.316281+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:20.368864+00:00</t>
+          <t>2025-10-31T07:02:28.316299+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:23.142240+00:00</t>
+          <t>2025-10-31T07:02:31.125876+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:23.142268+00:00</t>
+          <t>2025-10-31T07:02:31.125903+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:23.142286+00:00</t>
+          <t>2025-10-31T07:02:31.125920+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:25.440004+00:00</t>
+          <t>2025-10-31T07:02:33.460988+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:25.440033+00:00</t>
+          <t>2025-10-31T07:02:33.461016+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:25.440052+00:00</t>
+          <t>2025-10-31T07:02:33.461034+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:25.440069+00:00</t>
+          <t>2025-10-31T07:02:33.461050+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:25.440085+00:00</t>
+          <t>2025-10-31T07:02:33.461065+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:25.440101+00:00</t>
+          <t>2025-10-31T07:02:33.461080+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:25.440121+00:00</t>
+          <t>2025-10-31T07:02:33.461099+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:25.440137+00:00</t>
+          <t>2025-10-31T07:02:33.461114+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:25.440151+00:00</t>
+          <t>2025-10-31T07:02:33.461128+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:28.297301+00:00</t>
+          <t>2025-10-31T07:02:36.189530+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:28.297333+00:00</t>
+          <t>2025-10-31T07:02:36.189559+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:33.361056+00:00</t>
+          <t>2025-10-31T07:02:40.887512+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:36.062893+00:00</t>
+          <t>2025-10-31T07:02:43.693787+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:36.062925+00:00</t>
+          <t>2025-10-31T07:02:43.693816+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:36.062944+00:00</t>
+          <t>2025-10-31T07:02:43.693834+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-10-31T03:02:36.062960+00:00</t>
+          <t>2025-10-31T07:02:43.693851+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-01 11:02:32)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,42 +495,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>АВГ</t>
+          <t>АВТ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Авангард</t>
+          <t>Автомобилист</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>avangard</t>
+          <t>avtomobilist</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Якупов Наиль</t>
+          <t>Зборовский Сергей</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>16391</t>
+          <t>20989</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1369_АВГ_якуповнаиль</t>
+          <t>1369_АВТ_зборовскийсергей</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -540,12 +540,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/avangard/team/</t>
+          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-31T07:01:50.533873+00:00</t>
+          <t>2025-11-01T03:01:22.830687+00:00</t>
         </is>
       </c>
     </row>
@@ -567,27 +567,27 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Зборовский Сергей</t>
+          <t>Кизимов Семён</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>20989</t>
+          <t>25697</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1369_АВТ_зборовскийсергей</t>
+          <t>1369_АВТ_кизимовсемен</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-31T07:01:53.208599+00:00</t>
+          <t>2025-11-01T03:01:22.830720+00:00</t>
         </is>
       </c>
     </row>
@@ -624,27 +624,27 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Кизимов Семён</t>
+          <t>Осипов Максим И</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>25697</t>
+          <t>17459</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1369_АВТ_кизимовсемен</t>
+          <t>1369_АВТ_осиповмаксими</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-31T07:01:53.208630+00:00</t>
+          <t>2025-11-01T03:01:22.830740+00:00</t>
         </is>
       </c>
     </row>
@@ -681,12 +681,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Осипов Максим И</t>
+          <t>Трямкин Никита</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -696,12 +696,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>17459</t>
+          <t>17594</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1369_АВТ_осиповмаксими</t>
+          <t>1369_АВТ_трямкинникита</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -716,34 +716,34 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-31T07:01:53.208650+00:00</t>
+          <t>2025-11-01T03:01:22.830757+00:00</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>avtomobilist</t>
+          <t>admiral</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Трямкин Никита</t>
+          <t>Грман Марио</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -753,12 +753,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>17594</t>
+          <t>31232</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1369_АВТ_трямкинникита</t>
+          <t>1369_АДМ_грманмарио</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -768,12 +768,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
+          <t>https://www.khl.ru/clubs/admiral/team/</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-31T07:01:53.208667+00:00</t>
+          <t>2025-11-01T03:01:25.721039+00:00</t>
         </is>
       </c>
     </row>
@@ -795,12 +795,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Грман Марио</t>
+          <t>Шепелев Александр</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -810,12 +810,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>31232</t>
+          <t>23447</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1369_АДМ_грманмарио</t>
+          <t>1369_АДМ_шепелевалександр</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -830,34 +830,34 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-31T07:01:55.564044+00:00</t>
+          <t>2025-11-01T03:01:25.721070+00:00</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>АКБ</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>admiral</t>
+          <t>ak_bars</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Шепелев Александр</t>
+          <t>Яруллин Альберт</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -867,12 +867,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>23447</t>
+          <t>16365</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1369_АДМ_шепелевалександр</t>
+          <t>1369_АКБ_яруллинальберт</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -882,39 +882,39 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/admiral/team/</t>
+          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-31T07:01:55.564076+00:00</t>
+          <t>2025-11-01T03:01:28.080084+00:00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>АКБ</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ak_bars</t>
+          <t>amur</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Яруллин Альберт</t>
+          <t>Абросимов Роман</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>94</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -924,12 +924,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>16365</t>
+          <t>17968</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1369_АКБ_яруллинальберт</t>
+          <t>1369_АМР_абросимовроман</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -939,12 +939,12 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-31T07:01:57.864150+00:00</t>
+          <t>2025-11-01T03:01:30.404865+00:00</t>
         </is>
       </c>
     </row>
@@ -966,27 +966,27 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Абросимов Роман</t>
+          <t>Гиздатуллин Артур</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>87</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>17968</t>
+          <t>22208</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1369_АМР_абросимовроман</t>
+          <t>1369_АМР_гиздатуллинартур</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1001,49 +1001,49 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:00.644788+00:00</t>
+          <t>2025-11-01T03:01:30.404894+00:00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Гиздатуллин Артур</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>22208</t>
+          <t>28244</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1369_АМР_гиздатуллинартур</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1053,12 +1053,12 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:00.644817+00:00</t>
+          <t>2025-11-01T03:01:33.230169+00:00</t>
         </is>
       </c>
     </row>
@@ -1080,27 +1080,27 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Галимов Эмиль</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>28244</t>
+          <t>15997</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_БАР_галимовэмиль</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:03.507666+00:00</t>
+          <t>2025-11-01T03:01:33.230197+00:00</t>
         </is>
       </c>
     </row>
@@ -1137,12 +1137,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Галимов Эмиль</t>
+          <t>Мухаметов Максим</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>15997</t>
+          <t>25207</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_БАР_галимовэмиль</t>
+          <t>1369_БАР_мухаметовмаксим</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1172,34 +1172,34 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:03.507694+00:00</t>
+          <t>2025-11-01T03:01:33.230214+00:00</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Мухаметов Максим</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1209,12 +1209,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>25207</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_БАР_мухаметовмаксим</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1224,54 +1224,54 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:03.507713+00:00</t>
+          <t>2025-11-01T03:01:41.680641+00:00</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1281,54 +1281,54 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:11.051218+00:00</t>
+          <t>2025-11-01T03:01:44.096808+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,39 +1338,39 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:13.408140+00:00</t>
+          <t>2025-11-01T03:01:46.480237+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1380,12 +1380,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,12 +1395,12 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:15.752756+00:00</t>
+          <t>2025-11-01T03:01:48.783875+00:00</t>
         </is>
       </c>
     </row>
@@ -1422,12 +1422,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Попугаев Никита О</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>22683</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_НХК_попугаевникитао</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:18.050314+00:00</t>
+          <t>2025-11-01T03:01:48.783903+00:00</t>
         </is>
       </c>
     </row>
@@ -1479,27 +1479,27 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>Профака Лука</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>22683</t>
+          <t>43943</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>1369_НХК_профакалука</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1514,34 +1514,34 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:18.050344+00:00</t>
+          <t>2025-11-01T03:01:48.783920+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Профака Лука</t>
+          <t>Ващенко Григорий</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1551,12 +1551,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>43943</t>
+          <t>14155</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_НХК_профакалука</t>
+          <t>1369_СЕВ_ващенкогригорий</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1566,12 +1566,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:18.050362+00:00</t>
+          <t>2025-11-01T03:01:51.519259+00:00</t>
         </is>
       </c>
     </row>
@@ -1593,12 +1593,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Ващенко Григорий</t>
+          <t>Грудинин Владимир</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>14155</t>
+          <t>35064</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_СЕВ_ващенкогригорий</t>
+          <t>1369_СЕВ_грудининвладимир</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:20.433948+00:00</t>
+          <t>2025-11-01T03:01:51.519287+00:00</t>
         </is>
       </c>
     </row>
@@ -1650,27 +1650,27 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Грудинин Владимир</t>
+          <t>Танков Кирилл</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>35064</t>
+          <t>32981</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СЕВ_грудининвладимир</t>
+          <t>1369_СЕВ_танковкирилл</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:20.433977+00:00</t>
+          <t>2025-11-01T03:01:51.519304+00:00</t>
         </is>
       </c>
     </row>
@@ -1707,12 +1707,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Лишка Адам</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1722,12 +1722,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>25514</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СЕВ_лишкаадам</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1742,34 +1742,34 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:20.433995+00:00</t>
+          <t>2025-11-01T03:01:51.519321+00:00</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Танков Кирилл</t>
+          <t>Гараев Амир</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>67</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1779,12 +1779,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>32981</t>
+          <t>28624</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СЕВ_танковкирилл</t>
+          <t>1369_СОЧ_гараевамир</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1794,54 +1794,54 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:20.434011+00:00</t>
+          <t>2025-11-01T03:01:59.530940+00:00</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1851,12 +1851,12 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:20.434028+00:00</t>
+          <t>2025-11-01T03:01:59.530970+00:00</t>
         </is>
       </c>
     </row>
@@ -1878,12 +1878,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Гараев Амир</t>
+          <t>Уткин Дмитрий А</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>28624</t>
+          <t>35195</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гараевамир</t>
+          <t>1369_СОЧ_уткиндмитрийа</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:28.316231+00:00</t>
+          <t>2025-11-01T03:01:59.530989+00:00</t>
         </is>
       </c>
     </row>
@@ -1935,27 +1935,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1970,34 +1970,34 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:28.316262+00:00</t>
+          <t>2025-11-01T03:01:59.531006+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Уткин Дмитрий А</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2007,12 +2007,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>35195</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_уткиндмитрийа</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,54 +2022,54 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:28.316281+00:00</t>
+          <t>2025-11-01T03:02:02.344696+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,12 +2079,12 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:28.316299+00:00</t>
+          <t>2025-11-01T03:02:02.344725+00:00</t>
         </is>
       </c>
     </row>
@@ -2106,12 +2106,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2121,12 +2121,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2141,34 +2141,34 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:31.125876+00:00</t>
+          <t>2025-11-01T03:02:02.344744+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2178,12 +2178,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,39 +2193,39 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:31.125903+00:00</t>
+          <t>2025-11-01T03:02:05.159163+00:00</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2235,12 +2235,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2250,12 +2250,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:31.125920+00:00</t>
+          <t>2025-11-01T03:02:05.159192+00:00</t>
         </is>
       </c>
     </row>
@@ -2277,27 +2277,27 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:33.460988+00:00</t>
+          <t>2025-11-01T03:02:05.159211+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,12 +2334,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2349,12 +2349,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:33.461016+00:00</t>
+          <t>2025-11-01T03:02:05.159226+00:00</t>
         </is>
       </c>
     </row>
@@ -2391,27 +2391,27 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Пименов Артём</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>68</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>21205</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_пименовартем</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:33.461034+00:00</t>
+          <t>2025-11-01T03:02:05.159243+00:00</t>
         </is>
       </c>
     </row>
@@ -2448,12 +2448,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2463,12 +2463,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:33.461050+00:00</t>
+          <t>2025-11-01T03:02:05.159259+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,12 +2505,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Набиев Артём</t>
+          <t>Хохряков Пётр</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2520,12 +2520,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>41187</t>
+          <t>15413</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_набиевартем</t>
+          <t>1369_СЮЛ_хохряковпетр</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:33.461065+00:00</t>
+          <t>2025-11-01T03:02:05.159275+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,12 +2562,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Пименов Артём</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>21205</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_пименовартем</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2597,49 +2597,49 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:33.461080+00:00</t>
+          <t>2025-11-01T03:02:05.159289+00:00</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2649,39 +2649,39 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:33.461099+00:00</t>
+          <t>2025-11-01T03:02:07.461507+00:00</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Хохряков Пётр</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2691,12 +2691,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>15413</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хохряковпетр</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2706,39 +2706,39 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:33.461114+00:00</t>
+          <t>2025-11-01T03:02:07.461536+00:00</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2748,12 +2748,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2763,39 +2763,39 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:33.461128+00:00</t>
+          <t>2025-11-01T03:02:13.252112+00:00</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2805,12 +2805,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2820,39 +2820,39 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:36.189530+00:00</t>
+          <t>2025-11-01T03:02:16.069397+00:00</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Попугаев Никита А</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2862,12 +2862,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>22684</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ШДР_попугаевникитаа</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2877,39 +2877,39 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:36.189559+00:00</t>
+          <t>2025-11-01T03:02:16.069425+00:00</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Саттер Райли</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2919,12 +2919,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>45491</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ШДР_саттеррайли</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2934,12 +2934,12 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:40.887512+00:00</t>
+          <t>2025-11-01T03:02:16.069443+00:00</t>
         </is>
       </c>
     </row>
@@ -2961,27 +2961,27 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Фу Спенсер</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>34934</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ШДР_фуспенсер</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2996,178 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-10-31T07:02:43.693787+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Попугаев Никита А</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>81</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>22684</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>1369_ШДР_попугаевникитаа</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>2025-10-31T07:02:43.693816+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Саттер Райли</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>45491</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>1369_ШДР_саттеррайли</t>
-        </is>
-      </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>2025-10-31T07:02:43.693834+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Фу Спенсер</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>34934</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>1369_ШДР_фуспенсер</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>2025-10-31T07:02:43.693851+00:00</t>
+          <t>2025-11-01T03:02:16.069458+00:00</t>
         </is>
       </c>
     </row>
@@ -3182,7 +3011,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3230,22 +3059,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>АВГ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>Авангард</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Буше Рид</t>
+          <t>Якупов Наиль</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_АВТ_бушерид</t>
+          <t>1369_АВГ_якуповнаиль</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -3255,34 +3084,34 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-10-31T11:02:36.570189+08:00</t>
+          <t>2025-11-01T11:02:16.576964+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Асетов Алихан</t>
+          <t>Лишка Адам</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1369_БАР_асетовалихан</t>
+          <t>1369_СЕВ_лишкаадам</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -3292,12 +3121,49 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-10-31T11:02:36.570189+08:00</t>
+          <t>2025-11-01T11:02:16.576964+08:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>СЮЛ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Салават Юлаев</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Набиев Артём</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1369_СЮЛ_набиевартем</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-11-01T11:02:16.576964+08:00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-01 15:02:24)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:22.830687+00:00</t>
+          <t>2025-11-01T07:01:19.485825+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:22.830720+00:00</t>
+          <t>2025-11-01T07:01:19.485857+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:22.830740+00:00</t>
+          <t>2025-11-01T07:01:19.485877+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:22.830757+00:00</t>
+          <t>2025-11-01T07:01:19.485894+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:25.721039+00:00</t>
+          <t>2025-11-01T07:01:21.810969+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:25.721070+00:00</t>
+          <t>2025-11-01T07:01:21.810997+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:28.080084+00:00</t>
+          <t>2025-11-01T07:01:24.647595+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:30.404865+00:00</t>
+          <t>2025-11-01T07:01:26.951777+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:30.404894+00:00</t>
+          <t>2025-11-01T07:01:26.951805+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:33.230169+00:00</t>
+          <t>2025-11-01T07:01:29.306865+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:33.230197+00:00</t>
+          <t>2025-11-01T07:01:29.306893+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:33.230214+00:00</t>
+          <t>2025-11-01T07:01:29.306911+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:41.680641+00:00</t>
+          <t>2025-11-01T07:01:37.664303+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:44.096808+00:00</t>
+          <t>2025-11-01T07:01:40.547189+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:46.480237+00:00</t>
+          <t>2025-11-01T07:01:43.301793+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:48.783875+00:00</t>
+          <t>2025-11-01T07:01:45.587999+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:48.783903+00:00</t>
+          <t>2025-11-01T07:01:45.588029+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:48.783920+00:00</t>
+          <t>2025-11-01T07:01:45.588047+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:51.519259+00:00</t>
+          <t>2025-11-01T07:01:47.911246+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:51.519287+00:00</t>
+          <t>2025-11-01T07:01:47.911302+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:51.519304+00:00</t>
+          <t>2025-11-01T07:01:47.911346+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:51.519321+00:00</t>
+          <t>2025-11-01T07:01:47.911368+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:59.530940+00:00</t>
+          <t>2025-11-01T07:01:55.949013+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:59.530970+00:00</t>
+          <t>2025-11-01T07:01:55.949040+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:59.530989+00:00</t>
+          <t>2025-11-01T07:01:55.949058+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-01T03:01:59.531006+00:00</t>
+          <t>2025-11-01T07:01:55.949074+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:02.344696+00:00</t>
+          <t>2025-11-01T07:01:58.732971+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:02.344725+00:00</t>
+          <t>2025-11-01T07:01:58.733006+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:02.344744+00:00</t>
+          <t>2025-11-01T07:01:58.733162+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:05.159163+00:00</t>
+          <t>2025-11-01T07:02:01.076243+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:05.159192+00:00</t>
+          <t>2025-11-01T07:02:01.076271+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:05.159211+00:00</t>
+          <t>2025-11-01T07:02:01.076287+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:05.159226+00:00</t>
+          <t>2025-11-01T07:02:01.076303+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:05.159243+00:00</t>
+          <t>2025-11-01T07:02:01.076319+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:05.159259+00:00</t>
+          <t>2025-11-01T07:02:01.076334+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:05.159275+00:00</t>
+          <t>2025-11-01T07:02:01.076349+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:05.159289+00:00</t>
+          <t>2025-11-01T07:02:01.076362+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:07.461507+00:00</t>
+          <t>2025-11-01T07:02:03.496711+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:07.461536+00:00</t>
+          <t>2025-11-01T07:02:03.496741+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:13.252112+00:00</t>
+          <t>2025-11-01T07:02:08.157926+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:16.069397+00:00</t>
+          <t>2025-11-01T07:02:10.514616+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:16.069425+00:00</t>
+          <t>2025-11-01T07:02:10.514645+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:16.069443+00:00</t>
+          <t>2025-11-01T07:02:10.514662+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-01T03:02:16.069458+00:00</t>
+          <t>2025-11-01T07:02:10.514678+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-01 21:40:01)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:19.485825+00:00</t>
+          <t>2025-11-01T13:38:56.494631+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:19.485857+00:00</t>
+          <t>2025-11-01T13:38:56.494651+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:19.485877+00:00</t>
+          <t>2025-11-01T13:38:56.494662+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:19.485894+00:00</t>
+          <t>2025-11-01T13:38:56.494670+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:21.810969+00:00</t>
+          <t>2025-11-01T13:38:58.709768+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:21.810997+00:00</t>
+          <t>2025-11-01T13:38:58.709785+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:24.647595+00:00</t>
+          <t>2025-11-01T13:39:00.789879+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:26.951777+00:00</t>
+          <t>2025-11-01T13:39:03.638515+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:26.951805+00:00</t>
+          <t>2025-11-01T13:39:03.638545+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:29.306865+00:00</t>
+          <t>2025-11-01T13:39:06.114648+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:29.306893+00:00</t>
+          <t>2025-11-01T13:39:06.114676+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:29.306911+00:00</t>
+          <t>2025-11-01T13:39:06.114696+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:37.664303+00:00</t>
+          <t>2025-11-01T13:39:13.523828+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:40.547189+00:00</t>
+          <t>2025-11-01T13:39:16.465445+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:43.301793+00:00</t>
+          <t>2025-11-01T13:39:18.732826+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:45.587999+00:00</t>
+          <t>2025-11-01T13:39:21.104280+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:45.588029+00:00</t>
+          <t>2025-11-01T13:39:21.104309+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:45.588047+00:00</t>
+          <t>2025-11-01T13:39:21.104327+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:47.911246+00:00</t>
+          <t>2025-11-01T13:39:23.465554+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:47.911302+00:00</t>
+          <t>2025-11-01T13:39:23.465584+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:47.911346+00:00</t>
+          <t>2025-11-01T13:39:23.465602+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:47.911368+00:00</t>
+          <t>2025-11-01T13:39:23.465620+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:55.949013+00:00</t>
+          <t>2025-11-01T13:39:32.189837+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:55.949040+00:00</t>
+          <t>2025-11-01T13:39:32.189868+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:55.949058+00:00</t>
+          <t>2025-11-01T13:39:32.189888+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:55.949074+00:00</t>
+          <t>2025-11-01T13:39:32.189906+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:58.732971+00:00</t>
+          <t>2025-11-01T13:39:35.019703+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:58.733006+00:00</t>
+          <t>2025-11-01T13:39:35.019732+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-01T07:01:58.733162+00:00</t>
+          <t>2025-11-01T13:39:35.019755+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:01.076243+00:00</t>
+          <t>2025-11-01T13:39:37.449019+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:01.076271+00:00</t>
+          <t>2025-11-01T13:39:37.449049+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:01.076287+00:00</t>
+          <t>2025-11-01T13:39:37.449067+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:01.076303+00:00</t>
+          <t>2025-11-01T13:39:37.449084+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:01.076319+00:00</t>
+          <t>2025-11-01T13:39:37.449101+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:01.076334+00:00</t>
+          <t>2025-11-01T13:39:37.449117+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:01.076349+00:00</t>
+          <t>2025-11-01T13:39:37.449138+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:01.076362+00:00</t>
+          <t>2025-11-01T13:39:37.449153+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:03.496711+00:00</t>
+          <t>2025-11-01T13:39:40.104671+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:03.496741+00:00</t>
+          <t>2025-11-01T13:39:40.104700+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:08.157926+00:00</t>
+          <t>2025-11-01T13:39:44.950042+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:10.514616+00:00</t>
+          <t>2025-11-01T13:39:47.733216+00:00</t>
         </is>
       </c>
     </row>
@@ -2847,12 +2847,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Попугаев Никита А</t>
+          <t>Саттер Райли</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2862,12 +2862,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>22684</t>
+          <t>45491</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_ШДР_попугаевникитаа</t>
+          <t>1369_ШДР_саттеррайли</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:10.514645+00:00</t>
+          <t>2025-11-01T13:39:47.733244+00:00</t>
         </is>
       </c>
     </row>
@@ -2904,12 +2904,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Саттер Райли</t>
+          <t>Фу Спенсер</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2919,12 +2919,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>45491</t>
+          <t>34934</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_ШДР_саттеррайли</t>
+          <t>1369_ШДР_фуспенсер</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2939,64 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-01T07:02:10.514662+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Фу Спенсер</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>34934</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>1369_ШДР_фуспенсер</t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>2025-11-01T07:02:10.514678+00:00</t>
+          <t>2025-11-01T13:39:47.733260+00:00</t>
         </is>
       </c>
     </row>
@@ -3011,7 +2954,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3162,6 +3105,43 @@
         </is>
       </c>
       <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Попугаев Никита А</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1369_ШДР_попугаевникитаа</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-11-01T21:39:48.237159+08:00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>2025-11-01</t>
         </is>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-02 11:02:34)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,42 +495,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>АВГ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>Авангард</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>avtomobilist</t>
+          <t>avangard</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Зборовский Сергей</t>
+          <t>Якупов Наиль</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>65</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>20989</t>
+          <t>16391</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1369_АВТ_зборовскийсергей</t>
+          <t>1369_АВГ_якуповнаиль</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -540,12 +540,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
+          <t>https://www.khl.ru/clubs/avangard/team/</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-01T13:38:56.494631+00:00</t>
+          <t>2025-11-02T03:01:23.368209+00:00</t>
         </is>
       </c>
     </row>
@@ -567,27 +567,27 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Кизимов Семён</t>
+          <t>Зборовский Сергей</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>25697</t>
+          <t>20989</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1369_АВТ_кизимовсемен</t>
+          <t>1369_АВТ_зборовскийсергей</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-01T13:38:56.494651+00:00</t>
+          <t>2025-11-02T03:01:25.670423+00:00</t>
         </is>
       </c>
     </row>
@@ -624,27 +624,27 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Осипов Максим И</t>
+          <t>Кизимов Семён</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>17459</t>
+          <t>25697</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1369_АВТ_осиповмаксими</t>
+          <t>1369_АВТ_кизимовсемен</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-01T13:38:56.494662+00:00</t>
+          <t>2025-11-02T03:01:25.670454+00:00</t>
         </is>
       </c>
     </row>
@@ -681,12 +681,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Трямкин Никита</t>
+          <t>Осипов Максим И</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -696,12 +696,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>17594</t>
+          <t>17459</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1369_АВТ_трямкинникита</t>
+          <t>1369_АВТ_осиповмаксими</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -716,34 +716,34 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-01T13:38:56.494670+00:00</t>
+          <t>2025-11-02T03:01:25.670472+00:00</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>АВТ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>Автомобилист</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>admiral</t>
+          <t>avtomobilist</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Грман Марио</t>
+          <t>Трямкин Никита</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -753,12 +753,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>31232</t>
+          <t>17594</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1369_АДМ_грманмарио</t>
+          <t>1369_АВТ_трямкинникита</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -768,12 +768,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/admiral/team/</t>
+          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-01T13:38:58.709768+00:00</t>
+          <t>2025-11-02T03:01:25.670487+00:00</t>
         </is>
       </c>
     </row>
@@ -795,12 +795,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Шепелев Александр</t>
+          <t>Грман Марио</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -810,12 +810,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>23447</t>
+          <t>31232</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1369_АДМ_шепелевалександр</t>
+          <t>1369_АДМ_грманмарио</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -830,49 +830,49 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-01T13:38:58.709785+00:00</t>
+          <t>2025-11-02T03:01:28.590193+00:00</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>АКБ</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ak_bars</t>
+          <t>admiral</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Яруллин Альберт</t>
+          <t>Старков Степан</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>16365</t>
+          <t>27000</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1369_АКБ_яруллинальберт</t>
+          <t>1369_АДМ_старковстепан</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -882,39 +882,39 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
+          <t>https://www.khl.ru/clubs/admiral/team/</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:00.789879+00:00</t>
+          <t>2025-11-02T03:01:28.590222+00:00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>admiral</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Абросимов Роман</t>
+          <t>Шепелев Александр</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -924,12 +924,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>17968</t>
+          <t>23447</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1369_АМР_абросимовроман</t>
+          <t>1369_АДМ_шепелевалександр</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -939,54 +939,54 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
+          <t>https://www.khl.ru/clubs/admiral/team/</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:03.638515+00:00</t>
+          <t>2025-11-02T03:01:28.590240+00:00</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>АКБ</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>ak_bars</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Гиздатуллин Артур</t>
+          <t>Яруллин Альберт</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>22208</t>
+          <t>16365</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1369_АМР_гиздатуллинартур</t>
+          <t>1369_АКБ_яруллинальберт</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -996,54 +996,54 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
+          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:03.638545+00:00</t>
+          <t>2025-11-02T03:01:31.359836+00:00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>amur</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Абросимов Роман</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>94</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>28244</t>
+          <t>17968</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_АМР_абросимовроман</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1053,39 +1053,39 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:06.114648+00:00</t>
+          <t>2025-11-02T03:01:33.747986+00:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>amur</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Галимов Эмиль</t>
+          <t>Гиздатуллин Артур</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>87</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1095,12 +1095,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>15997</t>
+          <t>22208</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_БАР_галимовэмиль</t>
+          <t>1369_АМР_гиздатуллинартур</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1110,12 +1110,12 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:06.114676+00:00</t>
+          <t>2025-11-02T03:01:33.748015+00:00</t>
         </is>
       </c>
     </row>
@@ -1137,27 +1137,27 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Мухаметов Максим</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>25207</t>
+          <t>28244</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_БАР_мухаметовмаксим</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1172,34 +1172,34 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:06.114696+00:00</t>
+          <t>2025-11-02T03:01:36.579113+00:00</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Галимов Эмиль</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1209,12 +1209,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>15997</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_БАР_галимовэмиль</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1224,54 +1224,54 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:13.523828+00:00</t>
+          <t>2025-11-02T03:01:36.579141+00:00</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Мухаметов Максим</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>25207</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_БАР_мухаметовмаксим</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1281,39 +1281,39 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:16.465445+00:00</t>
+          <t>2025-11-02T03:01:36.579158+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1323,12 +1323,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,54 +1338,54 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:18.732826+00:00</t>
+          <t>2025-11-02T03:01:44.908863+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,39 +1395,39 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:21.104280+00:00</t>
+          <t>2025-11-02T03:01:47.647311+00:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>22683</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1452,12 +1452,12 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:21.104309+00:00</t>
+          <t>2025-11-02T03:01:50.456038+00:00</t>
         </is>
       </c>
     </row>
@@ -1479,27 +1479,27 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Профака Лука</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>43943</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_НХК_профакалука</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1514,49 +1514,49 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:21.104327+00:00</t>
+          <t>2025-11-02T03:01:53.299648+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Ващенко Григорий</t>
+          <t>Попугаев Никита О</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>14155</t>
+          <t>22683</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_СЕВ_ващенкогригорий</t>
+          <t>1369_НХК_попугаевникитао</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1566,39 +1566,39 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:23.465554+00:00</t>
+          <t>2025-11-02T03:01:53.299677+00:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Грудинин Владимир</t>
+          <t>Профака Лука</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>35064</t>
+          <t>43943</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_СЕВ_грудининвладимир</t>
+          <t>1369_НХК_профакалука</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1623,12 +1623,12 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:23.465584+00:00</t>
+          <t>2025-11-02T03:01:53.299694+00:00</t>
         </is>
       </c>
     </row>
@@ -1650,27 +1650,27 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Танков Кирилл</t>
+          <t>Ващенко Григорий</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>32981</t>
+          <t>14155</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СЕВ_танковкирилл</t>
+          <t>1369_СЕВ_ващенкогригорий</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:23.465602+00:00</t>
+          <t>2025-11-02T03:01:56.054565+00:00</t>
         </is>
       </c>
     </row>
@@ -1707,27 +1707,27 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Грудинин Владимир</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>35064</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СЕВ_грудининвладимир</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1742,34 +1742,34 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:23.465620+00:00</t>
+          <t>2025-11-02T03:01:56.054595+00:00</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Гараев Амир</t>
+          <t>Танков Кирилл</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1779,12 +1779,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>28624</t>
+          <t>32981</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гараевамир</t>
+          <t>1369_СЕВ_танковкирилл</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1794,54 +1794,54 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:32.189837+00:00</t>
+          <t>2025-11-02T03:01:56.054613+00:00</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1851,12 +1851,12 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:32.189868+00:00</t>
+          <t>2025-11-02T03:01:56.054629+00:00</t>
         </is>
       </c>
     </row>
@@ -1878,12 +1878,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Уткин Дмитрий А</t>
+          <t>Гараев Амир</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>67</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>35195</t>
+          <t>28624</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СОЧ_уткиндмитрийа</t>
+          <t>1369_СОЧ_гараевамир</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:32.189888+00:00</t>
+          <t>2025-11-02T03:02:03.131667+00:00</t>
         </is>
       </c>
     </row>
@@ -1935,27 +1935,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1970,34 +1970,34 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:32.189906+00:00</t>
+          <t>2025-11-02T03:02:03.131694+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Уткин Дмитрий А</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2007,12 +2007,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>35195</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СОЧ_уткиндмитрийа</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,54 +2022,54 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:35.019703+00:00</t>
+          <t>2025-11-02T03:02:03.131712+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,12 +2079,12 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:35.019732+00:00</t>
+          <t>2025-11-02T03:02:03.131729+00:00</t>
         </is>
       </c>
     </row>
@@ -2106,12 +2106,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2121,12 +2121,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2141,34 +2141,34 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:35.019755+00:00</t>
+          <t>2025-11-02T03:02:06.023896+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2178,12 +2178,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,39 +2193,39 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:37.449019+00:00</t>
+          <t>2025-11-02T03:02:06.023923+00:00</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2235,12 +2235,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2250,12 +2250,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:37.449049+00:00</t>
+          <t>2025-11-02T03:02:06.023940+00:00</t>
         </is>
       </c>
     </row>
@@ -2277,27 +2277,27 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:37.449067+00:00</t>
+          <t>2025-11-02T03:02:08.768466+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,12 +2334,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2349,12 +2349,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:37.449084+00:00</t>
+          <t>2025-11-02T03:02:08.768496+00:00</t>
         </is>
       </c>
     </row>
@@ -2391,27 +2391,27 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Пименов Артём</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>21205</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_пименовартем</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:37.449101+00:00</t>
+          <t>2025-11-02T03:02:08.768515+00:00</t>
         </is>
       </c>
     </row>
@@ -2448,12 +2448,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2463,12 +2463,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:37.449117+00:00</t>
+          <t>2025-11-02T03:02:08.768532+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,12 +2505,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Хохряков Пётр</t>
+          <t>Пименов Артём</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>68</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2520,12 +2520,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>15413</t>
+          <t>21205</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хохряковпетр</t>
+          <t>1369_СЮЛ_пименовартем</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:37.449138+00:00</t>
+          <t>2025-11-02T03:02:08.768549+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,12 +2562,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2597,49 +2597,49 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:37.449153+00:00</t>
+          <t>2025-11-02T03:02:08.768565+00:00</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Хохряков Пётр</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>15413</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_СЮЛ_хохряковпетр</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2649,39 +2649,39 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:40.104671+00:00</t>
+          <t>2025-11-02T03:02:08.768584+00:00</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2691,12 +2691,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2706,54 +2706,54 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:40.104700+00:00</t>
+          <t>2025-11-02T03:02:08.768598+00:00</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2763,54 +2763,54 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:44.950042+00:00</t>
+          <t>2025-11-02T03:02:11.554596+00:00</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2820,39 +2820,39 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:47.733216+00:00</t>
+          <t>2025-11-02T03:02:11.554625+00:00</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Саттер Райли</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2862,12 +2862,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>45491</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_ШДР_саттеррайли</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2877,12 +2877,12 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-01T13:39:47.733244+00:00</t>
+          <t>2025-11-02T03:02:16.899918+00:00</t>
         </is>
       </c>
     </row>
@@ -2904,42 +2904,156 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
+          <t>Гроло Жереми</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>45343</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>1369_ШДР_гроложереми</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>2025-11-02T03:02:19.257502+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Саттер Райли</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>45491</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>1369_ШДР_саттеррайли</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>2025-11-02T03:02:19.257529+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
           <t>Фу Спенсер</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="F46" t="inlineStr">
         <is>
           <t>нападающий</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="G46" t="inlineStr">
         <is>
           <t>34934</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr">
+      <c r="H46" t="inlineStr">
         <is>
           <t>1369_ШДР_фуспенсер</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
         <is>
           <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>2025-11-01T13:39:47.733260+00:00</t>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>2025-11-02T03:02:19.257545+00:00</t>
         </is>
       </c>
     </row>
@@ -2949,210 +3063,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>team_abbr</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>team_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>player_name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>player_uid</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>changed_at</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>changed_day</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>АВГ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Авангард</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Якупов Наиль</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_АВГ_якуповнаиль</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-01T11:02:16.576964+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-01</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>СЕВ</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Северсталь</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Лишка Адам</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1369_СЕВ_лишкаадам</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-11-01T11:02:16.576964+08:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-11-01</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>СЮЛ</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Салават Юлаев</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Набиев Артём</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1369_СЮЛ_набиевартем</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-11-01T11:02:16.576964+08:00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2025-11-01</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Попугаев Никита А</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>1369_ШДР_попугаевникитаа</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2025-11-01T21:39:48.237159+08:00</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2025-11-01</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3206,4 +3116,134 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>team_abbr</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>team_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>player_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>player_uid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>changed_at</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>changed_day</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>АВГ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Авангард</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Якупов Наиль</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_АВГ_якуповнаиль</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-02T11:02:19.765734+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>АДМ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Адмирал</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Старков Степан</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1369_АДМ_старковстепан</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-11-02T11:02:19.765734+08:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-11-02</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-03 18:36:28)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:23.368209+00:00</t>
+          <t>2025-11-03T09:37:27.922910+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:25.670423+00:00</t>
+          <t>2025-11-03T09:37:30.005876+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:25.670454+00:00</t>
+          <t>2025-11-03T09:37:30.005894+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:25.670472+00:00</t>
+          <t>2025-11-03T09:37:30.005902+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:25.670487+00:00</t>
+          <t>2025-11-03T09:37:30.005909+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:28.590193+00:00</t>
+          <t>2025-11-03T09:37:32.604079+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:28.590222+00:00</t>
+          <t>2025-11-03T09:37:32.604098+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:28.590240+00:00</t>
+          <t>2025-11-03T09:37:32.604106+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:31.359836+00:00</t>
+          <t>2025-11-03T09:37:34.605644+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:33.747986+00:00</t>
+          <t>2025-11-03T09:37:37.107772+00:00</t>
         </is>
       </c>
     </row>
@@ -1080,12 +1080,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Гиздатуллин Артур</t>
+          <t>Броадхёрст Алекс</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>25</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1095,12 +1095,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>22208</t>
+          <t>27232</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_АМР_гиздатуллинартур</t>
+          <t>1369_АМР_броадхерсталекс</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1115,49 +1115,49 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:33.748015+00:00</t>
+          <t>2025-11-03T09:37:37.107790+00:00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>amur</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Гиздатуллин Артур</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>87</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>28244</t>
+          <t>22208</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_АМР_гиздатуллинартур</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1167,12 +1167,12 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:36.579113+00:00</t>
+          <t>2025-11-03T09:37:37.107799+00:00</t>
         </is>
       </c>
     </row>
@@ -1194,27 +1194,27 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Галимов Эмиль</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>15997</t>
+          <t>28244</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_БАР_галимовэмиль</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:36.579141+00:00</t>
+          <t>2025-11-03T09:37:39.164043+00:00</t>
         </is>
       </c>
     </row>
@@ -1251,12 +1251,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Мухаметов Максим</t>
+          <t>Галимов Эмиль</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1266,12 +1266,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>25207</t>
+          <t>15997</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_БАР_мухаметовмаксим</t>
+          <t>1369_БАР_галимовэмиль</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1286,34 +1286,34 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:36.579158+00:00</t>
+          <t>2025-11-03T09:37:39.164060+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Мухаметов Максим</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1323,12 +1323,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>25207</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_БАР_мухаметовмаксим</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,54 +1338,54 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:44.908863+00:00</t>
+          <t>2025-11-03T09:37:39.164068+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,54 +1395,54 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:47.647311+00:00</t>
+          <t>2025-11-03T09:37:46.923301+00:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1452,39 +1452,39 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:50.456038+00:00</t>
+          <t>2025-11-03T09:37:49.502514+00:00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1494,12 +1494,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1509,12 +1509,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:53.299648+00:00</t>
+          <t>2025-11-03T09:37:51.554584+00:00</t>
         </is>
       </c>
     </row>
@@ -1536,12 +1536,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1551,12 +1551,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>22683</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:53.299677+00:00</t>
+          <t>2025-11-03T09:37:53.551575+00:00</t>
         </is>
       </c>
     </row>
@@ -1593,27 +1593,27 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Профака Лука</t>
+          <t>Попугаев Никита О</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>43943</t>
+          <t>22683</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_НХК_профакалука</t>
+          <t>1369_НХК_попугаевникитао</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1628,34 +1628,34 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:53.299694+00:00</t>
+          <t>2025-11-03T09:37:53.551592+00:00</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Ващенко Григорий</t>
+          <t>Профака Лука</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1665,12 +1665,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>14155</t>
+          <t>43943</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СЕВ_ващенкогригорий</t>
+          <t>1369_НХК_профакалука</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1680,12 +1680,12 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:56.054565+00:00</t>
+          <t>2025-11-03T09:37:53.551600+00:00</t>
         </is>
       </c>
     </row>
@@ -1707,12 +1707,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Грудинин Владимир</t>
+          <t>Ващенко Григорий</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1722,12 +1722,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>35064</t>
+          <t>14155</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СЕВ_грудининвладимир</t>
+          <t>1369_СЕВ_ващенкогригорий</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:56.054595+00:00</t>
+          <t>2025-11-03T09:37:56.001375+00:00</t>
         </is>
       </c>
     </row>
@@ -1764,27 +1764,27 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Танков Кирилл</t>
+          <t>Грудинин Владимир</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>32981</t>
+          <t>35064</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СЕВ_танковкирилл</t>
+          <t>1369_СЕВ_грудининвладимир</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:56.054613+00:00</t>
+          <t>2025-11-03T09:37:56.001396+00:00</t>
         </is>
       </c>
     </row>
@@ -1821,12 +1821,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Танков Кирилл</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1836,12 +1836,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>32981</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СЕВ_танковкирилл</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1856,34 +1856,34 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-02T03:01:56.054629+00:00</t>
+          <t>2025-11-03T09:37:56.001405+00:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Гараев Амир</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>28624</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гараевамир</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1908,12 +1908,12 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:03.131667+00:00</t>
+          <t>2025-11-03T09:37:56.001414+00:00</t>
         </is>
       </c>
     </row>
@@ -1935,27 +1935,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Гараев Амир</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>67</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>28624</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СОЧ_гараевамир</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:03.131694+00:00</t>
+          <t>2025-11-03T09:38:02.443318+00:00</t>
         </is>
       </c>
     </row>
@@ -1992,12 +1992,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Уткин Дмитрий А</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2007,12 +2007,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>35195</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_уткиндмитрийа</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:03.131712+00:00</t>
+          <t>2025-11-03T09:38:02.443359+00:00</t>
         </is>
       </c>
     </row>
@@ -2049,27 +2049,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2084,34 +2084,34 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:03.131729+00:00</t>
+          <t>2025-11-03T09:38:02.443370+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Уткин Дмитрий А</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2121,12 +2121,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>35195</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СОЧ_уткиндмитрийа</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2136,54 +2136,54 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:06.023896+00:00</t>
+          <t>2025-11-03T09:38:02.443379+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,12 +2193,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:06.023923+00:00</t>
+          <t>2025-11-03T09:38:02.443388+00:00</t>
         </is>
       </c>
     </row>
@@ -2220,12 +2220,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2235,12 +2235,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2255,34 +2255,34 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:06.023940+00:00</t>
+          <t>2025-11-03T09:38:04.864622+00:00</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2292,12 +2292,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2307,39 +2307,39 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:08.768466+00:00</t>
+          <t>2025-11-03T09:38:04.864642+00:00</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2349,12 +2349,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2364,12 +2364,12 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:08.768496+00:00</t>
+          <t>2025-11-03T09:38:04.864649+00:00</t>
         </is>
       </c>
     </row>
@@ -2391,27 +2391,27 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:08.768515+00:00</t>
+          <t>2025-11-03T09:38:06.900515+00:00</t>
         </is>
       </c>
     </row>
@@ -2448,12 +2448,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2463,12 +2463,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:08.768532+00:00</t>
+          <t>2025-11-03T09:38:06.900533+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,27 +2505,27 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Пименов Артём</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>21205</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_пименовартем</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:08.768549+00:00</t>
+          <t>2025-11-03T09:38:06.900540+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,12 +2562,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:08.768565+00:00</t>
+          <t>2025-11-03T09:38:06.900551+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,12 +2619,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Хохряков Пётр</t>
+          <t>Пименов Артём</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>68</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2634,12 +2634,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>15413</t>
+          <t>21205</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хохряковпетр</t>
+          <t>1369_СЮЛ_пименовартем</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:08.768584+00:00</t>
+          <t>2025-11-03T09:38:06.900558+00:00</t>
         </is>
       </c>
     </row>
@@ -2676,12 +2676,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2691,12 +2691,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2711,49 +2711,49 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:08.768598+00:00</t>
+          <t>2025-11-03T09:38:06.900565+00:00</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Хохряков Пётр</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>15413</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_СЮЛ_хохряковпетр</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2763,39 +2763,39 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:11.554596+00:00</t>
+          <t>2025-11-03T09:38:06.900572+00:00</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2805,12 +2805,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2820,54 +2820,54 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:11.554625+00:00</t>
+          <t>2025-11-03T09:38:06.900579+00:00</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2877,54 +2877,54 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:16.899918+00:00</t>
+          <t>2025-11-03T09:38:09.011798+00:00</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2934,39 +2934,39 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:19.257502+00:00</t>
+          <t>2025-11-03T09:38:09.011831+00:00</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Саттер Райли</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2976,12 +2976,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>45491</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_ШДР_саттеррайли</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2991,12 +2991,12 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-02T03:02:19.257529+00:00</t>
+          <t>2025-11-03T09:38:13.382184+00:00</t>
         </is>
       </c>
     </row>
@@ -3018,42 +3018,156 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
+          <t>Гроло Жереми</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>45343</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>1369_ШДР_гроложереми</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>2025-11-03T09:38:15.886898+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Саттер Райли</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>45491</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>1369_ШДР_саттеррайли</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>2025-11-03T09:38:15.886918+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
           <t>Фу Спенсер</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="F48" t="inlineStr">
         <is>
           <t>нападающий</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="G48" t="inlineStr">
         <is>
           <t>34934</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr">
+      <c r="H48" t="inlineStr">
         <is>
           <t>1369_ШДР_фуспенсер</t>
         </is>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
         <is>
           <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>2025-11-02T03:02:19.257545+00:00</t>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>2025-11-03T09:38:15.886925+00:00</t>
         </is>
       </c>
     </row>
@@ -3172,22 +3286,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>АВГ</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Авангард</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Якупов Наиль</t>
+          <t>Броадхёрст Алекс</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_АВГ_якуповнаиль</t>
+          <t>1369_АМР_броадхерсталекс</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -3197,34 +3311,34 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-02T11:02:19.765734+08:00</t>
+          <t>2025-11-03T17:38:16.389140+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-02</t>
+          <t>2025-11-03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Старков Степан</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1369_АДМ_старковстепан</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -3234,12 +3348,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-02T11:02:19.765734+08:00</t>
+          <t>2025-11-03T17:38:16.389140+08:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-11-02</t>
+          <t>2025-11-03</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-03 19:20:19)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:27.922910+00:00</t>
+          <t>2025-11-03T10:55:08.594127+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:30.005876+00:00</t>
+          <t>2025-11-03T10:55:10.750751+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:30.005894+00:00</t>
+          <t>2025-11-03T10:55:10.750773+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:30.005902+00:00</t>
+          <t>2025-11-03T10:55:10.750781+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:30.005909+00:00</t>
+          <t>2025-11-03T10:55:10.750788+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:32.604079+00:00</t>
+          <t>2025-11-03T10:55:13.334977+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:32.604098+00:00</t>
+          <t>2025-11-03T10:55:13.335009+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:32.604106+00:00</t>
+          <t>2025-11-03T10:55:13.335030+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:34.605644+00:00</t>
+          <t>2025-11-03T10:55:15.906289+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:37.107772+00:00</t>
+          <t>2025-11-03T10:55:18.068454+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:37.107790+00:00</t>
+          <t>2025-11-03T10:55:18.068486+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:37.107799+00:00</t>
+          <t>2025-11-03T10:55:18.068509+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:39.164043+00:00</t>
+          <t>2025-11-03T10:55:20.424177+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:39.164060+00:00</t>
+          <t>2025-11-03T10:55:20.424207+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:39.164068+00:00</t>
+          <t>2025-11-03T10:55:20.424227+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:46.923301+00:00</t>
+          <t>2025-11-03T10:55:27.741224+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:49.502514+00:00</t>
+          <t>2025-11-03T10:55:29.834442+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:51.554584+00:00</t>
+          <t>2025-11-03T10:55:31.955401+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:53.551575+00:00</t>
+          <t>2025-11-03T10:55:34.117199+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:53.551592+00:00</t>
+          <t>2025-11-03T10:55:34.117231+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:53.551600+00:00</t>
+          <t>2025-11-03T10:55:34.117249+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:56.001375+00:00</t>
+          <t>2025-11-03T10:55:36.701819+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:56.001396+00:00</t>
+          <t>2025-11-03T10:55:36.701838+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:56.001405+00:00</t>
+          <t>2025-11-03T10:55:36.701847+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-03T09:37:56.001414+00:00</t>
+          <t>2025-11-03T10:55:36.701855+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:02.443318+00:00</t>
+          <t>2025-11-03T10:55:43.780492+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:02.443359+00:00</t>
+          <t>2025-11-03T10:55:43.780524+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:02.443370+00:00</t>
+          <t>2025-11-03T10:55:43.780560+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:02.443379+00:00</t>
+          <t>2025-11-03T10:55:43.780589+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:02.443388+00:00</t>
+          <t>2025-11-03T10:55:43.780609+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:04.864622+00:00</t>
+          <t>2025-11-03T10:55:45.812428+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:04.864642+00:00</t>
+          <t>2025-11-03T10:55:45.812445+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:04.864649+00:00</t>
+          <t>2025-11-03T10:55:45.812453+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:06.900515+00:00</t>
+          <t>2025-11-03T10:55:48.397722+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:06.900533+00:00</t>
+          <t>2025-11-03T10:55:48.397752+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:06.900540+00:00</t>
+          <t>2025-11-03T10:55:48.397772+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:06.900551+00:00</t>
+          <t>2025-11-03T10:55:48.397793+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:06.900558+00:00</t>
+          <t>2025-11-03T10:55:48.397811+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:06.900565+00:00</t>
+          <t>2025-11-03T10:55:48.397826+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:06.900572+00:00</t>
+          <t>2025-11-03T10:55:48.397866+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:06.900579+00:00</t>
+          <t>2025-11-03T10:55:48.397900+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:09.011798+00:00</t>
+          <t>2025-11-03T10:55:50.975196+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:09.011831+00:00</t>
+          <t>2025-11-03T10:55:50.975230+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:13.382184+00:00</t>
+          <t>2025-11-03T10:55:56.197421+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:15.886898+00:00</t>
+          <t>2025-11-03T10:55:58.242309+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:15.886918+00:00</t>
+          <t>2025-11-03T10:55:58.242343+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-03T09:38:15.886925+00:00</t>
+          <t>2025-11-03T10:55:58.242365+00:00</t>
         </is>
       </c>
     </row>
@@ -3238,7 +3238,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3283,80 +3283,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>АМР</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Амур</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Броадхёрст Алекс</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_АМР_броадхерсталекс</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-03T17:38:16.389140+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-03</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>СОЧ</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ХК Сочи</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Гуськов Матвей</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1369_СОЧ_гуськовматвей</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-11-03T17:38:16.389140+08:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-11-03</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-03 19:35:26)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:08.594127+00:00</t>
+          <t>2025-11-03T11:34:29.777784+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:10.750751+00:00</t>
+          <t>2025-11-03T11:34:32.305167+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:10.750773+00:00</t>
+          <t>2025-11-03T11:34:32.305220+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:10.750781+00:00</t>
+          <t>2025-11-03T11:34:32.305229+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:10.750788+00:00</t>
+          <t>2025-11-03T11:34:32.305236+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:13.334977+00:00</t>
+          <t>2025-11-03T11:34:34.306472+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:13.335009+00:00</t>
+          <t>2025-11-03T11:34:34.306489+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:13.335030+00:00</t>
+          <t>2025-11-03T11:34:34.306498+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:15.906289+00:00</t>
+          <t>2025-11-03T11:34:36.390291+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:18.068454+00:00</t>
+          <t>2025-11-03T11:34:38.883808+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:18.068486+00:00</t>
+          <t>2025-11-03T11:34:38.883826+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:18.068509+00:00</t>
+          <t>2025-11-03T11:34:38.883835+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:20.424177+00:00</t>
+          <t>2025-11-03T11:34:40.942724+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:20.424207+00:00</t>
+          <t>2025-11-03T11:34:40.942739+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:20.424227+00:00</t>
+          <t>2025-11-03T11:34:40.942747+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:27.741224+00:00</t>
+          <t>2025-11-03T11:34:47.417874+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:29.834442+00:00</t>
+          <t>2025-11-03T11:34:49.392150+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:31.955401+00:00</t>
+          <t>2025-11-03T11:34:51.403987+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:34.117199+00:00</t>
+          <t>2025-11-03T11:34:53.417579+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:34.117231+00:00</t>
+          <t>2025-11-03T11:34:53.417626+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:34.117249+00:00</t>
+          <t>2025-11-03T11:34:53.417650+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:36.701819+00:00</t>
+          <t>2025-11-03T11:34:55.436531+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:36.701838+00:00</t>
+          <t>2025-11-03T11:34:55.436564+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:36.701847+00:00</t>
+          <t>2025-11-03T11:34:55.436584+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:36.701855+00:00</t>
+          <t>2025-11-03T11:34:55.436603+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:43.780492+00:00</t>
+          <t>2025-11-03T11:35:01.960182+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:43.780524+00:00</t>
+          <t>2025-11-03T11:35:01.960211+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:43.780560+00:00</t>
+          <t>2025-11-03T11:35:01.960230+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:43.780589+00:00</t>
+          <t>2025-11-03T11:35:01.960247+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:43.780609+00:00</t>
+          <t>2025-11-03T11:35:01.960263+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:45.812428+00:00</t>
+          <t>2025-11-03T11:35:04.845955+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:45.812445+00:00</t>
+          <t>2025-11-03T11:35:04.845972+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:45.812453+00:00</t>
+          <t>2025-11-03T11:35:04.845980+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:48.397722+00:00</t>
+          <t>2025-11-03T11:35:06.879023+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:48.397752+00:00</t>
+          <t>2025-11-03T11:35:06.879039+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:48.397772+00:00</t>
+          <t>2025-11-03T11:35:06.879047+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:48.397793+00:00</t>
+          <t>2025-11-03T11:35:06.879057+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:48.397811+00:00</t>
+          <t>2025-11-03T11:35:06.879064+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:48.397826+00:00</t>
+          <t>2025-11-03T11:35:06.879071+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:48.397866+00:00</t>
+          <t>2025-11-03T11:35:06.879078+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:48.397900+00:00</t>
+          <t>2025-11-03T11:35:06.879084+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:50.975196+00:00</t>
+          <t>2025-11-03T11:35:09.438651+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:50.975230+00:00</t>
+          <t>2025-11-03T11:35:09.438671+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:56.197421+00:00</t>
+          <t>2025-11-03T11:35:14.477756+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:58.242309+00:00</t>
+          <t>2025-11-03T11:35:16.558785+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:58.242343+00:00</t>
+          <t>2025-11-03T11:35:16.558804+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-03T10:55:58.242365+00:00</t>
+          <t>2025-11-03T11:35:16.558812+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-03 22:31:23)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:29.777784+00:00</t>
+          <t>2025-11-03T14:30:16.951441+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:32.305167+00:00</t>
+          <t>2025-11-03T14:30:19.565726+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:32.305220+00:00</t>
+          <t>2025-11-03T14:30:19.565745+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:32.305229+00:00</t>
+          <t>2025-11-03T14:30:19.565753+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:32.305236+00:00</t>
+          <t>2025-11-03T14:30:19.565760+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:34.306472+00:00</t>
+          <t>2025-11-03T14:30:21.628152+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:34.306489+00:00</t>
+          <t>2025-11-03T14:30:21.628171+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:34.306498+00:00</t>
+          <t>2025-11-03T14:30:21.628184+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:36.390291+00:00</t>
+          <t>2025-11-03T14:30:24.732073+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:38.883808+00:00</t>
+          <t>2025-11-03T14:30:27.124900+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:38.883826+00:00</t>
+          <t>2025-11-03T14:30:27.124933+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:38.883835+00:00</t>
+          <t>2025-11-03T14:30:27.124959+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:40.942724+00:00</t>
+          <t>2025-11-03T14:30:29.609195+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:40.942739+00:00</t>
+          <t>2025-11-03T14:30:29.609225+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:40.942747+00:00</t>
+          <t>2025-11-03T14:30:29.609244+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:47.417874+00:00</t>
+          <t>2025-11-03T14:30:37.332189+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:49.392150+00:00</t>
+          <t>2025-11-03T14:30:39.748394+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:51.403987+00:00</t>
+          <t>2025-11-03T14:30:42.156581+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:53.417579+00:00</t>
+          <t>2025-11-03T14:30:44.565479+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:53.417626+00:00</t>
+          <t>2025-11-03T14:30:44.565510+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:53.417650+00:00</t>
+          <t>2025-11-03T14:30:44.565528+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:55.436531+00:00</t>
+          <t>2025-11-03T14:30:47.572804+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:55.436564+00:00</t>
+          <t>2025-11-03T14:30:47.572859+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:55.436584+00:00</t>
+          <t>2025-11-03T14:30:47.572884+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,49 +1913,49 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-03T11:34:55.436603+00:00</t>
+          <t>2025-11-03T14:30:47.572907+00:00</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Гараев Амир</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>28624</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гараевамир</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1965,12 +1965,12 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:01.960182+00:00</t>
+          <t>2025-11-03T14:30:50.485280+00:00</t>
         </is>
       </c>
     </row>
@@ -1992,12 +1992,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Гараев Амир</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>67</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2007,12 +2007,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>28624</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СОЧ_гараевамир</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:01.960211+00:00</t>
+          <t>2025-11-03T14:30:56.186888+00:00</t>
         </is>
       </c>
     </row>
@@ -2049,27 +2049,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:01.960230+00:00</t>
+          <t>2025-11-03T14:30:56.186922+00:00</t>
         </is>
       </c>
     </row>
@@ -2106,27 +2106,27 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Уткин Дмитрий А</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>35195</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СОЧ_уткиндмитрийа</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:01.960247+00:00</t>
+          <t>2025-11-03T14:30:56.186948+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:01.960263+00:00</t>
+          <t>2025-11-03T14:30:56.186969+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:04.845955+00:00</t>
+          <t>2025-11-03T14:30:59.156697+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:04.845972+00:00</t>
+          <t>2025-11-03T14:30:59.156740+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:04.845980+00:00</t>
+          <t>2025-11-03T14:30:59.156828+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:06.879023+00:00</t>
+          <t>2025-11-03T14:31:01.635698+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:06.879039+00:00</t>
+          <t>2025-11-03T14:31:01.635731+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:06.879047+00:00</t>
+          <t>2025-11-03T14:31:01.635750+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:06.879057+00:00</t>
+          <t>2025-11-03T14:31:01.635772+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:06.879064+00:00</t>
+          <t>2025-11-03T14:31:01.635791+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:06.879071+00:00</t>
+          <t>2025-11-03T14:31:01.635809+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:06.879078+00:00</t>
+          <t>2025-11-03T14:31:01.635827+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:06.879084+00:00</t>
+          <t>2025-11-03T14:31:01.635843+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:09.438651+00:00</t>
+          <t>2025-11-03T14:31:04.674641+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:09.438671+00:00</t>
+          <t>2025-11-03T14:31:04.674671+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:14.477756+00:00</t>
+          <t>2025-11-03T14:31:09.448830+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:16.558785+00:00</t>
+          <t>2025-11-03T14:31:11.823436+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:16.558804+00:00</t>
+          <t>2025-11-03T14:31:11.823465+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-03T11:35:16.558812+00:00</t>
+          <t>2025-11-03T14:31:11.823482+00:00</t>
         </is>
       </c>
     </row>
@@ -3182,7 +3182,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3224,6 +3224,43 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>changed_day</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>СОЧ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Уткин Дмитрий А</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_СОЧ_уткиндмитрийа</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-03T22:31:12.326868+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-03</t>
         </is>
       </c>
     </row>
@@ -3238,7 +3275,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3283,6 +3320,43 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>СИБ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Приски Чейз Эванс</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_СИБ_прискичейзэванс</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-03T22:31:12.326868+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-03</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-03 23:41:17)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:16.951441+00:00</t>
+          <t>2025-11-03T15:40:13.087744+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:19.565726+00:00</t>
+          <t>2025-11-03T15:40:15.194452+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:19.565745+00:00</t>
+          <t>2025-11-03T15:40:15.194471+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:19.565753+00:00</t>
+          <t>2025-11-03T15:40:15.194479+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:19.565760+00:00</t>
+          <t>2025-11-03T15:40:15.194487+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:21.628152+00:00</t>
+          <t>2025-11-03T15:40:17.351523+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:21.628171+00:00</t>
+          <t>2025-11-03T15:40:17.351578+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:21.628184+00:00</t>
+          <t>2025-11-03T15:40:17.351604+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:24.732073+00:00</t>
+          <t>2025-11-03T15:40:19.611904+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:27.124900+00:00</t>
+          <t>2025-11-03T15:40:22.490728+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:27.124933+00:00</t>
+          <t>2025-11-03T15:40:22.490759+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:27.124959+00:00</t>
+          <t>2025-11-03T15:40:22.490779+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:29.609195+00:00</t>
+          <t>2025-11-03T15:40:24.847730+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:29.609225+00:00</t>
+          <t>2025-11-03T15:40:24.847758+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:29.609244+00:00</t>
+          <t>2025-11-03T15:40:24.847776+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:37.332189+00:00</t>
+          <t>2025-11-03T15:40:32.598800+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:39.748394+00:00</t>
+          <t>2025-11-03T15:40:34.937654+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:42.156581+00:00</t>
+          <t>2025-11-03T15:40:37.424167+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:44.565479+00:00</t>
+          <t>2025-11-03T15:40:39.850285+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:44.565510+00:00</t>
+          <t>2025-11-03T15:40:39.850317+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:44.565528+00:00</t>
+          <t>2025-11-03T15:40:39.850335+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:47.572804+00:00</t>
+          <t>2025-11-03T15:40:42.368164+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:47.572859+00:00</t>
+          <t>2025-11-03T15:40:42.368198+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:47.572884+00:00</t>
+          <t>2025-11-03T15:40:42.368219+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:47.572907+00:00</t>
+          <t>2025-11-03T15:40:42.368240+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:50.485280+00:00</t>
+          <t>2025-11-03T15:40:44.738644+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:56.186888+00:00</t>
+          <t>2025-11-03T15:40:49.938718+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:56.186922+00:00</t>
+          <t>2025-11-03T15:40:49.938752+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:56.186948+00:00</t>
+          <t>2025-11-03T15:40:49.938770+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:56.186969+00:00</t>
+          <t>2025-11-03T15:40:49.938786+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:59.156697+00:00</t>
+          <t>2025-11-03T15:40:52.319933+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:59.156740+00:00</t>
+          <t>2025-11-03T15:40:52.319965+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-03T14:30:59.156828+00:00</t>
+          <t>2025-11-03T15:40:52.319985+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:01.635698+00:00</t>
+          <t>2025-11-03T15:40:54.647538+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:01.635731+00:00</t>
+          <t>2025-11-03T15:40:54.647570+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:01.635750+00:00</t>
+          <t>2025-11-03T15:40:54.647589+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:01.635772+00:00</t>
+          <t>2025-11-03T15:40:54.647606+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:01.635791+00:00</t>
+          <t>2025-11-03T15:40:54.647623+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:01.635809+00:00</t>
+          <t>2025-11-03T15:40:54.647669+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:01.635827+00:00</t>
+          <t>2025-11-03T15:40:54.647688+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:01.635843+00:00</t>
+          <t>2025-11-03T15:40:54.647708+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:04.674641+00:00</t>
+          <t>2025-11-03T15:40:57.622509+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:04.674671+00:00</t>
+          <t>2025-11-03T15:40:57.622539+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:09.448830+00:00</t>
+          <t>2025-11-03T15:41:02.919375+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:11.823436+00:00</t>
+          <t>2025-11-03T15:41:05.312080+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:11.823465+00:00</t>
+          <t>2025-11-03T15:41:05.312108+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-03T14:31:11.823482+00:00</t>
+          <t>2025-11-03T15:41:05.312125+00:00</t>
         </is>
       </c>
     </row>
@@ -3275,7 +3275,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3320,43 +3320,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>СИБ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Сибирь</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Приски Чейз Эванс</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_СИБ_прискичейзэванс</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-03T22:31:12.326868+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-03</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-04 11:02:35)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:13.087744+00:00</t>
+          <t>2025-11-04T03:01:21.943800+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:15.194452+00:00</t>
+          <t>2025-11-04T03:01:24.400433+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:15.194471+00:00</t>
+          <t>2025-11-04T03:01:24.400465+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:15.194479+00:00</t>
+          <t>2025-11-04T03:01:24.400486+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:15.194487+00:00</t>
+          <t>2025-11-04T03:01:24.400504+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:17.351523+00:00</t>
+          <t>2025-11-04T03:01:27.230266+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:17.351578+00:00</t>
+          <t>2025-11-04T03:01:27.230297+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:17.351604+00:00</t>
+          <t>2025-11-04T03:01:27.230318+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:19.611904+00:00</t>
+          <t>2025-11-04T03:01:29.710602+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:22.490728+00:00</t>
+          <t>2025-11-04T03:01:32.526580+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:22.490759+00:00</t>
+          <t>2025-11-04T03:01:32.526610+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:22.490779+00:00</t>
+          <t>2025-11-04T03:01:32.526629+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:24.847730+00:00</t>
+          <t>2025-11-04T03:01:34.962576+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:24.847758+00:00</t>
+          <t>2025-11-04T03:01:34.962606+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:24.847776+00:00</t>
+          <t>2025-11-04T03:01:34.962625+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:32.598800+00:00</t>
+          <t>2025-11-04T03:01:42.962209+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:34.937654+00:00</t>
+          <t>2025-11-04T03:01:45.794200+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:37.424167+00:00</t>
+          <t>2025-11-04T03:01:48.643522+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:39.850285+00:00</t>
+          <t>2025-11-04T03:01:51.465313+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:39.850317+00:00</t>
+          <t>2025-11-04T03:01:51.465347+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:39.850335+00:00</t>
+          <t>2025-11-04T03:01:51.465366+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:42.368164+00:00</t>
+          <t>2025-11-04T03:01:54.294694+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:42.368198+00:00</t>
+          <t>2025-11-04T03:01:54.294732+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:42.368219+00:00</t>
+          <t>2025-11-04T03:01:54.294758+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:42.368240+00:00</t>
+          <t>2025-11-04T03:01:54.294781+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:44.738644+00:00</t>
+          <t>2025-11-04T03:01:57.183621+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:49.938718+00:00</t>
+          <t>2025-11-04T03:02:02.767469+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:49.938752+00:00</t>
+          <t>2025-11-04T03:02:02.767499+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:49.938770+00:00</t>
+          <t>2025-11-04T03:02:02.767518+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:49.938786+00:00</t>
+          <t>2025-11-04T03:02:02.767536+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:52.319933+00:00</t>
+          <t>2025-11-04T03:02:05.197237+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:52.319965+00:00</t>
+          <t>2025-11-04T03:02:05.197266+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:52.319985+00:00</t>
+          <t>2025-11-04T03:02:05.197284+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:54.647538+00:00</t>
+          <t>2025-11-04T03:02:07.878221+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:54.647570+00:00</t>
+          <t>2025-11-04T03:02:07.878258+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:54.647589+00:00</t>
+          <t>2025-11-04T03:02:07.878278+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:54.647606+00:00</t>
+          <t>2025-11-04T03:02:07.878296+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:54.647623+00:00</t>
+          <t>2025-11-04T03:02:07.878314+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:54.647669+00:00</t>
+          <t>2025-11-04T03:02:07.878330+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:54.647688+00:00</t>
+          <t>2025-11-04T03:02:07.878345+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:54.647708+00:00</t>
+          <t>2025-11-04T03:02:07.878360+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:57.622509+00:00</t>
+          <t>2025-11-04T03:02:10.818065+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-03T15:40:57.622539+00:00</t>
+          <t>2025-11-04T03:02:10.818095+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-03T15:41:02.919375+00:00</t>
+          <t>2025-11-04T03:02:16.783416+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-03T15:41:05.312080+00:00</t>
+          <t>2025-11-04T03:02:19.654083+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-03T15:41:05.312108+00:00</t>
+          <t>2025-11-04T03:02:19.654112+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-03T15:41:05.312125+00:00</t>
+          <t>2025-11-04T03:02:19.654130+00:00</t>
         </is>
       </c>
     </row>
@@ -3182,7 +3182,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3224,43 +3224,6 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>changed_day</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>СОЧ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ХК Сочи</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Уткин Дмитрий А</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_СОЧ_уткиндмитрийа</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-03T22:31:12.326868+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-03</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-04 15:02:29)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:21.943800+00:00</t>
+          <t>2025-11-04T07:01:19.713733+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:24.400433+00:00</t>
+          <t>2025-11-04T07:01:22.038322+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:24.400465+00:00</t>
+          <t>2025-11-04T07:01:22.038357+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:24.400486+00:00</t>
+          <t>2025-11-04T07:01:22.038377+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:24.400504+00:00</t>
+          <t>2025-11-04T07:01:22.038394+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:27.230266+00:00</t>
+          <t>2025-11-04T07:01:24.391853+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:27.230297+00:00</t>
+          <t>2025-11-04T07:01:24.391883+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:27.230318+00:00</t>
+          <t>2025-11-04T07:01:24.391903+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:29.710602+00:00</t>
+          <t>2025-11-04T07:01:27.199711+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:32.526580+00:00</t>
+          <t>2025-11-04T07:01:29.652989+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:32.526610+00:00</t>
+          <t>2025-11-04T07:01:29.653021+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:32.526629+00:00</t>
+          <t>2025-11-04T07:01:29.653040+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:34.962576+00:00</t>
+          <t>2025-11-04T07:01:32.034472+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:34.962606+00:00</t>
+          <t>2025-11-04T07:01:32.034501+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:34.962625+00:00</t>
+          <t>2025-11-04T07:01:32.034520+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:42.962209+00:00</t>
+          <t>2025-11-04T07:01:40.359711+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:45.794200+00:00</t>
+          <t>2025-11-04T07:01:43.168626+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:48.643522+00:00</t>
+          <t>2025-11-04T07:01:45.558741+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:51.465313+00:00</t>
+          <t>2025-11-04T07:01:48.459900+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:51.465347+00:00</t>
+          <t>2025-11-04T07:01:48.459933+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:51.465366+00:00</t>
+          <t>2025-11-04T07:01:48.459953+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:54.294694+00:00</t>
+          <t>2025-11-04T07:01:51.229533+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:54.294732+00:00</t>
+          <t>2025-11-04T07:01:51.229565+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:54.294758+00:00</t>
+          <t>2025-11-04T07:01:51.229585+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:54.294781+00:00</t>
+          <t>2025-11-04T07:01:51.229604+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-04T03:01:57.183621+00:00</t>
+          <t>2025-11-04T07:01:53.600381+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:02.767469+00:00</t>
+          <t>2025-11-04T07:01:59.412704+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:02.767499+00:00</t>
+          <t>2025-11-04T07:01:59.412733+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:02.767518+00:00</t>
+          <t>2025-11-04T07:01:59.412751+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:02.767536+00:00</t>
+          <t>2025-11-04T07:01:59.412768+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:05.197237+00:00</t>
+          <t>2025-11-04T07:02:02.190670+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:05.197266+00:00</t>
+          <t>2025-11-04T07:02:02.190700+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:05.197284+00:00</t>
+          <t>2025-11-04T07:02:02.190717+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:07.878221+00:00</t>
+          <t>2025-11-04T07:02:04.547944+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:07.878258+00:00</t>
+          <t>2025-11-04T07:02:04.547974+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:07.878278+00:00</t>
+          <t>2025-11-04T07:02:04.547991+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:07.878296+00:00</t>
+          <t>2025-11-04T07:02:04.548011+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:07.878314+00:00</t>
+          <t>2025-11-04T07:02:04.548028+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:07.878330+00:00</t>
+          <t>2025-11-04T07:02:04.548044+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:07.878345+00:00</t>
+          <t>2025-11-04T07:02:04.548060+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:07.878360+00:00</t>
+          <t>2025-11-04T07:02:04.548074+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:10.818065+00:00</t>
+          <t>2025-11-04T07:02:07.540940+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:10.818095+00:00</t>
+          <t>2025-11-04T07:02:07.540970+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:16.783416+00:00</t>
+          <t>2025-11-04T07:02:12.225726+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:19.654083+00:00</t>
+          <t>2025-11-04T07:02:14.586792+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:19.654112+00:00</t>
+          <t>2025-11-04T07:02:14.586823+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-04T03:02:19.654130+00:00</t>
+          <t>2025-11-04T07:02:14.586842+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-04 16:10:48)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:19.713733+00:00</t>
+          <t>2025-11-04T08:09:42.195876+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:22.038322+00:00</t>
+          <t>2025-11-04T08:09:44.363659+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:22.038357+00:00</t>
+          <t>2025-11-04T08:09:44.363705+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:22.038377+00:00</t>
+          <t>2025-11-04T08:09:44.363722+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:22.038394+00:00</t>
+          <t>2025-11-04T08:09:44.363733+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:24.391853+00:00</t>
+          <t>2025-11-04T08:09:46.433019+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:24.391883+00:00</t>
+          <t>2025-11-04T08:09:46.433037+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:24.391903+00:00</t>
+          <t>2025-11-04T08:09:46.433045+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:27.199711+00:00</t>
+          <t>2025-11-04T08:09:48.531867+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:29.652989+00:00</t>
+          <t>2025-11-04T08:09:50.897622+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:29.653021+00:00</t>
+          <t>2025-11-04T08:09:50.897652+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:29.653040+00:00</t>
+          <t>2025-11-04T08:09:50.897675+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:32.034472+00:00</t>
+          <t>2025-11-04T08:09:53.727805+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:32.034501+00:00</t>
+          <t>2025-11-04T08:09:53.727836+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:32.034520+00:00</t>
+          <t>2025-11-04T08:09:53.727856+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:40.359711+00:00</t>
+          <t>2025-11-04T08:10:01.279786+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:43.168626+00:00</t>
+          <t>2025-11-04T08:10:03.707815+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:45.558741+00:00</t>
+          <t>2025-11-04T08:10:06.460254+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:48.459900+00:00</t>
+          <t>2025-11-04T08:10:08.848527+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:48.459933+00:00</t>
+          <t>2025-11-04T08:10:08.848563+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:48.459953+00:00</t>
+          <t>2025-11-04T08:10:08.848582+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:51.229533+00:00</t>
+          <t>2025-11-04T08:10:11.932232+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:51.229565+00:00</t>
+          <t>2025-11-04T08:10:11.932261+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:51.229585+00:00</t>
+          <t>2025-11-04T08:10:11.932278+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:51.229604+00:00</t>
+          <t>2025-11-04T08:10:11.932294+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:53.600381+00:00</t>
+          <t>2025-11-04T08:10:14.768267+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:59.412704+00:00</t>
+          <t>2025-11-04T08:10:20.082879+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:59.412733+00:00</t>
+          <t>2025-11-04T08:10:20.082907+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:59.412751+00:00</t>
+          <t>2025-11-04T08:10:20.082925+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-04T07:01:59.412768+00:00</t>
+          <t>2025-11-04T08:10:20.082940+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:02.190670+00:00</t>
+          <t>2025-11-04T08:10:22.942530+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:02.190700+00:00</t>
+          <t>2025-11-04T08:10:22.942562+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:02.190717+00:00</t>
+          <t>2025-11-04T08:10:22.942582+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:04.547944+00:00</t>
+          <t>2025-11-04T08:10:25.295460+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:04.547974+00:00</t>
+          <t>2025-11-04T08:10:25.295491+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:04.547991+00:00</t>
+          <t>2025-11-04T08:10:25.295509+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:04.548011+00:00</t>
+          <t>2025-11-04T08:10:25.295529+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:04.548028+00:00</t>
+          <t>2025-11-04T08:10:25.295546+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:04.548044+00:00</t>
+          <t>2025-11-04T08:10:25.295562+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:04.548060+00:00</t>
+          <t>2025-11-04T08:10:25.295578+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:04.548074+00:00</t>
+          <t>2025-11-04T08:10:25.295592+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:07.540940+00:00</t>
+          <t>2025-11-04T08:10:28.147609+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:07.540970+00:00</t>
+          <t>2025-11-04T08:10:28.147643+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:12.225726+00:00</t>
+          <t>2025-11-04T08:10:32.846275+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:14.586792+00:00</t>
+          <t>2025-11-04T08:10:35.260010+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:14.586823+00:00</t>
+          <t>2025-11-04T08:10:35.260040+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-04T07:02:14.586842+00:00</t>
+          <t>2025-11-04T08:10:35.260060+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-04 17:23:59)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:42.195876+00:00</t>
+          <t>2025-11-04T09:22:56.615985+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:44.363659+00:00</t>
+          <t>2025-11-04T09:22:59.139224+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:44.363705+00:00</t>
+          <t>2025-11-04T09:22:59.139245+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:44.363722+00:00</t>
+          <t>2025-11-04T09:22:59.139272+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:44.363733+00:00</t>
+          <t>2025-11-04T09:22:59.139280+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:46.433019+00:00</t>
+          <t>2025-11-04T09:23:01.216155+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:46.433037+00:00</t>
+          <t>2025-11-04T09:23:01.216195+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:46.433045+00:00</t>
+          <t>2025-11-04T09:23:01.216219+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:48.531867+00:00</t>
+          <t>2025-11-04T09:23:03.917959+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:50.897622+00:00</t>
+          <t>2025-11-04T09:23:06.320029+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:50.897652+00:00</t>
+          <t>2025-11-04T09:23:06.320060+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:50.897675+00:00</t>
+          <t>2025-11-04T09:23:06.320079+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:53.727805+00:00</t>
+          <t>2025-11-04T09:23:08.784893+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:53.727836+00:00</t>
+          <t>2025-11-04T09:23:08.784924+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,49 +1343,49 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-04T08:09:53.727856+00:00</t>
+          <t>2025-11-04T09:23:08.784944+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Уотерспун Тайлер</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>26</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>45769</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_БАР_уотерспунтайлер</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,54 +1395,54 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:01.279786+00:00</t>
+          <t>2025-11-04T09:23:08.784962+00:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1452,54 +1452,54 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:03.707815+00:00</t>
+          <t>2025-11-04T09:23:16.357275+00:00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1509,39 +1509,39 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:06.460254+00:00</t>
+          <t>2025-11-04T09:23:18.733981+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1551,12 +1551,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1566,12 +1566,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:08.848527+00:00</t>
+          <t>2025-11-04T09:23:21.645334+00:00</t>
         </is>
       </c>
     </row>
@@ -1593,12 +1593,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>22683</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:08.848563+00:00</t>
+          <t>2025-11-04T09:23:24.489597+00:00</t>
         </is>
       </c>
     </row>
@@ -1650,27 +1650,27 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Профака Лука</t>
+          <t>Попугаев Никита О</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>43943</t>
+          <t>22683</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_НХК_профакалука</t>
+          <t>1369_НХК_попугаевникитао</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1685,34 +1685,34 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:08.848582+00:00</t>
+          <t>2025-11-04T09:23:24.489629+00:00</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Ващенко Григорий</t>
+          <t>Профака Лука</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1722,12 +1722,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>14155</t>
+          <t>43943</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СЕВ_ващенкогригорий</t>
+          <t>1369_НХК_профакалука</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1737,12 +1737,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:11.932232+00:00</t>
+          <t>2025-11-04T09:23:24.489647+00:00</t>
         </is>
       </c>
     </row>
@@ -1764,12 +1764,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Грудинин Владимир</t>
+          <t>Ващенко Григорий</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1779,12 +1779,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>35064</t>
+          <t>14155</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СЕВ_грудининвладимир</t>
+          <t>1369_СЕВ_ващенкогригорий</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:11.932261+00:00</t>
+          <t>2025-11-04T09:23:27.113355+00:00</t>
         </is>
       </c>
     </row>
@@ -1821,27 +1821,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Танков Кирилл</t>
+          <t>Грудинин Владимир</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>32981</t>
+          <t>35064</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СЕВ_танковкирилл</t>
+          <t>1369_СЕВ_грудининвладимир</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:11.932278+00:00</t>
+          <t>2025-11-04T09:23:27.113386+00:00</t>
         </is>
       </c>
     </row>
@@ -1878,12 +1878,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Танков Кирилл</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>32981</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СЕВ_танковкирилл</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1913,49 +1913,49 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:11.932294+00:00</t>
+          <t>2025-11-04T09:23:27.113406+00:00</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1965,54 +1965,54 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:14.768267+00:00</t>
+          <t>2025-11-04T09:23:27.113424+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Гараев Амир</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>28624</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гараевамир</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,12 +2022,12 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:20.082879+00:00</t>
+          <t>2025-11-04T09:23:29.222616+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:20.082907+00:00</t>
+          <t>2025-11-04T09:23:33.391115+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:20.082925+00:00</t>
+          <t>2025-11-04T09:23:33.391147+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:20.082940+00:00</t>
+          <t>2025-11-04T09:23:33.391167+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:22.942530+00:00</t>
+          <t>2025-11-04T09:23:35.898391+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:22.942562+00:00</t>
+          <t>2025-11-04T09:23:35.898421+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:22.942582+00:00</t>
+          <t>2025-11-04T09:23:35.898440+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:25.295460+00:00</t>
+          <t>2025-11-04T09:23:38.075626+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:25.295491+00:00</t>
+          <t>2025-11-04T09:23:38.075661+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:25.295509+00:00</t>
+          <t>2025-11-04T09:23:38.075675+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:25.295529+00:00</t>
+          <t>2025-11-04T09:23:38.075688+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:25.295546+00:00</t>
+          <t>2025-11-04T09:23:38.075701+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:25.295562+00:00</t>
+          <t>2025-11-04T09:23:38.075714+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:25.295578+00:00</t>
+          <t>2025-11-04T09:23:38.075734+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:25.295592+00:00</t>
+          <t>2025-11-04T09:23:38.075745+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:28.147609+00:00</t>
+          <t>2025-11-04T09:23:40.181569+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:28.147643+00:00</t>
+          <t>2025-11-04T09:23:40.181602+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:32.846275+00:00</t>
+          <t>2025-11-04T09:23:44.806068+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:35.260010+00:00</t>
+          <t>2025-11-04T09:23:47.510765+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:35.260040+00:00</t>
+          <t>2025-11-04T09:23:47.510794+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-04T08:10:35.260060+00:00</t>
+          <t>2025-11-04T09:23:47.510812+00:00</t>
         </is>
       </c>
     </row>
@@ -3182,7 +3182,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3224,6 +3224,43 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>changed_day</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>СОЧ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Гараев Амир</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_СОЧ_гараевамир</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-04T17:23:48.013752+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
         </is>
       </c>
     </row>
@@ -3238,7 +3275,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3283,6 +3320,43 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>БАР</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Барыс</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Уотерспун Тайлер</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_БАР_уотерспунтайлер</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-04T17:23:48.013752+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-06 11:04:34)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,42 +495,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>АВГ</t>
+          <t>АВТ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Авангард</t>
+          <t>Автомобилист</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>avangard</t>
+          <t>avtomobilist</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Якупов Наиль</t>
+          <t>Зборовский Сергей</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>16391</t>
+          <t>20989</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1369_АВГ_якуповнаиль</t>
+          <t>1369_АВТ_зборовскийсергей</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -540,12 +540,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/avangard/team/</t>
+          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-04T09:22:56.615985+00:00</t>
+          <t>2025-11-06T03:03:07.232150+00:00</t>
         </is>
       </c>
     </row>
@@ -567,27 +567,27 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Зборовский Сергей</t>
+          <t>Кизимов Семён</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>20989</t>
+          <t>25697</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1369_АВТ_зборовскийсергей</t>
+          <t>1369_АВТ_кизимовсемен</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-04T09:22:59.139224+00:00</t>
+          <t>2025-11-06T03:03:07.232183+00:00</t>
         </is>
       </c>
     </row>
@@ -624,27 +624,27 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Кизимов Семён</t>
+          <t>Трямкин Никита</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>25697</t>
+          <t>17594</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1369_АВТ_кизимовсемен</t>
+          <t>1369_АВТ_трямкинникита</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -659,34 +659,34 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-04T09:22:59.139245+00:00</t>
+          <t>2025-11-06T03:03:07.232202+00:00</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>avtomobilist</t>
+          <t>admiral</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Осипов Максим И</t>
+          <t>Грман Марио</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -696,12 +696,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>17459</t>
+          <t>31232</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1369_АВТ_осиповмаксими</t>
+          <t>1369_АДМ_грманмарио</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -711,54 +711,54 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
+          <t>https://www.khl.ru/clubs/admiral/team/</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-04T09:22:59.139272+00:00</t>
+          <t>2025-11-06T03:03:09.942523+00:00</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>avtomobilist</t>
+          <t>admiral</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Трямкин Никита</t>
+          <t>Старков Степан</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>17594</t>
+          <t>27000</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1369_АВТ_трямкинникита</t>
+          <t>1369_АДМ_старковстепан</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -768,12 +768,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
+          <t>https://www.khl.ru/clubs/admiral/team/</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-04T09:22:59.139280+00:00</t>
+          <t>2025-11-06T03:03:09.942551+00:00</t>
         </is>
       </c>
     </row>
@@ -795,12 +795,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Грман Марио</t>
+          <t>Шепелев Александр</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -810,12 +810,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>31232</t>
+          <t>23447</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1369_АДМ_грманмарио</t>
+          <t>1369_АДМ_шепелевалександр</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -830,49 +830,49 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:01.216155+00:00</t>
+          <t>2025-11-06T03:03:09.942569+00:00</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>АКБ</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>admiral</t>
+          <t>ak_bars</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Старков Степан</t>
+          <t>Яруллин Альберт</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>27000</t>
+          <t>16365</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1369_АДМ_старковстепан</t>
+          <t>1369_АКБ_яруллинальберт</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -882,39 +882,39 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/admiral/team/</t>
+          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:01.216195+00:00</t>
+          <t>2025-11-06T03:03:12.784177+00:00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>admiral</t>
+          <t>amur</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Шепелев Александр</t>
+          <t>Абросимов Роман</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>94</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -924,12 +924,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>23447</t>
+          <t>17968</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1369_АДМ_шепелевалександр</t>
+          <t>1369_АМР_абросимовроман</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -939,54 +939,54 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/admiral/team/</t>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:01.216219+00:00</t>
+          <t>2025-11-06T03:03:15.639309+00:00</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>АКБ</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ak_bars</t>
+          <t>amur</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Яруллин Альберт</t>
+          <t>Броадхёрст Алекс</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>25</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>16365</t>
+          <t>27232</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1369_АКБ_яруллинальберт</t>
+          <t>1369_АМР_броадхерсталекс</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -996,12 +996,12 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:03.917959+00:00</t>
+          <t>2025-11-06T03:03:15.639339+00:00</t>
         </is>
       </c>
     </row>
@@ -1023,27 +1023,27 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Абросимов Роман</t>
+          <t>Гиздатуллин Артур</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>87</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>17968</t>
+          <t>22208</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1369_АМР_абросимовроман</t>
+          <t>1369_АМР_гиздатуллинартур</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1058,49 +1058,49 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:06.320029+00:00</t>
+          <t>2025-11-06T03:03:15.639356+00:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Броадхёрст Алекс</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>27232</t>
+          <t>28244</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_АМР_броадхерсталекс</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1110,39 +1110,39 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:06.320060+00:00</t>
+          <t>2025-11-06T03:03:18.553449+00:00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Гиздатуллин Артур</t>
+          <t>Галимов Эмиль</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>22208</t>
+          <t>15997</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_АМР_гиздатуллинартур</t>
+          <t>1369_БАР_галимовэмиль</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1167,12 +1167,12 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:06.320079+00:00</t>
+          <t>2025-11-06T03:03:18.553480+00:00</t>
         </is>
       </c>
     </row>
@@ -1194,27 +1194,27 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Мухаметов Максим</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>28244</t>
+          <t>25207</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_БАР_мухаметовмаксим</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:08.784893+00:00</t>
+          <t>2025-11-06T03:03:18.553497+00:00</t>
         </is>
       </c>
     </row>
@@ -1251,27 +1251,27 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Галимов Эмиль</t>
+          <t>Уотерспун Тайлер</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>26</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>15997</t>
+          <t>45769</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_БАР_галимовэмиль</t>
+          <t>1369_БАР_уотерспунтайлер</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1286,49 +1286,49 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:08.784924+00:00</t>
+          <t>2025-11-06T03:03:18.553512+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>ДМН</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>dinamo_mn</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Мухаметов Максим</t>
+          <t>Уэлле Ксавье</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>25207</t>
+          <t>19692</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_БАР_мухаметовмаксим</t>
+          <t>1369_ДМН_уэллексавье</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,54 +1338,54 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:08.784944+00:00</t>
+          <t>2025-11-06T03:03:23.666647+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Уотерспун Тайлер</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>45769</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_БАР_уотерспунтайлер</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,39 +1395,39 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:08.784962+00:00</t>
+          <t>2025-11-06T03:03:30.751192+00:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Волков Александр С</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_ЛОК_волковалександрс</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1452,12 +1452,12 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:16.357275+00:00</t>
+          <t>2025-11-06T03:03:33.507697+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:18.733981+00:00</t>
+          <t>2025-11-06T03:03:33.507727+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:21.645334+00:00</t>
+          <t>2025-11-06T03:03:36.297199+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:24.489597+00:00</t>
+          <t>2025-11-06T03:03:39.088707+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:24.489629+00:00</t>
+          <t>2025-11-06T03:03:39.088736+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:24.489647+00:00</t>
+          <t>2025-11-06T03:03:39.088753+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:27.113355+00:00</t>
+          <t>2025-11-06T03:03:42.011481+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:27.113386+00:00</t>
+          <t>2025-11-06T03:03:42.011509+00:00</t>
         </is>
       </c>
     </row>
@@ -1878,12 +1878,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Танков Кирилл</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>32981</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СЕВ_танковкирилл</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1913,49 +1913,49 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:27.113406+00:00</t>
+          <t>2025-11-06T03:03:42.011526+00:00</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Гордеев Фёдор</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>43049</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СИБ_гордеевфедор</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1965,12 +1965,12 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:27.113424+00:00</t>
+          <t>2025-11-06T03:03:44.304124+00:00</t>
         </is>
       </c>
     </row>
@@ -1992,12 +1992,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Калиниченко Роман</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2007,12 +2007,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>26690</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СИБ_калиниченкороман</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2027,49 +2027,49 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:29.222616+00:00</t>
+          <t>2025-11-06T03:03:44.304153+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,54 +2079,54 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:33.391115+00:00</t>
+          <t>2025-11-06T03:03:44.304171+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2136,54 +2136,54 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:33.391147+00:00</t>
+          <t>2025-11-06T03:03:44.304187+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,39 +2193,39 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:33.391167+00:00</t>
+          <t>2025-11-06T03:03:47.022280+00:00</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2235,12 +2235,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2250,54 +2250,54 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:35.898391+00:00</t>
+          <t>2025-11-06T03:03:49.360588+00:00</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2307,54 +2307,54 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:35.898421+00:00</t>
+          <t>2025-11-06T03:03:49.360633+00:00</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2364,39 +2364,39 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:35.898440+00:00</t>
+          <t>2025-11-06T03:03:49.360650+00:00</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2406,12 +2406,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2421,39 +2421,39 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:38.075626+00:00</t>
+          <t>2025-11-06T03:03:52.096236+00:00</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2463,12 +2463,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2478,54 +2478,54 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:38.075661+00:00</t>
+          <t>2025-11-06T03:03:52.096264+00:00</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2535,12 +2535,12 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:38.075675+00:00</t>
+          <t>2025-11-06T03:03:52.096281+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,12 +2562,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:38.075688+00:00</t>
+          <t>2025-11-06T03:04:02.818935+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,12 +2619,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Пименов Артём</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2634,12 +2634,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>21205</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_пименовартем</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:38.075701+00:00</t>
+          <t>2025-11-06T03:04:02.818969+00:00</t>
         </is>
       </c>
     </row>
@@ -2676,27 +2676,27 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:38.075714+00:00</t>
+          <t>2025-11-06T03:04:02.818987+00:00</t>
         </is>
       </c>
     </row>
@@ -2733,12 +2733,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Хохряков Пётр</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2748,12 +2748,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>15413</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хохряковпетр</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:38.075734+00:00</t>
+          <t>2025-11-06T03:04:02.819002+00:00</t>
         </is>
       </c>
     </row>
@@ -2790,12 +2790,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Пименов Артём</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>68</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2805,12 +2805,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>21205</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_СЮЛ_пименовартем</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2825,49 +2825,49 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:38.075745+00:00</t>
+          <t>2025-11-06T03:04:02.819018+00:00</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2877,39 +2877,39 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:40.181569+00:00</t>
+          <t>2025-11-06T03:04:02.819047+00:00</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Хохряков Пётр</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2919,12 +2919,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>15413</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_СЮЛ_хохряковпетр</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2934,39 +2934,39 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:40.181602+00:00</t>
+          <t>2025-11-06T03:04:02.819063+00:00</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2976,12 +2976,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2991,39 +2991,39 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:44.806068+00:00</t>
+          <t>2025-11-06T03:04:02.819076+00:00</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3033,12 +3033,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3048,39 +3048,39 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:47.510765+00:00</t>
+          <t>2025-11-06T03:04:05.716507+00:00</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Саттер Райли</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3090,12 +3090,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>45491</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>1369_ШДР_саттеррайли</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -3105,69 +3105,240 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-04T09:23:47.510794+00:00</t>
+          <t>2025-11-06T03:04:05.716536+00:00</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>cska</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Моисеев Данила</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>23931</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_моисеевданила</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>2025-11-06T03:04:15.611382+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>cska</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Уильямс Колби</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>41896</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_уильямсколби</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>2025-11-06T03:04:15.611411+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
           <t>ШДР</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B50" t="inlineStr">
         <is>
           <t>Драконы</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>kunlun</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Фу Спенсер</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Гроло Жереми</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>45343</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>1369_ШДР_гроложереми</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>2025-11-06T03:04:18.419858+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Саттер Райли</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
         <is>
           <t>нападающий</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>34934</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>1369_ШДР_фуспенсер</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>45491</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>1369_ШДР_саттеррайли</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
         <is>
           <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>2025-11-04T09:23:47.510812+00:00</t>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>2025-11-06T03:04:18.419886+00:00</t>
         </is>
       </c>
     </row>
@@ -3230,22 +3401,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Гараев Амир</t>
+          <t>Фу Спенсер</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гараевамир</t>
+          <t>1369_ШДР_фуспенсер</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -3255,12 +3426,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-04T17:23:48.013752+08:00</t>
+          <t>2025-11-06T11:04:18.942775+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-11-06</t>
         </is>
       </c>
     </row>
@@ -3275,7 +3446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3323,22 +3494,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Уотерспун Тайлер</t>
+          <t>Гордеев Фёдор</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_БАР_уотерспунтайлер</t>
+          <t>1369_СИБ_гордеевфедор</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -3348,12 +3519,160 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-04T17:23:48.013752+08:00</t>
+          <t>2025-11-06T11:04:18.942775+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-11-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>СИБ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Калиниченко Роман</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1369_СИБ_калиниченкороман</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-11-06T11:04:18.942775+08:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-11-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>СИБ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Широков Сергей</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1369_СИБ_широковсергей</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-11-06T11:04:18.942775+08:00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-11-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>СКА</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>СКА</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Зайцев Никита И</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1369_СКА_зайцевникитаи</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-11-06T11:04:18.942775+08:00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025-11-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Уильямс Колби</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_уильямсколби</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-11-06T11:04:18.942775+08:00</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025-11-06</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-06 15:04:11)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:07.232150+00:00</t>
+          <t>2025-11-06T07:03:01.991828+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:07.232183+00:00</t>
+          <t>2025-11-06T07:03:01.991864+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:07.232202+00:00</t>
+          <t>2025-11-06T07:03:01.991886+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:09.942523+00:00</t>
+          <t>2025-11-06T07:03:04.726184+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:09.942551+00:00</t>
+          <t>2025-11-06T07:03:04.726268+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:09.942569+00:00</t>
+          <t>2025-11-06T07:03:04.726295+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:12.784177+00:00</t>
+          <t>2025-11-06T07:03:07.107912+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:15.639309+00:00</t>
+          <t>2025-11-06T07:03:10.023490+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:15.639339+00:00</t>
+          <t>2025-11-06T07:03:10.023519+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:15.639356+00:00</t>
+          <t>2025-11-06T07:03:10.023538+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:18.553449+00:00</t>
+          <t>2025-11-06T07:03:12.892711+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:18.553480+00:00</t>
+          <t>2025-11-06T07:03:12.892738+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:18.553497+00:00</t>
+          <t>2025-11-06T07:03:12.892756+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:18.553512+00:00</t>
+          <t>2025-11-06T07:03:12.892773+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:23.666647+00:00</t>
+          <t>2025-11-06T07:03:18.088455+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:30.751192+00:00</t>
+          <t>2025-11-06T07:03:20.861505+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:33.507697+00:00</t>
+          <t>2025-11-06T07:03:23.117517+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:33.507727+00:00</t>
+          <t>2025-11-06T07:03:23.117546+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:36.297199+00:00</t>
+          <t>2025-11-06T07:03:25.451066+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:39.088707+00:00</t>
+          <t>2025-11-06T07:03:28.248153+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:39.088736+00:00</t>
+          <t>2025-11-06T07:03:28.248182+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:39.088753+00:00</t>
+          <t>2025-11-06T07:03:28.248200+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:42.011481+00:00</t>
+          <t>2025-11-06T07:03:31.003838+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:42.011509+00:00</t>
+          <t>2025-11-06T07:03:31.003867+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:42.011526+00:00</t>
+          <t>2025-11-06T07:03:31.003885+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:44.304124+00:00</t>
+          <t>2025-11-06T07:03:33.445499+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:44.304153+00:00</t>
+          <t>2025-11-06T07:03:33.445536+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:44.304171+00:00</t>
+          <t>2025-11-06T07:03:33.445557+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:44.304187+00:00</t>
+          <t>2025-11-06T07:03:33.445575+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:47.022280+00:00</t>
+          <t>2025-11-06T07:03:35.739318+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:49.360588+00:00</t>
+          <t>2025-11-06T07:03:38.110110+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:49.360633+00:00</t>
+          <t>2025-11-06T07:03:38.110145+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:49.360650+00:00</t>
+          <t>2025-11-06T07:03:38.110165+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:52.096236+00:00</t>
+          <t>2025-11-06T07:03:40.932906+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:52.096264+00:00</t>
+          <t>2025-11-06T07:03:40.932935+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-06T03:03:52.096281+00:00</t>
+          <t>2025-11-06T07:03:40.932952+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:02.818935+00:00</t>
+          <t>2025-11-06T07:03:43.403327+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:02.818969+00:00</t>
+          <t>2025-11-06T07:03:43.403357+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:02.818987+00:00</t>
+          <t>2025-11-06T07:03:43.403378+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:02.819002+00:00</t>
+          <t>2025-11-06T07:03:43.403393+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:02.819018+00:00</t>
+          <t>2025-11-06T07:03:43.403408+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:02.819047+00:00</t>
+          <t>2025-11-06T07:03:43.403424+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:02.819063+00:00</t>
+          <t>2025-11-06T07:03:43.403438+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:02.819076+00:00</t>
+          <t>2025-11-06T07:03:43.403452+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:05.716507+00:00</t>
+          <t>2025-11-06T07:03:46.260731+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:05.716536+00:00</t>
+          <t>2025-11-06T07:03:46.260761+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:15.611382+00:00</t>
+          <t>2025-11-06T07:03:51.480274+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:15.611411+00:00</t>
+          <t>2025-11-06T07:03:51.480303+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:18.419858+00:00</t>
+          <t>2025-11-06T07:03:54.403582+00:00</t>
         </is>
       </c>
     </row>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>2025-11-06T03:04:18.419886+00:00</t>
+          <t>2025-11-06T07:03:54.403611+00:00</t>
         </is>
       </c>
     </row>
@@ -3446,7 +3446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3491,191 +3491,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>СИБ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Сибирь</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Гордеев Фёдор</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_СИБ_гордеевфедор</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-06T11:04:18.942775+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-06</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>СИБ</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Сибирь</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Калиниченко Роман</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1369_СИБ_калиниченкороман</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-11-06T11:04:18.942775+08:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-11-06</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>СИБ</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Сибирь</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Широков Сергей</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1369_СИБ_широковсергей</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-11-06T11:04:18.942775+08:00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2025-11-06</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>СКА</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>СКА</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Зайцев Никита И</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>1369_СКА_зайцевникитаи</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2025-11-06T11:04:18.942775+08:00</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2025-11-06</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Уильямс Колби</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_уильямсколби</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2025-11-06T11:04:18.942775+08:00</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2025-11-06</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-06 18:30:09)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:01.991828+00:00</t>
+          <t>2025-11-06T10:28:57.749887+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:01.991864+00:00</t>
+          <t>2025-11-06T10:28:57.749910+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:01.991886+00:00</t>
+          <t>2025-11-06T10:28:57.749920+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:04.726184+00:00</t>
+          <t>2025-11-06T10:29:00.205323+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:04.726268+00:00</t>
+          <t>2025-11-06T10:29:00.205368+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:04.726295+00:00</t>
+          <t>2025-11-06T10:29:00.205380+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:07.107912+00:00</t>
+          <t>2025-11-06T10:29:02.297230+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:10.023490+00:00</t>
+          <t>2025-11-06T10:29:04.381037+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:10.023519+00:00</t>
+          <t>2025-11-06T10:29:04.381066+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:10.023538+00:00</t>
+          <t>2025-11-06T10:29:04.381084+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:12.892711+00:00</t>
+          <t>2025-11-06T10:29:06.496405+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:12.892738+00:00</t>
+          <t>2025-11-06T10:29:06.496434+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:12.892756+00:00</t>
+          <t>2025-11-06T10:29:06.496453+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:12.892773+00:00</t>
+          <t>2025-11-06T10:29:06.496482+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:18.088455+00:00</t>
+          <t>2025-11-06T10:29:10.636477+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:20.861505+00:00</t>
+          <t>2025-11-06T10:29:24.889672+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:23.117517+00:00</t>
+          <t>2025-11-06T10:29:27.417126+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:23.117546+00:00</t>
+          <t>2025-11-06T10:29:27.417148+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:25.451066+00:00</t>
+          <t>2025-11-06T10:29:29.477017+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:28.248153+00:00</t>
+          <t>2025-11-06T10:29:31.940378+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:28.248182+00:00</t>
+          <t>2025-11-06T10:29:31.940408+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:28.248200+00:00</t>
+          <t>2025-11-06T10:29:31.940424+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:31.003838+00:00</t>
+          <t>2025-11-06T10:29:34.558169+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:31.003867+00:00</t>
+          <t>2025-11-06T10:29:34.558212+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:31.003885+00:00</t>
+          <t>2025-11-06T10:29:34.558223+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:33.445499+00:00</t>
+          <t>2025-11-06T10:29:37.172296+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:33.445536+00:00</t>
+          <t>2025-11-06T10:29:37.172329+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:33.445557+00:00</t>
+          <t>2025-11-06T10:29:37.172353+00:00</t>
         </is>
       </c>
     </row>
@@ -2106,12 +2106,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2121,12 +2121,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2141,49 +2141,49 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:33.445575+00:00</t>
+          <t>2025-11-06T10:29:37.172373+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,54 +2193,54 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:35.739318+00:00</t>
+          <t>2025-11-06T10:29:37.172392+00:00</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2250,12 +2250,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:38.110110+00:00</t>
+          <t>2025-11-06T10:29:39.266602+00:00</t>
         </is>
       </c>
     </row>
@@ -2277,27 +2277,27 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:38.110145+00:00</t>
+          <t>2025-11-06T10:29:41.372693+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,27 +2334,27 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,49 +2369,49 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:38.110165+00:00</t>
+          <t>2025-11-06T10:29:41.372721+00:00</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2421,12 +2421,12 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:40.932906+00:00</t>
+          <t>2025-11-06T10:29:41.372739+00:00</t>
         </is>
       </c>
     </row>
@@ -2448,12 +2448,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2463,12 +2463,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:40.932935+00:00</t>
+          <t>2025-11-06T10:29:43.881798+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,12 +2505,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2520,12 +2520,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,34 +2540,34 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:40.932952+00:00</t>
+          <t>2025-11-06T10:29:43.881825+00:00</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2592,12 +2592,12 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:43.403327+00:00</t>
+          <t>2025-11-06T10:29:43.881847+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,12 +2619,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2634,12 +2634,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:43.403357+00:00</t>
+          <t>2025-11-06T10:29:46.072260+00:00</t>
         </is>
       </c>
     </row>
@@ -2676,27 +2676,27 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:43.403378+00:00</t>
+          <t>2025-11-06T10:29:46.072290+00:00</t>
         </is>
       </c>
     </row>
@@ -2733,27 +2733,27 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:43.403393+00:00</t>
+          <t>2025-11-06T10:29:46.072308+00:00</t>
         </is>
       </c>
     </row>
@@ -2790,12 +2790,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Пименов Артём</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2805,12 +2805,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>21205</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_пименовартем</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:43.403408+00:00</t>
+          <t>2025-11-06T10:29:46.072324+00:00</t>
         </is>
       </c>
     </row>
@@ -2847,12 +2847,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Пименов Артём</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>68</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2862,12 +2862,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>21205</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_пименовартем</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:43.403424+00:00</t>
+          <t>2025-11-06T10:29:46.072341+00:00</t>
         </is>
       </c>
     </row>
@@ -2904,12 +2904,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Хохряков Пётр</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2919,12 +2919,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>15413</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хохряковпетр</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:43.403438+00:00</t>
+          <t>2025-11-06T10:29:46.072357+00:00</t>
         </is>
       </c>
     </row>
@@ -2961,12 +2961,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Хохряков Пётр</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2976,12 +2976,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>15413</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_СЮЛ_хохряковпетр</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2996,49 +2996,49 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:43.403452+00:00</t>
+          <t>2025-11-06T10:29:46.072381+00:00</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3048,12 +3048,12 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:46.260731+00:00</t>
+          <t>2025-11-06T10:29:46.072396+00:00</t>
         </is>
       </c>
     </row>
@@ -3075,27 +3075,27 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -3110,34 +3110,34 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:46.260761+00:00</t>
+          <t>2025-11-06T10:29:48.698581+00:00</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -3147,12 +3147,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3162,12 +3162,12 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:51.480274+00:00</t>
+          <t>2025-11-06T10:29:48.698612+00:00</t>
         </is>
       </c>
     </row>
@@ -3189,27 +3189,27 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>41896</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -3224,34 +3224,34 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:51.480303+00:00</t>
+          <t>2025-11-06T10:29:53.420364+00:00</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -3261,12 +3261,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>41896</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -3276,12 +3276,12 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-06T07:03:54.403582+00:00</t>
+          <t>2025-11-06T10:29:53.420392+00:00</t>
         </is>
       </c>
     </row>
@@ -3303,42 +3303,99 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
+          <t>Гроло Жереми</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>45343</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>1369_ШДР_гроложереми</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>2025-11-06T10:29:55.612485+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
           <t>Саттер Райли</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
+      <c r="F52" t="inlineStr">
         <is>
           <t>нападающий</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr">
+      <c r="G52" t="inlineStr">
         <is>
           <t>45491</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr">
+      <c r="H52" t="inlineStr">
         <is>
           <t>1369_ШДР_саттеррайли</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
         <is>
           <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>2025-11-06T07:03:54.403611+00:00</t>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>2025-11-06T10:29:55.612502+00:00</t>
         </is>
       </c>
     </row>
@@ -3446,7 +3503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3491,6 +3548,43 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>СИБ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Пьянов Валентин</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_СИБ_пьяноввалентин</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-06T18:29:56.120235+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-06</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-07 10:49:23)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-06T10:28:57.749887+00:00</t>
+          <t>2025-11-07T02:48:24.023086+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-06T10:28:57.749910+00:00</t>
+          <t>2025-11-07T02:48:24.023108+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-06T10:28:57.749920+00:00</t>
+          <t>2025-11-07T02:48:24.023118+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:00.205323+00:00</t>
+          <t>2025-11-07T02:48:26.025171+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:00.205368+00:00</t>
+          <t>2025-11-07T02:48:26.025250+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:00.205380+00:00</t>
+          <t>2025-11-07T02:48:26.025287+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:02.297230+00:00</t>
+          <t>2025-11-07T02:48:28.469890+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:04.381037+00:00</t>
+          <t>2025-11-07T02:48:30.833939+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:04.381066+00:00</t>
+          <t>2025-11-07T02:48:30.833956+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:04.381084+00:00</t>
+          <t>2025-11-07T02:48:30.833965+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:06.496405+00:00</t>
+          <t>2025-11-07T02:48:33.243613+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:06.496434+00:00</t>
+          <t>2025-11-07T02:48:33.243637+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:06.496453+00:00</t>
+          <t>2025-11-07T02:48:33.243647+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:06.496482+00:00</t>
+          <t>2025-11-07T02:48:33.243656+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:10.636477+00:00</t>
+          <t>2025-11-07T02:48:38.123709+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:24.889672+00:00</t>
+          <t>2025-11-07T02:48:40.615052+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:27.417126+00:00</t>
+          <t>2025-11-07T02:48:43.101589+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:27.417148+00:00</t>
+          <t>2025-11-07T02:48:43.101609+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:29.477017+00:00</t>
+          <t>2025-11-07T02:48:45.558452+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:31.940378+00:00</t>
+          <t>2025-11-07T02:48:47.964830+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:31.940408+00:00</t>
+          <t>2025-11-07T02:48:47.964850+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:31.940424+00:00</t>
+          <t>2025-11-07T02:48:47.964858+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:34.558169+00:00</t>
+          <t>2025-11-07T02:48:50.088811+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:34.558212+00:00</t>
+          <t>2025-11-07T02:48:50.088843+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:34.558223+00:00</t>
+          <t>2025-11-07T02:48:50.088864+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:37.172296+00:00</t>
+          <t>2025-11-07T02:48:52.541358+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:37.172329+00:00</t>
+          <t>2025-11-07T02:48:52.541391+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:37.172353+00:00</t>
+          <t>2025-11-07T02:48:52.541412+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:37.172373+00:00</t>
+          <t>2025-11-07T02:48:52.541431+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:37.172392+00:00</t>
+          <t>2025-11-07T02:48:52.541448+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:39.266602+00:00</t>
+          <t>2025-11-07T02:48:55.059239+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:41.372693+00:00</t>
+          <t>2025-11-07T02:48:57.499048+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:41.372721+00:00</t>
+          <t>2025-11-07T02:48:57.499083+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:41.372739+00:00</t>
+          <t>2025-11-07T02:48:57.499106+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:43.881798+00:00</t>
+          <t>2025-11-07T02:48:59.959114+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:43.881825+00:00</t>
+          <t>2025-11-07T02:48:59.959146+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:43.881847+00:00</t>
+          <t>2025-11-07T02:48:59.959166+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:46.072260+00:00</t>
+          <t>2025-11-07T02:49:01.984797+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:46.072290+00:00</t>
+          <t>2025-11-07T02:49:01.984832+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:46.072308+00:00</t>
+          <t>2025-11-07T02:49:01.984852+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:46.072324+00:00</t>
+          <t>2025-11-07T02:49:01.984870+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:46.072341+00:00</t>
+          <t>2025-11-07T02:49:01.984889+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:46.072357+00:00</t>
+          <t>2025-11-07T02:49:01.984906+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:46.072381+00:00</t>
+          <t>2025-11-07T02:49:01.984922+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:46.072396+00:00</t>
+          <t>2025-11-07T02:49:01.984938+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:48.698581+00:00</t>
+          <t>2025-11-07T02:49:04.097065+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:48.698612+00:00</t>
+          <t>2025-11-07T02:49:04.097113+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:53.420364+00:00</t>
+          <t>2025-11-07T02:49:08.175464+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:53.420392+00:00</t>
+          <t>2025-11-07T02:49:08.175495+00:00</t>
         </is>
       </c>
     </row>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:55.612485+00:00</t>
+          <t>2025-11-07T02:49:10.212178+00:00</t>
         </is>
       </c>
     </row>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>2025-11-06T10:29:55.612502+00:00</t>
+          <t>2025-11-07T02:49:10.212199+00:00</t>
         </is>
       </c>
     </row>
@@ -3410,7 +3410,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3452,43 +3452,6 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>changed_day</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Фу Спенсер</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_ШДР_фуспенсер</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-06T11:04:18.942775+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-06</t>
         </is>
       </c>
     </row>
@@ -3503,7 +3466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3548,43 +3511,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>СИБ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Сибирь</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Пьянов Валентин</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_СИБ_пьяноввалентин</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-06T18:29:56.120235+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-06</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-07 11:03:49)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:24.023086+00:00</t>
+          <t>2025-11-07T03:02:39.709539+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:24.023108+00:00</t>
+          <t>2025-11-07T03:02:39.709576+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:24.023118+00:00</t>
+          <t>2025-11-07T03:02:39.709596+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:26.025171+00:00</t>
+          <t>2025-11-07T03:02:42.082762+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:26.025250+00:00</t>
+          <t>2025-11-07T03:02:42.082795+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:26.025287+00:00</t>
+          <t>2025-11-07T03:02:42.082816+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:28.469890+00:00</t>
+          <t>2025-11-07T03:02:44.267908+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:30.833939+00:00</t>
+          <t>2025-11-07T03:02:46.638705+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:30.833956+00:00</t>
+          <t>2025-11-07T03:02:46.638735+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:30.833965+00:00</t>
+          <t>2025-11-07T03:02:46.638754+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:33.243613+00:00</t>
+          <t>2025-11-07T03:02:49.466407+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:33.243637+00:00</t>
+          <t>2025-11-07T03:02:49.466438+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:33.243647+00:00</t>
+          <t>2025-11-07T03:02:49.466456+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:33.243656+00:00</t>
+          <t>2025-11-07T03:02:49.466473+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:38.123709+00:00</t>
+          <t>2025-11-07T03:02:54.535477+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:40.615052+00:00</t>
+          <t>2025-11-07T03:02:56.890756+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:43.101589+00:00</t>
+          <t>2025-11-07T03:02:59.191953+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:43.101609+00:00</t>
+          <t>2025-11-07T03:02:59.191988+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:45.558452+00:00</t>
+          <t>2025-11-07T03:03:01.546961+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:47.964830+00:00</t>
+          <t>2025-11-07T03:03:04.292237+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:47.964850+00:00</t>
+          <t>2025-11-07T03:03:04.292270+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:47.964858+00:00</t>
+          <t>2025-11-07T03:03:04.292289+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:50.088811+00:00</t>
+          <t>2025-11-07T03:03:06.746167+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:50.088843+00:00</t>
+          <t>2025-11-07T03:03:06.746195+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:50.088864+00:00</t>
+          <t>2025-11-07T03:03:06.746212+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:52.541358+00:00</t>
+          <t>2025-11-07T03:03:09.118326+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:52.541391+00:00</t>
+          <t>2025-11-07T03:03:09.118356+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:52.541412+00:00</t>
+          <t>2025-11-07T03:03:09.118373+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:52.541431+00:00</t>
+          <t>2025-11-07T03:03:09.118388+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:52.541448+00:00</t>
+          <t>2025-11-07T03:03:09.118402+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:55.059239+00:00</t>
+          <t>2025-11-07T03:03:11.904464+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:57.499048+00:00</t>
+          <t>2025-11-07T03:03:14.292718+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:57.499083+00:00</t>
+          <t>2025-11-07T03:03:14.292749+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:57.499106+00:00</t>
+          <t>2025-11-07T03:03:14.292769+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:59.959114+00:00</t>
+          <t>2025-11-07T03:03:16.723060+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:59.959146+00:00</t>
+          <t>2025-11-07T03:03:16.723093+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-07T02:48:59.959166+00:00</t>
+          <t>2025-11-07T03:03:16.723112+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:01.984797+00:00</t>
+          <t>2025-11-07T03:03:19.109452+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:01.984832+00:00</t>
+          <t>2025-11-07T03:03:19.109483+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:01.984852+00:00</t>
+          <t>2025-11-07T03:03:19.109501+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:01.984870+00:00</t>
+          <t>2025-11-07T03:03:19.109517+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:01.984889+00:00</t>
+          <t>2025-11-07T03:03:19.109534+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:01.984906+00:00</t>
+          <t>2025-11-07T03:03:19.109549+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:01.984922+00:00</t>
+          <t>2025-11-07T03:03:19.109566+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:01.984938+00:00</t>
+          <t>2025-11-07T03:03:19.109581+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:04.097065+00:00</t>
+          <t>2025-11-07T03:03:21.502555+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:04.097113+00:00</t>
+          <t>2025-11-07T03:03:21.502586+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:08.175464+00:00</t>
+          <t>2025-11-07T03:03:27.128353+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:08.175495+00:00</t>
+          <t>2025-11-07T03:03:27.128382+00:00</t>
         </is>
       </c>
     </row>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:10.212178+00:00</t>
+          <t>2025-11-07T03:03:37.760233+00:00</t>
         </is>
       </c>
     </row>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>2025-11-07T02:49:10.212199+00:00</t>
+          <t>2025-11-07T03:03:37.760265+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-07 15:03:32)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:39.709539+00:00</t>
+          <t>2025-11-07T07:02:27.221228+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:39.709576+00:00</t>
+          <t>2025-11-07T07:02:27.221264+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:39.709596+00:00</t>
+          <t>2025-11-07T07:02:27.221283+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:42.082762+00:00</t>
+          <t>2025-11-07T07:02:29.962744+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:42.082795+00:00</t>
+          <t>2025-11-07T07:02:29.962772+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:42.082816+00:00</t>
+          <t>2025-11-07T07:02:29.962792+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:44.267908+00:00</t>
+          <t>2025-11-07T07:02:32.691794+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:46.638705+00:00</t>
+          <t>2025-11-07T07:02:35.501998+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:46.638735+00:00</t>
+          <t>2025-11-07T07:02:35.502028+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:46.638754+00:00</t>
+          <t>2025-11-07T07:02:35.502046+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:49.466407+00:00</t>
+          <t>2025-11-07T07:02:38.366426+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:49.466438+00:00</t>
+          <t>2025-11-07T07:02:38.366459+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:49.466456+00:00</t>
+          <t>2025-11-07T07:02:38.366478+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:49.466473+00:00</t>
+          <t>2025-11-07T07:02:38.366503+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:54.535477+00:00</t>
+          <t>2025-11-07T07:02:43.739940+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:56.890756+00:00</t>
+          <t>2025-11-07T07:02:46.487628+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:59.191953+00:00</t>
+          <t>2025-11-07T07:02:48.884537+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-07T03:02:59.191988+00:00</t>
+          <t>2025-11-07T07:02:48.884571+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:01.546961+00:00</t>
+          <t>2025-11-07T07:02:51.716394+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:04.292237+00:00</t>
+          <t>2025-11-07T07:02:54.077386+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:04.292270+00:00</t>
+          <t>2025-11-07T07:02:54.077417+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:04.292289+00:00</t>
+          <t>2025-11-07T07:02:54.077435+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:06.746167+00:00</t>
+          <t>2025-11-07T07:02:56.385463+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:06.746195+00:00</t>
+          <t>2025-11-07T07:02:56.385493+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:06.746212+00:00</t>
+          <t>2025-11-07T07:02:56.385513+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:09.118326+00:00</t>
+          <t>2025-11-07T07:02:59.121532+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:09.118356+00:00</t>
+          <t>2025-11-07T07:02:59.121560+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:09.118373+00:00</t>
+          <t>2025-11-07T07:02:59.121578+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:09.118388+00:00</t>
+          <t>2025-11-07T07:02:59.121593+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:09.118402+00:00</t>
+          <t>2025-11-07T07:02:59.121608+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:11.904464+00:00</t>
+          <t>2025-11-07T07:03:01.467494+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:14.292718+00:00</t>
+          <t>2025-11-07T07:03:04.370984+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:14.292749+00:00</t>
+          <t>2025-11-07T07:03:04.371014+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:14.292769+00:00</t>
+          <t>2025-11-07T07:03:04.371033+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:16.723060+00:00</t>
+          <t>2025-11-07T07:03:07.127198+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:16.723093+00:00</t>
+          <t>2025-11-07T07:03:07.127226+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:16.723112+00:00</t>
+          <t>2025-11-07T07:03:07.127244+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:19.109452+00:00</t>
+          <t>2025-11-07T07:03:09.411035+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:19.109483+00:00</t>
+          <t>2025-11-07T07:03:09.411065+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:19.109501+00:00</t>
+          <t>2025-11-07T07:03:09.411083+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:19.109517+00:00</t>
+          <t>2025-11-07T07:03:09.411098+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:19.109534+00:00</t>
+          <t>2025-11-07T07:03:09.411114+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:19.109549+00:00</t>
+          <t>2025-11-07T07:03:09.411129+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:19.109566+00:00</t>
+          <t>2025-11-07T07:03:09.411144+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:19.109581+00:00</t>
+          <t>2025-11-07T07:03:09.411158+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:21.502555+00:00</t>
+          <t>2025-11-07T07:03:12.361501+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:21.502586+00:00</t>
+          <t>2025-11-07T07:03:12.361531+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:27.128353+00:00</t>
+          <t>2025-11-07T07:03:17.013705+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:27.128382+00:00</t>
+          <t>2025-11-07T07:03:17.013733+00:00</t>
         </is>
       </c>
     </row>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:37.760233+00:00</t>
+          <t>2025-11-07T07:03:19.284191+00:00</t>
         </is>
       </c>
     </row>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>2025-11-07T03:03:37.760265+00:00</t>
+          <t>2025-11-07T07:03:19.284219+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-08 11:04:01)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:27.221228+00:00</t>
+          <t>2025-11-08T03:02:53.664217+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:27.221264+00:00</t>
+          <t>2025-11-08T03:02:53.664252+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:27.221283+00:00</t>
+          <t>2025-11-08T03:02:53.664277+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:29.962744+00:00</t>
+          <t>2025-11-08T03:02:56.438192+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:29.962772+00:00</t>
+          <t>2025-11-08T03:02:56.438221+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:29.962792+00:00</t>
+          <t>2025-11-08T03:02:56.438240+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:32.691794+00:00</t>
+          <t>2025-11-08T03:02:59.346418+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:35.501998+00:00</t>
+          <t>2025-11-08T03:03:01.737685+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:35.502028+00:00</t>
+          <t>2025-11-08T03:03:01.737715+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:35.502046+00:00</t>
+          <t>2025-11-08T03:03:01.737733+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:38.366426+00:00</t>
+          <t>2025-11-08T03:03:04.537647+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:38.366459+00:00</t>
+          <t>2025-11-08T03:03:04.537675+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:38.366478+00:00</t>
+          <t>2025-11-08T03:03:04.537692+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:38.366503+00:00</t>
+          <t>2025-11-08T03:03:04.537708+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:43.739940+00:00</t>
+          <t>2025-11-08T03:03:09.141509+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:46.487628+00:00</t>
+          <t>2025-11-08T03:03:11.477838+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:48.884537+00:00</t>
+          <t>2025-11-08T03:03:14.245804+00:00</t>
         </is>
       </c>
     </row>
@@ -1479,27 +1479,27 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Паник Рихард</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>16071</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ЛОК_паникрихард</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1514,49 +1514,49 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:48.884571+00:00</t>
+          <t>2025-11-08T03:03:14.245871+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1566,39 +1566,39 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:51.716394+00:00</t>
+          <t>2025-11-08T03:03:14.245899+00:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1623,12 +1623,12 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:54.077386+00:00</t>
+          <t>2025-11-08T03:03:16.521996+00:00</t>
         </is>
       </c>
     </row>
@@ -1650,12 +1650,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1665,12 +1665,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>22683</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:54.077417+00:00</t>
+          <t>2025-11-08T03:03:19.232236+00:00</t>
         </is>
       </c>
     </row>
@@ -1707,27 +1707,27 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Профака Лука</t>
+          <t>Попугаев Никита О</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>43943</t>
+          <t>22683</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_НХК_профакалука</t>
+          <t>1369_НХК_попугаевникитао</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:54.077435+00:00</t>
+          <t>2025-11-08T03:03:19.232266+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:56.385463+00:00</t>
+          <t>2025-11-08T03:03:22.151013+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:56.385493+00:00</t>
+          <t>2025-11-08T03:03:22.151047+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:56.385513+00:00</t>
+          <t>2025-11-08T03:03:22.151067+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:59.121532+00:00</t>
+          <t>2025-11-08T03:03:25.118685+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:59.121560+00:00</t>
+          <t>2025-11-08T03:03:25.118718+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:59.121578+00:00</t>
+          <t>2025-11-08T03:03:25.118744+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:59.121593+00:00</t>
+          <t>2025-11-08T03:03:25.118762+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-07T07:02:59.121608+00:00</t>
+          <t>2025-11-08T03:03:25.118782+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:01.467494+00:00</t>
+          <t>2025-11-08T03:03:27.873012+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:04.370984+00:00</t>
+          <t>2025-11-08T03:03:30.152503+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:04.371014+00:00</t>
+          <t>2025-11-08T03:03:30.152533+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:04.371033+00:00</t>
+          <t>2025-11-08T03:03:30.152552+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:07.127198+00:00</t>
+          <t>2025-11-08T03:03:32.406671+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:07.127226+00:00</t>
+          <t>2025-11-08T03:03:32.406699+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:07.127244+00:00</t>
+          <t>2025-11-08T03:03:32.406716+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:09.411035+00:00</t>
+          <t>2025-11-08T03:03:35.218024+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:09.411065+00:00</t>
+          <t>2025-11-08T03:03:35.218053+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:09.411083+00:00</t>
+          <t>2025-11-08T03:03:35.218073+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:09.411098+00:00</t>
+          <t>2025-11-08T03:03:35.218091+00:00</t>
         </is>
       </c>
     </row>
@@ -2847,12 +2847,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Пименов Артём</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2862,12 +2862,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>21205</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_пименовартем</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:09.411114+00:00</t>
+          <t>2025-11-08T03:03:35.218107+00:00</t>
         </is>
       </c>
     </row>
@@ -2904,12 +2904,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2919,12 +2919,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2939,49 +2939,49 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:09.411129+00:00</t>
+          <t>2025-11-08T03:03:35.218121+00:00</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Хохряков Пётр</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>15413</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хохряковпетр</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2991,39 +2991,39 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:09.411144+00:00</t>
+          <t>2025-11-08T03:03:38.123971+00:00</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3033,12 +3033,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3048,54 +3048,54 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:09.411158+00:00</t>
+          <t>2025-11-08T03:03:38.124004+00:00</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -3105,54 +3105,54 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:12.361501+00:00</t>
+          <t>2025-11-08T03:03:43.722175+00:00</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>41896</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3162,54 +3162,54 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:12.361531+00:00</t>
+          <t>2025-11-08T03:03:43.722204+00:00</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -3219,54 +3219,54 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:17.013705+00:00</t>
+          <t>2025-11-08T03:03:46.028334+00:00</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Саттер Райли</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>41896</t>
+          <t>45491</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_ШДР_саттеррайли</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -3276,126 +3276,12 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-07T07:03:17.013733+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Гроло Жереми</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>45343</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>1369_ШДР_гроложереми</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>2025-11-07T07:03:19.284191+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Саттер Райли</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>45491</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>1369_ШДР_саттеррайли</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>2025-11-07T07:03:19.284219+00:00</t>
+          <t>2025-11-08T03:03:46.028363+00:00</t>
         </is>
       </c>
     </row>
@@ -3410,7 +3296,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3452,6 +3338,117 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>changed_day</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>НХК</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Нефтехимик</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Профака Лука</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_НХК_профакалука</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-08T11:03:46.545097+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>СЮЛ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Салават Юлаев</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Пименов Артём</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1369_СЮЛ_пименовартем</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-11-08T11:03:46.545097+08:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-11-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>СЮЛ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Салават Юлаев</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Хохряков Пётр</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1369_СЮЛ_хохряковпетр</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-11-08T11:03:46.545097+08:00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-11-08</t>
         </is>
       </c>
     </row>
@@ -3466,7 +3463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3511,6 +3508,43 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ЛОК</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Локомотив</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Паник Рихард</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_ЛОК_паникрихард</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-08T11:03:46.545097+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-08</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-08 15:03:53)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-08T03:02:53.664217+00:00</t>
+          <t>2025-11-08T07:02:45.456129+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-08T03:02:53.664252+00:00</t>
+          <t>2025-11-08T07:02:45.456166+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-08T03:02:53.664277+00:00</t>
+          <t>2025-11-08T07:02:45.456190+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-08T03:02:56.438192+00:00</t>
+          <t>2025-11-08T07:02:48.318846+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-08T03:02:56.438221+00:00</t>
+          <t>2025-11-08T07:02:48.318877+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-08T03:02:56.438240+00:00</t>
+          <t>2025-11-08T07:02:48.318895+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-08T03:02:59.346418+00:00</t>
+          <t>2025-11-08T07:02:50.624461+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:01.737685+00:00</t>
+          <t>2025-11-08T07:02:52.914848+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:01.737715+00:00</t>
+          <t>2025-11-08T07:02:52.914877+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:01.737733+00:00</t>
+          <t>2025-11-08T07:02:52.914895+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:04.537647+00:00</t>
+          <t>2025-11-08T07:02:55.619058+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:04.537675+00:00</t>
+          <t>2025-11-08T07:02:55.619088+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:04.537692+00:00</t>
+          <t>2025-11-08T07:02:55.619105+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:04.537708+00:00</t>
+          <t>2025-11-08T07:02:55.619120+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:09.141509+00:00</t>
+          <t>2025-11-08T07:03:01.072475+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:11.477838+00:00</t>
+          <t>2025-11-08T07:03:03.407651+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:14.245804+00:00</t>
+          <t>2025-11-08T07:03:06.213073+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:14.245871+00:00</t>
+          <t>2025-11-08T07:03:06.213102+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:14.245899+00:00</t>
+          <t>2025-11-08T07:03:06.213120+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:16.521996+00:00</t>
+          <t>2025-11-08T07:03:08.908819+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:19.232236+00:00</t>
+          <t>2025-11-08T07:03:11.322693+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:19.232266+00:00</t>
+          <t>2025-11-08T07:03:11.322721+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:22.151013+00:00</t>
+          <t>2025-11-08T07:03:14.123250+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:22.151047+00:00</t>
+          <t>2025-11-08T07:03:14.123280+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:22.151067+00:00</t>
+          <t>2025-11-08T07:03:14.123298+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:25.118685+00:00</t>
+          <t>2025-11-08T07:03:16.419196+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:25.118718+00:00</t>
+          <t>2025-11-08T07:03:16.419227+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:25.118744+00:00</t>
+          <t>2025-11-08T07:03:16.419245+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:25.118762+00:00</t>
+          <t>2025-11-08T07:03:16.419260+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:25.118782+00:00</t>
+          <t>2025-11-08T07:03:16.419275+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:27.873012+00:00</t>
+          <t>2025-11-08T07:03:19.142429+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:30.152503+00:00</t>
+          <t>2025-11-08T07:03:21.918807+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:30.152533+00:00</t>
+          <t>2025-11-08T07:03:21.918837+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:30.152552+00:00</t>
+          <t>2025-11-08T07:03:21.918856+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:32.406671+00:00</t>
+          <t>2025-11-08T07:03:24.627984+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:32.406699+00:00</t>
+          <t>2025-11-08T07:03:24.628011+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:32.406716+00:00</t>
+          <t>2025-11-08T07:03:24.628029+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:35.218024+00:00</t>
+          <t>2025-11-08T07:03:26.939387+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:35.218053+00:00</t>
+          <t>2025-11-08T07:03:26.939417+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:35.218073+00:00</t>
+          <t>2025-11-08T07:03:26.939435+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:35.218091+00:00</t>
+          <t>2025-11-08T07:03:26.939451+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:35.218107+00:00</t>
+          <t>2025-11-08T07:03:26.939468+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:35.218121+00:00</t>
+          <t>2025-11-08T07:03:26.939484+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:38.123971+00:00</t>
+          <t>2025-11-08T07:03:29.320924+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:38.124004+00:00</t>
+          <t>2025-11-08T07:03:29.320954+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:43.722175+00:00</t>
+          <t>2025-11-08T07:03:34.459660+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:43.722204+00:00</t>
+          <t>2025-11-08T07:03:34.459688+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:46.028334+00:00</t>
+          <t>2025-11-08T07:03:36.846196+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-08T03:03:46.028363+00:00</t>
+          <t>2025-11-08T07:03:36.846224+00:00</t>
         </is>
       </c>
     </row>
@@ -3463,7 +3463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3508,43 +3508,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ЛОК</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Локомотив</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Паник Рихард</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_ЛОК_паникрихард</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-08T11:03:46.545097+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-08</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-09 11:02:40)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:45.456129+00:00</t>
+          <t>2025-11-09T03:01:32.374659+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:45.456166+00:00</t>
+          <t>2025-11-09T03:01:32.374693+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:45.456190+00:00</t>
+          <t>2025-11-09T03:01:32.374713+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:48.318846+00:00</t>
+          <t>2025-11-09T03:01:34.876621+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:48.318877+00:00</t>
+          <t>2025-11-09T03:01:34.876649+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:48.318895+00:00</t>
+          <t>2025-11-09T03:01:34.876668+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:50.624461+00:00</t>
+          <t>2025-11-09T03:01:37.103364+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:52.914848+00:00</t>
+          <t>2025-11-09T03:01:39.393740+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:52.914877+00:00</t>
+          <t>2025-11-09T03:01:39.393770+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:52.914895+00:00</t>
+          <t>2025-11-09T03:01:39.393788+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:55.619058+00:00</t>
+          <t>2025-11-09T03:01:42.209378+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:55.619088+00:00</t>
+          <t>2025-11-09T03:01:42.209406+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:55.619105+00:00</t>
+          <t>2025-11-09T03:01:42.209425+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-08T07:02:55.619120+00:00</t>
+          <t>2025-11-09T03:01:42.209441+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:01.072475+00:00</t>
+          <t>2025-11-09T03:01:47.291388+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:03.407651+00:00</t>
+          <t>2025-11-09T03:01:49.981590+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:06.213073+00:00</t>
+          <t>2025-11-09T03:01:52.849415+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:06.213102+00:00</t>
+          <t>2025-11-09T03:01:52.849443+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:06.213120+00:00</t>
+          <t>2025-11-09T03:01:52.849459+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:08.908819+00:00</t>
+          <t>2025-11-09T03:01:55.964029+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:11.322693+00:00</t>
+          <t>2025-11-09T03:01:58.782620+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:11.322721+00:00</t>
+          <t>2025-11-09T03:01:58.782650+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:14.123250+00:00</t>
+          <t>2025-11-09T03:02:01.599862+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:14.123280+00:00</t>
+          <t>2025-11-09T03:02:01.599890+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:14.123298+00:00</t>
+          <t>2025-11-09T03:02:01.599907+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:16.419196+00:00</t>
+          <t>2025-11-09T03:02:03.936657+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:16.419227+00:00</t>
+          <t>2025-11-09T03:02:03.936687+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:16.419245+00:00</t>
+          <t>2025-11-09T03:02:03.936705+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:16.419260+00:00</t>
+          <t>2025-11-09T03:02:03.936721+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:16.419275+00:00</t>
+          <t>2025-11-09T03:02:03.936737+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,34 +2255,34 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:19.142429+00:00</t>
+          <t>2025-11-09T03:02:06.257693+00:00</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2292,12 +2292,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2307,12 +2307,12 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:21.918807+00:00</t>
+          <t>2025-11-09T03:02:06.257723+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,27 +2334,27 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:21.918837+00:00</t>
+          <t>2025-11-09T03:02:08.956061+00:00</t>
         </is>
       </c>
     </row>
@@ -2391,27 +2391,27 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2426,49 +2426,49 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:21.918856+00:00</t>
+          <t>2025-11-09T03:02:08.956090+00:00</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2478,12 +2478,12 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:24.627984+00:00</t>
+          <t>2025-11-09T03:02:08.956107+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,12 +2505,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2520,12 +2520,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:24.628011+00:00</t>
+          <t>2025-11-09T03:02:11.667187+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,12 +2562,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2597,34 +2597,34 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:24.628029+00:00</t>
+          <t>2025-11-09T03:02:11.667215+00:00</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2634,12 +2634,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2649,12 +2649,12 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:26.939387+00:00</t>
+          <t>2025-11-09T03:02:11.667231+00:00</t>
         </is>
       </c>
     </row>
@@ -2676,12 +2676,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2691,12 +2691,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:26.939417+00:00</t>
+          <t>2025-11-09T03:02:13.924509+00:00</t>
         </is>
       </c>
     </row>
@@ -2733,27 +2733,27 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:26.939435+00:00</t>
+          <t>2025-11-09T03:02:13.924557+00:00</t>
         </is>
       </c>
     </row>
@@ -2790,27 +2790,27 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:26.939451+00:00</t>
+          <t>2025-11-09T03:02:13.924580+00:00</t>
         </is>
       </c>
     </row>
@@ -2847,12 +2847,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2862,12 +2862,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:26.939468+00:00</t>
+          <t>2025-11-09T03:02:13.924603+00:00</t>
         </is>
       </c>
     </row>
@@ -2904,12 +2904,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2919,12 +2919,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2939,49 +2939,49 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:26.939484+00:00</t>
+          <t>2025-11-09T03:02:13.924623+00:00</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2991,12 +2991,12 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:29.320924+00:00</t>
+          <t>2025-11-09T03:02:13.924642+00:00</t>
         </is>
       </c>
     </row>
@@ -3018,27 +3018,27 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3053,34 +3053,34 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:29.320954+00:00</t>
+          <t>2025-11-09T03:02:16.710147+00:00</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3090,12 +3090,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -3105,12 +3105,12 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:34.459660+00:00</t>
+          <t>2025-11-09T03:02:16.710176+00:00</t>
         </is>
       </c>
     </row>
@@ -3132,27 +3132,27 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>41896</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3167,34 +3167,34 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:34.459688+00:00</t>
+          <t>2025-11-09T03:02:21.874595+00:00</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Саморуков Дмитрий</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -3204,12 +3204,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>24005</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ЦСК_саморуковдмитрий</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -3219,69 +3219,183 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-08T07:03:36.846196+00:00</t>
+          <t>2025-11-09T03:02:21.874627+00:00</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>cska</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Уильямс Колби</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>41896</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_уильямсколби</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>2025-11-09T03:02:21.874647+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
           <t>ШДР</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B51" t="inlineStr">
         <is>
           <t>Драконы</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>kunlun</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Гроло Жереми</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>45343</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>1369_ШДР_гроложереми</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>2025-11-09T03:02:24.228115+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
         <is>
           <t>Саттер Райли</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="F52" t="inlineStr">
         <is>
           <t>нападающий</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr">
+      <c r="G52" t="inlineStr">
         <is>
           <t>45491</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr">
+      <c r="H52" t="inlineStr">
         <is>
           <t>1369_ШДР_саттеррайли</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
         <is>
           <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>2025-11-08T07:03:36.846224+00:00</t>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>2025-11-09T03:02:24.228142+00:00</t>
         </is>
       </c>
     </row>
@@ -3291,173 +3405,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>team_abbr</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>team_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>player_name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>player_uid</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>changed_at</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>changed_day</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>НХК</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Нефтехимик</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Профака Лука</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_НХК_профакалука</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-08T11:03:46.545097+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-08</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>СЮЛ</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Салават Юлаев</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Пименов Артём</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1369_СЮЛ_пименовартем</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-11-08T11:03:46.545097+08:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-11-08</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>СЮЛ</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Салават Юлаев</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Хохряков Пётр</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1369_СЮЛ_хохряковпетр</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-11-08T11:03:46.545097+08:00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2025-11-08</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3511,4 +3458,134 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>team_abbr</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>team_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>player_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>player_uid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>changed_at</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>changed_day</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>СКА</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>СКА</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Короткий Матвей</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_СКА_короткийматвей</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-09T11:02:24.737696+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Саморуков Дмитрий</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_саморуковдмитрий</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-11-09T11:02:24.737696+08:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-11-09</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-09 12:53:55)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:32.374659+00:00</t>
+          <t>2025-11-09T04:51:32.557554+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:32.374693+00:00</t>
+          <t>2025-11-09T04:51:32.557619+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:32.374713+00:00</t>
+          <t>2025-11-09T04:51:32.557648+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:34.876621+00:00</t>
+          <t>2025-11-09T04:51:34.658854+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:34.876649+00:00</t>
+          <t>2025-11-09T04:51:34.658869+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:34.876668+00:00</t>
+          <t>2025-11-09T04:51:34.658877+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:37.103364+00:00</t>
+          <t>2025-11-09T04:51:37.178423+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:39.393740+00:00</t>
+          <t>2025-11-09T04:51:39.623657+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:39.393770+00:00</t>
+          <t>2025-11-09T04:51:39.623688+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:39.393788+00:00</t>
+          <t>2025-11-09T04:51:39.623708+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:42.209378+00:00</t>
+          <t>2025-11-09T04:51:42.349622+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:42.209406+00:00</t>
+          <t>2025-11-09T04:51:42.349651+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:42.209425+00:00</t>
+          <t>2025-11-09T04:51:42.349670+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:42.209441+00:00</t>
+          <t>2025-11-09T04:51:42.349688+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:47.291388+00:00</t>
+          <t>2025-11-09T04:51:47.324466+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:49.981590+00:00</t>
+          <t>2025-11-09T04:51:49.714643+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:52.849415+00:00</t>
+          <t>2025-11-09T04:51:52.542628+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:52.849443+00:00</t>
+          <t>2025-11-09T04:51:52.542657+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:52.849459+00:00</t>
+          <t>2025-11-09T04:51:52.542676+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:55.964029+00:00</t>
+          <t>2025-11-09T04:51:55.253319+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:58.782620+00:00</t>
+          <t>2025-11-09T04:51:57.988689+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-09T03:01:58.782650+00:00</t>
+          <t>2025-11-09T04:51:57.988720+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:01.599862+00:00</t>
+          <t>2025-11-09T04:52:00.755599+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:01.599890+00:00</t>
+          <t>2025-11-09T04:52:00.755629+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:01.599907+00:00</t>
+          <t>2025-11-09T04:52:00.755648+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:03.936657+00:00</t>
+          <t>2025-11-09T04:52:03.068364+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:03.936687+00:00</t>
+          <t>2025-11-09T04:52:03.068407+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:03.936705+00:00</t>
+          <t>2025-11-09T04:52:03.068428+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:03.936721+00:00</t>
+          <t>2025-11-09T04:52:03.068438+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:03.936737+00:00</t>
+          <t>2025-11-09T04:52:03.068445+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:06.257693+00:00</t>
+          <t>2025-11-09T04:52:05.527655+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:06.257723+00:00</t>
+          <t>2025-11-09T04:52:05.527691+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:08.956061+00:00</t>
+          <t>2025-11-09T04:52:07.619053+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:08.956090+00:00</t>
+          <t>2025-11-09T04:52:07.619071+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:08.956107+00:00</t>
+          <t>2025-11-09T04:52:07.619079+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:11.667187+00:00</t>
+          <t>2025-11-09T04:52:10.053713+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:11.667215+00:00</t>
+          <t>2025-11-09T04:52:10.053746+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:11.667231+00:00</t>
+          <t>2025-11-09T04:52:10.053766+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:13.924509+00:00</t>
+          <t>2025-11-09T04:52:12.060906+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:13.924557+00:00</t>
+          <t>2025-11-09T04:52:12.060938+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:13.924580+00:00</t>
+          <t>2025-11-09T04:52:12.060957+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:13.924603+00:00</t>
+          <t>2025-11-09T04:52:12.060975+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:13.924623+00:00</t>
+          <t>2025-11-09T04:52:12.060991+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:13.924642+00:00</t>
+          <t>2025-11-09T04:52:12.061006+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:16.710147+00:00</t>
+          <t>2025-11-09T04:52:14.516175+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:16.710176+00:00</t>
+          <t>2025-11-09T04:52:14.516193+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:21.874595+00:00</t>
+          <t>2025-11-09T04:52:18.605382+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:21.874627+00:00</t>
+          <t>2025-11-09T04:52:18.605413+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:21.874647+00:00</t>
+          <t>2025-11-09T04:52:18.605431+00:00</t>
         </is>
       </c>
     </row>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:24.228115+00:00</t>
+          <t>2025-11-09T04:52:21.024079+00:00</t>
         </is>
       </c>
     </row>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>2025-11-09T03:02:24.228142+00:00</t>
+          <t>2025-11-09T04:52:21.024100+00:00</t>
         </is>
       </c>
     </row>
@@ -3466,7 +3466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3511,80 +3511,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>СКА</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>СКА</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Короткий Матвей</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_СКА_короткийматвей</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-09T11:02:24.737696+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Саморуков Дмитрий</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_саморуковдмитрий</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-11-09T11:02:24.737696+08:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-11-09</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-09 15:04:16)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:32.557554+00:00</t>
+          <t>2025-11-09T07:01:32.302554+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:32.557619+00:00</t>
+          <t>2025-11-09T07:01:32.302592+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:32.557648+00:00</t>
+          <t>2025-11-09T07:01:32.302614+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:34.658854+00:00</t>
+          <t>2025-11-09T07:01:36.291526+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:34.658869+00:00</t>
+          <t>2025-11-09T07:01:36.291555+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:34.658877+00:00</t>
+          <t>2025-11-09T07:01:36.291574+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:37.178423+00:00</t>
+          <t>2025-11-09T07:01:38.752747+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:39.623657+00:00</t>
+          <t>2025-11-09T07:01:41.480364+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:39.623688+00:00</t>
+          <t>2025-11-09T07:01:41.480395+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:39.623708+00:00</t>
+          <t>2025-11-09T07:01:41.480414+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:42.349622+00:00</t>
+          <t>2025-11-09T07:01:44.328725+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:42.349651+00:00</t>
+          <t>2025-11-09T07:01:44.328756+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:42.349670+00:00</t>
+          <t>2025-11-09T07:01:44.328775+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:42.349688+00:00</t>
+          <t>2025-11-09T07:01:44.328791+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:47.324466+00:00</t>
+          <t>2025-11-09T07:01:49.981378+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:49.714643+00:00</t>
+          <t>2025-11-09T07:01:52.290199+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:52.542628+00:00</t>
+          <t>2025-11-09T07:01:54.669928+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:52.542657+00:00</t>
+          <t>2025-11-09T07:01:54.669958+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:52.542676+00:00</t>
+          <t>2025-11-09T07:01:54.669976+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:55.253319+00:00</t>
+          <t>2025-11-09T07:01:57.414117+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:57.988689+00:00</t>
+          <t>2025-11-09T07:01:59.690018+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-09T04:51:57.988720+00:00</t>
+          <t>2025-11-09T07:01:59.690057+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:00.755599+00:00</t>
+          <t>2025-11-09T07:02:02.436000+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:00.755629+00:00</t>
+          <t>2025-11-09T07:02:02.436032+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:00.755648+00:00</t>
+          <t>2025-11-09T07:02:02.436051+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:03.068364+00:00</t>
+          <t>2025-11-09T07:02:04.699123+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:03.068407+00:00</t>
+          <t>2025-11-09T07:02:04.699151+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:03.068428+00:00</t>
+          <t>2025-11-09T07:02:04.699169+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:03.068438+00:00</t>
+          <t>2025-11-09T07:02:04.699195+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:03.068445+00:00</t>
+          <t>2025-11-09T07:02:04.699210+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:05.527655+00:00</t>
+          <t>2025-11-09T07:02:07.576189+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:05.527691+00:00</t>
+          <t>2025-11-09T07:02:07.576216+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:07.619053+00:00</t>
+          <t>2025-11-09T07:02:09.938292+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:07.619071+00:00</t>
+          <t>2025-11-09T07:02:09.938320+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:07.619079+00:00</t>
+          <t>2025-11-09T07:02:09.938337+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:10.053713+00:00</t>
+          <t>2025-11-09T07:02:12.662184+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:10.053746+00:00</t>
+          <t>2025-11-09T07:02:12.662221+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:10.053766+00:00</t>
+          <t>2025-11-09T07:02:12.662239+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:12.060906+00:00</t>
+          <t>2025-11-09T07:02:14.954024+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:12.060938+00:00</t>
+          <t>2025-11-09T07:02:14.954053+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:12.060957+00:00</t>
+          <t>2025-11-09T07:02:14.954071+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:12.060975+00:00</t>
+          <t>2025-11-09T07:02:14.954088+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:12.060991+00:00</t>
+          <t>2025-11-09T07:02:14.954103+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:12.061006+00:00</t>
+          <t>2025-11-09T07:02:14.954119+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:14.516175+00:00</t>
+          <t>2025-11-09T07:02:17.721687+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:14.516193+00:00</t>
+          <t>2025-11-09T07:02:17.721722+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:18.605382+00:00</t>
+          <t>2025-11-09T07:02:22.844268+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:18.605413+00:00</t>
+          <t>2025-11-09T07:02:22.844298+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:18.605431+00:00</t>
+          <t>2025-11-09T07:02:22.844316+00:00</t>
         </is>
       </c>
     </row>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:21.024079+00:00</t>
+          <t>2025-11-09T07:02:25.636361+00:00</t>
         </is>
       </c>
     </row>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>2025-11-09T04:52:21.024100+00:00</t>
+          <t>2025-11-09T07:02:25.636392+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-10 11:06:44)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:32.302554+00:00</t>
+          <t>2025-11-10T03:01:27.013571+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:32.302592+00:00</t>
+          <t>2025-11-10T03:01:27.013608+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:32.302614+00:00</t>
+          <t>2025-11-10T03:01:27.013629+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:36.291526+00:00</t>
+          <t>2025-11-10T03:01:29.757790+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:36.291555+00:00</t>
+          <t>2025-11-10T03:01:29.757826+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:36.291574+00:00</t>
+          <t>2025-11-10T03:01:29.757848+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:38.752747+00:00</t>
+          <t>2025-11-10T03:01:32.071178+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:41.480364+00:00</t>
+          <t>2025-11-10T03:01:34.749013+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:41.480395+00:00</t>
+          <t>2025-11-10T03:01:34.749044+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:41.480414+00:00</t>
+          <t>2025-11-10T03:01:34.749064+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:44.328725+00:00</t>
+          <t>2025-11-10T03:01:37.039071+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:44.328756+00:00</t>
+          <t>2025-11-10T03:01:37.039103+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:44.328775+00:00</t>
+          <t>2025-11-10T03:01:37.039123+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:44.328791+00:00</t>
+          <t>2025-11-10T03:01:37.039140+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:49.981378+00:00</t>
+          <t>2025-11-10T03:01:42.093260+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:52.290199+00:00</t>
+          <t>2025-11-10T03:01:44.750388+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:54.669928+00:00</t>
+          <t>2025-11-10T03:01:47.538425+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:54.669958+00:00</t>
+          <t>2025-11-10T03:01:47.538456+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:54.669976+00:00</t>
+          <t>2025-11-10T03:01:47.538479+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:57.414117+00:00</t>
+          <t>2025-11-10T03:01:49.820511+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:59.690018+00:00</t>
+          <t>2025-11-10T03:01:52.571095+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-09T07:01:59.690057+00:00</t>
+          <t>2025-11-10T03:01:52.571128+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:02.436000+00:00</t>
+          <t>2025-11-10T03:01:54.886852+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:02.436032+00:00</t>
+          <t>2025-11-10T03:01:54.886888+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:02.436051+00:00</t>
+          <t>2025-11-10T03:01:54.886912+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:04.699123+00:00</t>
+          <t>2025-11-10T03:01:57.677184+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:04.699151+00:00</t>
+          <t>2025-11-10T03:01:57.677216+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:04.699169+00:00</t>
+          <t>2025-11-10T03:01:57.677237+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:04.699195+00:00</t>
+          <t>2025-11-10T03:01:57.677254+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:04.699210+00:00</t>
+          <t>2025-11-10T03:01:57.677271+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:07.576189+00:00</t>
+          <t>2025-11-10T03:02:00.358373+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:07.576216+00:00</t>
+          <t>2025-11-10T03:02:00.358403+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:09.938292+00:00</t>
+          <t>2025-11-10T03:02:03.086739+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:09.938320+00:00</t>
+          <t>2025-11-10T03:02:03.086773+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:09.938337+00:00</t>
+          <t>2025-11-10T03:02:03.086791+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:12.662184+00:00</t>
+          <t>2025-11-10T03:02:05.339741+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:12.662221+00:00</t>
+          <t>2025-11-10T03:02:05.339771+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:12.662239+00:00</t>
+          <t>2025-11-10T03:02:05.339789+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:14.954024+00:00</t>
+          <t>2025-11-10T03:02:07.676227+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:14.954053+00:00</t>
+          <t>2025-11-10T03:02:07.676265+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:14.954071+00:00</t>
+          <t>2025-11-10T03:02:07.676286+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:14.954088+00:00</t>
+          <t>2025-11-10T03:02:07.676304+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:14.954103+00:00</t>
+          <t>2025-11-10T03:02:07.676323+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:14.954119+00:00</t>
+          <t>2025-11-10T03:02:07.676339+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:17.721687+00:00</t>
+          <t>2025-11-10T03:02:10.420265+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:17.721722+00:00</t>
+          <t>2025-11-10T03:02:10.420295+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:22.844268+00:00</t>
+          <t>2025-11-10T03:02:15.509065+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:22.844298+00:00</t>
+          <t>2025-11-10T03:02:15.509096+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:22.844316+00:00</t>
+          <t>2025-11-10T03:02:15.509114+00:00</t>
         </is>
       </c>
     </row>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:25.636361+00:00</t>
+          <t>2025-11-10T03:02:17.895401+00:00</t>
         </is>
       </c>
     </row>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>2025-11-09T07:02:25.636392+00:00</t>
+          <t>2025-11-10T03:02:17.895429+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-10 15:06:46)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:27.013571+00:00</t>
+          <t>2025-11-10T07:01:26.910693+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:27.013608+00:00</t>
+          <t>2025-11-10T07:01:26.910729+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:27.013629+00:00</t>
+          <t>2025-11-10T07:01:26.910750+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:29.757790+00:00</t>
+          <t>2025-11-10T07:01:29.329086+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:29.757826+00:00</t>
+          <t>2025-11-10T07:01:29.329118+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:29.757848+00:00</t>
+          <t>2025-11-10T07:01:29.329139+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:32.071178+00:00</t>
+          <t>2025-11-10T07:01:31.645250+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:34.749013+00:00</t>
+          <t>2025-11-10T07:01:34.014152+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:34.749044+00:00</t>
+          <t>2025-11-10T07:01:34.014182+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:34.749064+00:00</t>
+          <t>2025-11-10T07:01:34.014201+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:37.039071+00:00</t>
+          <t>2025-11-10T07:01:36.803766+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:37.039103+00:00</t>
+          <t>2025-11-10T07:01:36.803796+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:37.039123+00:00</t>
+          <t>2025-11-10T07:01:36.803815+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:37.039140+00:00</t>
+          <t>2025-11-10T07:01:36.803831+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:42.093260+00:00</t>
+          <t>2025-11-10T07:01:42.335403+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:44.750388+00:00</t>
+          <t>2025-11-10T07:01:44.793298+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:47.538425+00:00</t>
+          <t>2025-11-10T07:01:47.105772+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:47.538456+00:00</t>
+          <t>2025-11-10T07:01:47.105801+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:47.538479+00:00</t>
+          <t>2025-11-10T07:01:47.105819+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:49.820511+00:00</t>
+          <t>2025-11-10T07:01:49.451508+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:52.571095+00:00</t>
+          <t>2025-11-10T07:01:52.210226+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:52.571128+00:00</t>
+          <t>2025-11-10T07:01:52.210259+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:54.886852+00:00</t>
+          <t>2025-11-10T07:01:54.980169+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:54.886888+00:00</t>
+          <t>2025-11-10T07:01:54.980205+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:54.886912+00:00</t>
+          <t>2025-11-10T07:01:54.980230+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:57.677184+00:00</t>
+          <t>2025-11-10T07:01:57.292229+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:57.677216+00:00</t>
+          <t>2025-11-10T07:01:57.292258+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:57.677237+00:00</t>
+          <t>2025-11-10T07:01:57.292277+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:57.677254+00:00</t>
+          <t>2025-11-10T07:01:57.292296+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-10T03:01:57.677271+00:00</t>
+          <t>2025-11-10T07:01:57.292311+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:00.358373+00:00</t>
+          <t>2025-11-10T07:01:59.997505+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:00.358403+00:00</t>
+          <t>2025-11-10T07:01:59.997538+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:03.086739+00:00</t>
+          <t>2025-11-10T07:02:02.276786+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:03.086773+00:00</t>
+          <t>2025-11-10T07:02:02.276816+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:03.086791+00:00</t>
+          <t>2025-11-10T07:02:02.276841+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:05.339741+00:00</t>
+          <t>2025-11-10T07:02:04.640557+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:05.339771+00:00</t>
+          <t>2025-11-10T07:02:04.640586+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:05.339789+00:00</t>
+          <t>2025-11-10T07:02:04.640605+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:07.676227+00:00</t>
+          <t>2025-11-10T07:02:07.071729+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:07.676265+00:00</t>
+          <t>2025-11-10T07:02:07.071766+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:07.676286+00:00</t>
+          <t>2025-11-10T07:02:07.071786+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:07.676304+00:00</t>
+          <t>2025-11-10T07:02:07.071805+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:07.676323+00:00</t>
+          <t>2025-11-10T07:02:07.071823+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:07.676339+00:00</t>
+          <t>2025-11-10T07:02:07.071839+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:10.420265+00:00</t>
+          <t>2025-11-10T07:02:09.304379+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:10.420295+00:00</t>
+          <t>2025-11-10T07:02:09.304409+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:15.509065+00:00</t>
+          <t>2025-11-10T07:02:14.138463+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:15.509096+00:00</t>
+          <t>2025-11-10T07:02:14.138505+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:15.509114+00:00</t>
+          <t>2025-11-10T07:02:14.138528+00:00</t>
         </is>
       </c>
     </row>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:17.895401+00:00</t>
+          <t>2025-11-10T07:02:16.453671+00:00</t>
         </is>
       </c>
     </row>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>2025-11-10T03:02:17.895429+00:00</t>
+          <t>2025-11-10T07:02:16.453702+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-11 15:06:06)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:26.910693+00:00</t>
+          <t>2025-11-11T07:03:33.328798+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:26.910729+00:00</t>
+          <t>2025-11-11T07:03:33.328841+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:26.910750+00:00</t>
+          <t>2025-11-11T07:03:33.328868+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:29.329086+00:00</t>
+          <t>2025-11-11T07:03:36.128766+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:29.329118+00:00</t>
+          <t>2025-11-11T07:03:36.128809+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:29.329139+00:00</t>
+          <t>2025-11-11T07:03:36.128830+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:31.645250+00:00</t>
+          <t>2025-11-11T07:03:38.959326+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:34.014152+00:00</t>
+          <t>2025-11-11T07:03:41.795700+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:34.014182+00:00</t>
+          <t>2025-11-11T07:03:41.795734+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:34.014201+00:00</t>
+          <t>2025-11-11T07:03:41.795756+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:36.803766+00:00</t>
+          <t>2025-11-11T07:03:44.565472+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:36.803796+00:00</t>
+          <t>2025-11-11T07:03:44.565507+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:36.803815+00:00</t>
+          <t>2025-11-11T07:03:44.565526+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:36.803831+00:00</t>
+          <t>2025-11-11T07:03:44.565543+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:42.335403+00:00</t>
+          <t>2025-11-11T07:03:49.132440+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:44.793298+00:00</t>
+          <t>2025-11-11T07:03:51.852141+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:47.105772+00:00</t>
+          <t>2025-11-11T07:03:54.047824+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:47.105801+00:00</t>
+          <t>2025-11-11T07:03:54.047863+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:47.105819+00:00</t>
+          <t>2025-11-11T07:03:54.047887+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:49.451508+00:00</t>
+          <t>2025-11-11T07:03:56.405613+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:52.210226+00:00</t>
+          <t>2025-11-11T07:03:59.179203+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:52.210259+00:00</t>
+          <t>2025-11-11T07:03:59.179255+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:54.980169+00:00</t>
+          <t>2025-11-11T07:04:01.915164+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:54.980205+00:00</t>
+          <t>2025-11-11T07:04:01.915198+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:54.980230+00:00</t>
+          <t>2025-11-11T07:04:01.915219+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:57.292229+00:00</t>
+          <t>2025-11-11T07:04:04.148967+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:57.292258+00:00</t>
+          <t>2025-11-11T07:04:04.148997+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:57.292277+00:00</t>
+          <t>2025-11-11T07:04:04.149017+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:57.292296+00:00</t>
+          <t>2025-11-11T07:04:04.149035+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:57.292311+00:00</t>
+          <t>2025-11-11T07:04:04.149052+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:59.997505+00:00</t>
+          <t>2025-11-11T07:04:06.946952+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-10T07:01:59.997538+00:00</t>
+          <t>2025-11-11T07:04:06.946984+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:02.276786+00:00</t>
+          <t>2025-11-11T07:04:09.641582+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:02.276816+00:00</t>
+          <t>2025-11-11T07:04:09.641616+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:02.276841+00:00</t>
+          <t>2025-11-11T07:04:09.641638+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:04.640557+00:00</t>
+          <t>2025-11-11T07:04:11.974401+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:04.640586+00:00</t>
+          <t>2025-11-11T07:04:11.974439+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:04.640605+00:00</t>
+          <t>2025-11-11T07:04:11.974460+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:07.071729+00:00</t>
+          <t>2025-11-11T07:04:14.277434+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:07.071766+00:00</t>
+          <t>2025-11-11T07:04:14.277468+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:07.071786+00:00</t>
+          <t>2025-11-11T07:04:14.277539+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:07.071805+00:00</t>
+          <t>2025-11-11T07:04:14.277568+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:07.071823+00:00</t>
+          <t>2025-11-11T07:04:14.277588+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:07.071839+00:00</t>
+          <t>2025-11-11T07:04:14.277605+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:09.304379+00:00</t>
+          <t>2025-11-11T07:04:16.556140+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:09.304409+00:00</t>
+          <t>2025-11-11T07:04:16.556171+00:00</t>
         </is>
       </c>
     </row>
@@ -3132,12 +3132,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Дроздов Иван</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -3147,12 +3147,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>30752</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ЦСК_дроздовиван</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:14.138463+00:00</t>
+          <t>2025-11-11T07:04:21.279309+00:00</t>
         </is>
       </c>
     </row>
@@ -3189,27 +3189,27 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Саморуков Дмитрий</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>24005</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>1369_ЦСК_саморуковдмитрий</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:14.138505+00:00</t>
+          <t>2025-11-11T07:04:21.279336+00:00</t>
         </is>
       </c>
     </row>
@@ -3246,12 +3246,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Саморуков Дмитрий</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -3261,12 +3261,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>41896</t>
+          <t>24005</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_ЦСК_саморуковдмитрий</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -3281,34 +3281,34 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:14.138528+00:00</t>
+          <t>2025-11-11T07:04:21.279354+00:00</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -3318,12 +3318,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>41896</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -3333,12 +3333,12 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>2025-11-10T07:02:16.453671+00:00</t>
+          <t>2025-11-11T07:04:21.279373+00:00</t>
         </is>
       </c>
     </row>
@@ -3360,42 +3360,99 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
+          <t>Гроло Жереми</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>45343</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>1369_ШДР_гроложереми</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>2025-11-11T07:04:23.979096+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
           <t>Саттер Райли</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr">
+      <c r="F53" t="inlineStr">
         <is>
           <t>нападающий</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="G53" t="inlineStr">
         <is>
           <t>45491</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr">
+      <c r="H53" t="inlineStr">
         <is>
           <t>1369_ШДР_саттеррайли</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
         <is>
           <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>2025-11-10T07:02:16.453702+00:00</t>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>2025-11-11T07:04:23.979125+00:00</t>
         </is>
       </c>
     </row>
@@ -3466,7 +3523,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3511,6 +3568,43 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Дроздов Иван</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_дроздовиван</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-11T15:04:24.488351+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-12 17:26:40)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:33.328798+00:00</t>
+          <t>2025-11-12T09:23:16.117744+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:33.328841+00:00</t>
+          <t>2025-11-12T09:23:16.117768+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:33.328868+00:00</t>
+          <t>2025-11-12T09:23:16.117781+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:36.128766+00:00</t>
+          <t>2025-11-12T09:23:18.816979+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:36.128809+00:00</t>
+          <t>2025-11-12T09:23:18.817023+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:36.128830+00:00</t>
+          <t>2025-11-12T09:23:18.817036+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:38.959326+00:00</t>
+          <t>2025-11-12T09:23:20.832321+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:41.795700+00:00</t>
+          <t>2025-11-12T09:23:23.281387+00:00</t>
         </is>
       </c>
     </row>
@@ -966,12 +966,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Броадхёрст Алекс</t>
+          <t>Гиздатуллин Артур</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>87</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -981,12 +981,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>27232</t>
+          <t>22208</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1369_АМР_броадхерсталекс</t>
+          <t>1369_АМР_гиздатуллинартур</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1001,49 +1001,49 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:41.795734+00:00</t>
+          <t>2025-11-12T09:23:23.281421+00:00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Гиздатуллин Артур</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>22208</t>
+          <t>28244</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1369_АМР_гиздатуллинартур</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1053,12 +1053,12 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:41.795756+00:00</t>
+          <t>2025-11-12T09:23:25.824617+00:00</t>
         </is>
       </c>
     </row>
@@ -1080,27 +1080,27 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Галимов Эмиль</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>28244</t>
+          <t>15997</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_БАР_галимовэмиль</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:44.565472+00:00</t>
+          <t>2025-11-12T09:23:25.824647+00:00</t>
         </is>
       </c>
     </row>
@@ -1137,12 +1137,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Галимов Эмиль</t>
+          <t>Мухаметов Максим</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>15997</t>
+          <t>25207</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_БАР_галимовэмиль</t>
+          <t>1369_БАР_мухаметовмаксим</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:44.565507+00:00</t>
+          <t>2025-11-12T09:23:25.824665+00:00</t>
         </is>
       </c>
     </row>
@@ -1194,27 +1194,27 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Мухаметов Максим</t>
+          <t>Уотерспун Тайлер</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>26</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>25207</t>
+          <t>45769</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_БАР_мухаметовмаксим</t>
+          <t>1369_БАР_уотерспунтайлер</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1229,34 +1229,34 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:44.565526+00:00</t>
+          <t>2025-11-12T09:23:25.824682+00:00</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>ДМН</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>dinamo_mn</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Уотерспун Тайлер</t>
+          <t>Уэлле Ксавье</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1266,12 +1266,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>45769</t>
+          <t>19692</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_БАР_уотерспунтайлер</t>
+          <t>1369_ДМН_уэллексавье</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1281,54 +1281,54 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:44.565543+00:00</t>
+          <t>2025-11-12T09:23:30.114612+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ДМН</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>dinamo_mn</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Уэлле Ксавье</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>19692</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_ДМН_уэллексавье</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,39 +1338,39 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:49.132440+00:00</t>
+          <t>2025-11-12T09:23:32.012341+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Волков Александр С</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1380,12 +1380,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_ЛОК_волковалександрс</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,12 +1395,12 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:51.852141+00:00</t>
+          <t>2025-11-12T09:23:33.975310+00:00</t>
         </is>
       </c>
     </row>
@@ -1422,12 +1422,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Волков Александр С</t>
+          <t>Паник Рихард</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>16071</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_ЛОК_волковалександрс</t>
+          <t>1369_ЛОК_паникрихард</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:54.047824+00:00</t>
+          <t>2025-11-12T09:23:33.975337+00:00</t>
         </is>
       </c>
     </row>
@@ -1479,27 +1479,27 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Паник Рихард</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>16071</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_ЛОК_паникрихард</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1514,49 +1514,49 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:54.047863+00:00</t>
+          <t>2025-11-12T09:23:33.975359+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1566,39 +1566,39 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:54.047887+00:00</t>
+          <t>2025-11-12T09:23:36.309807+00:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1623,12 +1623,12 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:56.405613+00:00</t>
+          <t>2025-11-12T09:23:39.395462+00:00</t>
         </is>
       </c>
     </row>
@@ -1650,12 +1650,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Попугаев Никита О</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1665,12 +1665,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>22683</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_НХК_попугаевникитао</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1685,49 +1685,49 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:59.179203+00:00</t>
+          <t>2025-11-12T09:23:39.395491+00:00</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>Ващенко Григорий</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>22683</t>
+          <t>14155</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>1369_СЕВ_ващенкогригорий</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1737,12 +1737,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-11T07:03:59.179255+00:00</t>
+          <t>2025-11-12T09:23:41.308603+00:00</t>
         </is>
       </c>
     </row>
@@ -1764,12 +1764,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Ващенко Григорий</t>
+          <t>Грудинин Владимир</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1779,12 +1779,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>14155</t>
+          <t>35064</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СЕВ_ващенкогригорий</t>
+          <t>1369_СЕВ_грудининвладимир</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:01.915164+00:00</t>
+          <t>2025-11-12T09:23:41.308634+00:00</t>
         </is>
       </c>
     </row>
@@ -1821,27 +1821,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Грудинин Владимир</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>35064</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СЕВ_грудининвладимир</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1856,49 +1856,49 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:01.915198+00:00</t>
+          <t>2025-11-12T09:23:41.308653+00:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Гордеев Фёдор</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>43049</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СИБ_гордеевфедор</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1908,12 +1908,12 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:01.915219+00:00</t>
+          <t>2025-11-12T09:23:43.623865+00:00</t>
         </is>
       </c>
     </row>
@@ -1935,12 +1935,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Гордеев Фёдор</t>
+          <t>Калиниченко Роман</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1950,12 +1950,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>43049</t>
+          <t>26690</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СИБ_гордеевфедор</t>
+          <t>1369_СИБ_калиниченкороман</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:04.148967+00:00</t>
+          <t>2025-11-12T09:23:43.623899+00:00</t>
         </is>
       </c>
     </row>
@@ -1992,12 +1992,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Калиниченко Роман</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2007,12 +2007,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>26690</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СИБ_калиниченкороман</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:04.148997+00:00</t>
+          <t>2025-11-12T09:23:43.623920+00:00</t>
         </is>
       </c>
     </row>
@@ -2049,27 +2049,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:04.149017+00:00</t>
+          <t>2025-11-12T09:23:43.623940+00:00</t>
         </is>
       </c>
     </row>
@@ -2106,12 +2106,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2121,12 +2121,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>16195</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2141,49 +2141,49 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:04.149035+00:00</t>
+          <t>2025-11-12T09:23:43.623957+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,12 +2193,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:04.149052+00:00</t>
+          <t>2025-11-12T09:23:45.568999+00:00</t>
         </is>
       </c>
     </row>
@@ -2220,27 +2220,27 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2255,34 +2255,34 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:06.946952+00:00</t>
+          <t>2025-11-12T09:23:45.569029+00:00</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2292,12 +2292,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>41566</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2307,12 +2307,12 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:06.946984+00:00</t>
+          <t>2025-11-12T09:23:48.492691+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,27 +2334,27 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:09.641582+00:00</t>
+          <t>2025-11-12T09:23:48.492726+00:00</t>
         </is>
       </c>
     </row>
@@ -2391,27 +2391,27 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2426,49 +2426,49 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:09.641616+00:00</t>
+          <t>2025-11-12T09:23:48.492751+00:00</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2478,12 +2478,12 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:09.641638+00:00</t>
+          <t>2025-11-12T09:23:50.808327+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,12 +2505,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2520,12 +2520,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:11.974401+00:00</t>
+          <t>2025-11-12T09:23:50.808363+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,12 +2562,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2597,34 +2597,34 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:11.974439+00:00</t>
+          <t>2025-11-12T09:23:50.808385+00:00</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2634,12 +2634,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2649,12 +2649,12 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:11.974460+00:00</t>
+          <t>2025-11-12T09:23:52.703282+00:00</t>
         </is>
       </c>
     </row>
@@ -2676,12 +2676,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2691,12 +2691,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:14.277434+00:00</t>
+          <t>2025-11-12T09:23:52.703312+00:00</t>
         </is>
       </c>
     </row>
@@ -2733,27 +2733,27 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:14.277468+00:00</t>
+          <t>2025-11-12T09:23:52.703331+00:00</t>
         </is>
       </c>
     </row>
@@ -2790,27 +2790,27 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:14.277539+00:00</t>
+          <t>2025-11-12T09:23:52.703351+00:00</t>
         </is>
       </c>
     </row>
@@ -2847,12 +2847,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2862,12 +2862,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:14.277568+00:00</t>
+          <t>2025-11-12T09:23:52.703369+00:00</t>
         </is>
       </c>
     </row>
@@ -2904,12 +2904,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2919,12 +2919,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2939,49 +2939,49 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:14.277588+00:00</t>
+          <t>2025-11-12T09:23:52.703388+00:00</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2991,12 +2991,12 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:14.277605+00:00</t>
+          <t>2025-11-12T09:23:54.549585+00:00</t>
         </is>
       </c>
     </row>
@@ -3018,27 +3018,27 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3053,34 +3053,34 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:16.556140+00:00</t>
+          <t>2025-11-12T09:23:54.549617+00:00</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Дроздов Иван</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3090,12 +3090,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>30752</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ЦСК_дроздовиван</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -3105,12 +3105,12 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:16.556171+00:00</t>
+          <t>2025-11-12T09:23:58.829989+00:00</t>
         </is>
       </c>
     </row>
@@ -3132,12 +3132,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Дроздов Иван</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -3147,12 +3147,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>30752</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1369_ЦСК_дроздовиван</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:21.279309+00:00</t>
+          <t>2025-11-12T09:23:58.830016+00:00</t>
         </is>
       </c>
     </row>
@@ -3189,27 +3189,27 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Саморуков Дмитрий</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>24005</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ЦСК_саморуковдмитрий</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:21.279336+00:00</t>
+          <t>2025-11-12T09:23:58.830034+00:00</t>
         </is>
       </c>
     </row>
@@ -3246,12 +3246,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Саморуков Дмитрий</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -3261,12 +3261,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>24005</t>
+          <t>41896</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>1369_ЦСК_саморуковдмитрий</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -3281,34 +3281,34 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:21.279354+00:00</t>
+          <t>2025-11-12T09:23:58.830051+00:00</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -3318,12 +3318,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>41896</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -3333,12 +3333,12 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:21.279373+00:00</t>
+          <t>2025-11-12T09:24:01.169066+00:00</t>
         </is>
       </c>
     </row>
@@ -3360,27 +3360,27 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Саттер Райли</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>45491</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ШДР_саттеррайли</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -3395,64 +3395,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>2025-11-11T07:04:23.979096+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Саттер Райли</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>45491</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>1369_ШДР_саттеррайли</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>2025-11-11T07:04:23.979125+00:00</t>
+          <t>2025-11-12T09:24:01.169097+00:00</t>
         </is>
       </c>
     </row>
@@ -3462,6 +3405,99 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>team_abbr</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>team_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>player_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>player_uid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>changed_at</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>changed_day</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>АМР</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Амур</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Броадхёрст Алекс</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_АМР_броадхерсталекс</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-12T17:24:01.672404+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3515,97 +3551,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>team_abbr</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>team_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>player_name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>player_uid</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>changed_at</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>changed_day</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Дроздов Иван</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_дроздовиван</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-11T15:04:24.488351+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-11</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-13 11:04:22)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:16.117744+00:00</t>
+          <t>2025-11-13T03:01:50.734844+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:16.117768+00:00</t>
+          <t>2025-11-13T03:01:50.734878+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:16.117781+00:00</t>
+          <t>2025-11-13T03:01:50.734897+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:18.816979+00:00</t>
+          <t>2025-11-13T03:01:53.012492+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:18.817023+00:00</t>
+          <t>2025-11-13T03:01:53.012524+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:18.817036+00:00</t>
+          <t>2025-11-13T03:01:53.012543+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:20.832321+00:00</t>
+          <t>2025-11-13T03:01:55.820295+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:23.281387+00:00</t>
+          <t>2025-11-13T03:01:58.415780+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:23.281421+00:00</t>
+          <t>2025-11-13T03:01:58.415810+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:25.824617+00:00</t>
+          <t>2025-11-13T03:02:01.201358+00:00</t>
         </is>
       </c>
     </row>
@@ -1080,27 +1080,27 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Галимов Эмиль</t>
+          <t>Уотерспун Тайлер</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>26</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>15997</t>
+          <t>45769</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_БАР_галимовэмиль</t>
+          <t>1369_БАР_уотерспунтайлер</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1115,49 +1115,49 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:25.824647+00:00</t>
+          <t>2025-11-13T03:02:01.201390+00:00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>ДМН</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>dinamo_mn</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Мухаметов Максим</t>
+          <t>Уэлле Ксавье</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>25207</t>
+          <t>19692</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_БАР_мухаметовмаксим</t>
+          <t>1369_ДМН_уэллексавье</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1167,54 +1167,54 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:25.824665+00:00</t>
+          <t>2025-11-13T03:02:06.354585+00:00</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Уотерспун Тайлер</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>45769</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_БАР_уотерспунтайлер</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1224,54 +1224,54 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:25.824682+00:00</t>
+          <t>2025-11-13T03:02:08.711291+00:00</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ДМН</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>dinamo_mn</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Уэлле Ксавье</t>
+          <t>Волков Александр С</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>19692</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_ДМН_уэллексавье</t>
+          <t>1369_ЛОК_волковалександрс</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1281,39 +1281,39 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:30.114612+00:00</t>
+          <t>2025-11-13T03:02:11.439894+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Паник Рихард</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1323,12 +1323,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>16071</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_ЛОК_паникрихард</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,12 +1338,12 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:32.012341+00:00</t>
+          <t>2025-11-13T03:02:11.439923+00:00</t>
         </is>
       </c>
     </row>
@@ -1365,27 +1365,27 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Волков Александр С</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_ЛОК_волковалександрс</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1400,34 +1400,34 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:33.975310+00:00</t>
+          <t>2025-11-13T03:02:11.439942+00:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Паник Рихард</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>16071</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_ЛОК_паникрихард</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1452,54 +1452,54 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:33.975337+00:00</t>
+          <t>2025-11-13T03:02:13.696800+00:00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1509,39 +1509,39 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:33.975359+00:00</t>
+          <t>2025-11-13T03:02:16.516971+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Попугаев Никита О</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1551,12 +1551,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>22683</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_НХК_попугаевникитао</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1566,54 +1566,54 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:36.309807+00:00</t>
+          <t>2025-11-13T03:02:16.517005+00:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Ващенко Григорий</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>14155</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_СЕВ_ващенкогригорий</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1623,54 +1623,54 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:39.395462+00:00</t>
+          <t>2025-11-13T03:02:19.220030+00:00</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>Грудинин Владимир</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>22683</t>
+          <t>35064</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>1369_СЕВ_грудининвладимир</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1680,12 +1680,12 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:39.395491+00:00</t>
+          <t>2025-11-13T03:02:19.220058+00:00</t>
         </is>
       </c>
     </row>
@@ -1707,27 +1707,27 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Ващенко Григорий</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>14155</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СЕВ_ващенкогригорий</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1742,34 +1742,34 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:41.308603+00:00</t>
+          <t>2025-11-13T03:02:19.220076+00:00</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Грудинин Владимир</t>
+          <t>Гордеев Фёдор</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1779,12 +1779,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>35064</t>
+          <t>43049</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СЕВ_грудининвладимир</t>
+          <t>1369_СИБ_гордеевфедор</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1794,54 +1794,54 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:41.308634+00:00</t>
+          <t>2025-11-13T03:02:21.543434+00:00</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Калиниченко Роман</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>26690</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СИБ_калиниченкороман</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1851,12 +1851,12 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:41.308653+00:00</t>
+          <t>2025-11-13T03:02:21.543478+00:00</t>
         </is>
       </c>
     </row>
@@ -1878,12 +1878,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Гордеев Фёдор</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>43049</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СИБ_гордеевфедор</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:43.623865+00:00</t>
+          <t>2025-11-13T03:02:21.543498+00:00</t>
         </is>
       </c>
     </row>
@@ -1935,27 +1935,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Калиниченко Роман</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>26690</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СИБ_калиниченкороман</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:43.623899+00:00</t>
+          <t>2025-11-13T03:02:21.543519+00:00</t>
         </is>
       </c>
     </row>
@@ -1992,27 +1992,27 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2027,49 +2027,49 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:43.623920+00:00</t>
+          <t>2025-11-13T03:02:21.543540+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>16195</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,39 +2079,39 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:43.623940+00:00</t>
+          <t>2025-11-13T03:02:24.499225+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2121,12 +2121,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2136,54 +2136,54 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:43.623957+00:00</t>
+          <t>2025-11-13T03:02:24.499255+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,54 +2193,54 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:45.568999+00:00</t>
+          <t>2025-11-13T03:02:26.784893+00:00</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>41566</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2250,12 +2250,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:45.569029+00:00</t>
+          <t>2025-11-13T03:02:26.784924+00:00</t>
         </is>
       </c>
     </row>
@@ -2277,27 +2277,27 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2312,49 +2312,49 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:48.492691+00:00</t>
+          <t>2025-11-13T03:02:26.784944+00:00</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2364,54 +2364,54 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:48.492726+00:00</t>
+          <t>2025-11-13T03:02:29.085973+00:00</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2421,12 +2421,12 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:48.492751+00:00</t>
+          <t>2025-11-13T03:02:29.086005+00:00</t>
         </is>
       </c>
     </row>
@@ -2448,12 +2448,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2463,12 +2463,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2483,34 +2483,34 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:50.808327+00:00</t>
+          <t>2025-11-13T03:02:29.086024+00:00</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2520,12 +2520,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2535,39 +2535,39 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:50.808363+00:00</t>
+          <t>2025-11-13T03:02:31.446412+00:00</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2592,12 +2592,12 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:50.808385+00:00</t>
+          <t>2025-11-13T03:02:31.446442+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,27 +2619,27 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:52.703282+00:00</t>
+          <t>2025-11-13T03:02:31.446461+00:00</t>
         </is>
       </c>
     </row>
@@ -2676,12 +2676,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2691,12 +2691,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:52.703312+00:00</t>
+          <t>2025-11-13T03:02:31.446479+00:00</t>
         </is>
       </c>
     </row>
@@ -2733,27 +2733,27 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:52.703331+00:00</t>
+          <t>2025-11-13T03:02:31.446496+00:00</t>
         </is>
       </c>
     </row>
@@ -2790,12 +2790,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2805,12 +2805,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2825,49 +2825,49 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:52.703351+00:00</t>
+          <t>2025-11-13T03:02:31.446512+00:00</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2877,39 +2877,39 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:52.703369+00:00</t>
+          <t>2025-11-13T03:02:34.240103+00:00</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2919,12 +2919,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2934,54 +2934,54 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:52.703388+00:00</t>
+          <t>2025-11-13T03:02:34.240134+00:00</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Дроздов Иван</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>30752</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ЦСК_дроздовиван</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2991,39 +2991,39 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:54.549585+00:00</t>
+          <t>2025-11-13T03:02:39.366117+00:00</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3033,12 +3033,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3048,12 +3048,12 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:54.549617+00:00</t>
+          <t>2025-11-13T03:02:39.366149+00:00</t>
         </is>
       </c>
     </row>
@@ -3075,27 +3075,27 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Дроздов Иван</t>
+          <t>Саморуков Дмитрий</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>30752</t>
+          <t>24005</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>1369_ЦСК_дроздовиван</t>
+          <t>1369_ЦСК_саморуковдмитрий</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:58.829989+00:00</t>
+          <t>2025-11-13T03:02:39.366169+00:00</t>
         </is>
       </c>
     </row>
@@ -3132,27 +3132,27 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>41896</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3167,34 +3167,34 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:58.830016+00:00</t>
+          <t>2025-11-13T03:02:39.366186+00:00</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Саморуков Дмитрий</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -3204,12 +3204,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>24005</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>1369_ЦСК_саморуковдмитрий</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -3219,54 +3219,54 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:58.830034+00:00</t>
+          <t>2025-11-13T03:02:42.022852+00:00</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Саттер Райли</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>41896</t>
+          <t>45491</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_ШДР_саттеррайли</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -3276,126 +3276,12 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-12T09:23:58.830051+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Гроло Жереми</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>45343</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>1369_ШДР_гроложереми</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>2025-11-12T09:24:01.169066+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Саттер Райли</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>45491</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>1369_ШДР_саттеррайли</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>2025-11-12T09:24:01.169097+00:00</t>
+          <t>2025-11-13T03:02:42.022881+00:00</t>
         </is>
       </c>
     </row>
@@ -3410,7 +3296,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3458,22 +3344,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Броадхёрст Алекс</t>
+          <t>Галимов Эмиль</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_АМР_броадхерсталекс</t>
+          <t>1369_БАР_галимовэмиль</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -3483,12 +3369,49 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-12T17:24:01.672404+08:00</t>
+          <t>2025-11-13T11:02:42.529087+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-12</t>
+          <t>2025-11-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>БАР</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Барыс</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Мухаметов Максим</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1369_БАР_мухаметовмаксим</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-11-13T11:02:42.529087+08:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-11-13</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-13 12:11:48)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-13T03:01:50.734844+00:00</t>
+          <t>2025-11-13T04:09:45.807995+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-13T03:01:50.734878+00:00</t>
+          <t>2025-11-13T04:09:45.808030+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-13T03:01:50.734897+00:00</t>
+          <t>2025-11-13T04:09:45.808051+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-13T03:01:53.012492+00:00</t>
+          <t>2025-11-13T04:09:48.295242+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-13T03:01:53.012524+00:00</t>
+          <t>2025-11-13T04:09:48.295268+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-13T03:01:53.012543+00:00</t>
+          <t>2025-11-13T04:09:48.295281+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-13T03:01:55.820295+00:00</t>
+          <t>2025-11-13T04:09:50.299829+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-13T03:01:58.415780+00:00</t>
+          <t>2025-11-13T04:09:52.810673+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-13T03:01:58.415810+00:00</t>
+          <t>2025-11-13T04:09:52.810704+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:01.201358+00:00</t>
+          <t>2025-11-13T04:09:55.374809+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:01.201390+00:00</t>
+          <t>2025-11-13T04:09:55.374841+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:06.354585+00:00</t>
+          <t>2025-11-13T04:09:59.448723+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:08.711291+00:00</t>
+          <t>2025-11-13T04:10:01.949244+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:11.439894+00:00</t>
+          <t>2025-11-13T04:10:03.989603+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:11.439923+00:00</t>
+          <t>2025-11-13T04:10:03.989621+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:11.439942+00:00</t>
+          <t>2025-11-13T04:10:03.989629+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:13.696800+00:00</t>
+          <t>2025-11-13T04:10:06.051236+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:16.516971+00:00</t>
+          <t>2025-11-13T04:10:08.089615+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:16.517005+00:00</t>
+          <t>2025-11-13T04:10:08.089645+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:19.220030+00:00</t>
+          <t>2025-11-13T04:10:10.108008+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:19.220058+00:00</t>
+          <t>2025-11-13T04:10:10.108031+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:19.220076+00:00</t>
+          <t>2025-11-13T04:10:10.108040+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:21.543434+00:00</t>
+          <t>2025-11-13T04:10:12.260466+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:21.543478+00:00</t>
+          <t>2025-11-13T04:10:12.260493+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:21.543498+00:00</t>
+          <t>2025-11-13T04:10:12.260511+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:21.543519+00:00</t>
+          <t>2025-11-13T04:10:12.260526+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:21.543540+00:00</t>
+          <t>2025-11-13T04:10:12.260540+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:24.499225+00:00</t>
+          <t>2025-11-13T04:10:14.783397+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:24.499255+00:00</t>
+          <t>2025-11-13T04:10:14.783419+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:26.784893+00:00</t>
+          <t>2025-11-13T04:10:17.272374+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:26.784924+00:00</t>
+          <t>2025-11-13T04:10:17.272404+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:26.784944+00:00</t>
+          <t>2025-11-13T04:10:17.272423+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:29.085973+00:00</t>
+          <t>2025-11-13T04:10:19.297982+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:29.086005+00:00</t>
+          <t>2025-11-13T04:10:19.298003+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:29.086024+00:00</t>
+          <t>2025-11-13T04:10:19.298011+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:31.446412+00:00</t>
+          <t>2025-11-13T04:10:21.386575+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:31.446442+00:00</t>
+          <t>2025-11-13T04:10:21.386591+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:31.446461+00:00</t>
+          <t>2025-11-13T04:10:21.386599+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:31.446479+00:00</t>
+          <t>2025-11-13T04:10:21.386606+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:31.446496+00:00</t>
+          <t>2025-11-13T04:10:21.386613+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:31.446512+00:00</t>
+          <t>2025-11-13T04:10:21.386620+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:34.240103+00:00</t>
+          <t>2025-11-13T04:10:23.846904+00:00</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:34.240134+00:00</t>
+          <t>2025-11-13T04:10:23.846926+00:00</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:39.366117+00:00</t>
+          <t>2025-11-13T04:10:28.795166+00:00</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:39.366149+00:00</t>
+          <t>2025-11-13T04:10:28.795187+00:00</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:39.366169+00:00</t>
+          <t>2025-11-13T04:10:28.795196+00:00</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:39.366186+00:00</t>
+          <t>2025-11-13T04:10:28.795204+00:00</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:42.022852+00:00</t>
+          <t>2025-11-13T04:10:30.796772+00:00</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>2025-11-13T03:02:42.022881+00:00</t>
+          <t>2025-11-13T04:10:30.796790+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-13 17:48:51)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-13T04:09:45.807995+00:00</t>
+          <t>2025-11-13T09:46:51.454806+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-13T04:09:45.808030+00:00</t>
+          <t>2025-11-13T09:46:51.454829+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-13T04:09:45.808051+00:00</t>
+          <t>2025-11-13T09:46:51.454887+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-13T04:09:48.295242+00:00</t>
+          <t>2025-11-13T09:46:54.045003+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-13T04:09:48.295268+00:00</t>
+          <t>2025-11-13T09:46:54.045042+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-13T04:09:48.295281+00:00</t>
+          <t>2025-11-13T09:46:54.045065+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-13T04:09:50.299829+00:00</t>
+          <t>2025-11-13T09:46:56.296170+00:00</t>
         </is>
       </c>
     </row>
@@ -944,49 +944,49 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-13T04:09:52.810673+00:00</t>
+          <t>2025-11-13T09:46:58.570210+00:00</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Гиздатуллин Артур</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>22208</t>
+          <t>28244</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1369_АМР_гиздатуллинартур</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -996,12 +996,12 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-13T04:09:52.810704+00:00</t>
+          <t>2025-11-13T09:47:01.414786+00:00</t>
         </is>
       </c>
     </row>
@@ -1023,27 +1023,27 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Уотерспун Тайлер</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>26</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>28244</t>
+          <t>45769</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_БАР_уотерспунтайлер</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1058,34 +1058,34 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-13T04:09:55.374809+00:00</t>
+          <t>2025-11-13T09:47:01.414857+00:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>ДМН</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>dinamo_mn</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Уотерспун Тайлер</t>
+          <t>Уэлле Ксавье</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1095,12 +1095,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>45769</t>
+          <t>19692</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_БАР_уотерспунтайлер</t>
+          <t>1369_ДМН_уэллексавье</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1110,54 +1110,54 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-13T04:09:55.374841+00:00</t>
+          <t>2025-11-13T09:47:06.077465+00:00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ДМН</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>dinamo_mn</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Уэлле Ксавье</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>19692</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_ДМН_уэллексавье</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1167,39 +1167,39 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-13T04:09:59.448723+00:00</t>
+          <t>2025-11-13T09:47:08.385171+00:00</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Волков Александр С</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1209,12 +1209,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_ЛОК_волковалександрс</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1224,12 +1224,12 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:01.949244+00:00</t>
+          <t>2025-11-13T09:47:11.266096+00:00</t>
         </is>
       </c>
     </row>
@@ -1251,12 +1251,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Волков Александр С</t>
+          <t>Паник Рихард</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1266,12 +1266,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>16071</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_ЛОК_волковалександрс</t>
+          <t>1369_ЛОК_паникрихард</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:03.989603+00:00</t>
+          <t>2025-11-13T09:47:11.266130+00:00</t>
         </is>
       </c>
     </row>
@@ -1308,27 +1308,27 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Паник Рихард</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>16071</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_ЛОК_паникрихард</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1343,49 +1343,49 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:03.989621+00:00</t>
+          <t>2025-11-13T09:47:11.266151+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,39 +1395,39 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:03.989629+00:00</t>
+          <t>2025-11-13T09:47:13.626142+00:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1452,12 +1452,12 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:06.051236+00:00</t>
+          <t>2025-11-13T09:47:16.482744+00:00</t>
         </is>
       </c>
     </row>
@@ -1479,12 +1479,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Попугаев Никита О</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1494,12 +1494,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>22683</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_НХК_попугаевникитао</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1514,34 +1514,34 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:08.089615+00:00</t>
+          <t>2025-11-13T09:47:16.482779+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1551,12 +1551,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>22683</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1566,39 +1566,39 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:08.089645+00:00</t>
+          <t>2025-11-13T09:47:19.333270+00:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Ващенко Григорий</t>
+          <t>Гордеев Фёдор</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>14155</t>
+          <t>43049</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_СЕВ_ващенкогригорий</t>
+          <t>1369_СИБ_гордеевфедор</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1623,39 +1623,39 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:10.108008+00:00</t>
+          <t>2025-11-13T09:47:21.674157+00:00</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Грудинин Владимир</t>
+          <t>Калиниченко Роман</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1665,12 +1665,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>35064</t>
+          <t>26690</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СЕВ_грудининвладимир</t>
+          <t>1369_СИБ_калиниченкороман</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1680,54 +1680,54 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:10.108031+00:00</t>
+          <t>2025-11-13T09:47:21.674188+00:00</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1737,12 +1737,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:10.108040+00:00</t>
+          <t>2025-11-13T09:47:21.674207+00:00</t>
         </is>
       </c>
     </row>
@@ -1764,27 +1764,27 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Гордеев Фёдор</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>43049</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СИБ_гордеевфедор</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:12.260466+00:00</t>
+          <t>2025-11-13T09:47:21.674224+00:00</t>
         </is>
       </c>
     </row>
@@ -1821,27 +1821,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Калиниченко Роман</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>26690</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СИБ_калиниченкороман</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1856,29 +1856,29 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:12.260493+00:00</t>
+          <t>2025-11-13T09:47:21.674241+00:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1908,39 +1908,39 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:12.260511+00:00</t>
+          <t>2025-11-13T09:47:24.023834+00:00</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1950,12 +1950,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>16195</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1965,39 +1965,39 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:12.260526+00:00</t>
+          <t>2025-11-13T09:47:24.023865+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2007,12 +2007,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,39 +2022,39 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:12.260540+00:00</t>
+          <t>2025-11-13T09:47:26.264440+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2064,12 +2064,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,54 +2079,54 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:14.783397+00:00</t>
+          <t>2025-11-13T09:47:26.264475+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>41566</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2136,39 +2136,39 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:14.783419+00:00</t>
+          <t>2025-11-13T09:47:26.264495+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2178,12 +2178,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,54 +2193,54 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:17.272374+00:00</t>
+          <t>2025-11-13T09:47:29.031770+00:00</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Порядин Павел</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СПР_порядинпавел</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2250,54 +2250,54 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:17.272404+00:00</t>
+          <t>2025-11-13T09:47:29.031798+00:00</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2307,39 +2307,39 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:17.272423+00:00</t>
+          <t>2025-11-13T09:47:29.031815+00:00</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2349,12 +2349,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2364,39 +2364,39 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:19.297982+00:00</t>
+          <t>2025-11-13T09:47:31.243083+00:00</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Порядин Павел</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2406,12 +2406,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СПР_порядинпавел</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2421,54 +2421,54 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:19.298003+00:00</t>
+          <t>2025-11-13T09:47:31.243112+00:00</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2478,12 +2478,12 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:19.298011+00:00</t>
+          <t>2025-11-13T09:47:31.243129+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,12 +2505,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2520,12 +2520,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:21.386575+00:00</t>
+          <t>2025-11-13T09:47:31.243144+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,12 +2562,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:21.386591+00:00</t>
+          <t>2025-11-13T09:47:31.243163+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,27 +2619,27 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,49 +2654,49 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:21.386599+00:00</t>
+          <t>2025-11-13T09:47:31.243179+00:00</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2706,39 +2706,39 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:21.386606+00:00</t>
+          <t>2025-11-13T09:47:34.060908+00:00</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2748,12 +2748,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2763,39 +2763,39 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:21.386613+00:00</t>
+          <t>2025-11-13T09:47:34.060939+00:00</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Дроздов Иван</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2805,12 +2805,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>30752</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ЦСК_дроздовиван</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2820,54 +2820,54 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:21.386620+00:00</t>
+          <t>2025-11-13T09:47:38.774881+00:00</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2877,54 +2877,54 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:23.846904+00:00</t>
+          <t>2025-11-13T09:47:38.774918+00:00</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Саморуков Дмитрий</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>24005</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ЦСК_саморуковдмитрий</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2934,12 +2934,12 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:23.846926+00:00</t>
+          <t>2025-11-13T09:47:38.774940+00:00</t>
         </is>
       </c>
     </row>
@@ -2961,27 +2961,27 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Дроздов Иван</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>30752</t>
+          <t>41896</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_ЦСК_дроздовиван</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2996,49 +2996,49 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:28.795166+00:00</t>
+          <t>2025-11-13T09:47:38.774959+00:00</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3048,54 +3048,54 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:28.795187+00:00</t>
+          <t>2025-11-13T09:47:41.488374+00:00</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Саморуков Дмитрий</t>
+          <t>Саттер Райли</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>24005</t>
+          <t>45491</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>1369_ЦСК_саморуковдмитрий</t>
+          <t>1369_ШДР_саттеррайли</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -3105,183 +3105,12 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2025-11-13T04:10:28.795196+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>cska</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Уильямс Колби</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>41896</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_уильямсколби</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>2025-11-13T04:10:28.795204+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Гроло Жереми</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>45343</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>1369_ШДР_гроложереми</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>2025-11-13T04:10:30.796772+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Саттер Райли</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>45491</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>1369_ШДР_саттеррайли</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>2025-11-13T04:10:30.796790+00:00</t>
+          <t>2025-11-13T09:47:41.488405+00:00</t>
         </is>
       </c>
     </row>
@@ -3296,7 +3125,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3410,6 +3239,117 @@
         </is>
       </c>
       <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-11-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>АМР</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Амур</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Гиздатуллин Артур</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1369_АМР_гиздатуллинартур</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-11-13T17:47:41.991047+08:00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-11-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>СЕВ</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Северсталь</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ващенко Григорий</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1369_СЕВ_ващенкогригорий</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-11-13T17:47:41.991047+08:00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025-11-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>СЕВ</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Северсталь</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Грудинин Владимир</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1369_СЕВ_грудининвладимир</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-11-13T17:47:41.991047+08:00</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>2025-11-13</t>
         </is>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-14 18:23:43)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:32.702746+00:00</t>
+          <t>2025-11-14T10:21:32.962284+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:32.702785+00:00</t>
+          <t>2025-11-14T10:21:32.962320+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:32.702809+00:00</t>
+          <t>2025-11-14T10:21:32.962341+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:34.635737+00:00</t>
+          <t>2025-11-14T10:21:34.993843+00:00</t>
         </is>
       </c>
     </row>
@@ -738,27 +738,27 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Старков Степан</t>
+          <t>Шепелев Александр</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>27000</t>
+          <t>23447</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1369_АДМ_старковстепан</t>
+          <t>1369_АДМ_шепелевалександр</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -773,34 +773,34 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:34.635769+00:00</t>
+          <t>2025-11-14T10:21:34.993876+00:00</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>АКБ</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>admiral</t>
+          <t>ak_bars</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Шепелев Александр</t>
+          <t>Яруллин Альберт</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -810,12 +810,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>23447</t>
+          <t>16365</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1369_АДМ_шепелевалександр</t>
+          <t>1369_АКБ_яруллинальберт</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -825,39 +825,39 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/admiral/team/</t>
+          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:34.635791+00:00</t>
+          <t>2025-11-14T10:21:37.063284+00:00</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>АКБ</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ak_bars</t>
+          <t>amur</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Яруллин Альберт</t>
+          <t>Абросимов Роман</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>94</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -867,12 +867,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>16365</t>
+          <t>17968</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1369_АКБ_яруллинальберт</t>
+          <t>1369_АМР_абросимовроман</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -882,54 +882,54 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:37.060110+00:00</t>
+          <t>2025-11-14T10:21:39.074441+00:00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Абросимов Роман</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>17968</t>
+          <t>28244</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1369_АМР_абросимовроман</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -939,12 +939,12 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:38.943707+00:00</t>
+          <t>2025-11-14T10:21:41.137384+00:00</t>
         </is>
       </c>
     </row>
@@ -966,27 +966,27 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Уотерспун Тайлер</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>26</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>28244</t>
+          <t>45769</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_БАР_уотерспунтайлер</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1001,34 +1001,34 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:41.006366+00:00</t>
+          <t>2025-11-14T10:21:41.137412+00:00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>ДМН</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>dinamo_mn</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Уотерспун Тайлер</t>
+          <t>Уэлле Ксавье</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1038,12 +1038,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>45769</t>
+          <t>19692</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1369_БАР_уотерспунтайлер</t>
+          <t>1369_ДМН_уэллексавье</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1053,54 +1053,54 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:41.006405+00:00</t>
+          <t>2025-11-14T10:21:45.563918+00:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ДМН</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>dinamo_mn</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Уэлле Ксавье</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>19692</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_ДМН_уэллексавье</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1110,39 +1110,39 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:46.108687+00:00</t>
+          <t>2025-11-14T10:21:48.040073+00:00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Волков Александр С</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_ЛОК_волковалександрс</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1167,12 +1167,12 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:48.433474+00:00</t>
+          <t>2025-11-14T10:21:50.506888+00:00</t>
         </is>
       </c>
     </row>
@@ -1194,12 +1194,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Волков Александр С</t>
+          <t>Паник Рихард</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1209,12 +1209,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>16071</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_ЛОК_волковалександрс</t>
+          <t>1369_ЛОК_паникрихард</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:50.302998+00:00</t>
+          <t>2025-11-14T10:21:50.506916+00:00</t>
         </is>
       </c>
     </row>
@@ -1251,27 +1251,27 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Паник Рихард</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>16071</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_ЛОК_паникрихард</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1286,49 +1286,49 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:50.303028+00:00</t>
+          <t>2025-11-14T10:21:50.506934+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,39 +1338,39 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:50.303047+00:00</t>
+          <t>2025-11-14T10:21:52.542325+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1380,12 +1380,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,12 +1395,12 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:52.669790+00:00</t>
+          <t>2025-11-14T10:21:54.558066+00:00</t>
         </is>
       </c>
     </row>
@@ -1422,12 +1422,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Попугаев Никита О</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>22683</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_НХК_попугаевникитао</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1457,34 +1457,34 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:54.591539+00:00</t>
+          <t>2025-11-14T10:21:54.558137+00:00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1494,12 +1494,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>22683</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1509,54 +1509,54 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:54.591571+00:00</t>
+          <t>2025-11-14T10:21:56.657045+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Гордеев Фёдор</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>43049</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СИБ_гордеевфедор</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1566,12 +1566,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:56.966902+00:00</t>
+          <t>2025-11-14T10:21:59.023420+00:00</t>
         </is>
       </c>
     </row>
@@ -1593,12 +1593,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Гордеев Фёдор</t>
+          <t>Калиниченко Роман</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>43049</t>
+          <t>26690</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_СИБ_гордеевфедор</t>
+          <t>1369_СИБ_калиниченкороман</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:58.957548+00:00</t>
+          <t>2025-11-14T10:21:59.023450+00:00</t>
         </is>
       </c>
     </row>
@@ -1650,12 +1650,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Калиниченко Роман</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1665,12 +1665,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>26690</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СИБ_калиниченкороман</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:58.957585+00:00</t>
+          <t>2025-11-14T10:21:59.023484+00:00</t>
         </is>
       </c>
     </row>
@@ -1707,27 +1707,27 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:58.957611+00:00</t>
+          <t>2025-11-14T10:21:59.023497+00:00</t>
         </is>
       </c>
     </row>
@@ -1764,12 +1764,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1779,12 +1779,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>16195</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1799,49 +1799,49 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:58.957631+00:00</t>
+          <t>2025-11-14T10:21:59.023505+00:00</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1851,12 +1851,12 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-14T07:02:58.957654+00:00</t>
+          <t>2025-11-14T10:22:01.699171+00:00</t>
         </is>
       </c>
     </row>
@@ -1878,27 +1878,27 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1913,34 +1913,34 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:01.371741+00:00</t>
+          <t>2025-11-14T10:22:01.699186+00:00</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1950,12 +1950,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>41566</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1965,12 +1965,12 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:01.371772+00:00</t>
+          <t>2025-11-14T10:22:03.884138+00:00</t>
         </is>
       </c>
     </row>
@@ -1992,27 +1992,27 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Мачулин Василий</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>33926</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СОЧ_мачулинвасилий</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:03.728395+00:00</t>
+          <t>2025-11-14T10:22:03.884168+00:00</t>
         </is>
       </c>
     </row>
@@ -2049,27 +2049,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Мачулин Василий</t>
+          <t>Хомченко Павел</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>33926</t>
+          <t>17592</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
+          <t>1369_СОЧ_хомченкопавел</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2084,49 +2084,49 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:03.728427+00:00</t>
+          <t>2025-11-14T10:22:03.884187+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Хомченко Павел</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>17592</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хомченкопавел</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2136,12 +2136,12 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:03.728446+00:00</t>
+          <t>2025-11-14T10:22:06.044713+00:00</t>
         </is>
       </c>
     </row>
@@ -2163,12 +2163,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2178,12 +2178,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2198,34 +2198,34 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:05.673334+00:00</t>
+          <t>2025-11-14T10:22:06.044758+00:00</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2235,12 +2235,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2250,12 +2250,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:05.673370+00:00</t>
+          <t>2025-11-14T10:22:08.151554+00:00</t>
         </is>
       </c>
     </row>
@@ -2277,12 +2277,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2292,12 +2292,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:07.514020+00:00</t>
+          <t>2025-11-14T10:22:08.151586+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,27 +2334,27 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:07.514051+00:00</t>
+          <t>2025-11-14T10:22:08.151605+00:00</t>
         </is>
       </c>
     </row>
@@ -2391,27 +2391,27 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Кузьмин Глеб</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>22170</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_кузьминглеб</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:07.514070+00:00</t>
+          <t>2025-11-14T10:22:08.151622+00:00</t>
         </is>
       </c>
     </row>
@@ -2448,12 +2448,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Кузьмин Глеб</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2463,12 +2463,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>22170</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:07.514086+00:00</t>
+          <t>2025-11-14T10:22:08.151638+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,12 +2505,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2520,12 +2520,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,49 +2540,49 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:07.514102+00:00</t>
+          <t>2025-11-14T10:22:08.151653+00:00</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2592,12 +2592,12 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:07.514125+00:00</t>
+          <t>2025-11-14T10:22:10.549949+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,27 +2619,27 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,34 +2654,34 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:09.403645+00:00</t>
+          <t>2025-11-14T10:22:10.549980+00:00</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Дроздов Иван</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2691,12 +2691,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>30752</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ЦСК_дроздовиван</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2706,12 +2706,12 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:09.403676+00:00</t>
+          <t>2025-11-14T10:22:14.627151+00:00</t>
         </is>
       </c>
     </row>
@@ -2733,12 +2733,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Дроздов Иван</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2748,12 +2748,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>30752</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_ЦСК_дроздовиван</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:13.834739+00:00</t>
+          <t>2025-11-14T10:22:14.627181+00:00</t>
         </is>
       </c>
     </row>
@@ -2790,27 +2790,27 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Саморуков Дмитрий</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>24005</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ЦСК_саморуковдмитрий</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:13.834781+00:00</t>
+          <t>2025-11-14T10:22:14.627201+00:00</t>
         </is>
       </c>
     </row>
@@ -2847,12 +2847,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Саморуков Дмитрий</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2862,12 +2862,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>24005</t>
+          <t>41896</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1369_ЦСК_саморуковдмитрий</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2882,34 +2882,34 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:13.834806+00:00</t>
+          <t>2025-11-14T10:22:14.627218+00:00</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2919,12 +2919,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>41896</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2934,12 +2934,12 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:13.834826+00:00</t>
+          <t>2025-11-14T10:22:16.666831+00:00</t>
         </is>
       </c>
     </row>
@@ -2961,27 +2961,27 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Саттер Райли</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>45343</t>
+          <t>45491</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ШДР_саттеррайли</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2996,64 +2996,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2025-11-14T07:03:16.279323+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Саттер Райли</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>45491</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>1369_ШДР_саттеррайли</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>2025-11-14T07:03:16.279352+00:00</t>
+          <t>2025-11-14T10:22:16.666850+00:00</t>
         </is>
       </c>
     </row>
@@ -3068,7 +3011,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3145,6 +3088,43 @@
         </is>
       </c>
       <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>АДМ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Адмирал</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Старков Степан</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1369_АДМ_старковстепан</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-11-14T18:22:17.171882+08:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>2025-11-14</t>
         </is>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-16 11:06:41)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:08.050729+00:00</t>
+          <t>2025-11-16T03:01:41.167735+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:08.050772+00:00</t>
+          <t>2025-11-16T03:01:41.167773+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:08.050795+00:00</t>
+          <t>2025-11-16T03:01:41.167795+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:10.672959+00:00</t>
+          <t>2025-11-16T03:01:43.861639+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:10.672990+00:00</t>
+          <t>2025-11-16T03:01:43.861671+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:13.430032+00:00</t>
+          <t>2025-11-16T03:01:46.213765+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:16.081522+00:00</t>
+          <t>2025-11-16T03:01:48.917073+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:18.376428+00:00</t>
+          <t>2025-11-16T03:01:51.677663+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:18.376459+00:00</t>
+          <t>2025-11-16T03:01:51.677692+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:23.456790+00:00</t>
+          <t>2025-11-16T03:01:56.695444+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:25.720710+00:00</t>
+          <t>2025-11-16T03:01:59.038251+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:28.025406+00:00</t>
+          <t>2025-11-16T03:02:01.764048+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:28.025438+00:00</t>
+          <t>2025-11-16T03:02:01.764080+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:28.025459+00:00</t>
+          <t>2025-11-16T03:02:01.764099+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:30.252069+00:00</t>
+          <t>2025-11-16T03:02:04.581142+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:32.480356+00:00</t>
+          <t>2025-11-16T03:02:07.280322+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:32.480392+00:00</t>
+          <t>2025-11-16T03:02:07.280357+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:35.247095+00:00</t>
+          <t>2025-11-16T03:02:09.951485+00:00</t>
         </is>
       </c>
     </row>
@@ -1536,12 +1536,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Гордеев Фёдор</t>
+          <t>Калиниченко Роман</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1551,12 +1551,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>43049</t>
+          <t>26690</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_СИБ_гордеевфедор</t>
+          <t>1369_СИБ_калиниченкороман</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:37.518757+00:00</t>
+          <t>2025-11-16T03:02:12.322779+00:00</t>
         </is>
       </c>
     </row>
@@ -1593,12 +1593,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Калиниченко Роман</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>26690</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_СИБ_калиниченкороман</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:37.518792+00:00</t>
+          <t>2025-11-16T03:02:12.322812+00:00</t>
         </is>
       </c>
     </row>
@@ -1650,27 +1650,27 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:37.518816+00:00</t>
+          <t>2025-11-16T03:02:12.322832+00:00</t>
         </is>
       </c>
     </row>
@@ -1707,12 +1707,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1722,12 +1722,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>16195</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1742,49 +1742,49 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:37.518840+00:00</t>
+          <t>2025-11-16T03:02:12.322849+00:00</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1794,12 +1794,12 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:37.518862+00:00</t>
+          <t>2025-11-16T03:02:15.147779+00:00</t>
         </is>
       </c>
     </row>
@@ -1821,27 +1821,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1856,34 +1856,34 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:40.286678+00:00</t>
+          <t>2025-11-16T03:02:15.147808+00:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>41566</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1908,12 +1908,12 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:40.286708+00:00</t>
+          <t>2025-11-16T03:02:17.921853+00:00</t>
         </is>
       </c>
     </row>
@@ -1935,27 +1935,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Самсонов Илья</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>21010</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СОЧ_самсоновилья</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:42.985477+00:00</t>
+          <t>2025-11-16T03:02:17.921884+00:00</t>
         </is>
       </c>
     </row>
@@ -1992,27 +1992,27 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Самсонов Илья</t>
+          <t>Хёфенмайер Ноэль</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>21010</t>
+          <t>44847</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_самсоновилья</t>
+          <t>1369_СОЧ_хефенмайерноэль</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2027,49 +2027,49 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:42.985507+00:00</t>
+          <t>2025-11-16T03:02:17.921905+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>44847</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,12 +2079,12 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:42.985527+00:00</t>
+          <t>2025-11-16T03:02:20.597059+00:00</t>
         </is>
       </c>
     </row>
@@ -2106,12 +2106,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2121,12 +2121,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2141,34 +2141,34 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:45.672530+00:00</t>
+          <t>2025-11-16T03:02:20.597088+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2178,12 +2178,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,12 +2193,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:45.672557+00:00</t>
+          <t>2025-11-16T03:02:23.359413+00:00</t>
         </is>
       </c>
     </row>
@@ -2220,12 +2220,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2235,12 +2235,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:47.966011+00:00</t>
+          <t>2025-11-16T03:02:23.359442+00:00</t>
         </is>
       </c>
     </row>
@@ -2277,27 +2277,27 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:47.966048+00:00</t>
+          <t>2025-11-16T03:02:23.359460+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,27 +2334,27 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:47.966070+00:00</t>
+          <t>2025-11-16T03:02:23.359476+00:00</t>
         </is>
       </c>
     </row>
@@ -2391,12 +2391,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2406,12 +2406,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2426,49 +2426,49 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:47.966092+00:00</t>
+          <t>2025-11-16T03:02:23.359490+00:00</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2478,12 +2478,12 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:47.966112+00:00</t>
+          <t>2025-11-16T03:02:26.167578+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,27 +2505,27 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,34 +2540,34 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:50.359413+00:00</t>
+          <t>2025-11-16T03:02:26.167607+00:00</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Дроздов Иван</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>30752</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ЦСК_дроздовиван</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2592,12 +2592,12 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:50.359445+00:00</t>
+          <t>2025-11-16T03:02:31.264393+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,12 +2619,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Дроздов Иван</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2634,12 +2634,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>30752</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_ЦСК_дроздовиван</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:55.182226+00:00</t>
+          <t>2025-11-16T03:02:31.264423+00:00</t>
         </is>
       </c>
     </row>
@@ -2676,27 +2676,27 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Саморуков Дмитрий</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>24005</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ЦСК_саморуковдмитрий</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:55.182258+00:00</t>
+          <t>2025-11-16T03:02:31.264440+00:00</t>
         </is>
       </c>
     </row>
@@ -2733,12 +2733,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Саморуков Дмитрий</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2748,12 +2748,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>24005</t>
+          <t>41896</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_ЦСК_саморуковдмитрий</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2768,34 +2768,34 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:55.182277+00:00</t>
+          <t>2025-11-16T03:02:31.264455+00:00</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2805,12 +2805,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>41896</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2820,126 +2820,12 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-15T07:03:55.182295+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Гроло Жереми</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>45343</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>1369_ШДР_гроложереми</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>2025-11-15T07:03:58.257072+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Саттер Райли</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>45491</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>1369_ШДР_саттеррайли</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>2025-11-15T07:03:58.257104+00:00</t>
+          <t>2025-11-16T03:02:33.640826+00:00</t>
         </is>
       </c>
     </row>
@@ -2949,173 +2835,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>team_abbr</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>team_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>player_name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>player_uid</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>changed_at</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>changed_day</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>СОЧ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ХК Сочи</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Мачулин Василий</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_СОЧ_мачулинвасилий</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-15T15:03:58.764737+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-15</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>СОЧ</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ХК Сочи</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Хомченко Павел</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1369_СОЧ_хомченкопавел</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-11-15T15:03:58.764737+08:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-11-15</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>СЮЛ</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Салават Юлаев</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Кузьмин Глеб</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1369_СЮЛ_кузьминглеб</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-11-15T15:03:58.764737+08:00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2025-11-15</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3169,74 +2888,130 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Самсонов Илья</t>
+          <t>Гордеев Фёдор</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_СОЧ_самсоновилья</t>
+          <t>1369_СИБ_гордеевфедор</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>INJURED_NEW</t>
+          <t>RETURN</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-15T15:03:58.764737+08:00</t>
+          <t>2025-11-16T11:02:34.145192+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-15</t>
+          <t>2025-11-16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Саттер Райли</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_ШДР_саттеррайли</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>INJURED_NEW</t>
+          <t>RETURN</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-15T15:03:58.764737+08:00</t>
+          <t>2025-11-16T11:02:34.145192+08:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-11-15</t>
+          <t>2025-11-16</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>team_abbr</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>team_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>player_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>player_uid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>changed_at</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>changed_day</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-17 11:04:16)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-16T03:01:41.167735+00:00</t>
+          <t>2025-11-17T03:01:37.969847+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-16T03:01:41.167773+00:00</t>
+          <t>2025-11-17T03:01:37.969887+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-16T03:01:41.167795+00:00</t>
+          <t>2025-11-17T03:01:37.969910+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-16T03:01:43.861639+00:00</t>
+          <t>2025-11-17T03:01:40.796335+00:00</t>
         </is>
       </c>
     </row>
@@ -738,27 +738,27 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Шепелев Александр</t>
+          <t>Сошников Никита</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>90</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>23447</t>
+          <t>16731</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1369_АДМ_шепелевалександр</t>
+          <t>1369_АДМ_сошниковникита</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -773,34 +773,34 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-16T03:01:43.861671+00:00</t>
+          <t>2025-11-17T03:01:40.796421+00:00</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>АКБ</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ak_bars</t>
+          <t>admiral</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Яруллин Альберт</t>
+          <t>Шепелев Александр</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -810,12 +810,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>16365</t>
+          <t>23447</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1369_АКБ_яруллинальберт</t>
+          <t>1369_АДМ_шепелевалександр</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -825,39 +825,39 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
+          <t>https://www.khl.ru/clubs/admiral/team/</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-16T03:01:46.213765+00:00</t>
+          <t>2025-11-17T03:01:40.796455+00:00</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>АКБ</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>ak_bars</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Абросимов Роман</t>
+          <t>Яруллин Альберт</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -867,12 +867,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>17968</t>
+          <t>16365</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1369_АМР_абросимовроман</t>
+          <t>1369_АКБ_яруллинальберт</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -882,54 +882,54 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
+          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-16T03:01:48.917073+00:00</t>
+          <t>2025-11-17T03:01:43.505813+00:00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>amur</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Абросимов Роман</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>94</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>28244</t>
+          <t>17968</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_АМР_абросимовроман</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -939,12 +939,12 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-16T03:01:51.677663+00:00</t>
+          <t>2025-11-17T03:01:46.253814+00:00</t>
         </is>
       </c>
     </row>
@@ -966,27 +966,27 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Уотерспун Тайлер</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>45769</t>
+          <t>28244</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1369_БАР_уотерспунтайлер</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1001,34 +1001,34 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-16T03:01:51.677692+00:00</t>
+          <t>2025-11-17T03:01:48.978753+00:00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ДМН</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dinamo_mn</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Уэлле Ксавье</t>
+          <t>Уотерспун Тайлер</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>26</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1038,12 +1038,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>19692</t>
+          <t>45769</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1369_ДМН_уэллексавье</t>
+          <t>1369_БАР_уотерспунтайлер</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1053,54 +1053,54 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-16T03:01:56.695444+00:00</t>
+          <t>2025-11-17T03:01:48.978786+00:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>ДМН</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>dinamo_mn</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Уэлле Ксавье</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>19692</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_ДМН_уэллексавье</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1110,39 +1110,39 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-16T03:01:59.038251+00:00</t>
+          <t>2025-11-17T03:01:53.901243+00:00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Волков Александр С</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_ЛОК_волковалександрс</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1167,12 +1167,12 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:01.764048+00:00</t>
+          <t>2025-11-17T03:01:56.142582+00:00</t>
         </is>
       </c>
     </row>
@@ -1194,12 +1194,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Паник Рихард</t>
+          <t>Волков Александр С</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1209,12 +1209,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>16071</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_ЛОК_паникрихард</t>
+          <t>1369_ЛОК_волковалександрс</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:01.764080+00:00</t>
+          <t>2025-11-17T03:01:58.402148+00:00</t>
         </is>
       </c>
     </row>
@@ -1251,27 +1251,27 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Паник Рихард</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>16071</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ЛОК_паникрихард</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1286,49 +1286,49 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:01.764099+00:00</t>
+          <t>2025-11-17T03:01:58.402176+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,39 +1338,39 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:04.581142+00:00</t>
+          <t>2025-11-17T03:01:58.402194+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1380,12 +1380,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,12 +1395,12 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:07.280322+00:00</t>
+          <t>2025-11-17T03:02:01.201920+00:00</t>
         </is>
       </c>
     </row>
@@ -1422,12 +1422,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>22683</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1457,34 +1457,34 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:07.280357+00:00</t>
+          <t>2025-11-17T03:02:03.957635+00:00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Попугаев Никита О</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1494,12 +1494,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>22683</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_НХК_попугаевникитао</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1509,54 +1509,54 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:09.951485+00:00</t>
+          <t>2025-11-17T03:02:03.957665+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Калиниченко Роман</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>26690</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_СИБ_калиниченкороман</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1566,12 +1566,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:12.322779+00:00</t>
+          <t>2025-11-17T03:02:06.623228+00:00</t>
         </is>
       </c>
     </row>
@@ -1593,12 +1593,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Калиниченко Роман</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>26690</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СИБ_калиниченкороман</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:12.322812+00:00</t>
+          <t>2025-11-17T03:02:09.371499+00:00</t>
         </is>
       </c>
     </row>
@@ -1650,27 +1650,27 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>16195</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:12.322832+00:00</t>
+          <t>2025-11-17T03:02:09.371531+00:00</t>
         </is>
       </c>
     </row>
@@ -1707,12 +1707,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1722,12 +1722,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1742,49 +1742,49 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:12.322849+00:00</t>
+          <t>2025-11-17T03:02:09.371550+00:00</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1794,12 +1794,12 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:15.147779+00:00</t>
+          <t>2025-11-17T03:02:09.371567+00:00</t>
         </is>
       </c>
     </row>
@@ -1821,27 +1821,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>41566</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1856,34 +1856,34 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:15.147808+00:00</t>
+          <t>2025-11-17T03:02:11.575637+00:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1908,12 +1908,12 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:17.921853+00:00</t>
+          <t>2025-11-17T03:02:11.575665+00:00</t>
         </is>
       </c>
     </row>
@@ -1935,27 +1935,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Самсонов Илья</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>21010</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СОЧ_самсоновилья</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:17.921884+00:00</t>
+          <t>2025-11-17T03:02:14.254704+00:00</t>
         </is>
       </c>
     </row>
@@ -1992,27 +1992,27 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Самсонов Илья</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>44847</t>
+          <t>21010</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_СОЧ_самсоновилья</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2027,49 +2027,49 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:17.921905+00:00</t>
+          <t>2025-11-17T03:02:14.254737+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Хёфенмайер Ноэль</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>44847</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СОЧ_хефенмайерноэль</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,12 +2079,12 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:20.597059+00:00</t>
+          <t>2025-11-17T03:02:14.254757+00:00</t>
         </is>
       </c>
     </row>
@@ -2106,12 +2106,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2121,12 +2121,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2141,34 +2141,34 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:20.597088+00:00</t>
+          <t>2025-11-17T03:02:16.905633+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2178,12 +2178,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,12 +2193,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:23.359413+00:00</t>
+          <t>2025-11-17T03:02:16.905662+00:00</t>
         </is>
       </c>
     </row>
@@ -2220,12 +2220,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2235,12 +2235,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:23.359442+00:00</t>
+          <t>2025-11-17T03:02:19.151370+00:00</t>
         </is>
       </c>
     </row>
@@ -2277,27 +2277,27 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:23.359460+00:00</t>
+          <t>2025-11-17T03:02:19.151398+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,27 +2334,27 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:23.359476+00:00</t>
+          <t>2025-11-17T03:02:19.151417+00:00</t>
         </is>
       </c>
     </row>
@@ -2391,12 +2391,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2406,12 +2406,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2426,49 +2426,49 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:23.359490+00:00</t>
+          <t>2025-11-17T03:02:19.151436+00:00</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2478,12 +2478,12 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:26.167578+00:00</t>
+          <t>2025-11-17T03:02:19.151452+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,27 +2505,27 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,34 +2540,34 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:26.167607+00:00</t>
+          <t>2025-11-17T03:02:21.868032+00:00</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Дроздов Иван</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>30752</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_ЦСК_дроздовиван</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2592,12 +2592,12 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:31.264393+00:00</t>
+          <t>2025-11-17T03:02:21.868062+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,12 +2619,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Дроздов Иван</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2634,12 +2634,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>30752</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ЦСК_дроздовиван</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:31.264423+00:00</t>
+          <t>2025-11-17T03:02:26.963326+00:00</t>
         </is>
       </c>
     </row>
@@ -2676,27 +2676,27 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Саморуков Дмитрий</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>24005</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_ЦСК_саморуковдмитрий</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:31.264440+00:00</t>
+          <t>2025-11-17T03:02:26.963353+00:00</t>
         </is>
       </c>
     </row>
@@ -2733,12 +2733,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Саморуков Дмитрий</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2748,12 +2748,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>41896</t>
+          <t>24005</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_ЦСК_саморуковдмитрий</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2768,64 +2768,121 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-16T03:02:31.264455+00:00</t>
+          <t>2025-11-17T03:02:26.963371+00:00</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>cska</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Уильямс Колби</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>41896</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_уильямсколби</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>2025-11-17T03:02:26.963388+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
           <t>ШДР</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B43" t="inlineStr">
         <is>
           <t>Драконы</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>kunlun</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>Гроло Жереми</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>75</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="F43" t="inlineStr">
         <is>
           <t>защитник</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="G43" t="inlineStr">
         <is>
           <t>45343</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr">
+      <c r="H43" t="inlineStr">
         <is>
           <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
         <is>
           <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>2025-11-16T03:02:33.640826+00:00</t>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>2025-11-17T03:02:29.278481+00:00</t>
         </is>
       </c>
     </row>
@@ -2835,136 +2892,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>team_abbr</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>team_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>player_name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>player_uid</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>changed_at</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>changed_day</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>СИБ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Сибирь</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Гордеев Фёдор</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_СИБ_гордеевфедор</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-16T11:02:34.145192+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-16</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Саттер Райли</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1369_ШДР_саттеррайли</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-11-16T11:02:34.145192+08:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-11-16</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3018,4 +2945,97 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>team_abbr</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>team_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>player_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>player_uid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>changed_at</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>changed_day</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>АДМ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Адмирал</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Сошников Никита</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_АДМ_сошниковникита</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-17T11:02:29.789806+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-17</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-17 19:13:33)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:37.969847+00:00</t>
+          <t>2025-11-17T11:11:06.343361+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:37.969887+00:00</t>
+          <t>2025-11-17T11:11:06.343381+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:37.969910+00:00</t>
+          <t>2025-11-17T11:11:06.343390+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:40.796335+00:00</t>
+          <t>2025-11-17T11:11:08.296613+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:40.796421+00:00</t>
+          <t>2025-11-17T11:11:08.296631+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:40.796455+00:00</t>
+          <t>2025-11-17T11:11:08.296640+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:43.505813+00:00</t>
+          <t>2025-11-17T11:11:10.950508+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:46.253814+00:00</t>
+          <t>2025-11-17T11:11:13.294859+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:48.978753+00:00</t>
+          <t>2025-11-17T11:11:15.987370+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:48.978786+00:00</t>
+          <t>2025-11-17T11:11:15.987401+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:53.901243+00:00</t>
+          <t>2025-11-17T11:11:21.029493+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:56.142582+00:00</t>
+          <t>2025-11-17T11:11:23.422784+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:58.402148+00:00</t>
+          <t>2025-11-17T11:11:26.100105+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:58.402176+00:00</t>
+          <t>2025-11-17T11:11:26.100133+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-17T03:01:58.402194+00:00</t>
+          <t>2025-11-17T11:11:26.100151+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:01.201920+00:00</t>
+          <t>2025-11-17T11:11:28.381254+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:03.957635+00:00</t>
+          <t>2025-11-17T11:11:30.754090+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:03.957665+00:00</t>
+          <t>2025-11-17T11:11:30.754178+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:06.623228+00:00</t>
+          <t>2025-11-17T11:11:33.057939+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:09.371499+00:00</t>
+          <t>2025-11-17T11:11:35.385590+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:09.371531+00:00</t>
+          <t>2025-11-17T11:11:35.385624+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:09.371550+00:00</t>
+          <t>2025-11-17T11:11:35.385645+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:09.371567+00:00</t>
+          <t>2025-11-17T11:11:35.385663+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:11.575637+00:00</t>
+          <t>2025-11-17T11:11:37.743881+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:11.575665+00:00</t>
+          <t>2025-11-17T11:11:37.743912+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:14.254704+00:00</t>
+          <t>2025-11-17T11:11:40.043951+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:14.254737+00:00</t>
+          <t>2025-11-17T11:11:40.043980+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:14.254757+00:00</t>
+          <t>2025-11-17T11:11:40.044000+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:16.905633+00:00</t>
+          <t>2025-11-17T11:11:42.401593+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:16.905662+00:00</t>
+          <t>2025-11-17T11:11:42.401624+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:19.151370+00:00</t>
+          <t>2025-11-17T11:11:44.804044+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:19.151398+00:00</t>
+          <t>2025-11-17T11:11:44.804074+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:19.151417+00:00</t>
+          <t>2025-11-17T11:11:44.804092+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:19.151436+00:00</t>
+          <t>2025-11-17T11:11:44.804109+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:19.151452+00:00</t>
+          <t>2025-11-17T11:11:44.804128+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:21.868032+00:00</t>
+          <t>2025-11-17T11:11:47.168150+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:21.868062+00:00</t>
+          <t>2025-11-17T11:11:47.168180+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:26.963326+00:00</t>
+          <t>2025-11-17T11:11:51.924215+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:26.963353+00:00</t>
+          <t>2025-11-17T11:11:51.924245+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:26.963371+00:00</t>
+          <t>2025-11-17T11:11:51.924265+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:26.963388+00:00</t>
+          <t>2025-11-17T11:11:51.924283+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-17T03:02:29.278481+00:00</t>
+          <t>2025-11-17T11:11:54.214357+00:00</t>
         </is>
       </c>
     </row>
@@ -2953,7 +2953,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2998,43 +2998,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>АДМ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Адмирал</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Сошников Никита</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_АДМ_сошниковникита</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-17T11:02:29.789806+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-17</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-18 07:26:55)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:06.343361+00:00</t>
+          <t>2025-11-17T23:21:26.318468+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:06.343381+00:00</t>
+          <t>2025-11-17T23:21:26.318504+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:06.343390+00:00</t>
+          <t>2025-11-17T23:21:26.318524+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:08.296613+00:00</t>
+          <t>2025-11-17T23:21:28.842913+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:08.296631+00:00</t>
+          <t>2025-11-17T23:21:28.842956+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:08.296640+00:00</t>
+          <t>2025-11-17T23:21:28.842968+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:10.950508+00:00</t>
+          <t>2025-11-17T23:21:31.231401+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:13.294859+00:00</t>
+          <t>2025-11-17T23:21:33.674152+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:15.987370+00:00</t>
+          <t>2025-11-17T23:21:35.774131+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:15.987401+00:00</t>
+          <t>2025-11-17T23:21:35.774160+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:21.029493+00:00</t>
+          <t>2025-11-17T23:21:40.753322+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:23.422784+00:00</t>
+          <t>2025-11-17T23:21:43.179370+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:26.100105+00:00</t>
+          <t>2025-11-17T23:21:45.691118+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:26.100133+00:00</t>
+          <t>2025-11-17T23:21:45.691139+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:26.100151+00:00</t>
+          <t>2025-11-17T23:21:45.691147+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:28.381254+00:00</t>
+          <t>2025-11-17T23:21:48.199767+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:30.754090+00:00</t>
+          <t>2025-11-17T23:21:50.648765+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:30.754178+00:00</t>
+          <t>2025-11-17T23:21:50.648782+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:33.057939+00:00</t>
+          <t>2025-11-17T23:21:52.821423+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:35.385590+00:00</t>
+          <t>2025-11-17T23:21:54.918571+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:35.385624+00:00</t>
+          <t>2025-11-17T23:21:54.918600+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:35.385645+00:00</t>
+          <t>2025-11-17T23:21:54.918618+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:35.385663+00:00</t>
+          <t>2025-11-17T23:21:54.918634+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:37.743881+00:00</t>
+          <t>2025-11-17T23:21:57.371555+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:37.743912+00:00</t>
+          <t>2025-11-17T23:21:57.371579+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:40.043951+00:00</t>
+          <t>2025-11-17T23:21:59.929884+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:40.043980+00:00</t>
+          <t>2025-11-17T23:21:59.929913+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:40.044000+00:00</t>
+          <t>2025-11-17T23:21:59.929933+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:42.401593+00:00</t>
+          <t>2025-11-17T23:22:02.388274+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:42.401624+00:00</t>
+          <t>2025-11-17T23:22:02.388316+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:44.804044+00:00</t>
+          <t>2025-11-17T23:22:04.818936+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:44.804074+00:00</t>
+          <t>2025-11-17T23:22:04.818971+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:44.804092+00:00</t>
+          <t>2025-11-17T23:22:04.818991+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:44.804109+00:00</t>
+          <t>2025-11-17T23:22:04.819009+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:44.804128+00:00</t>
+          <t>2025-11-17T23:22:04.819024+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:47.168150+00:00</t>
+          <t>2025-11-17T23:22:07.484526+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:47.168180+00:00</t>
+          <t>2025-11-17T23:22:07.484556+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:51.924215+00:00</t>
+          <t>2025-11-17T23:22:12.529691+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:51.924245+00:00</t>
+          <t>2025-11-17T23:22:12.529722+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:51.924265+00:00</t>
+          <t>2025-11-17T23:22:12.529741+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:51.924283+00:00</t>
+          <t>2025-11-17T23:22:12.529758+00:00</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>2025-11-17T11:11:54.214357+00:00</t>
+          <t>2025-11-17T23:22:14.922456+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-18 11:06:39)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:26.318468+00:00</t>
+          <t>2025-11-18T03:01:44.309977+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:26.318504+00:00</t>
+          <t>2025-11-18T03:01:44.310029+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:26.318524+00:00</t>
+          <t>2025-11-18T03:01:44.310054+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:28.842913+00:00</t>
+          <t>2025-11-18T03:01:46.615968+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:28.842956+00:00</t>
+          <t>2025-11-18T03:01:46.615998+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:28.842968+00:00</t>
+          <t>2025-11-18T03:01:46.616016+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:31.231401+00:00</t>
+          <t>2025-11-18T03:01:49.311060+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:33.674152+00:00</t>
+          <t>2025-11-18T03:01:51.985673+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:35.774131+00:00</t>
+          <t>2025-11-18T03:01:54.735786+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:35.774160+00:00</t>
+          <t>2025-11-18T03:01:54.735816+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:40.753322+00:00</t>
+          <t>2025-11-18T03:02:00.268573+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:43.179370+00:00</t>
+          <t>2025-11-18T03:02:02.585561+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:45.691118+00:00</t>
+          <t>2025-11-18T03:02:05.335773+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:45.691139+00:00</t>
+          <t>2025-11-18T03:02:05.335801+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:45.691147+00:00</t>
+          <t>2025-11-18T03:02:05.335818+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:48.199767+00:00</t>
+          <t>2025-11-18T03:02:07.491227+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,34 +1457,34 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:50.648765+00:00</t>
+          <t>2025-11-18T03:02:09.777437+00:00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1494,12 +1494,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>22683</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1509,54 +1509,54 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:50.648782+00:00</t>
+          <t>2025-11-18T03:02:12.475519+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Калиниченко Роман</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>26690</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СИБ_калиниченкороман</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1566,12 +1566,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:52.821423+00:00</t>
+          <t>2025-11-18T03:02:14.721931+00:00</t>
         </is>
       </c>
     </row>
@@ -1593,12 +1593,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Калиниченко Роман</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>26690</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_СИБ_калиниченкороман</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:54.918571+00:00</t>
+          <t>2025-11-18T03:02:14.721961+00:00</t>
         </is>
       </c>
     </row>
@@ -1650,27 +1650,27 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:54.918600+00:00</t>
+          <t>2025-11-18T03:02:14.721979+00:00</t>
         </is>
       </c>
     </row>
@@ -1707,12 +1707,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1722,12 +1722,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>16195</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1742,49 +1742,49 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:54.918618+00:00</t>
+          <t>2025-11-18T03:02:14.721996+00:00</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1794,12 +1794,12 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:54.918634+00:00</t>
+          <t>2025-11-18T03:02:16.976173+00:00</t>
         </is>
       </c>
     </row>
@@ -1821,27 +1821,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1856,34 +1856,34 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:57.371555+00:00</t>
+          <t>2025-11-18T03:02:16.976201+00:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>41566</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1908,12 +1908,12 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:57.371579+00:00</t>
+          <t>2025-11-18T03:02:19.701676+00:00</t>
         </is>
       </c>
     </row>
@@ -1935,27 +1935,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Самсонов Илья</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>21010</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СОЧ_самсоновилья</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:59.929884+00:00</t>
+          <t>2025-11-18T03:02:19.701706+00:00</t>
         </is>
       </c>
     </row>
@@ -1992,27 +1992,27 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Самсонов Илья</t>
+          <t>Хёфенмайер Ноэль</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>21010</t>
+          <t>44847</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_самсоновилья</t>
+          <t>1369_СОЧ_хефенмайерноэль</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2027,49 +2027,49 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:59.929913+00:00</t>
+          <t>2025-11-18T03:02:19.701729+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>44847</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,12 +2079,12 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-17T23:21:59.929933+00:00</t>
+          <t>2025-11-18T03:02:22.368414+00:00</t>
         </is>
       </c>
     </row>
@@ -2106,12 +2106,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2121,12 +2121,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2141,34 +2141,34 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-17T23:22:02.388274+00:00</t>
+          <t>2025-11-18T03:02:22.368444+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2178,12 +2178,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,12 +2193,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-17T23:22:02.388316+00:00</t>
+          <t>2025-11-18T03:02:24.582577+00:00</t>
         </is>
       </c>
     </row>
@@ -2220,12 +2220,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2235,12 +2235,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-17T23:22:04.818936+00:00</t>
+          <t>2025-11-18T03:02:24.582608+00:00</t>
         </is>
       </c>
     </row>
@@ -2277,27 +2277,27 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-17T23:22:04.818971+00:00</t>
+          <t>2025-11-18T03:02:24.582626+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,27 +2334,27 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-17T23:22:04.818991+00:00</t>
+          <t>2025-11-18T03:02:24.582643+00:00</t>
         </is>
       </c>
     </row>
@@ -2391,12 +2391,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2406,12 +2406,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2426,49 +2426,49 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-17T23:22:04.819009+00:00</t>
+          <t>2025-11-18T03:02:24.582662+00:00</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2478,12 +2478,12 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-17T23:22:04.819024+00:00</t>
+          <t>2025-11-18T03:02:27.369992+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,27 +2505,27 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,34 +2540,34 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-17T23:22:07.484526+00:00</t>
+          <t>2025-11-18T03:02:27.370022+00:00</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Дроздов Иван</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>30752</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ЦСК_дроздовиван</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2592,12 +2592,12 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-17T23:22:07.484556+00:00</t>
+          <t>2025-11-18T03:02:32.691620+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,12 +2619,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Дроздов Иван</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2634,12 +2634,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>30752</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_ЦСК_дроздовиван</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-17T23:22:12.529691+00:00</t>
+          <t>2025-11-18T03:02:32.691654+00:00</t>
         </is>
       </c>
     </row>
@@ -2676,27 +2676,27 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>41896</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2711,34 +2711,34 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-17T23:22:12.529722+00:00</t>
+          <t>2025-11-18T03:02:32.691675+00:00</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Саморуков Дмитрий</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2748,12 +2748,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>24005</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1369_ЦСК_саморуковдмитрий</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2763,126 +2763,12 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-17T23:22:12.529741+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>cska</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Уильямс Колби</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>41896</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_уильямсколби</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>2025-11-17T23:22:12.529758+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Гроло Жереми</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>45343</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>1369_ШДР_гроложереми</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>2025-11-17T23:22:14.922456+00:00</t>
+          <t>2025-11-18T03:02:34.914959+00:00</t>
         </is>
       </c>
     </row>
@@ -2897,7 +2783,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2939,6 +2825,80 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>changed_day</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>НХК</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Нефтехимик</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Попугаев Никита О</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_НХК_попугаевникитао</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-18T11:02:35.425573+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Саморуков Дмитрий</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_саморуковдмитрий</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-11-18T11:02:35.425573+08:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-11-18</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-18 15:06:25)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-18T03:01:44.309977+00:00</t>
+          <t>2025-11-18T07:01:32.615610+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-18T03:01:44.310029+00:00</t>
+          <t>2025-11-18T07:01:32.615650+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-18T03:01:44.310054+00:00</t>
+          <t>2025-11-18T07:01:32.615676+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-18T03:01:46.615968+00:00</t>
+          <t>2025-11-18T07:01:34.848092+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-18T03:01:46.615998+00:00</t>
+          <t>2025-11-18T07:01:34.848123+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-18T03:01:46.616016+00:00</t>
+          <t>2025-11-18T07:01:34.848143+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-18T03:01:49.311060+00:00</t>
+          <t>2025-11-18T07:01:37.205852+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-18T03:01:51.985673+00:00</t>
+          <t>2025-11-18T07:01:39.515610+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-18T03:01:54.735786+00:00</t>
+          <t>2025-11-18T07:01:42.257925+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-18T03:01:54.735816+00:00</t>
+          <t>2025-11-18T07:01:42.257955+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:00.268573+00:00</t>
+          <t>2025-11-18T07:01:46.813264+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:02.585561+00:00</t>
+          <t>2025-11-18T07:01:49.200195+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:05.335773+00:00</t>
+          <t>2025-11-18T07:01:51.936011+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:05.335801+00:00</t>
+          <t>2025-11-18T07:01:51.936042+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:05.335818+00:00</t>
+          <t>2025-11-18T07:01:51.936061+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:07.491227+00:00</t>
+          <t>2025-11-18T07:01:54.294484+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:09.777437+00:00</t>
+          <t>2025-11-18T07:01:57.146845+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:12.475519+00:00</t>
+          <t>2025-11-18T07:01:59.907052+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:14.721931+00:00</t>
+          <t>2025-11-18T07:02:02.234397+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:14.721961+00:00</t>
+          <t>2025-11-18T07:02:02.234425+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:14.721979+00:00</t>
+          <t>2025-11-18T07:02:02.234443+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:14.721996+00:00</t>
+          <t>2025-11-18T07:02:02.234459+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:16.976173+00:00</t>
+          <t>2025-11-18T07:02:04.531384+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:16.976201+00:00</t>
+          <t>2025-11-18T07:02:04.531434+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:19.701676+00:00</t>
+          <t>2025-11-18T07:02:07.277607+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:19.701706+00:00</t>
+          <t>2025-11-18T07:02:07.277656+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:19.701729+00:00</t>
+          <t>2025-11-18T07:02:07.277687+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:22.368414+00:00</t>
+          <t>2025-11-18T07:02:09.639905+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:22.368444+00:00</t>
+          <t>2025-11-18T07:02:09.639934+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:24.582577+00:00</t>
+          <t>2025-11-18T07:02:11.993217+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:24.582608+00:00</t>
+          <t>2025-11-18T07:02:11.993247+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:24.582626+00:00</t>
+          <t>2025-11-18T07:02:11.993266+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:24.582643+00:00</t>
+          <t>2025-11-18T07:02:11.993283+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:24.582662+00:00</t>
+          <t>2025-11-18T07:02:11.993299+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:27.369992+00:00</t>
+          <t>2025-11-18T07:02:14.939887+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:27.370022+00:00</t>
+          <t>2025-11-18T07:02:14.939920+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:32.691620+00:00</t>
+          <t>2025-11-18T07:02:20.018845+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:32.691654+00:00</t>
+          <t>2025-11-18T07:02:20.018876+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:32.691675+00:00</t>
+          <t>2025-11-18T07:02:20.018894+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-18T03:02:34.914959+00:00</t>
+          <t>2025-11-18T07:02:22.281504+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-18 18:36:17)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:32.615610+00:00</t>
+          <t>2025-11-18T10:31:16.794522+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:32.615650+00:00</t>
+          <t>2025-11-18T10:31:16.794542+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:32.615676+00:00</t>
+          <t>2025-11-18T10:31:16.794552+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:34.848092+00:00</t>
+          <t>2025-11-18T10:31:18.775475+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:34.848123+00:00</t>
+          <t>2025-11-18T10:31:18.775509+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:34.848143+00:00</t>
+          <t>2025-11-18T10:31:18.775532+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:37.205852+00:00</t>
+          <t>2025-11-18T10:31:21.202617+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:39.515610+00:00</t>
+          <t>2025-11-18T10:31:24.025578+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:42.257925+00:00</t>
+          <t>2025-11-18T10:31:26.763751+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:42.257955+00:00</t>
+          <t>2025-11-18T10:31:26.763785+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:46.813264+00:00</t>
+          <t>2025-11-18T10:31:31.726344+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:49.200195+00:00</t>
+          <t>2025-11-18T10:31:34.028830+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:51.936011+00:00</t>
+          <t>2025-11-18T10:31:36.735706+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:51.936042+00:00</t>
+          <t>2025-11-18T10:31:36.735737+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:51.936061+00:00</t>
+          <t>2025-11-18T10:31:36.735762+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:54.294484+00:00</t>
+          <t>2025-11-18T10:31:39.002586+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:57.146845+00:00</t>
+          <t>2025-11-18T10:31:41.722696+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-18T07:01:59.907052+00:00</t>
+          <t>2025-11-18T10:31:44.050412+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:02.234397+00:00</t>
+          <t>2025-11-18T10:31:46.761208+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:02.234425+00:00</t>
+          <t>2025-11-18T10:31:46.761241+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:02.234443+00:00</t>
+          <t>2025-11-18T10:31:46.761261+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:02.234459+00:00</t>
+          <t>2025-11-18T10:31:46.761279+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:04.531384+00:00</t>
+          <t>2025-11-18T10:31:49.159066+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:04.531434+00:00</t>
+          <t>2025-11-18T10:31:49.159097+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:07.277607+00:00</t>
+          <t>2025-11-18T10:31:51.515759+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:07.277656+00:00</t>
+          <t>2025-11-18T10:31:51.515788+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:07.277687+00:00</t>
+          <t>2025-11-18T10:31:51.515808+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:09.639905+00:00</t>
+          <t>2025-11-18T10:31:54.808892+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:09.639934+00:00</t>
+          <t>2025-11-18T10:31:54.808923+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:11.993217+00:00</t>
+          <t>2025-11-18T10:31:57.118478+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:11.993247+00:00</t>
+          <t>2025-11-18T10:31:57.118531+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:11.993266+00:00</t>
+          <t>2025-11-18T10:31:57.118554+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:11.993283+00:00</t>
+          <t>2025-11-18T10:31:57.118575+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:11.993299+00:00</t>
+          <t>2025-11-18T10:31:57.118593+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:14.939887+00:00</t>
+          <t>2025-11-18T10:31:59.544301+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:14.939920+00:00</t>
+          <t>2025-11-18T10:31:59.544332+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:20.018845+00:00</t>
+          <t>2025-11-18T10:32:04.209999+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:20.018876+00:00</t>
+          <t>2025-11-18T10:32:04.210030+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:20.018894+00:00</t>
+          <t>2025-11-18T10:32:04.210049+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-18T07:02:22.281504+00:00</t>
+          <t>2025-11-18T10:32:06.458674+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-19 11:11:41)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:16.794522+00:00</t>
+          <t>2025-11-19T03:06:26.519705+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:16.794542+00:00</t>
+          <t>2025-11-19T03:06:26.519745+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:16.794552+00:00</t>
+          <t>2025-11-19T03:06:26.519766+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:18.775475+00:00</t>
+          <t>2025-11-19T03:06:31.003614+00:00</t>
         </is>
       </c>
     </row>
@@ -773,34 +773,34 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:18.775509+00:00</t>
+          <t>2025-11-19T03:06:31.003648+00:00</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>АКБ</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>admiral</t>
+          <t>ak_bars</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Шепелев Александр</t>
+          <t>Яруллин Альберт</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -810,12 +810,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>23447</t>
+          <t>16365</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1369_АДМ_шепелевалександр</t>
+          <t>1369_АКБ_яруллинальберт</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -825,39 +825,39 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/admiral/team/</t>
+          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:18.775532+00:00</t>
+          <t>2025-11-19T03:06:36.636032+00:00</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>АКБ</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ak_bars</t>
+          <t>amur</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Яруллин Альберт</t>
+          <t>Абросимов Роман</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>94</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -867,12 +867,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>16365</t>
+          <t>17968</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1369_АКБ_яруллинальберт</t>
+          <t>1369_АМР_абросимовроман</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -882,54 +882,54 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:21.202617+00:00</t>
+          <t>2025-11-19T03:06:42.103802+00:00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Абросимов Роман</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>17968</t>
+          <t>28244</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1369_АМР_абросимовроман</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -939,12 +939,12 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:24.025578+00:00</t>
+          <t>2025-11-19T03:06:47.664169+00:00</t>
         </is>
       </c>
     </row>
@@ -966,27 +966,27 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Уотерспун Тайлер</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>26</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>28244</t>
+          <t>45769</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_БАР_уотерспунтайлер</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1001,34 +1001,34 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:26.763751+00:00</t>
+          <t>2025-11-19T03:06:47.664204+00:00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>ДМН</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>dinamo_mn</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Уотерспун Тайлер</t>
+          <t>Уэлле Ксавье</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1038,12 +1038,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>45769</t>
+          <t>19692</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1369_БАР_уотерспунтайлер</t>
+          <t>1369_ДМН_уэллексавье</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1053,54 +1053,54 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:26.763785+00:00</t>
+          <t>2025-11-19T03:06:58.676781+00:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ДМН</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>dinamo_mn</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Уэлле Ксавье</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>19692</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_ДМН_уэллексавье</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1110,39 +1110,39 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:31.726344+00:00</t>
+          <t>2025-11-19T03:07:04.141876+00:00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Волков Александр С</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_ЛОК_волковалександрс</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1167,12 +1167,12 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:34.028830+00:00</t>
+          <t>2025-11-19T03:07:09.208161+00:00</t>
         </is>
       </c>
     </row>
@@ -1194,12 +1194,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Волков Александр С</t>
+          <t>Паник Рихард</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1209,12 +1209,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>16071</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_ЛОК_волковалександрс</t>
+          <t>1369_ЛОК_паникрихард</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:36.735706+00:00</t>
+          <t>2025-11-19T03:07:09.208189+00:00</t>
         </is>
       </c>
     </row>
@@ -1251,27 +1251,27 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Паник Рихард</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>16071</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_ЛОК_паникрихард</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1286,49 +1286,49 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:36.735737+00:00</t>
+          <t>2025-11-19T03:07:09.208208+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,39 +1338,39 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:36.735762+00:00</t>
+          <t>2025-11-19T03:07:14.311102+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1380,12 +1380,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,39 +1395,39 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:39.002586+00:00</t>
+          <t>2025-11-19T03:07:19.862461+00:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1452,54 +1452,54 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:41.722696+00:00</t>
+          <t>2025-11-19T03:07:25.555802+00:00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Калиниченко Роман</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>26690</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СИБ_калиниченкороман</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1509,12 +1509,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:44.050412+00:00</t>
+          <t>2025-11-19T03:07:30.748719+00:00</t>
         </is>
       </c>
     </row>
@@ -1536,12 +1536,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Калиниченко Роман</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1551,12 +1551,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>26690</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_СИБ_калиниченкороман</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:46.761208+00:00</t>
+          <t>2025-11-19T03:07:30.748748+00:00</t>
         </is>
       </c>
     </row>
@@ -1593,27 +1593,27 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:46.761241+00:00</t>
+          <t>2025-11-19T03:07:30.748767+00:00</t>
         </is>
       </c>
     </row>
@@ -1650,12 +1650,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1665,12 +1665,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>16195</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1685,49 +1685,49 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:46.761261+00:00</t>
+          <t>2025-11-19T03:07:30.748783+00:00</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1737,12 +1737,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:46.761279+00:00</t>
+          <t>2025-11-19T03:07:36.331556+00:00</t>
         </is>
       </c>
     </row>
@@ -1764,27 +1764,27 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1799,34 +1799,34 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:49.159066+00:00</t>
+          <t>2025-11-19T03:07:36.331585+00:00</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1836,12 +1836,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>41566</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1851,12 +1851,12 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:49.159097+00:00</t>
+          <t>2025-11-19T03:07:41.532617+00:00</t>
         </is>
       </c>
     </row>
@@ -1878,27 +1878,27 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Самсонов Илья</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>21010</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СОЧ_самсоновилья</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:51.515759+00:00</t>
+          <t>2025-11-19T03:07:41.532648+00:00</t>
         </is>
       </c>
     </row>
@@ -1935,27 +1935,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Самсонов Илья</t>
+          <t>Хёфенмайер Ноэль</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>21010</t>
+          <t>44847</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СОЧ_самсоновилья</t>
+          <t>1369_СОЧ_хефенмайерноэль</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1970,49 +1970,49 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:51.515788+00:00</t>
+          <t>2025-11-19T03:07:41.532671+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>44847</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,12 +2022,12 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:51.515808+00:00</t>
+          <t>2025-11-19T03:07:47.098378+00:00</t>
         </is>
       </c>
     </row>
@@ -2049,12 +2049,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2064,12 +2064,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2084,34 +2084,34 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:54.808892+00:00</t>
+          <t>2025-11-19T03:07:47.098404+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2121,12 +2121,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2136,12 +2136,12 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:54.808923+00:00</t>
+          <t>2025-11-19T03:07:52.165812+00:00</t>
         </is>
       </c>
     </row>
@@ -2163,12 +2163,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2178,12 +2178,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:57.118478+00:00</t>
+          <t>2025-11-19T03:07:52.165847+00:00</t>
         </is>
       </c>
     </row>
@@ -2220,27 +2220,27 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:57.118531+00:00</t>
+          <t>2025-11-19T03:07:52.165865+00:00</t>
         </is>
       </c>
     </row>
@@ -2277,27 +2277,27 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:57.118554+00:00</t>
+          <t>2025-11-19T03:07:52.165881+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,12 +2334,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2349,12 +2349,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,49 +2369,49 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:57.118575+00:00</t>
+          <t>2025-11-19T03:07:52.165895+00:00</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2421,12 +2421,12 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:57.118593+00:00</t>
+          <t>2025-11-19T03:07:57.271425+00:00</t>
         </is>
       </c>
     </row>
@@ -2448,27 +2448,27 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2483,34 +2483,34 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:59.544301+00:00</t>
+          <t>2025-11-19T03:07:57.271456+00:00</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Дроздов Иван</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2520,12 +2520,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>30752</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ЦСК_дроздовиван</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2535,12 +2535,12 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-18T10:31:59.544332+00:00</t>
+          <t>2025-11-19T03:08:08.347526+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,12 +2562,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Дроздов Иван</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>30752</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_ЦСК_дроздовиван</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-18T10:32:04.209999+00:00</t>
+          <t>2025-11-19T03:08:08.347560+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,27 +2619,27 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>41896</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,34 +2654,34 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-18T10:32:04.210030+00:00</t>
+          <t>2025-11-19T03:08:08.347583+00:00</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2691,12 +2691,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>41896</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2706,69 +2706,12 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-18T10:32:04.210049+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Гроло Жереми</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>45343</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>1369_ШДР_гроложереми</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>2025-11-18T10:32:06.458674+00:00</t>
+          <t>2025-11-19T03:08:13.846901+00:00</t>
         </is>
       </c>
     </row>
@@ -2783,7 +2726,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2831,22 +2774,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Попугаев Никита О</t>
+          <t>Шепелев Александр</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_НХК_попугаевникитао</t>
+          <t>1369_АДМ_шепелевалександр</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2856,49 +2799,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-18T11:02:35.425573+08:00</t>
+          <t>2025-11-19T11:08:14.354550+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-18</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Саморуков Дмитрий</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_саморуковдмитрий</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-11-18T11:02:35.425573+08:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-11-18</t>
+          <t>2025-11-19</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-19 15:08:42)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-19T03:06:26.519705+00:00</t>
+          <t>2025-11-19T07:03:27.845460+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-19T03:06:26.519745+00:00</t>
+          <t>2025-11-19T07:03:27.845498+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-19T03:06:26.519766+00:00</t>
+          <t>2025-11-19T07:03:27.845518+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-19T03:06:31.003614+00:00</t>
+          <t>2025-11-19T07:03:33.207622+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-19T03:06:31.003648+00:00</t>
+          <t>2025-11-19T07:03:33.207652+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-19T03:06:36.636032+00:00</t>
+          <t>2025-11-19T07:03:38.176178+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-19T03:06:42.103802+00:00</t>
+          <t>2025-11-19T07:03:43.721083+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-19T03:06:47.664169+00:00</t>
+          <t>2025-11-19T07:03:49.643389+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-19T03:06:47.664204+00:00</t>
+          <t>2025-11-19T07:03:49.643417+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-19T03:06:58.676781+00:00</t>
+          <t>2025-11-19T07:04:00.098071+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:04.141876+00:00</t>
+          <t>2025-11-19T07:04:05.448928+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:09.208161+00:00</t>
+          <t>2025-11-19T07:04:10.876331+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:09.208189+00:00</t>
+          <t>2025-11-19T07:04:10.876357+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:09.208208+00:00</t>
+          <t>2025-11-19T07:04:10.876374+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:14.311102+00:00</t>
+          <t>2025-11-19T07:04:15.853810+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:19.862461+00:00</t>
+          <t>2025-11-19T07:04:32.370178+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:25.555802+00:00</t>
+          <t>2025-11-19T07:04:37.828847+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:30.748719+00:00</t>
+          <t>2025-11-19T07:04:42.824636+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:30.748748+00:00</t>
+          <t>2025-11-19T07:04:42.824667+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:30.748767+00:00</t>
+          <t>2025-11-19T07:04:42.824686+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:30.748783+00:00</t>
+          <t>2025-11-19T07:04:42.824702+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:36.331556+00:00</t>
+          <t>2025-11-19T07:04:48.274853+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:36.331585+00:00</t>
+          <t>2025-11-19T07:04:48.274883+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:41.532617+00:00</t>
+          <t>2025-11-19T07:04:53.273312+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:41.532648+00:00</t>
+          <t>2025-11-19T07:04:53.273338+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:41.532671+00:00</t>
+          <t>2025-11-19T07:04:53.273357+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:47.098378+00:00</t>
+          <t>2025-11-19T07:04:58.744787+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:47.098404+00:00</t>
+          <t>2025-11-19T07:04:58.744814+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:52.165812+00:00</t>
+          <t>2025-11-19T07:05:03.852997+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:52.165847+00:00</t>
+          <t>2025-11-19T07:05:03.853024+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:52.165865+00:00</t>
+          <t>2025-11-19T07:05:03.853041+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:52.165881+00:00</t>
+          <t>2025-11-19T07:05:03.853057+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:52.165895+00:00</t>
+          <t>2025-11-19T07:05:03.853071+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:57.271425+00:00</t>
+          <t>2025-11-19T07:05:09.254832+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-19T03:07:57.271456+00:00</t>
+          <t>2025-11-19T07:05:09.254884+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-19T03:08:08.347526+00:00</t>
+          <t>2025-11-19T07:05:19.480005+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-19T03:08:08.347560+00:00</t>
+          <t>2025-11-19T07:05:19.480035+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-19T03:08:08.347583+00:00</t>
+          <t>2025-11-19T07:05:19.480058+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-19T03:08:13.846901+00:00</t>
+          <t>2025-11-19T07:05:24.561921+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-19 18:05:43)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-19T07:03:27.845460+00:00</t>
+          <t>2025-11-19T10:01:07.669188+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-19T07:03:27.845498+00:00</t>
+          <t>2025-11-19T10:01:07.669233+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-19T07:03:27.845518+00:00</t>
+          <t>2025-11-19T10:01:07.669316+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-19T07:03:33.207622+00:00</t>
+          <t>2025-11-19T10:01:12.752236+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-19T07:03:33.207652+00:00</t>
+          <t>2025-11-19T10:01:12.752269+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-19T07:03:38.176178+00:00</t>
+          <t>2025-11-19T10:01:17.774573+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-19T07:03:43.721083+00:00</t>
+          <t>2025-11-19T10:01:23.267471+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-19T07:03:49.643389+00:00</t>
+          <t>2025-11-19T10:01:28.356018+00:00</t>
         </is>
       </c>
     </row>
@@ -966,27 +966,27 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Уотерспун Тайлер</t>
+          <t>Савицкий Кирилл</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>84</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>45769</t>
+          <t>17901</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1369_БАР_уотерспунтайлер</t>
+          <t>1369_БАР_савицкийкирилл</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1001,34 +1001,34 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-19T07:03:49.643417+00:00</t>
+          <t>2025-11-19T10:01:28.356049+00:00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ДМН</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dinamo_mn</t>
+          <t>barys</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Уэлле Ксавье</t>
+          <t>Уотерспун Тайлер</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>26</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1038,12 +1038,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>19692</t>
+          <t>45769</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1369_ДМН_уэллексавье</t>
+          <t>1369_БАР_уотерспунтайлер</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1053,54 +1053,54 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:00.098071+00:00</t>
+          <t>2025-11-19T10:01:28.356068+00:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>ДМН</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>dinamo_mn</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Уэлле Ксавье</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>19692</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_ДМН_уэллексавье</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1110,39 +1110,39 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:05.448928+00:00</t>
+          <t>2025-11-19T10:01:38.456213+00:00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Волков Александр С</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_ЛОК_волковалександрс</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1167,12 +1167,12 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:10.876331+00:00</t>
+          <t>2025-11-19T10:01:43.553855+00:00</t>
         </is>
       </c>
     </row>
@@ -1194,12 +1194,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Паник Рихард</t>
+          <t>Волков Александр С</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1209,12 +1209,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>16071</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_ЛОК_паникрихард</t>
+          <t>1369_ЛОК_волковалександрс</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:10.876357+00:00</t>
+          <t>2025-11-19T10:01:48.568090+00:00</t>
         </is>
       </c>
     </row>
@@ -1251,27 +1251,27 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Паник Рихард</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>16071</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ЛОК_паникрихард</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1286,49 +1286,49 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:10.876374+00:00</t>
+          <t>2025-11-19T10:01:48.568125+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,39 +1338,39 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:15.853810+00:00</t>
+          <t>2025-11-19T10:01:48.568146+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1380,12 +1380,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,39 +1395,39 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:32.370178+00:00</t>
+          <t>2025-11-19T10:01:53.536030+00:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1452,54 +1452,54 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:37.828847+00:00</t>
+          <t>2025-11-19T10:01:58.571368+00:00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Калиниченко Роман</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>26690</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_СИБ_калиниченкороман</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1509,12 +1509,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:42.824636+00:00</t>
+          <t>2025-11-19T10:02:03.602987+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:42.824667+00:00</t>
+          <t>2025-11-19T10:02:08.617446+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:42.824686+00:00</t>
+          <t>2025-11-19T10:02:08.617480+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:42.824702+00:00</t>
+          <t>2025-11-19T10:02:08.617500+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:48.274853+00:00</t>
+          <t>2025-11-19T10:02:13.763035+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:48.274883+00:00</t>
+          <t>2025-11-19T10:02:13.763070+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:53.273312+00:00</t>
+          <t>2025-11-19T10:02:18.797388+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:53.273338+00:00</t>
+          <t>2025-11-19T10:02:18.797423+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:53.273357+00:00</t>
+          <t>2025-11-19T10:02:18.797447+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:58.744787+00:00</t>
+          <t>2025-11-19T10:02:24.223155+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-19T07:04:58.744814+00:00</t>
+          <t>2025-11-19T10:02:24.223191+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-19T07:05:03.852997+00:00</t>
+          <t>2025-11-19T10:02:29.257514+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-19T07:05:03.853024+00:00</t>
+          <t>2025-11-19T10:02:29.257547+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-19T07:05:03.853041+00:00</t>
+          <t>2025-11-19T10:02:29.257570+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-19T07:05:03.853057+00:00</t>
+          <t>2025-11-19T10:02:29.257591+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-19T07:05:03.853071+00:00</t>
+          <t>2025-11-19T10:02:29.257609+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-19T07:05:09.254832+00:00</t>
+          <t>2025-11-19T10:02:34.771679+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-19T07:05:09.254884+00:00</t>
+          <t>2025-11-19T10:02:34.771717+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-19T07:05:19.480005+00:00</t>
+          <t>2025-11-19T10:02:44.866643+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-19T07:05:19.480035+00:00</t>
+          <t>2025-11-19T10:02:44.866676+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-19T07:05:19.480058+00:00</t>
+          <t>2025-11-19T10:02:44.866694+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-19T07:05:24.561921+00:00</t>
+          <t>2025-11-19T10:02:49.904008+00:00</t>
         </is>
       </c>
     </row>
@@ -2721,6 +2721,136 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>team_abbr</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>team_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>player_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>player_uid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>changed_at</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>changed_day</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>АДМ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Адмирал</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Шепелев Александр</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_АДМ_шепелевалександр</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-19T11:08:14.354550+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>СИБ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Калиниченко Роман</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1369_СИБ_калиниченкороман</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-11-19T18:02:50.406848+08:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-11-19</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2774,93 +2904,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Шепелев Александр</t>
+          <t>Савицкий Кирилл</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_АДМ_шепелевалександр</t>
+          <t>1369_БАР_савицкийкирилл</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>RETURN</t>
+          <t>INJURED_NEW</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-19T11:08:14.354550+08:00</t>
+          <t>2025-11-19T18:02:50.406848+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>2025-11-19</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>team_abbr</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>team_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>player_name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>player_uid</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>changed_at</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>changed_day</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-20 11:04:17)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:07.669188+00:00</t>
+          <t>2025-11-20T03:01:01.798042+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:07.669233+00:00</t>
+          <t>2025-11-20T03:01:01.798074+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:07.669316+00:00</t>
+          <t>2025-11-20T03:01:01.798093+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:12.752236+00:00</t>
+          <t>2025-11-20T03:01:03.998942+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:12.752269+00:00</t>
+          <t>2025-11-20T03:01:03.998971+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:17.774573+00:00</t>
+          <t>2025-11-20T03:01:06.172975+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:23.267471+00:00</t>
+          <t>2025-11-20T03:01:08.375815+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:28.356018+00:00</t>
+          <t>2025-11-20T03:01:10.598659+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:28.356049+00:00</t>
+          <t>2025-11-20T03:01:10.598690+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,34 +1058,34 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:28.356068+00:00</t>
+          <t>2025-11-20T03:01:10.598709+00:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ДМН</t>
+          <t>ДИН</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>dinamo_mn</t>
+          <t>dynamo_msk</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Уэлле Ксавье</t>
+          <t>Готовец Кирилл</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>41</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1095,12 +1095,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>19692</t>
+          <t>16034</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_ДМН_уэллексавье</t>
+          <t>1369_ДИН_готовецкирилл</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1110,54 +1110,54 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
+          <t>https://www.khl.ru/clubs/dynamo_msk/team/</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:38.456213+00:00</t>
+          <t>2025-11-20T03:01:12.745208+00:00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>ДМН</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>dinamo_mn</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Уэлле Ксавье</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>19692</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_ДМН_уэллексавье</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1167,39 +1167,39 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:43.553855+00:00</t>
+          <t>2025-11-20T03:01:14.953208+00:00</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Волков Александр С</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1209,12 +1209,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_ЛОК_волковалександрс</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1224,12 +1224,12 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:48.568090+00:00</t>
+          <t>2025-11-20T03:01:17.113763+00:00</t>
         </is>
       </c>
     </row>
@@ -1251,12 +1251,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Паник Рихард</t>
+          <t>Волков Александр С</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>97</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1266,12 +1266,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>16071</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_ЛОК_паникрихард</t>
+          <t>1369_ЛОК_волковалександрс</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:48.568125+00:00</t>
+          <t>2025-11-20T03:01:19.370721+00:00</t>
         </is>
       </c>
     </row>
@@ -1308,27 +1308,27 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Паник Рихард</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>16071</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ЛОК_паникрихард</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1343,49 +1343,49 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:48.568146+00:00</t>
+          <t>2025-11-20T03:01:19.370748+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,39 +1395,39 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:53.536030+00:00</t>
+          <t>2025-11-20T03:01:19.370764+00:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>20592</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1452,39 +1452,39 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-19T10:01:58.571368+00:00</t>
+          <t>2025-11-20T03:01:21.183192+00:00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Дергачёв Александр</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1494,12 +1494,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>20592</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_НХК_дергачевалександр</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1509,39 +1509,39 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:03.602987+00:00</t>
+          <t>2025-11-20T03:01:23.376804+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Фомин Макар</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1551,12 +1551,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>42087</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СЕВ_фоминмакар</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1566,39 +1566,39 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:08.617446+00:00</t>
+          <t>2025-11-20T03:01:25.528590+00:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>16195</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1623,12 +1623,12 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:08.617480+00:00</t>
+          <t>2025-11-20T03:01:25.528621+00:00</t>
         </is>
       </c>
     </row>
@@ -1650,27 +1650,27 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1685,49 +1685,49 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:08.617500+00:00</t>
+          <t>2025-11-20T03:01:27.339044+00:00</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1737,39 +1737,39 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:13.763035+00:00</t>
+          <t>2025-11-20T03:01:27.339071+00:00</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1779,12 +1779,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>41566</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1794,54 +1794,54 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:13.763070+00:00</t>
+          <t>2025-11-20T03:01:27.339087+00:00</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1851,54 +1851,54 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:18.797388+00:00</t>
+          <t>2025-11-20T03:01:29.173263+00:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Самсонов Илья</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>21010</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СОЧ_самсоновилья</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1908,12 +1908,12 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:18.797423+00:00</t>
+          <t>2025-11-20T03:01:29.173290+00:00</t>
         </is>
       </c>
     </row>
@@ -1935,27 +1935,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>44847</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1970,49 +1970,49 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:18.797447+00:00</t>
+          <t>2025-11-20T03:01:31.501049+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Самсонов Илья</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>21010</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СОЧ_самсоновилья</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,54 +2022,54 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:24.223155+00:00</t>
+          <t>2025-11-20T03:01:31.501081+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Хёфенмайер Ноэль</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>44847</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СОЧ_хефенмайерноэль</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,39 +2079,39 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:24.223191+00:00</t>
+          <t>2025-11-20T03:01:31.501102+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2121,12 +2121,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2136,39 +2136,39 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:29.257514+00:00</t>
+          <t>2025-11-20T03:01:33.445103+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2178,12 +2178,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,12 +2193,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:29.257547+00:00</t>
+          <t>2025-11-20T03:01:33.445131+00:00</t>
         </is>
       </c>
     </row>
@@ -2220,27 +2220,27 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>61</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>34493</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:29.257570+00:00</t>
+          <t>2025-11-20T03:01:35.337644+00:00</t>
         </is>
       </c>
     </row>
@@ -2277,12 +2277,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2292,12 +2292,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:29.257591+00:00</t>
+          <t>2025-11-20T03:01:35.337674+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,27 +2334,27 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,49 +2369,49 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:29.257609+00:00</t>
+          <t>2025-11-20T03:01:35.337692+00:00</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2421,39 +2421,39 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:34.771679+00:00</t>
+          <t>2025-11-20T03:01:35.337709+00:00</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2463,12 +2463,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2478,54 +2478,54 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:34.771717+00:00</t>
+          <t>2025-11-20T03:01:35.337723+00:00</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Дроздов Иван</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>30752</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_ЦСК_дроздовиван</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2535,39 +2535,39 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:44.866643+00:00</t>
+          <t>2025-11-20T03:01:37.257238+00:00</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2592,12 +2592,12 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:44.866676+00:00</t>
+          <t>2025-11-20T03:01:37.257270+00:00</t>
         </is>
       </c>
     </row>
@@ -2619,27 +2619,27 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Дроздов Иван</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>41896</t>
+          <t>30752</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_ЦСК_дроздовиван</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2654,64 +2654,178 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-19T10:02:44.866694+00:00</t>
+          <t>2025-11-20T03:01:41.934613+00:00</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>cska</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Моисеев Данила</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>23931</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_моисеевданила</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>2025-11-20T03:01:41.934643+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>cska</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Уильямс Колби</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>41896</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_уильямсколби</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>2025-11-20T03:01:41.934662+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>ШДР</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B42" t="inlineStr">
         <is>
           <t>Драконы</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>kunlun</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>Гроло Жереми</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>75</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>защитник</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="G42" t="inlineStr">
         <is>
           <t>45343</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
+      <c r="H42" t="inlineStr">
         <is>
           <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
         <is>
           <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>2025-11-19T10:02:49.904008+00:00</t>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>2025-11-20T03:01:43.829999+00:00</t>
         </is>
       </c>
     </row>
@@ -2721,6 +2835,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>team_abbr</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>team_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>player_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>player_uid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>changed_at</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>changed_day</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2774,167 +2944,74 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>ДИН</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Шепелев Александр</t>
+          <t>Готовец Кирилл</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_АДМ_шепелевалександр</t>
+          <t>1369_ДИН_готовецкирилл</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>RETURN</t>
+          <t>INJURED_NEW</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-19T11:08:14.354550+08:00</t>
+          <t>2025-11-20T11:01:44.337091+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-19</t>
+          <t>2025-11-20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Калиниченко Роман</t>
+          <t>Фомин Макар</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1369_СИБ_калиниченкороман</t>
+          <t>1369_СЕВ_фоминмакар</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>RETURN</t>
+          <t>INJURED_NEW</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-19T18:02:50.406848+08:00</t>
+          <t>2025-11-20T11:01:44.337091+08:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-11-19</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>team_abbr</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>team_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>player_name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>player_uid</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>changed_at</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>changed_day</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>БАР</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Барыс</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Савицкий Кирилл</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_БАР_савицкийкирилл</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-19T18:02:50.406848+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-19</t>
+          <t>2025-11-20</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-20 15:05:44)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:01.798042+00:00</t>
+          <t>2025-11-20T07:02:29.457744+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:01.798074+00:00</t>
+          <t>2025-11-20T07:02:29.457784+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:01.798093+00:00</t>
+          <t>2025-11-20T07:02:29.457807+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:03.998942+00:00</t>
+          <t>2025-11-20T07:02:31.249288+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:03.998971+00:00</t>
+          <t>2025-11-20T07:02:31.249316+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:06.172975+00:00</t>
+          <t>2025-11-20T07:02:33.417184+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:08.375815+00:00</t>
+          <t>2025-11-20T07:02:35.610758+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:10.598659+00:00</t>
+          <t>2025-11-20T07:02:37.472431+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:10.598690+00:00</t>
+          <t>2025-11-20T07:02:37.472461+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:10.598709+00:00</t>
+          <t>2025-11-20T07:02:37.472481+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:12.745208+00:00</t>
+          <t>2025-11-20T07:02:39.686287+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:14.953208+00:00</t>
+          <t>2025-11-20T07:02:41.863254+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:17.113763+00:00</t>
+          <t>2025-11-20T07:02:43.982007+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:19.370721+00:00</t>
+          <t>2025-11-20T07:02:46.164684+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:19.370748+00:00</t>
+          <t>2025-11-20T07:02:46.164710+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:19.370764+00:00</t>
+          <t>2025-11-20T07:02:46.164726+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:21.183192+00:00</t>
+          <t>2025-11-20T07:02:48.337397+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:23.376804+00:00</t>
+          <t>2025-11-20T07:02:50.059858+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:25.528590+00:00</t>
+          <t>2025-11-20T07:02:52.168678+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:25.528621+00:00</t>
+          <t>2025-11-20T07:02:52.168709+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:27.339044+00:00</t>
+          <t>2025-11-20T07:02:54.341930+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:27.339071+00:00</t>
+          <t>2025-11-20T07:02:54.341960+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:27.339087+00:00</t>
+          <t>2025-11-20T07:02:54.341978+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:29.173263+00:00</t>
+          <t>2025-11-20T07:02:56.171514+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:29.173290+00:00</t>
+          <t>2025-11-20T07:02:56.171543+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:31.501049+00:00</t>
+          <t>2025-11-20T07:02:57.919886+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:31.501081+00:00</t>
+          <t>2025-11-20T07:02:57.919913+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:31.501102+00:00</t>
+          <t>2025-11-20T07:02:57.919931+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:33.445103+00:00</t>
+          <t>2025-11-20T07:02:59.747695+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:33.445131+00:00</t>
+          <t>2025-11-20T07:02:59.747726+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:35.337644+00:00</t>
+          <t>2025-11-20T07:03:02.003831+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:35.337674+00:00</t>
+          <t>2025-11-20T07:03:02.003859+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:35.337692+00:00</t>
+          <t>2025-11-20T07:03:02.003884+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:35.337709+00:00</t>
+          <t>2025-11-20T07:03:02.003901+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:35.337723+00:00</t>
+          <t>2025-11-20T07:03:02.003917+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:37.257238+00:00</t>
+          <t>2025-11-20T07:03:04.006091+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:37.257270+00:00</t>
+          <t>2025-11-20T07:03:04.006122+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:41.934613+00:00</t>
+          <t>2025-11-20T07:03:08.646488+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:41.934643+00:00</t>
+          <t>2025-11-20T07:03:08.646518+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:41.934662+00:00</t>
+          <t>2025-11-20T07:03:08.646536+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-20T03:01:43.829999+00:00</t>
+          <t>2025-11-20T07:03:10.557541+00:00</t>
         </is>
       </c>
     </row>
@@ -2896,7 +2896,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2941,80 +2941,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ДИН</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Динамо М</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Готовец Кирилл</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_ДИН_готовецкирилл</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-20T11:01:44.337091+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-20</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>СЕВ</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Северсталь</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Фомин Макар</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1369_СЕВ_фоминмакар</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-11-20T11:01:44.337091+08:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-11-20</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-20 20:15:06)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:29.457744+00:00</t>
+          <t>2025-11-20T12:11:09.853953+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:29.457784+00:00</t>
+          <t>2025-11-20T12:11:09.853986+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:29.457807+00:00</t>
+          <t>2025-11-20T12:11:09.854005+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:31.249288+00:00</t>
+          <t>2025-11-20T12:11:11.823315+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:31.249316+00:00</t>
+          <t>2025-11-20T12:11:11.823345+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:33.417184+00:00</t>
+          <t>2025-11-20T12:11:13.686998+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:35.610758+00:00</t>
+          <t>2025-11-20T12:11:16.341718+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:37.472431+00:00</t>
+          <t>2025-11-20T12:11:18.608285+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:37.472461+00:00</t>
+          <t>2025-11-20T12:11:18.608314+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:37.472481+00:00</t>
+          <t>2025-11-20T12:11:18.608334+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:39.686287+00:00</t>
+          <t>2025-11-20T12:11:21.275996+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:41.863254+00:00</t>
+          <t>2025-11-20T12:11:23.996460+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:43.982007+00:00</t>
+          <t>2025-11-20T12:11:26.728213+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:46.164684+00:00</t>
+          <t>2025-11-20T12:11:28.928182+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:46.164710+00:00</t>
+          <t>2025-11-20T12:11:28.928211+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:46.164726+00:00</t>
+          <t>2025-11-20T12:11:28.928228+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:48.337397+00:00</t>
+          <t>2025-11-20T12:11:31.165844+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:50.059858+00:00</t>
+          <t>2025-11-20T12:11:33.471252+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:52.168678+00:00</t>
+          <t>2025-11-20T12:11:36.155866+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:52.168709+00:00</t>
+          <t>2025-11-20T12:11:36.155898+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:54.341930+00:00</t>
+          <t>2025-11-20T12:11:38.390554+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:54.341960+00:00</t>
+          <t>2025-11-20T12:11:38.390583+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:54.341978+00:00</t>
+          <t>2025-11-20T12:11:38.390600+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:56.171514+00:00</t>
+          <t>2025-11-20T12:11:40.978804+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:56.171543+00:00</t>
+          <t>2025-11-20T12:11:40.978833+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:57.919886+00:00</t>
+          <t>2025-11-20T12:11:43.601049+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:57.919913+00:00</t>
+          <t>2025-11-20T12:11:43.601080+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:57.919931+00:00</t>
+          <t>2025-11-20T12:11:43.601101+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:59.747695+00:00</t>
+          <t>2025-11-20T12:11:45.919960+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-20T07:02:59.747726+00:00</t>
+          <t>2025-11-20T12:11:45.919992+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-20T07:03:02.003831+00:00</t>
+          <t>2025-11-20T12:11:48.210729+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-20T07:03:02.003859+00:00</t>
+          <t>2025-11-20T12:11:48.210761+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-20T07:03:02.003884+00:00</t>
+          <t>2025-11-20T12:11:48.210782+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-20T07:03:02.003901+00:00</t>
+          <t>2025-11-20T12:11:48.210803+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-20T07:03:02.003917+00:00</t>
+          <t>2025-11-20T12:11:48.210819+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-20T07:03:04.006091+00:00</t>
+          <t>2025-11-20T12:11:50.520050+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-20T07:03:04.006122+00:00</t>
+          <t>2025-11-20T12:11:50.520085+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-20T07:03:08.646488+00:00</t>
+          <t>2025-11-20T12:11:55.580757+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-20T07:03:08.646518+00:00</t>
+          <t>2025-11-20T12:11:55.580787+00:00</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2025-11-20T07:03:08.646536+00:00</t>
+          <t>2025-11-20T12:11:55.580805+00:00</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2025-11-20T07:03:10.557541+00:00</t>
+          <t>2025-11-20T12:11:57.822736+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-21 15:04:15)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:40.482673+00:00</t>
+          <t>2025-11-21T07:01:52.039165+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:40.482705+00:00</t>
+          <t>2025-11-21T07:01:52.039197+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:42.726478+00:00</t>
+          <t>2025-11-21T07:01:54.321165+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:42.726507+00:00</t>
+          <t>2025-11-21T07:01:54.321192+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:45.074404+00:00</t>
+          <t>2025-11-21T07:01:56.589072+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:47.699807+00:00</t>
+          <t>2025-11-21T07:01:59.248078+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:50.562316+00:00</t>
+          <t>2025-11-21T07:02:01.407983+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:50.562346+00:00</t>
+          <t>2025-11-21T07:02:01.408011+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:50.562374+00:00</t>
+          <t>2025-11-21T07:02:01.408031+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:52.804251+00:00</t>
+          <t>2025-11-21T07:02:03.653028+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:55.026165+00:00</t>
+          <t>2025-11-21T07:02:05.895929+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:57.673962+00:00</t>
+          <t>2025-11-21T07:02:08.698251+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:59.788791+00:00</t>
+          <t>2025-11-21T07:02:11.344156+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:59.788823+00:00</t>
+          <t>2025-11-21T07:02:11.344185+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-21T03:01:59.788842+00:00</t>
+          <t>2025-11-21T07:02:11.344201+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:02.126742+00:00</t>
+          <t>2025-11-21T07:02:13.562906+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:07.440766+00:00</t>
+          <t>2025-11-21T07:02:18.824051+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:07.440794+00:00</t>
+          <t>2025-11-21T07:02:18.824081+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:10.143592+00:00</t>
+          <t>2025-11-21T07:02:21.078373+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:10.143621+00:00</t>
+          <t>2025-11-21T07:02:21.078404+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:10.143638+00:00</t>
+          <t>2025-11-21T07:02:21.078420+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:12.836980+00:00</t>
+          <t>2025-11-21T07:02:23.725915+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:12.837009+00:00</t>
+          <t>2025-11-21T07:02:23.725943+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:15.040992+00:00</t>
+          <t>2025-11-21T07:02:26.316174+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:15.041018+00:00</t>
+          <t>2025-11-21T07:02:26.316202+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:15.041037+00:00</t>
+          <t>2025-11-21T07:02:26.316220+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:17.736298+00:00</t>
+          <t>2025-11-21T07:02:28.975965+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:17.736327+00:00</t>
+          <t>2025-11-21T07:02:28.975994+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:20.020564+00:00</t>
+          <t>2025-11-21T07:02:31.550064+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:20.020628+00:00</t>
+          <t>2025-11-21T07:02:31.550093+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:20.020679+00:00</t>
+          <t>2025-11-21T07:02:31.550112+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:20.020712+00:00</t>
+          <t>2025-11-21T07:02:31.550127+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:20.020732+00:00</t>
+          <t>2025-11-21T07:02:31.550142+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:22.623304+00:00</t>
+          <t>2025-11-21T07:02:33.835510+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:22.623331+00:00</t>
+          <t>2025-11-21T07:02:33.835538+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:27.657792+00:00</t>
+          <t>2025-11-21T07:02:39.145985+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:27.657820+00:00</t>
+          <t>2025-11-21T07:02:39.146015+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:27.657837+00:00</t>
+          <t>2025-11-21T07:02:39.146044+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-21T03:02:30.356017+00:00</t>
+          <t>2025-11-21T07:02:41.375942+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-21 15:19:59)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-21T07:01:52.039165+00:00</t>
+          <t>2025-11-21T07:18:01.126050+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-21T07:01:52.039197+00:00</t>
+          <t>2025-11-21T07:18:01.126073+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-21T07:01:54.321165+00:00</t>
+          <t>2025-11-21T07:18:03.552946+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-21T07:01:54.321192+00:00</t>
+          <t>2025-11-21T07:18:03.552966+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-21T07:01:56.589072+00:00</t>
+          <t>2025-11-21T07:18:05.501753+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-21T07:01:59.248078+00:00</t>
+          <t>2025-11-21T07:18:07.926509+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:01.407983+00:00</t>
+          <t>2025-11-21T07:18:09.893076+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:01.408011+00:00</t>
+          <t>2025-11-21T07:18:09.893094+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:01.408031+00:00</t>
+          <t>2025-11-21T07:18:09.893103+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:03.653028+00:00</t>
+          <t>2025-11-21T07:18:11.775082+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:05.895929+00:00</t>
+          <t>2025-11-21T07:18:14.141960+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:08.698251+00:00</t>
+          <t>2025-11-21T07:18:16.099426+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:11.344156+00:00</t>
+          <t>2025-11-21T07:18:18.046280+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:11.344185+00:00</t>
+          <t>2025-11-21T07:18:18.046309+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:11.344201+00:00</t>
+          <t>2025-11-21T07:18:18.046327+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:13.562906+00:00</t>
+          <t>2025-11-21T07:18:20.441560+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:18.824051+00:00</t>
+          <t>2025-11-21T07:18:25.270869+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:18.824081+00:00</t>
+          <t>2025-11-21T07:18:25.270898+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:21.078373+00:00</t>
+          <t>2025-11-21T07:18:27.732052+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:21.078404+00:00</t>
+          <t>2025-11-21T07:18:27.732084+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:21.078420+00:00</t>
+          <t>2025-11-21T07:18:27.732092+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:23.725915+00:00</t>
+          <t>2025-11-21T07:18:29.683547+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:23.725943+00:00</t>
+          <t>2025-11-21T07:18:29.683574+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:26.316174+00:00</t>
+          <t>2025-11-21T07:18:32.144628+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:26.316202+00:00</t>
+          <t>2025-11-21T07:18:32.144660+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:26.316220+00:00</t>
+          <t>2025-11-21T07:18:32.144680+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:28.975965+00:00</t>
+          <t>2025-11-21T07:18:34.530998+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:28.975994+00:00</t>
+          <t>2025-11-21T07:18:34.531016+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:31.550064+00:00</t>
+          <t>2025-11-21T07:18:36.338509+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:31.550093+00:00</t>
+          <t>2025-11-21T07:18:36.338530+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:31.550112+00:00</t>
+          <t>2025-11-21T07:18:36.338540+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:31.550127+00:00</t>
+          <t>2025-11-21T07:18:36.338548+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:31.550142+00:00</t>
+          <t>2025-11-21T07:18:36.338556+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:33.835510+00:00</t>
+          <t>2025-11-21T07:18:38.292961+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:33.835538+00:00</t>
+          <t>2025-11-21T07:18:38.292994+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:39.145985+00:00</t>
+          <t>2025-11-21T07:18:42.775204+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:39.146015+00:00</t>
+          <t>2025-11-21T07:18:42.775233+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:39.146044+00:00</t>
+          <t>2025-11-21T07:18:42.775251+00:00</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2025-11-21T07:02:41.375942+00:00</t>
+          <t>2025-11-21T07:18:45.096816+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-22 11:03:42)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:01.126050+00:00</t>
+          <t>2025-11-22T03:01:08.186413+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:01.126073+00:00</t>
+          <t>2025-11-22T03:01:08.186446+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:03.552946+00:00</t>
+          <t>2025-11-22T03:01:10.114883+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:03.552966+00:00</t>
+          <t>2025-11-22T03:01:10.114917+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:05.501753+00:00</t>
+          <t>2025-11-22T03:01:12.518758+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:07.926509+00:00</t>
+          <t>2025-11-22T03:01:14.864753+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:09.893076+00:00</t>
+          <t>2025-11-22T03:01:17.317155+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:09.893094+00:00</t>
+          <t>2025-11-22T03:01:17.317185+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:09.893103+00:00</t>
+          <t>2025-11-22T03:01:17.317205+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:11.775082+00:00</t>
+          <t>2025-11-22T03:01:19.258026+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:14.141960+00:00</t>
+          <t>2025-11-22T03:01:21.638880+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:16.099426+00:00</t>
+          <t>2025-11-22T03:01:23.598735+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:18.046280+00:00</t>
+          <t>2025-11-22T03:01:25.980554+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:18.046309+00:00</t>
+          <t>2025-11-22T03:01:25.980598+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:18.046327+00:00</t>
+          <t>2025-11-22T03:01:25.980618+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:20.441560+00:00</t>
+          <t>2025-11-22T03:01:28.440461+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:25.270869+00:00</t>
+          <t>2025-11-22T03:01:32.645356+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:25.270898+00:00</t>
+          <t>2025-11-22T03:01:32.645389+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:27.732052+00:00</t>
+          <t>2025-11-22T03:01:34.958855+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:27.732084+00:00</t>
+          <t>2025-11-22T03:01:34.958887+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:27.732092+00:00</t>
+          <t>2025-11-22T03:01:34.958906+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:29.683547+00:00</t>
+          <t>2025-11-22T03:01:37.263097+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:29.683574+00:00</t>
+          <t>2025-11-22T03:01:37.263126+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:32.144628+00:00</t>
+          <t>2025-11-22T03:01:39.643497+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:32.144660+00:00</t>
+          <t>2025-11-22T03:01:39.643529+00:00</t>
         </is>
       </c>
     </row>
@@ -1935,12 +1935,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Сушко Илья</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1950,12 +1950,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>44847</t>
+          <t>22691</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_СОЧ_сушкоилья</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1970,49 +1970,49 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:32.144680+00:00</t>
+          <t>2025-11-22T03:01:39.643547+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Хёфенмайер Ноэль</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>44847</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СОЧ_хефенмайерноэль</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,12 +2022,12 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:34.530998+00:00</t>
+          <t>2025-11-22T03:01:39.643565+00:00</t>
         </is>
       </c>
     </row>
@@ -2049,12 +2049,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2064,12 +2064,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2084,34 +2084,34 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:34.531016+00:00</t>
+          <t>2025-11-22T03:01:41.568188+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Алалыкин Данил</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2121,12 +2121,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>34493</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2136,12 +2136,12 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:36.338509+00:00</t>
+          <t>2025-11-22T03:01:41.568216+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:36.338530+00:00</t>
+          <t>2025-11-22T03:01:43.911305+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:36.338540+00:00</t>
+          <t>2025-11-22T03:01:43.911333+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:36.338548+00:00</t>
+          <t>2025-11-22T03:01:43.911353+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:36.338556+00:00</t>
+          <t>2025-11-22T03:01:43.911369+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:38.292961+00:00</t>
+          <t>2025-11-22T03:01:45.823695+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:38.292994+00:00</t>
+          <t>2025-11-22T03:01:45.823724+00:00</t>
         </is>
       </c>
     </row>
@@ -2505,12 +2505,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Дроздов Иван</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2520,12 +2520,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>30752</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_ЦСК_дроздовиван</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:42.775204+00:00</t>
+          <t>2025-11-22T03:01:50.195971+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,27 +2562,27 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>41896</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2597,121 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-21T07:18:42.775233+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>cska</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Уильямс Колби</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>41896</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_уильямсколби</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>2025-11-21T07:18:42.775251+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Гроло Жереми</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>45343</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>1369_ШДР_гроложереми</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>2025-11-21T07:18:45.096816+00:00</t>
+          <t>2025-11-22T03:01:50.195998+00:00</t>
         </is>
       </c>
     </row>
@@ -2726,7 +2612,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2774,22 +2660,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Кизимов Семён</t>
+          <t>Алалыкин Данил</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_АВТ_кизимовсемен</t>
+          <t>1369_СЮЛ_алалыкинданил</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2799,34 +2685,34 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-21T11:02:30.862605+08:00</t>
+          <t>2025-11-22T11:01:51.769380+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Дергачёв Александр</t>
+          <t>Дроздов Иван</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1369_НХК_дергачевалександр</t>
+          <t>1369_ЦСК_дроздовиван</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2836,12 +2722,49 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-21T11:02:30.862605+08:00</t>
+          <t>2025-11-22T11:01:51.769380+08:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Гроло Жереми</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1369_ШДР_гроложереми</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-11-22T11:01:51.769380+08:00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-11-22</t>
         </is>
       </c>
     </row>
@@ -2856,7 +2779,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2901,6 +2824,43 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>СОЧ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Сушко Илья</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_СОЧ_сушкоилья</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-22T11:01:51.769380+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-22 15:05:04)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:08.186413+00:00</t>
+          <t>2025-11-22T07:01:28.473056+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:08.186446+00:00</t>
+          <t>2025-11-22T07:01:28.473096+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:10.114883+00:00</t>
+          <t>2025-11-22T07:01:30.701134+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:10.114917+00:00</t>
+          <t>2025-11-22T07:01:30.701165+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:12.518758+00:00</t>
+          <t>2025-11-22T07:01:32.928080+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:14.864753+00:00</t>
+          <t>2025-11-22T07:01:35.697573+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:17.317155+00:00</t>
+          <t>2025-11-22T07:01:37.980803+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:17.317185+00:00</t>
+          <t>2025-11-22T07:01:37.980838+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:17.317205+00:00</t>
+          <t>2025-11-22T07:01:37.980858+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:19.258026+00:00</t>
+          <t>2025-11-22T07:01:40.672857+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:21.638880+00:00</t>
+          <t>2025-11-22T07:01:44.131877+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:23.598735+00:00</t>
+          <t>2025-11-22T07:01:46.782943+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:25.980554+00:00</t>
+          <t>2025-11-22T07:01:50.042332+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:25.980598+00:00</t>
+          <t>2025-11-22T07:01:50.042359+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:25.980618+00:00</t>
+          <t>2025-11-22T07:01:50.042376+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:28.440461+00:00</t>
+          <t>2025-11-22T07:01:53.484114+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:32.645356+00:00</t>
+          <t>2025-11-22T07:01:59.563184+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:32.645389+00:00</t>
+          <t>2025-11-22T07:01:59.563218+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:34.958855+00:00</t>
+          <t>2025-11-22T07:02:02.088010+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:34.958887+00:00</t>
+          <t>2025-11-22T07:02:02.088051+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:34.958906+00:00</t>
+          <t>2025-11-22T07:02:02.088076+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:37.263097+00:00</t>
+          <t>2025-11-22T07:02:05.633267+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:37.263126+00:00</t>
+          <t>2025-11-22T07:02:05.633299+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:39.643497+00:00</t>
+          <t>2025-11-22T07:02:08.351107+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:39.643529+00:00</t>
+          <t>2025-11-22T07:02:08.351138+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:39.643547+00:00</t>
+          <t>2025-11-22T07:02:08.351156+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:39.643565+00:00</t>
+          <t>2025-11-22T07:02:08.351175+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:41.568188+00:00</t>
+          <t>2025-11-22T07:02:11.621206+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:41.568216+00:00</t>
+          <t>2025-11-22T07:02:11.621235+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:43.911305+00:00</t>
+          <t>2025-11-22T07:02:13.873172+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:43.911333+00:00</t>
+          <t>2025-11-22T07:02:13.873201+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:43.911353+00:00</t>
+          <t>2025-11-22T07:02:13.873219+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:43.911369+00:00</t>
+          <t>2025-11-22T07:02:13.873234+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:45.823695+00:00</t>
+          <t>2025-11-22T07:02:17.024935+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:45.823724+00:00</t>
+          <t>2025-11-22T07:02:17.024963+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:50.195971+00:00</t>
+          <t>2025-11-22T07:02:22.770316+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,121 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-22T03:01:50.195998+00:00</t>
+          <t>2025-11-22T07:02:22.770345+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Бишофф Джейк</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>45490</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>1369_ШДР_бишоффджейк</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>2025-11-22T07:02:26.136759+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Гроло Жереми</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>45343</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>1369_ШДР_гроложереми</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>2025-11-22T07:02:26.136791+00:00</t>
         </is>
       </c>
     </row>
@@ -2779,7 +2893,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2827,22 +2941,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Сушко Илья</t>
+          <t>Бишофф Джейк</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_СОЧ_сушкоилья</t>
+          <t>1369_ШДР_бишоффджейк</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2852,10 +2966,47 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-22T11:01:51.769380+08:00</t>
+          <t>2025-11-22T15:02:26.639804+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Гроло Жереми</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1369_ШДР_гроложереми</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-11-22T15:02:26.639804+08:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>2025-11-22</t>
         </is>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-23 09:57:07)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:28.473056+00:00</t>
+          <t>2025-11-23T01:54:07.841824+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:28.473096+00:00</t>
+          <t>2025-11-23T01:54:07.841843+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:30.701134+00:00</t>
+          <t>2025-11-23T01:54:10.356347+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:30.701165+00:00</t>
+          <t>2025-11-23T01:54:10.356365+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:32.928080+00:00</t>
+          <t>2025-11-23T01:54:13.079258+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:35.697573+00:00</t>
+          <t>2025-11-23T01:54:15.402052+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:37.980803+00:00</t>
+          <t>2025-11-23T01:54:18.145103+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:37.980838+00:00</t>
+          <t>2025-11-23T01:54:18.145133+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:37.980858+00:00</t>
+          <t>2025-11-23T01:54:18.145151+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:40.672857+00:00</t>
+          <t>2025-11-23T01:54:20.440432+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:44.131877+00:00</t>
+          <t>2025-11-23T01:54:23.106146+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:46.782943+00:00</t>
+          <t>2025-11-23T01:54:25.908887+00:00</t>
         </is>
       </c>
     </row>
@@ -1194,27 +1194,27 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Волков Александр С</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_ЛОК_волковалександрс</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1229,34 +1229,34 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:50.042332+00:00</t>
+          <t>2025-11-23T01:54:28.660366+00:00</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Паник Рихард</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1266,12 +1266,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>16071</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_ЛОК_паникрихард</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1281,39 +1281,39 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:50.042359+00:00</t>
+          <t>2025-11-23T01:54:31.029127+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Фомин Макар</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1323,12 +1323,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>42087</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_СЕВ_фоминмакар</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,39 +1338,39 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:50.042376+00:00</t>
+          <t>2025-11-23T01:54:36.170434+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1380,12 +1380,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,39 +1395,39 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:53.484114+00:00</t>
+          <t>2025-11-23T01:54:36.170465+00:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Фомин Макар</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>42087</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_СЕВ_фоминмакар</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1452,39 +1452,39 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:59.563184+00:00</t>
+          <t>2025-11-23T01:54:38.336611+00:00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1494,12 +1494,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1509,12 +1509,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-22T07:01:59.563218+00:00</t>
+          <t>2025-11-23T01:54:38.336643+00:00</t>
         </is>
       </c>
     </row>
@@ -1536,27 +1536,27 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1571,49 +1571,49 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:02.088010+00:00</t>
+          <t>2025-11-23T01:54:38.336662+00:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>16195</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1623,39 +1623,39 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:02.088051+00:00</t>
+          <t>2025-11-23T01:54:41.045630+00:00</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1665,12 +1665,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1680,54 +1680,54 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:02.088076+00:00</t>
+          <t>2025-11-23T01:54:41.045660+00:00</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1737,54 +1737,54 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:05.633267+00:00</t>
+          <t>2025-11-23T01:54:43.706448+00:00</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Самсонов Илья</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>41566</t>
+          <t>21010</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СОЧ_самсоновилья</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1794,12 +1794,12 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:05.633299+00:00</t>
+          <t>2025-11-23T01:54:43.706480+00:00</t>
         </is>
       </c>
     </row>
@@ -1821,27 +1821,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Сушко Илья</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>22691</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СОЧ_сушкоилья</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:08.351107+00:00</t>
+          <t>2025-11-23T01:54:43.706502+00:00</t>
         </is>
       </c>
     </row>
@@ -1878,27 +1878,27 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Самсонов Илья</t>
+          <t>Хёфенмайер Ноэль</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>21010</t>
+          <t>44847</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СОЧ_самсоновилья</t>
+          <t>1369_СОЧ_хефенмайерноэль</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1913,49 +1913,49 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:08.351138+00:00</t>
+          <t>2025-11-23T01:54:43.706523+00:00</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Сушко Илья</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>88</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>22691</t>
+          <t>33545</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СОЧ_сушкоилья</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1965,54 +1965,54 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:08.351156+00:00</t>
+          <t>2025-11-23T01:54:46.510282+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>95</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>44847</t>
+          <t>22494</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,39 +2022,39 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:08.351175+00:00</t>
+          <t>2025-11-23T01:54:46.510317+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2064,12 +2064,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,54 +2079,54 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:11.621206+00:00</t>
+          <t>2025-11-23T01:54:49.281171+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2136,12 +2136,12 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:11.621235+00:00</t>
+          <t>2025-11-23T01:54:49.281203+00:00</t>
         </is>
       </c>
     </row>
@@ -2163,12 +2163,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2178,12 +2178,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:13.873172+00:00</t>
+          <t>2025-11-23T01:54:49.281222+00:00</t>
         </is>
       </c>
     </row>
@@ -2220,27 +2220,27 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2255,49 +2255,49 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:13.873201+00:00</t>
+          <t>2025-11-23T01:54:49.281238+00:00</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2307,39 +2307,39 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:13.873219+00:00</t>
+          <t>2025-11-23T01:54:51.982443+00:00</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2349,12 +2349,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2364,54 +2364,54 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:13.873234+00:00</t>
+          <t>2025-11-23T01:54:51.982477+00:00</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2421,54 +2421,54 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:17.024935+00:00</t>
+          <t>2025-11-23T01:54:57.139100+00:00</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>41896</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2478,54 +2478,54 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:17.024963+00:00</t>
+          <t>2025-11-23T01:54:57.139133+00:00</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Бишофф Джейк</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>28</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>45490</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ШДР_бишоффджейк</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2535,39 +2535,39 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:22.770316+00:00</t>
+          <t>2025-11-23T01:54:59.864667+00:00</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>41896</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2592,126 +2592,12 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-22T07:02:22.770345+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Бишофф Джейк</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>45490</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>1369_ШДР_бишоффджейк</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>2025-11-22T07:02:26.136759+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Гроло Жереми</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>45343</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>1369_ШДР_гроложереми</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>2025-11-22T07:02:26.136791+00:00</t>
+          <t>2025-11-23T01:54:59.864694+00:00</t>
         </is>
       </c>
     </row>
@@ -2721,173 +2607,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>team_abbr</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>team_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>player_name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>player_uid</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>changed_at</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>changed_day</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>СЮЛ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Салават Юлаев</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Алалыкин Данил</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_СЮЛ_алалыкинданил</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-22T11:01:51.769380+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-22</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Дроздов Иван</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_дроздовиван</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-11-22T11:01:51.769380+08:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-11-22</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Гроло Жереми</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1369_ШДР_гроложереми</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-11-22T11:01:51.769380+08:00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2025-11-22</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2941,74 +2660,130 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Бишофф Джейк</t>
+          <t>Волков Александр С</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_ШДР_бишоффджейк</t>
+          <t>1369_ЛОК_волковалександрс</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>INJURED_NEW</t>
+          <t>RETURN</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-22T15:02:26.639804+08:00</t>
+          <t>2025-11-23T09:55:00.367713+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Гроло Жереми</t>
+          <t>Паник Рихард</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1369_ШДР_гроложереми</t>
+          <t>1369_ЛОК_паникрихард</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>INJURED_NEW</t>
+          <t>RETURN</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-22T15:02:26.639804+08:00</t>
+          <t>2025-11-23T09:55:00.367713+08:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>team_abbr</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>team_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>player_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>player_uid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>changed_at</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>changed_day</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-23 11:05:06)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:07.841824+00:00</t>
+          <t>2025-11-23T03:01:50.494957+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:07.841843+00:00</t>
+          <t>2025-11-23T03:01:50.494995+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:10.356347+00:00</t>
+          <t>2025-11-23T03:01:53.135597+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:10.356365+00:00</t>
+          <t>2025-11-23T03:01:53.135629+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:13.079258+00:00</t>
+          <t>2025-11-23T03:01:55.857638+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:15.402052+00:00</t>
+          <t>2025-11-23T03:01:58.572287+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:18.145103+00:00</t>
+          <t>2025-11-23T03:02:00.951950+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:18.145133+00:00</t>
+          <t>2025-11-23T03:02:00.951980+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:18.145151+00:00</t>
+          <t>2025-11-23T03:02:00.951999+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:20.440432+00:00</t>
+          <t>2025-11-23T03:02:03.585113+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:23.106146+00:00</t>
+          <t>2025-11-23T03:02:05.879462+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:25.908887+00:00</t>
+          <t>2025-11-23T03:02:08.627346+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:28.660366+00:00</t>
+          <t>2025-11-23T03:02:10.915961+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:31.029127+00:00</t>
+          <t>2025-11-23T03:02:13.741583+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:36.170434+00:00</t>
+          <t>2025-11-23T03:02:18.786635+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:36.170465+00:00</t>
+          <t>2025-11-23T03:02:18.786666+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:38.336611+00:00</t>
+          <t>2025-11-23T03:02:21.489255+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:38.336643+00:00</t>
+          <t>2025-11-23T03:02:21.489289+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:38.336662+00:00</t>
+          <t>2025-11-23T03:02:21.489308+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:41.045630+00:00</t>
+          <t>2025-11-23T03:02:23.825051+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:41.045660+00:00</t>
+          <t>2025-11-23T03:02:23.825082+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:43.706448+00:00</t>
+          <t>2025-11-23T03:02:26.584481+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:43.706480+00:00</t>
+          <t>2025-11-23T03:02:26.584513+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:43.706502+00:00</t>
+          <t>2025-11-23T03:02:26.584532+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:43.706523+00:00</t>
+          <t>2025-11-23T03:02:26.584552+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:46.510282+00:00</t>
+          <t>2025-11-23T03:02:29.362414+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:46.510317+00:00</t>
+          <t>2025-11-23T03:02:29.362445+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:49.281171+00:00</t>
+          <t>2025-11-23T03:02:32.003050+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:49.281203+00:00</t>
+          <t>2025-11-23T03:02:32.003080+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:49.281222+00:00</t>
+          <t>2025-11-23T03:02:32.003099+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:49.281238+00:00</t>
+          <t>2025-11-23T03:02:32.003121+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:51.982443+00:00</t>
+          <t>2025-11-23T03:02:34.766140+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:51.982477+00:00</t>
+          <t>2025-11-23T03:02:34.766172+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:57.139100+00:00</t>
+          <t>2025-11-23T03:02:40.337064+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:57.139133+00:00</t>
+          <t>2025-11-23T03:02:40.337093+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:59.864667+00:00</t>
+          <t>2025-11-23T03:02:42.545420+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-23T01:54:59.864694+00:00</t>
+          <t>2025-11-23T03:02:42.545450+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-23 15:05:08)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-23T03:01:50.494957+00:00</t>
+          <t>2025-11-23T07:01:50.451543+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-23T03:01:50.494995+00:00</t>
+          <t>2025-11-23T07:01:50.451586+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-23T03:01:53.135597+00:00</t>
+          <t>2025-11-23T07:01:53.104468+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-23T03:01:53.135629+00:00</t>
+          <t>2025-11-23T07:01:53.104502+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-23T03:01:55.857638+00:00</t>
+          <t>2025-11-23T07:01:55.900574+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-23T03:01:58.572287+00:00</t>
+          <t>2025-11-23T07:01:58.212978+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:00.951950+00:00</t>
+          <t>2025-11-23T07:02:00.971759+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:00.951980+00:00</t>
+          <t>2025-11-23T07:02:00.971791+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:00.951999+00:00</t>
+          <t>2025-11-23T07:02:00.971811+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:03.585113+00:00</t>
+          <t>2025-11-23T07:02:03.701568+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:05.879462+00:00</t>
+          <t>2025-11-23T07:02:05.856455+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:08.627346+00:00</t>
+          <t>2025-11-23T07:02:08.128877+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:10.915961+00:00</t>
+          <t>2025-11-23T07:02:10.880350+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:13.741583+00:00</t>
+          <t>2025-11-23T07:02:13.665840+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:18.786635+00:00</t>
+          <t>2025-11-23T07:02:18.882252+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:18.786666+00:00</t>
+          <t>2025-11-23T07:02:18.882282+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:21.489255+00:00</t>
+          <t>2025-11-23T07:02:21.188261+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:21.489289+00:00</t>
+          <t>2025-11-23T07:02:21.188291+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:21.489308+00:00</t>
+          <t>2025-11-23T07:02:21.188309+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:23.825051+00:00</t>
+          <t>2025-11-23T07:02:24.030987+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:23.825082+00:00</t>
+          <t>2025-11-23T07:02:24.031019+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:26.584481+00:00</t>
+          <t>2025-11-23T07:02:26.756830+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:26.584513+00:00</t>
+          <t>2025-11-23T07:02:26.756861+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:26.584532+00:00</t>
+          <t>2025-11-23T07:02:26.756878+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:26.584552+00:00</t>
+          <t>2025-11-23T07:02:26.756896+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:29.362414+00:00</t>
+          <t>2025-11-23T07:02:29.129823+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:29.362445+00:00</t>
+          <t>2025-11-23T07:02:29.129852+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:32.003050+00:00</t>
+          <t>2025-11-23T07:02:31.580411+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:32.003080+00:00</t>
+          <t>2025-11-23T07:02:31.580440+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:32.003099+00:00</t>
+          <t>2025-11-23T07:02:31.580457+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:32.003121+00:00</t>
+          <t>2025-11-23T07:02:31.580472+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:34.766140+00:00</t>
+          <t>2025-11-23T07:02:33.874991+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:34.766172+00:00</t>
+          <t>2025-11-23T07:02:33.875021+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:40.337064+00:00</t>
+          <t>2025-11-23T07:02:38.606109+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:40.337093+00:00</t>
+          <t>2025-11-23T07:02:38.606140+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:42.545420+00:00</t>
+          <t>2025-11-23T07:02:41.377707+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-23T03:02:42.545450+00:00</t>
+          <t>2025-11-23T07:02:41.377735+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-23 19:07:21)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-23T07:01:50.451543+00:00</t>
+          <t>2025-11-23T11:04:25.502898+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-23T07:01:50.451586+00:00</t>
+          <t>2025-11-23T11:04:25.502935+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-23T07:01:53.104468+00:00</t>
+          <t>2025-11-23T11:04:28.092503+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-23T07:01:53.104502+00:00</t>
+          <t>2025-11-23T11:04:28.092536+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-23T07:01:55.900574+00:00</t>
+          <t>2025-11-23T11:04:30.212849+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-23T07:01:58.212978+00:00</t>
+          <t>2025-11-23T11:04:32.257060+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:00.971759+00:00</t>
+          <t>2025-11-23T11:04:34.346951+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:00.971791+00:00</t>
+          <t>2025-11-23T11:04:34.346968+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:00.971811+00:00</t>
+          <t>2025-11-23T11:04:34.346976+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:03.701568+00:00</t>
+          <t>2025-11-23T11:04:36.430325+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:05.856455+00:00</t>
+          <t>2025-11-23T11:04:38.529464+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:08.128877+00:00</t>
+          <t>2025-11-23T11:04:40.593521+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:10.880350+00:00</t>
+          <t>2025-11-23T11:04:42.642253+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:13.665840+00:00</t>
+          <t>2025-11-23T11:04:45.185838+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:18.882252+00:00</t>
+          <t>2025-11-23T11:04:49.384022+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:18.882282+00:00</t>
+          <t>2025-11-23T11:04:49.384051+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:21.188261+00:00</t>
+          <t>2025-11-23T11:04:51.339839+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:21.188291+00:00</t>
+          <t>2025-11-23T11:04:51.339885+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:21.188309+00:00</t>
+          <t>2025-11-23T11:04:51.339897+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:24.030987+00:00</t>
+          <t>2025-11-23T11:04:53.859383+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:24.031019+00:00</t>
+          <t>2025-11-23T11:04:53.859412+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:26.756830+00:00</t>
+          <t>2025-11-23T11:04:55.902959+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:26.756861+00:00</t>
+          <t>2025-11-23T11:04:55.902978+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:26.756878+00:00</t>
+          <t>2025-11-23T11:04:55.902989+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:26.756896+00:00</t>
+          <t>2025-11-23T11:04:55.902997+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:29.129823+00:00</t>
+          <t>2025-11-23T11:04:58.359933+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:29.129852+00:00</t>
+          <t>2025-11-23T11:04:58.359978+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:31.580411+00:00</t>
+          <t>2025-11-23T11:05:00.396057+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:31.580440+00:00</t>
+          <t>2025-11-23T11:05:00.396087+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:31.580457+00:00</t>
+          <t>2025-11-23T11:05:00.396105+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:31.580472+00:00</t>
+          <t>2025-11-23T11:05:00.396121+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:33.874991+00:00</t>
+          <t>2025-11-23T11:05:02.943085+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:33.875021+00:00</t>
+          <t>2025-11-23T11:05:02.943102+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:38.606109+00:00</t>
+          <t>2025-11-23T11:05:07.979970+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:38.606140+00:00</t>
+          <t>2025-11-23T11:05:07.979999+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:41.377707+00:00</t>
+          <t>2025-11-23T11:05:09.990261+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-23T07:02:41.377735+00:00</t>
+          <t>2025-11-23T11:05:09.990293+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-23 19:31:45)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:25.502898+00:00</t>
+          <t>2025-11-23T11:28:38.156335+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:25.502935+00:00</t>
+          <t>2025-11-23T11:28:38.156368+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:28.092503+00:00</t>
+          <t>2025-11-23T11:28:40.211442+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:28.092536+00:00</t>
+          <t>2025-11-23T11:28:40.211472+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:30.212849+00:00</t>
+          <t>2025-11-23T11:28:42.262328+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:32.257060+00:00</t>
+          <t>2025-11-23T11:28:44.274086+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:34.346951+00:00</t>
+          <t>2025-11-23T11:28:46.365788+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:34.346968+00:00</t>
+          <t>2025-11-23T11:28:46.365805+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:34.346976+00:00</t>
+          <t>2025-11-23T11:28:46.365813+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:36.430325+00:00</t>
+          <t>2025-11-23T11:28:48.410769+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:38.529464+00:00</t>
+          <t>2025-11-23T11:28:50.511452+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:40.593521+00:00</t>
+          <t>2025-11-23T11:28:53.030961+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:42.642253+00:00</t>
+          <t>2025-11-23T11:28:55.106932+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:45.185838+00:00</t>
+          <t>2025-11-23T11:28:57.241116+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:49.384022+00:00</t>
+          <t>2025-11-23T11:29:01.771944+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:49.384051+00:00</t>
+          <t>2025-11-23T11:29:01.771975+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:51.339839+00:00</t>
+          <t>2025-11-23T11:29:04.252782+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:51.339885+00:00</t>
+          <t>2025-11-23T11:29:04.252825+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:51.339897+00:00</t>
+          <t>2025-11-23T11:29:04.252836+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:53.859383+00:00</t>
+          <t>2025-11-23T11:29:06.388260+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:53.859412+00:00</t>
+          <t>2025-11-23T11:29:06.388277+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:55.902959+00:00</t>
+          <t>2025-11-23T11:29:08.458157+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:55.902978+00:00</t>
+          <t>2025-11-23T11:29:08.458185+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:55.902989+00:00</t>
+          <t>2025-11-23T11:29:08.458194+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:55.902997+00:00</t>
+          <t>2025-11-23T11:29:08.458202+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:58.359933+00:00</t>
+          <t>2025-11-23T11:29:10.581664+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-23T11:04:58.359978+00:00</t>
+          <t>2025-11-23T11:29:10.581708+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-23T11:05:00.396057+00:00</t>
+          <t>2025-11-23T11:29:13.075546+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-23T11:05:00.396087+00:00</t>
+          <t>2025-11-23T11:29:13.075573+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-23T11:05:00.396105+00:00</t>
+          <t>2025-11-23T11:29:13.075589+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-23T11:05:00.396121+00:00</t>
+          <t>2025-11-23T11:29:13.075603+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-23T11:05:02.943085+00:00</t>
+          <t>2025-11-23T11:29:15.622114+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-23T11:05:02.943102+00:00</t>
+          <t>2025-11-23T11:29:15.622141+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-23T11:05:07.979970+00:00</t>
+          <t>2025-11-23T11:29:19.887165+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-23T11:05:07.979999+00:00</t>
+          <t>2025-11-23T11:29:19.887180+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-23T11:05:09.990261+00:00</t>
+          <t>2025-11-23T11:29:22.706590+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-23T11:05:09.990293+00:00</t>
+          <t>2025-11-23T11:29:22.706617+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-24 11:04:37)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,2115 @@
       <c r="K1" s="1" t="inlineStr">
         <is>
           <t>scraped_at</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>АВТ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Автомобилист</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>avtomobilist</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Зборовский Сергей</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>20989</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1369_АВТ_зборовскийсергей</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/avtomobilist/team/</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:01:43.715385+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>АДМ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Адмирал</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>admiral</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Грман Марио</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>31232</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1369_АДМ_грманмарио</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/admiral/team/</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:01:45.986051+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>АДМ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Адмирал</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>admiral</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Сошников Никита</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>16731</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1369_АДМ_сошниковникита</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/admiral/team/</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:01:45.986081+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>АКБ</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Ак Барс</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ak_bars</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Яруллин Альберт</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>16365</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1369_АКБ_яруллинальберт</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:01:48.252137+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>АМР</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Амур</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>amur</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Абросимов Роман</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>17968</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1369_АМР_абросимовроман</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:01:50.972297+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>БАР</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Барыс</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>barys</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Бояркин Никита</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>вратарь</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>28244</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>1369_БАР_бояркинникита</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:01:53.758950+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>БАР</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Барыс</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>barys</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Савицкий Кирилл</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>17901</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1369_БАР_савицкийкирилл</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:01:53.758979+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>БАР</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Барыс</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>barys</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Уотерспун Тайлер</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>45769</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1369_БАР_уотерспунтайлер</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/barys/team/</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:01:53.758997+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ДИН</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Динамо М</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>dynamo_msk</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Готовец Кирилл</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>16034</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>1369_ДИН_готовецкирилл</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/dynamo_msk/team/</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:01:56.428329+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ДМН</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Динамо Мн</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>dinamo_mn</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Уэлле Ксавье</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>19692</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>1369_ДМН_уэллексавье</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:01:58.778170+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ЛАД</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Лада</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>lada</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Ожгихин Алексей</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>23021</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>1369_ЛАД_ожгихиналексей</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:01.472830+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ЛОК</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Локомотив</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>lokomotiv</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Сергеев Андрей</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>15416</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>1369_ЛОК_сергеевандрей</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:04.199319+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ММГ</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Металлург Мг</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>metallurg_mg</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Козлов Андрей Е</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>40899</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>1369_ММГ_козловандрейе</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:06.601383+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>СЕВ</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Северсталь</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>severstal</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Квочко Илья</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>39445</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>1369_СЕВ_квочкоилья</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:11.919783+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>СЕВ</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Северсталь</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>severstal</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Фомин Макар</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>42087</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>1369_СЕВ_фоминмакар</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:11.919812+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>СЕВ</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Северсталь</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>severstal</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Цицюра Владислав</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>23840</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>1369_СЕВ_цицюравладислав</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:11.919832+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>СИБ</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>sibir</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Приски Чейз Эванс</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>45392</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>1369_СИБ_прискичейзэванс</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:14.628109+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>СИБ</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>sibir</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Пьянов Валентин</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>16195</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>1369_СИБ_пьяноввалентин</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:14.628142+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>СИБ</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>sibir</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Широков Сергей</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>524</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>1369_СИБ_широковсергей</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:14.628159+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>СКА</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>СКА</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ska</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Зайцев Никита И</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>16024</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>1369_СКА_зайцевникитаи</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:17.212290+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>СКА</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>СКА</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ska</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Короткий Матвей</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>41566</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>1369_СКА_короткийматвей</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:17.212319+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>СОЧ</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>hc_sochi</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Гуськов Матвей</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>29136</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>1369_СОЧ_гуськовматвей</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:19.893359+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>СОЧ</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>hc_sochi</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Самсонов Илья</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>вратарь</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>21010</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>1369_СОЧ_самсоновилья</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:19.893390+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>СОЧ</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>hc_sochi</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Сушко Илья</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>22691</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>1369_СОЧ_сушкоилья</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:19.893407+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>СОЧ</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>hc_sochi</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Хёфенмайер Ноэль</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>44847</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>1369_СОЧ_хефенмайерноэль</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:19.893427+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>СПР</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Спартак</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>spartak</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Воробьёв Иван В</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>33545</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>1369_СПР_воробьевиванв</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:22.607221+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>СПР</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Спартак</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>spartak</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Рубцов Герман</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>22494</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>1369_СПР_рубцовгерман</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:22.607251+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>СЮЛ</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Салават Юлаев</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>salavat_yulaev</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Берлёв Антон</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>20546</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>1369_СЮЛ_берлевантон</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:24.933696+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>СЮЛ</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Салават Юлаев</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>salavat_yulaev</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Зоркин Никита</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>26738</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>1369_СЮЛ_зоркинникита</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:24.933725+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>СЮЛ</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Салават Юлаев</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>salavat_yulaev</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Хворов Николай</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>39828</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>1369_СЮЛ_хворовниколай</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:24.933741+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>СЮЛ</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Салават Юлаев</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>salavat_yulaev</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Ян Денис</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>22166</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>1369_СЮЛ_янденис</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:24.933757+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>ТОР</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Торпедо</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>torpedo</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Науменков Михаил</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>16400</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>1369_ТОР_науменковмихаил</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:27.466113+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ТОР</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Торпедо</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>torpedo</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Рожков Никита А</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>27912</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>1369_ТОР_рожковникитаа</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:27.466142+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>cska</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Моисеев Данила</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>23931</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_моисеевданила</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:32.531649+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>cska</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Уильямс Колби</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>41896</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_уильямсколби</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:32.531676+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Бишофф Джейк</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>45490</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>1369_ШДР_бишоффджейк</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:35.112234+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Гроло Жереми</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>45343</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>1369_ШДР_гроложереми</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>2025-11-24T03:02:35.112262+00:00</t>
         </is>
       </c>
     </row>
@@ -588,22 +2697,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>АВТ</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Автомобилист</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Трямкин Никита</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_АВТ_трямкинникита</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -625,22 +2734,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Грман Марио</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_АДМ_грманмарио</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -662,22 +2771,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Самсонов Илья</t>
+          <t>Сошников Никита</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1369_СОЧ_самсоновилья</t>
+          <t>1369_АДМ_сошниковникита</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -699,22 +2808,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>АКБ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Сушко Илья</t>
+          <t>Яруллин Альберт</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1369_СОЧ_сушкоилья</t>
+          <t>1369_АКБ_яруллинальберт</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -736,22 +2845,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Абросимов Роман</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_АМР_абросимовроман</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -773,22 +2882,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -810,22 +2919,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Савицкий Кирилл</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_БАР_савицкийкирилл</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -847,22 +2956,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Уотерспун Тайлер</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_БАР_уотерспунтайлер</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -884,22 +2993,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ДИН</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Готовец Кирилл</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_ДИН_готовецкирилл</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -921,22 +3030,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ДМН</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Уэлле Ксавье</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_ДМН_уэллексавье</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -958,22 +3067,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -995,22 +3104,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1032,22 +3141,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1069,22 +3178,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Фомин Макар</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_СЕВ_фоминмакар</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1106,22 +3215,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1143,22 +3252,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1180,22 +3289,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Бишофф Джейк</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1369_ШДР_бишоффджейк</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1254,22 +3363,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1291,22 +3400,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Трямкин Никита</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1369_АВТ_трямкинникита</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1328,22 +3437,22 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Грман Марио</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1369_АДМ_грманмарио</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1365,22 +3474,22 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Сошников Никита</t>
+          <t>Самсонов Илья</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1369_АДМ_сошниковникита</t>
+          <t>1369_СОЧ_самсоновилья</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1402,22 +3511,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>АКБ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Яруллин Альберт</t>
+          <t>Сушко Илья</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1369_АКБ_яруллинальберт</t>
+          <t>1369_СОЧ_сушкоилья</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1439,22 +3548,22 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Абросимов Роман</t>
+          <t>Хёфенмайер Ноэль</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1369_АМР_абросимовроман</t>
+          <t>1369_СОЧ_хефенмайерноэль</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1476,22 +3585,22 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1513,22 +3622,22 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Савицкий Кирилл</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1369_БАР_савицкийкирилл</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1550,22 +3659,22 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Уотерспун Тайлер</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1369_БАР_уотерспунтайлер</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1587,22 +3696,22 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ДИН</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Динамо М</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Готовец Кирилл</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1369_ДИН_готовецкирилл</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1624,22 +3733,22 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ДМН</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Уэлле Ксавье</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1369_ДМН_уэллексавье</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1661,22 +3770,22 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1698,22 +3807,22 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1735,22 +3844,22 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1772,22 +3881,22 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Фомин Макар</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1369_СЕВ_фоминмакар</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1809,22 +3918,22 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1846,22 +3955,22 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Бишофф Джейк</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_ШДР_бишоффджейк</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-24 15:04:54)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-24T03:01:43.715385+00:00</t>
+          <t>2025-11-24T07:01:37.931377+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-24T03:01:45.986051+00:00</t>
+          <t>2025-11-24T07:01:40.163933+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-24T03:01:45.986081+00:00</t>
+          <t>2025-11-24T07:01:40.163973+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-24T03:01:48.252137+00:00</t>
+          <t>2025-11-24T07:01:42.870526+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-24T03:01:50.972297+00:00</t>
+          <t>2025-11-24T07:01:45.661702+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-24T03:01:53.758950+00:00</t>
+          <t>2025-11-24T07:01:48.084064+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-24T03:01:53.758979+00:00</t>
+          <t>2025-11-24T07:01:48.084095+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-24T03:01:53.758997+00:00</t>
+          <t>2025-11-24T07:01:48.084114+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-24T03:01:56.428329+00:00</t>
+          <t>2025-11-24T07:01:50.400606+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-24T03:01:58.778170+00:00</t>
+          <t>2025-11-24T07:01:53.177641+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:01.472830+00:00</t>
+          <t>2025-11-24T07:01:55.924296+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:04.199319+00:00</t>
+          <t>2025-11-24T07:01:58.225214+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:06.601383+00:00</t>
+          <t>2025-11-24T07:02:00.541929+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:11.919783+00:00</t>
+          <t>2025-11-24T07:02:05.509866+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:11.919812+00:00</t>
+          <t>2025-11-24T07:02:05.509894+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:11.919832+00:00</t>
+          <t>2025-11-24T07:02:05.509913+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:14.628109+00:00</t>
+          <t>2025-11-24T07:02:07.889722+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:14.628142+00:00</t>
+          <t>2025-11-24T07:02:07.889754+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:14.628159+00:00</t>
+          <t>2025-11-24T07:02:07.889771+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:17.212290+00:00</t>
+          <t>2025-11-24T07:02:10.267375+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:17.212319+00:00</t>
+          <t>2025-11-24T07:02:10.267405+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:19.893359+00:00</t>
+          <t>2025-11-24T07:02:12.975236+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:19.893390+00:00</t>
+          <t>2025-11-24T07:02:12.975263+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:19.893407+00:00</t>
+          <t>2025-11-24T07:02:12.975283+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:19.893427+00:00</t>
+          <t>2025-11-24T07:02:12.975301+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:22.607221+00:00</t>
+          <t>2025-11-24T07:02:15.669380+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:22.607251+00:00</t>
+          <t>2025-11-24T07:02:15.669408+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:24.933696+00:00</t>
+          <t>2025-11-24T07:02:18.399603+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:24.933725+00:00</t>
+          <t>2025-11-24T07:02:18.399637+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:24.933741+00:00</t>
+          <t>2025-11-24T07:02:18.399655+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:24.933757+00:00</t>
+          <t>2025-11-24T07:02:18.399671+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:27.466113+00:00</t>
+          <t>2025-11-24T07:02:20.704368+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:27.466142+00:00</t>
+          <t>2025-11-24T07:02:20.704400+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:32.531649+00:00</t>
+          <t>2025-11-24T07:02:25.876730+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:32.531676+00:00</t>
+          <t>2025-11-24T07:02:25.876759+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:35.112234+00:00</t>
+          <t>2025-11-24T07:02:28.606522+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-24T03:02:35.112262+00:00</t>
+          <t>2025-11-24T07:02:28.606552+00:00</t>
         </is>
       </c>
     </row>
@@ -2697,22 +2697,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Трямкин Никита</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1369_АВТ_трямкинникита</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2734,22 +2734,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Грман Марио</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1369_АДМ_грманмарио</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -2771,22 +2771,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>АДМ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Сошников Никита</t>
+          <t>Самсонов Илья</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1369_АДМ_сошниковникита</t>
+          <t>1369_СОЧ_самсоновилья</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -2808,22 +2808,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>АКБ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Яруллин Альберт</t>
+          <t>Сушко Илья</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1369_АКБ_яруллинальберт</t>
+          <t>1369_СОЧ_сушкоилья</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -2845,22 +2845,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Абросимов Роман</t>
+          <t>Хёфенмайер Ноэль</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1369_АМР_абросимовроман</t>
+          <t>1369_СОЧ_хефенмайерноэль</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -2882,22 +2882,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -2919,22 +2919,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Савицкий Кирилл</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1369_БАР_савицкийкирилл</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -2956,22 +2956,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Уотерспун Тайлер</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1369_БАР_уотерспунтайлер</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -2993,22 +2993,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ДИН</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Динамо М</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Готовец Кирилл</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1369_ДИН_готовецкирилл</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -3030,22 +3030,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ДМН</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Уэлле Ксавье</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1369_ДМН_уэллексавье</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -3067,22 +3067,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -3104,22 +3104,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -3141,22 +3141,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -3178,22 +3178,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Фомин Макар</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1369_СЕВ_фоминмакар</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -3215,22 +3215,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -3252,22 +3252,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -3289,22 +3289,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Бишофф Джейк</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_ШДР_бишоффджейк</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -3363,22 +3363,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -3400,22 +3400,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>АВТ</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Автомобилист</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Трямкин Никита</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_АВТ_трямкинникита</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -3437,22 +3437,22 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Грман Марио</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_АДМ_грманмарио</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -3474,22 +3474,22 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Самсонов Илья</t>
+          <t>Сошников Никита</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1369_СОЧ_самсоновилья</t>
+          <t>1369_АДМ_сошниковникита</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -3511,22 +3511,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>АКБ</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Сушко Илья</t>
+          <t>Яруллин Альберт</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1369_СОЧ_сушкоилья</t>
+          <t>1369_АКБ_яруллинальберт</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -3548,22 +3548,22 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Абросимов Роман</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_АМР_абросимовроман</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -3585,22 +3585,22 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -3622,22 +3622,22 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Савицкий Кирилл</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_БАР_савицкийкирилл</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -3659,22 +3659,22 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Уотерспун Тайлер</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_БАР_уотерспунтайлер</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -3696,22 +3696,22 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ДИН</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Готовец Кирилл</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_ДИН_готовецкирилл</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -3733,22 +3733,22 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ДМН</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Уэлле Ксавье</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_ДМН_уэллексавье</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -3770,22 +3770,22 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -3807,22 +3807,22 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -3844,22 +3844,22 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -3881,22 +3881,22 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Фомин Макар</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_СЕВ_фоминмакар</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -3918,22 +3918,22 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -3955,22 +3955,22 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Бишофф Джейк</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1369_ШДР_бишоффджейк</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-25 11:03:43)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-24T07:01:37.931377+00:00</t>
+          <t>2025-11-25T03:01:11.456802+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-24T07:01:40.163933+00:00</t>
+          <t>2025-11-25T03:01:13.785575+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-24T07:01:40.163973+00:00</t>
+          <t>2025-11-25T03:01:13.785604+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-24T07:01:42.870526+00:00</t>
+          <t>2025-11-25T03:01:15.684829+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-24T07:01:45.661702+00:00</t>
+          <t>2025-11-25T03:01:18.010400+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-24T07:01:48.084064+00:00</t>
+          <t>2025-11-25T03:01:20.419727+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-24T07:01:48.084095+00:00</t>
+          <t>2025-11-25T03:01:20.419755+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-24T07:01:48.084114+00:00</t>
+          <t>2025-11-25T03:01:20.419773+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-24T07:01:50.400606+00:00</t>
+          <t>2025-11-25T03:01:22.790529+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-24T07:01:53.177641+00:00</t>
+          <t>2025-11-25T03:01:25.154010+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-24T07:01:55.924296+00:00</t>
+          <t>2025-11-25T03:01:27.502192+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-24T07:01:58.225214+00:00</t>
+          <t>2025-11-25T03:01:29.861433+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:00.541929+00:00</t>
+          <t>2025-11-25T03:01:32.221036+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:05.509866+00:00</t>
+          <t>2025-11-25T03:01:36.958360+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:05.509894+00:00</t>
+          <t>2025-11-25T03:01:36.958390+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:05.509913+00:00</t>
+          <t>2025-11-25T03:01:36.958407+00:00</t>
         </is>
       </c>
     </row>
@@ -1422,12 +1422,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Аланов Егор</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>26698</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СИБ_алановегор</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:07.889722+00:00</t>
+          <t>2025-11-25T03:01:38.875530+00:00</t>
         </is>
       </c>
     </row>
@@ -1479,27 +1479,27 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>16195</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:07.889754+00:00</t>
+          <t>2025-11-25T03:01:38.875559+00:00</t>
         </is>
       </c>
     </row>
@@ -1536,12 +1536,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1551,12 +1551,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1571,49 +1571,49 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:07.889771+00:00</t>
+          <t>2025-11-25T03:01:38.875576+00:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1623,12 +1623,12 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:10.267375+00:00</t>
+          <t>2025-11-25T03:01:38.875591+00:00</t>
         </is>
       </c>
     </row>
@@ -1650,27 +1650,27 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>41566</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1685,34 +1685,34 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:10.267405+00:00</t>
+          <t>2025-11-25T03:01:40.832965+00:00</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1722,12 +1722,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1737,12 +1737,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:12.975236+00:00</t>
+          <t>2025-11-25T03:01:40.832992+00:00</t>
         </is>
       </c>
     </row>
@@ -1764,27 +1764,27 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Самсонов Илья</t>
+          <t>Венгрыжановский Денис</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>21010</t>
+          <t>31892</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СОЧ_самсоновилья</t>
+          <t>1369_СОЧ_венгрыжановскийденис</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:12.975263+00:00</t>
+          <t>2025-11-25T03:01:43.254915+00:00</t>
         </is>
       </c>
     </row>
@@ -1821,27 +1821,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Сушко Илья</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>22691</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СОЧ_сушкоилья</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:12.975283+00:00</t>
+          <t>2025-11-25T03:01:43.254943+00:00</t>
         </is>
       </c>
     </row>
@@ -1878,27 +1878,27 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Самсонов Илья</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>вратарь</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>44847</t>
+          <t>21010</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_СОЧ_самсоновилья</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1913,49 +1913,49 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:12.975301+00:00</t>
+          <t>2025-11-25T03:01:43.254960+00:00</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Сушко Илья</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>33545</t>
+          <t>22691</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СОЧ_сушкоилья</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1965,54 +1965,54 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:15.669380+00:00</t>
+          <t>2025-11-25T03:01:43.254976+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Хёфенмайер Ноэль</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>22494</t>
+          <t>44847</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СОЧ_хефенмайерноэль</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,54 +2022,54 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:15.669408+00:00</t>
+          <t>2025-11-25T03:01:43.254993+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Вишневский Дмитрий</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>55</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>15299</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_СПР_вишневскийдмитрий</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,12 +2079,12 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:18.399603+00:00</t>
+          <t>2025-11-25T03:01:45.634035+00:00</t>
         </is>
       </c>
     </row>
@@ -2106,27 +2106,27 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>20546</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:18.399637+00:00</t>
+          <t>2025-11-25T03:01:48.034459+00:00</t>
         </is>
       </c>
     </row>
@@ -2163,27 +2163,27 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Зоркин Никита</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>26738</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СЮЛ_зоркинникита</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:18.399655+00:00</t>
+          <t>2025-11-25T03:01:48.034486+00:00</t>
         </is>
       </c>
     </row>
@@ -2220,12 +2220,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2235,12 +2235,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2255,49 +2255,49 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:18.399671+00:00</t>
+          <t>2025-11-25T03:01:48.034503+00:00</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Ян Денис</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>22166</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_СЮЛ_янденис</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2307,12 +2307,12 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:20.704368+00:00</t>
+          <t>2025-11-25T03:01:48.034518+00:00</t>
         </is>
       </c>
     </row>
@@ -2334,27 +2334,27 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2369,34 +2369,34 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:20.704400+00:00</t>
+          <t>2025-11-25T03:01:49.978674+00:00</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2406,12 +2406,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2421,12 +2421,12 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:25.876730+00:00</t>
+          <t>2025-11-25T03:01:49.978705+00:00</t>
         </is>
       </c>
     </row>
@@ -2448,27 +2448,27 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Уильямс Колби</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>41896</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1369_ЦСК_уильямсколби</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2483,34 +2483,34 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:25.876759+00:00</t>
+          <t>2025-11-25T03:01:54.386714+00:00</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Бишофф Джейк</t>
+          <t>Уильямс Колби</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2520,12 +2520,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>45490</t>
+          <t>41896</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1369_ШДР_бишоффджейк</t>
+          <t>1369_ЦСК_уильямсколби</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2535,12 +2535,12 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-24T07:02:28.606522+00:00</t>
+          <t>2025-11-25T03:01:54.386743+00:00</t>
         </is>
       </c>
     </row>
@@ -2562,42 +2562,99 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
+          <t>Бишофф Джейк</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>45490</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>1369_ШДР_бишоффджейк</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>2025-11-25T03:01:56.843467+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
           <t>Гроло Жереми</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>75</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>защитник</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="G39" t="inlineStr">
         <is>
           <t>45343</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
+      <c r="H39" t="inlineStr">
         <is>
           <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
         <is>
           <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>2025-11-24T07:02:28.606552+00:00</t>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>2025-11-25T03:01:56.843495+00:00</t>
         </is>
       </c>
     </row>
@@ -2612,7 +2669,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2660,22 +2717,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>АВТ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Автомобилист</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Зборовский Сергей</t>
+          <t>Воробьёв Иван В</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_АВТ_зборовскийсергей</t>
+          <t>1369_СПР_воробьевиванв</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2685,34 +2742,34 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
+          <t>2025-11-25T11:01:57.351677+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Рубцов Герман</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СПР_рубцовгерман</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2722,1307 +2779,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
+          <t>2025-11-25T11:01:57.351677+08:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>СОЧ</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ХК Сочи</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Гуськов Матвей</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1369_СОЧ_гуськовматвей</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>СОЧ</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ХК Сочи</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Самсонов Илья</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>1369_СОЧ_самсоновилья</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>СОЧ</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ХК Сочи</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Сушко Илья</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>1369_СОЧ_сушкоилья</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>СОЧ</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ХК Сочи</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Хёфенмайер Ноэль</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>СПР</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Спартак</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Воробьёв Иван В</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>1369_СПР_воробьевиванв</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>СПР</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Спартак</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Рубцов Герман</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>1369_СПР_рубцовгерман</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>СЮЛ</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Салават Юлаев</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Берлёв Антон</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1369_СЮЛ_берлевантон</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>СЮЛ</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Салават Юлаев</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Зоркин Никита</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>1369_СЮЛ_зоркинникита</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>СЮЛ</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Салават Юлаев</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Хворов Николай</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>1369_СЮЛ_хворовниколай</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>СЮЛ</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Салават Юлаев</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Ян Денис</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>1369_СЮЛ_янденис</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>ТОР</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Торпедо</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Науменков Михаил</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>1369_ТОР_науменковмихаил</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>ТОР</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Торпедо</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Рожков Никита А</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>1369_ТОР_рожковникитаа</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Моисеев Данила</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_моисеевданила</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Уильямс Колби</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_уильямсколби</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>СКА</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>СКА</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Зайцев Никита И</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>1369_СКА_зайцевникитаи</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Бишофф Джейк</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>1369_ШДР_бишоффджейк</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>СИБ</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Сибирь</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Широков Сергей</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>1369_СИБ_широковсергей</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>СИБ</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Сибирь</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Приски Чейз Эванс</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>1369_СИБ_прискичейзэванс</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>АВТ</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Автомобилист</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Трямкин Никита</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>1369_АВТ_трямкинникита</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>АДМ</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Адмирал</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Грман Марио</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>1369_АДМ_грманмарио</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>АДМ</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Адмирал</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Сошников Никита</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>1369_АДМ_сошниковникита</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>АКБ</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Ак Барс</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Яруллин Альберт</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>1369_АКБ_яруллинальберт</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>АМР</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Амур</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Абросимов Роман</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>1369_АМР_абросимовроман</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>БАР</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Барыс</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Бояркин Никита</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>1369_БАР_бояркинникита</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>БАР</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Барыс</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Савицкий Кирилл</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>1369_БАР_савицкийкирилл</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>БАР</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Барыс</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Уотерспун Тайлер</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>1369_БАР_уотерспунтайлер</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>ДИН</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Динамо М</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Готовец Кирилл</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>1369_ДИН_готовецкирилл</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>ДМН</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Динамо Мн</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Уэлле Ксавье</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>1369_ДМН_уэллексавье</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>ЛАД</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Лада</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Ожгихин Алексей</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>ЛОК</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Локомотив</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Сергеев Андрей</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>1369_ЛОК_сергеевандрей</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>ММГ</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Металлург Мг</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Козлов Андрей Е</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>1369_ММГ_козловандрейе</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>СЕВ</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Северсталь</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Фомин Макар</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>1369_СЕВ_фоминмакар</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>СЕВ</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Северсталь</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Цицюра Владислав</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>1369_СЕВ_цицюравладислав</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>СИБ</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Сибирь</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Пьянов Валентин</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>1369_СИБ_пьяноввалентин</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Гроло Жереми</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>1369_ШДР_гроложереми</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:12:27.061191+08:00</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
     </row>
@@ -4037,7 +2799,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4082,6 +2844,117 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>СИБ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Аланов Егор</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_СИБ_алановегор</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-25T11:01:57.351677+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>СОЧ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Венгрыжановский Денис</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1369_СОЧ_венгрыжановскийденис</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-11-25T11:01:57.351677+08:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-11-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>СПР</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Спартак</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Вишневский Дмитрий</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1369_СПР_вишневскийдмитрий</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-11-25T11:01:57.351677+08:00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-11-25</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-25 15:10:20)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:11.456802+00:00</t>
+          <t>2025-11-25T07:03:18.195425+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:13.785575+00:00</t>
+          <t>2025-11-25T07:03:23.626509+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:13.785604+00:00</t>
+          <t>2025-11-25T07:03:23.626538+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:15.684829+00:00</t>
+          <t>2025-11-25T07:03:28.703000+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:18.010400+00:00</t>
+          <t>2025-11-25T07:03:34.110071+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:20.419727+00:00</t>
+          <t>2025-11-25T07:03:39.247569+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:20.419755+00:00</t>
+          <t>2025-11-25T07:03:39.247598+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:20.419773+00:00</t>
+          <t>2025-11-25T07:03:39.247616+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:22.790529+00:00</t>
+          <t>2025-11-25T07:03:44.268907+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:25.154010+00:00</t>
+          <t>2025-11-25T07:03:49.314295+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:27.502192+00:00</t>
+          <t>2025-11-25T07:03:54.860386+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:29.861433+00:00</t>
+          <t>2025-11-25T07:03:59.898052+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:32.221036+00:00</t>
+          <t>2025-11-25T07:04:04.938364+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:36.958360+00:00</t>
+          <t>2025-11-25T07:04:15.376276+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:36.958390+00:00</t>
+          <t>2025-11-25T07:04:15.376309+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:36.958407+00:00</t>
+          <t>2025-11-25T07:04:15.376325+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:38.875530+00:00</t>
+          <t>2025-11-25T07:04:20.323809+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:38.875559+00:00</t>
+          <t>2025-11-25T07:04:20.323844+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:38.875576+00:00</t>
+          <t>2025-11-25T07:04:20.323864+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:38.875591+00:00</t>
+          <t>2025-11-25T07:04:20.323880+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:40.832965+00:00</t>
+          <t>2025-11-25T07:04:25.914629+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:40.832992+00:00</t>
+          <t>2025-11-25T07:04:25.914661+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:43.254915+00:00</t>
+          <t>2025-11-25T07:04:31.470219+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:43.254943+00:00</t>
+          <t>2025-11-25T07:04:31.470248+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:43.254960+00:00</t>
+          <t>2025-11-25T07:04:31.470265+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:43.254976+00:00</t>
+          <t>2025-11-25T07:04:31.470283+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:43.254993+00:00</t>
+          <t>2025-11-25T07:04:31.470302+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:45.634035+00:00</t>
+          <t>2025-11-25T07:04:36.517041+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:48.034459+00:00</t>
+          <t>2025-11-25T07:04:41.502560+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:48.034486+00:00</t>
+          <t>2025-11-25T07:04:41.502588+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:48.034503+00:00</t>
+          <t>2025-11-25T07:04:41.502607+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:48.034518+00:00</t>
+          <t>2025-11-25T07:04:41.502622+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:49.978674+00:00</t>
+          <t>2025-11-25T07:04:46.703897+00:00</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:49.978705+00:00</t>
+          <t>2025-11-25T07:04:46.703928+00:00</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:54.386714+00:00</t>
+          <t>2025-11-25T07:04:56.964000+00:00</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:54.386743+00:00</t>
+          <t>2025-11-25T07:04:56.964027+00:00</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:56.843467+00:00</t>
+          <t>2025-11-25T07:05:02.027092+00:00</t>
         </is>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2025-11-25T03:01:56.843495+00:00</t>
+          <t>2025-11-25T07:05:02.027122+00:00</t>
         </is>
       </c>
     </row>
@@ -2799,7 +2799,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2844,117 +2844,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>СИБ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Сибирь</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Аланов Егор</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_СИБ_алановегор</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-25T11:01:57.351677+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-25</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>СОЧ</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ХК Сочи</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Венгрыжановский Денис</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1369_СОЧ_венгрыжановскийденис</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-11-25T11:01:57.351677+08:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-11-25</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>СПР</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Спартак</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Вишневский Дмитрий</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1369_СПР_вишневскийдмитрий</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-11-25T11:01:57.351677+08:00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2025-11-25</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-26 11:06:23)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-25T07:03:18.195425+00:00</t>
+          <t>2025-11-26T03:02:55.353047+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-25T07:03:23.626509+00:00</t>
+          <t>2025-11-26T03:02:57.632335+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-25T07:03:23.626538+00:00</t>
+          <t>2025-11-26T03:02:57.632369+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-25T07:03:28.703000+00:00</t>
+          <t>2025-11-26T03:03:00.428256+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-25T07:03:34.110071+00:00</t>
+          <t>2025-11-26T03:03:02.776613+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-25T07:03:39.247569+00:00</t>
+          <t>2025-11-26T03:03:05.108922+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-25T07:03:39.247598+00:00</t>
+          <t>2025-11-26T03:03:05.108951+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-25T07:03:39.247616+00:00</t>
+          <t>2025-11-26T03:03:05.108969+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-25T07:03:44.268907+00:00</t>
+          <t>2025-11-26T03:03:07.338385+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-25T07:03:49.314295+00:00</t>
+          <t>2025-11-26T03:03:10.063262+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-25T07:03:54.860386+00:00</t>
+          <t>2025-11-26T03:03:12.738729+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-25T07:03:59.898052+00:00</t>
+          <t>2025-11-26T03:03:15.456918+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:04.938364+00:00</t>
+          <t>2025-11-26T03:03:18.209923+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:15.376276+00:00</t>
+          <t>2025-11-26T03:03:23.199849+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:15.376309+00:00</t>
+          <t>2025-11-26T03:03:23.199875+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:15.376325+00:00</t>
+          <t>2025-11-26T03:03:23.199897+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:20.323809+00:00</t>
+          <t>2025-11-26T03:03:25.977597+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:20.323844+00:00</t>
+          <t>2025-11-26T03:03:25.977627+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:20.323864+00:00</t>
+          <t>2025-11-26T03:03:25.977645+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:20.323880+00:00</t>
+          <t>2025-11-26T03:03:25.977661+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:25.914629+00:00</t>
+          <t>2025-11-26T03:03:28.293905+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:25.914661+00:00</t>
+          <t>2025-11-26T03:03:28.293937+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:31.470219+00:00</t>
+          <t>2025-11-26T03:03:31.027453+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:31.470248+00:00</t>
+          <t>2025-11-26T03:03:31.027484+00:00</t>
         </is>
       </c>
     </row>
@@ -1878,27 +1878,27 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Самсонов Илья</t>
+          <t>Сушко Илья</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>21010</t>
+          <t>22691</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СОЧ_самсоновилья</t>
+          <t>1369_СОЧ_сушкоилья</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:31.470265+00:00</t>
+          <t>2025-11-26T03:03:31.027502+00:00</t>
         </is>
       </c>
     </row>
@@ -1935,12 +1935,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Сушко Илья</t>
+          <t>Хёфенмайер Ноэль</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1950,12 +1950,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>22691</t>
+          <t>44847</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СОЧ_сушкоилья</t>
+          <t>1369_СОЧ_хефенмайерноэль</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1970,34 +1970,34 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:31.470283+00:00</t>
+          <t>2025-11-26T03:03:31.027522+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Вишневский Дмитрий</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>55</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2007,12 +2007,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>44847</t>
+          <t>15299</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_СПР_вишневскийдмитрий</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,54 +2022,54 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:31.470302+00:00</t>
+          <t>2025-11-26T03:03:33.803880+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Вишневский Дмитрий</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>15299</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СПР_вишневскийдмитрий</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,54 +2079,54 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:36.517041+00:00</t>
+          <t>2025-11-26T03:03:36.088681+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>20546</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2136,54 +2136,54 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:41.502560+00:00</t>
+          <t>2025-11-26T03:03:38.931494+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>26738</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,39 +2193,39 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:41.502588+00:00</t>
+          <t>2025-11-26T03:03:38.931526+00:00</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2235,12 +2235,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2250,54 +2250,54 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:41.502607+00:00</t>
+          <t>2025-11-26T03:03:44.044564+00:00</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Ян Денис</t>
+          <t>Бишофф Джейк</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>28</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>22166</t>
+          <t>45490</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_янденис</t>
+          <t>1369_ШДР_бишоффджейк</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2307,39 +2307,39 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:41.502622+00:00</t>
+          <t>2025-11-26T03:03:46.754572+00:00</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2349,12 +2349,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2364,297 +2364,12 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-25T07:04:46.703897+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>ТОР</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Торпедо</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>torpedo</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Рожков Никита А</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>71</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>27912</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>1369_ТОР_рожковникитаа</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>2025-11-25T07:04:46.703928+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>cska</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Моисеев Данила</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>93</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>нападающий</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>23931</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_моисеевданила</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>2025-11-25T07:04:56.964000+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>cska</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Уильямс Колби</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>41896</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_уильямсколби</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>2025-11-25T07:04:56.964027+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Бишофф Джейк</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>45490</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>1369_ШДР_бишоффджейк</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>2025-11-25T07:05:02.027092+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Гроло Жереми</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>45343</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>1369_ШДР_гроложереми</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>2025-11-25T07:05:02.027122+00:00</t>
+          <t>2025-11-26T03:03:46.754603+00:00</t>
         </is>
       </c>
     </row>
@@ -2669,7 +2384,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2717,22 +2432,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Воробьёв Иван В</t>
+          <t>Самсонов Илья</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_СПР_воробьевиванв</t>
+          <t>1369_СОЧ_самсоновилья</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2742,34 +2457,34 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-25T11:01:57.351677+08:00</t>
+          <t>2025-11-26T11:03:47.264605+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Рубцов Герман</t>
+          <t>Берлёв Антон</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1369_СПР_рубцовгерман</t>
+          <t>1369_СЮЛ_берлевантон</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2779,12 +2494,123 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-25T11:01:57.351677+08:00</t>
+          <t>2025-11-26T11:03:47.264605+08:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>СЮЛ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Салават Юлаев</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Зоркин Никита</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1369_СЮЛ_зоркинникита</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-11-26T11:03:47.264605+08:00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-11-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>СЮЛ</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Салават Юлаев</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ян Денис</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1369_СЮЛ_янденис</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-11-26T11:03:47.264605+08:00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025-11-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Уильямс Колби</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_уильямсколби</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-11-26T11:03:47.264605+08:00</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025-11-26</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-26 15:07:03)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-26T03:02:55.353047+00:00</t>
+          <t>2025-11-26T07:03:15.210224+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-26T03:02:57.632335+00:00</t>
+          <t>2025-11-26T07:03:17.528074+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-26T03:02:57.632369+00:00</t>
+          <t>2025-11-26T07:03:17.528113+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:00.428256+00:00</t>
+          <t>2025-11-26T07:03:20.297265+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:02.776613+00:00</t>
+          <t>2025-11-26T07:03:22.674197+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:05.108922+00:00</t>
+          <t>2025-11-26T07:03:25.519572+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:05.108951+00:00</t>
+          <t>2025-11-26T07:03:25.519599+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:05.108969+00:00</t>
+          <t>2025-11-26T07:03:25.519618+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:07.338385+00:00</t>
+          <t>2025-11-26T07:03:28.239812+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:10.063262+00:00</t>
+          <t>2025-11-26T07:03:30.596197+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:12.738729+00:00</t>
+          <t>2025-11-26T07:03:32.936403+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:15.456918+00:00</t>
+          <t>2025-11-26T07:03:35.296026+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:18.209923+00:00</t>
+          <t>2025-11-26T07:03:38.055390+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:23.199849+00:00</t>
+          <t>2025-11-26T07:03:42.994691+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:23.199875+00:00</t>
+          <t>2025-11-26T07:03:42.994724+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:23.199897+00:00</t>
+          <t>2025-11-26T07:03:42.994744+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:25.977597+00:00</t>
+          <t>2025-11-26T07:03:45.801991+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:25.977627+00:00</t>
+          <t>2025-11-26T07:03:45.802031+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:25.977645+00:00</t>
+          <t>2025-11-26T07:03:45.802050+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:25.977661+00:00</t>
+          <t>2025-11-26T07:03:45.802066+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:28.293905+00:00</t>
+          <t>2025-11-26T07:03:48.063525+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:28.293937+00:00</t>
+          <t>2025-11-26T07:03:48.063554+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:31.027453+00:00</t>
+          <t>2025-11-26T07:03:50.316307+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:31.027484+00:00</t>
+          <t>2025-11-26T07:03:50.316336+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:31.027502+00:00</t>
+          <t>2025-11-26T07:03:50.316353+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:31.027522+00:00</t>
+          <t>2025-11-26T07:03:50.316370+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:33.803880+00:00</t>
+          <t>2025-11-26T07:03:52.601170+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:36.088681+00:00</t>
+          <t>2025-11-26T07:03:55.117445+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:38.931494+00:00</t>
+          <t>2025-11-26T07:03:57.918244+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:38.931526+00:00</t>
+          <t>2025-11-26T07:03:57.918274+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:44.044564+00:00</t>
+          <t>2025-11-26T07:04:03.048924+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:46.754572+00:00</t>
+          <t>2025-11-26T07:04:05.928816+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-26T03:03:46.754603+00:00</t>
+          <t>2025-11-26T07:04:05.928843+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-27 11:06:26)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:15.210224+00:00</t>
+          <t>2025-11-27T03:02:43.290403+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:17.528074+00:00</t>
+          <t>2025-11-27T03:02:45.704479+00:00</t>
         </is>
       </c>
     </row>
@@ -624,12 +624,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Сошников Никита</t>
+          <t>Дарьин Александр</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>41</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -639,12 +639,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>16731</t>
+          <t>26282</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1369_АДМ_сошниковникита</t>
+          <t>1369_АДМ_дарьиналександр</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -659,49 +659,49 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:17.528113+00:00</t>
+          <t>2025-11-27T03:02:45.704515+00:00</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>АКБ</t>
+          <t>АДМ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Адмирал</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ak_bars</t>
+          <t>admiral</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Яруллин Альберт</t>
+          <t>Сошников Никита</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>90</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>16365</t>
+          <t>16731</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1369_АКБ_яруллинальберт</t>
+          <t>1369_АДМ_сошниковникита</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -711,39 +711,39 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
+          <t>https://www.khl.ru/clubs/admiral/team/</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:20.297265+00:00</t>
+          <t>2025-11-27T03:02:45.704534+00:00</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>АМР</t>
+          <t>АКБ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>amur</t>
+          <t>ak_bars</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Абросимов Роман</t>
+          <t>Яруллин Альберт</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -753,12 +753,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>17968</t>
+          <t>16365</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1369_АМР_абросимовроман</t>
+          <t>1369_АКБ_яруллинальберт</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -768,54 +768,54 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/amur/team/</t>
+          <t>https://www.khl.ru/clubs/ak_bars/team/</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:22.674197+00:00</t>
+          <t>2025-11-27T03:02:48.038723+00:00</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>АМР</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Амур</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>amur</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Абросимов Роман</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>94</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>вратарь</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>28244</t>
+          <t>17968</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_АМР_абросимовроман</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -825,12 +825,12 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/amur/team/</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:25.519572+00:00</t>
+          <t>2025-11-27T03:02:50.618549+00:00</t>
         </is>
       </c>
     </row>
@@ -852,27 +852,27 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Савицкий Кирилл</t>
+          <t>Уотерспун Тайлер</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>26</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>17901</t>
+          <t>45769</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1369_БАР_савицкийкирилл</t>
+          <t>1369_БАР_уотерспунтайлер</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -887,34 +887,34 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:25.519599+00:00</t>
+          <t>2025-11-27T03:02:52.945903+00:00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>ДИН</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>barys</t>
+          <t>dynamo_msk</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Уотерспун Тайлер</t>
+          <t>Готовец Кирилл</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>41</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -924,12 +924,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>45769</t>
+          <t>16034</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1369_БАР_уотерспунтайлер</t>
+          <t>1369_ДИН_готовецкирилл</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -939,54 +939,54 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/barys/team/</t>
+          <t>https://www.khl.ru/clubs/dynamo_msk/team/</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:25.519618+00:00</t>
+          <t>2025-11-27T03:02:55.615622+00:00</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ДИН</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Динамо М</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dynamo_msk</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Готовец Кирилл</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>16034</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1369_ДИН_готовецкирилл</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -996,39 +996,39 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/dynamo_msk/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:28.239812+00:00</t>
+          <t>2025-11-27T03:03:01.726044+00:00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ДМН</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dinamo_mn</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Уэлле Ксавье</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1038,12 +1038,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>19692</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1369_ДМН_уэллексавье</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1053,39 +1053,39 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/dinamo_mn/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:30.596197+00:00</t>
+          <t>2025-11-27T03:03:04.539506+00:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ЛАД</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>lada</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1095,12 +1095,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1110,54 +1110,54 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lada/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:32.936403+00:00</t>
+          <t>2025-11-27T03:03:07.318657+00:00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Квочко Илья</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>39445</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_СЕВ_квочкоилья</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1167,54 +1167,54 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:35.296026+00:00</t>
+          <t>2025-11-27T03:03:12.914962+00:00</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Фомин Макар</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>42087</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_СЕВ_фоминмакар</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1224,12 +1224,12 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:38.055390+00:00</t>
+          <t>2025-11-27T03:03:12.915000+00:00</t>
         </is>
       </c>
     </row>
@@ -1251,12 +1251,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Квочко Илья</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1266,12 +1266,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>39445</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_СЕВ_квочкоилья</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1286,34 +1286,34 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:42.994691+00:00</t>
+          <t>2025-11-27T03:03:12.915022+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Фомин Макар</t>
+          <t>Аланов Егор</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1323,12 +1323,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>42087</t>
+          <t>26698</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_СЕВ_фоминмакар</t>
+          <t>1369_СИБ_алановегор</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,54 +1338,54 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:42.994724+00:00</t>
+          <t>2025-11-27T03:03:15.293254+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,12 +1395,12 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:42.994744+00:00</t>
+          <t>2025-11-27T03:03:15.293285+00:00</t>
         </is>
       </c>
     </row>
@@ -1422,27 +1422,27 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Аланов Егор</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>26698</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_СИБ_алановегор</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:45.801991+00:00</t>
+          <t>2025-11-27T03:03:15.293308+00:00</t>
         </is>
       </c>
     </row>
@@ -1479,27 +1479,27 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1514,49 +1514,49 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:45.802031+00:00</t>
+          <t>2025-11-27T03:03:15.293326+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>16195</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1566,39 +1566,39 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:45.802050+00:00</t>
+          <t>2025-11-27T03:03:18.101414+00:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1623,54 +1623,54 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:45.802066+00:00</t>
+          <t>2025-11-27T03:03:18.101447+00:00</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Венгрыжановский Денис</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>31892</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СОЧ_венгрыжановскийденис</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1680,39 +1680,39 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:48.063525+00:00</t>
+          <t>2025-11-27T03:03:20.469126+00:00</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1722,12 +1722,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>41566</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1737,12 +1737,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:48.063554+00:00</t>
+          <t>2025-11-27T03:03:20.469159+00:00</t>
         </is>
       </c>
     </row>
@@ -1764,27 +1764,27 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Венгрыжановский Денис</t>
+          <t>Сушко Илья</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>31892</t>
+          <t>22691</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СОЧ_венгрыжановскийденис</t>
+          <t>1369_СОЧ_сушкоилья</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:50.316307+00:00</t>
+          <t>2025-11-27T03:03:20.469179+00:00</t>
         </is>
       </c>
     </row>
@@ -1821,27 +1821,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Хёфенмайер Ноэль</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>44847</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СОЧ_хефенмайерноэль</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1856,34 +1856,34 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:50.316336+00:00</t>
+          <t>2025-11-27T03:03:20.469201+00:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Сушко Илья</t>
+          <t>Вишневский Дмитрий</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>55</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>22691</t>
+          <t>15299</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СОЧ_сушкоилья</t>
+          <t>1369_СПР_вишневскийдмитрий</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1908,54 +1908,54 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:50.316353+00:00</t>
+          <t>2025-11-27T03:03:23.262287+00:00</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>44847</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1965,39 +1965,39 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:50.316370+00:00</t>
+          <t>2025-11-27T03:03:26.108549+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Вишневский Дмитрий</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2007,12 +2007,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>15299</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_СПР_вишневскийдмитрий</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,39 +2022,39 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:52.601170+00:00</t>
+          <t>2025-11-27T03:03:28.907700+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Рожков Никита А</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2064,12 +2064,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>27912</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_ТОР_рожковникитаа</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,54 +2079,54 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:55.117445+00:00</t>
+          <t>2025-11-27T03:03:28.907733+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Моисеев Данила</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>23931</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_ЦСК_моисеевданила</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2136,54 +2136,54 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:57.918244+00:00</t>
+          <t>2025-11-27T03:03:33.602589+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Бишофф Джейк</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>28</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>45490</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_ШДР_бишоффджейк</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,54 +2193,54 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-26T07:03:57.918274+00:00</t>
+          <t>2025-11-27T03:03:35.888048+00:00</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ШДР</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>kunlun</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Гроло Жереми</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>45343</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2250,126 +2250,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-26T07:04:03.048924+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Бишофф Джейк</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>45490</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>1369_ШДР_бишоффджейк</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>2025-11-26T07:04:05.928816+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>ШДР</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Драконы</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>kunlun</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Гроло Жереми</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>защитник</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>45343</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>1369_ШДР_гроложереми</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>2025-11-26T07:04:05.928843+00:00</t>
+          <t>2025-11-27T03:03:35.888079+00:00</t>
         </is>
       </c>
     </row>
@@ -2384,7 +2270,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2432,22 +2318,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Самсонов Илья</t>
+          <t>Бояркин Никита</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_СОЧ_самсоновилья</t>
+          <t>1369_БАР_бояркинникита</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2457,34 +2343,34 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-26T11:03:47.264605+08:00</t>
+          <t>2025-11-27T11:03:36.391116+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>БАР</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Берлёв Антон</t>
+          <t>Савицкий Кирилл</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_берлевантон</t>
+          <t>1369_БАР_савицкийкирилл</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2494,34 +2380,34 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-26T11:03:47.264605+08:00</t>
+          <t>2025-11-27T11:03:36.391116+08:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>ДМН</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Зоркин Никита</t>
+          <t>Уэлле Ксавье</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_зоркинникита</t>
+          <t>1369_ДМН_уэллексавье</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -2531,86 +2417,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-11-26T11:03:47.264605+08:00</t>
+          <t>2025-11-27T11:03:36.391116+08:00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>СЮЛ</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Салават Юлаев</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Ян Денис</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>1369_СЮЛ_янденис</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2025-11-26T11:03:47.264605+08:00</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2025-11-26</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Уильямс Колби</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_уильямсколби</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2025-11-26T11:03:47.264605+08:00</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
     </row>
@@ -2625,7 +2437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2670,6 +2482,43 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>АДМ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Адмирал</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Дарьин Александр</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_АДМ_дарьиналександр</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>INJURED_NEW</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-27T11:03:36.391116+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-27</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-27 15:05:59)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-27T03:02:43.290403+00:00</t>
+          <t>2025-11-27T07:02:15.813256+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-27T03:02:45.704479+00:00</t>
+          <t>2025-11-27T07:02:18.505254+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-27T03:02:45.704515+00:00</t>
+          <t>2025-11-27T07:02:18.505287+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-27T03:02:45.704534+00:00</t>
+          <t>2025-11-27T07:02:18.505307+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-27T03:02:48.038723+00:00</t>
+          <t>2025-11-27T07:02:21.358081+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-27T03:02:50.618549+00:00</t>
+          <t>2025-11-27T07:02:24.168007+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-27T03:02:52.945903+00:00</t>
+          <t>2025-11-27T07:02:26.589564+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-27T03:02:55.615622+00:00</t>
+          <t>2025-11-27T07:02:30.008443+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:01.726044+00:00</t>
+          <t>2025-11-27T07:02:35.012012+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:04.539506+00:00</t>
+          <t>2025-11-27T07:02:37.948007+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:07.318657+00:00</t>
+          <t>2025-11-27T07:02:40.266757+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:12.914962+00:00</t>
+          <t>2025-11-27T07:02:45.572430+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:12.915000+00:00</t>
+          <t>2025-11-27T07:02:45.572462+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:12.915022+00:00</t>
+          <t>2025-11-27T07:02:45.572487+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:15.293254+00:00</t>
+          <t>2025-11-27T07:02:48.217316+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:15.293285+00:00</t>
+          <t>2025-11-27T07:02:48.217351+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:15.293308+00:00</t>
+          <t>2025-11-27T07:02:48.217372+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:15.293326+00:00</t>
+          <t>2025-11-27T07:02:48.217391+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:18.101414+00:00</t>
+          <t>2025-11-27T07:02:50.538544+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:18.101447+00:00</t>
+          <t>2025-11-27T07:02:50.538576+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:20.469126+00:00</t>
+          <t>2025-11-27T07:02:52.826512+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:20.469159+00:00</t>
+          <t>2025-11-27T07:02:52.826543+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:20.469179+00:00</t>
+          <t>2025-11-27T07:02:52.826562+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:20.469201+00:00</t>
+          <t>2025-11-27T07:02:52.826581+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:23.262287+00:00</t>
+          <t>2025-11-27T07:02:55.587073+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:26.108549+00:00</t>
+          <t>2025-11-27T07:02:58.365887+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:28.907700+00:00</t>
+          <t>2025-11-27T07:03:01.416339+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:28.907733+00:00</t>
+          <t>2025-11-27T07:03:01.416374+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:33.602589+00:00</t>
+          <t>2025-11-27T07:03:06.486007+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:35.888048+00:00</t>
+          <t>2025-11-27T07:03:08.783400+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-27T03:03:35.888079+00:00</t>
+          <t>2025-11-27T07:03:08.783429+00:00</t>
         </is>
       </c>
     </row>
@@ -2437,7 +2437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2482,43 +2482,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>АДМ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Адмирал</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Дарьин Александр</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_АДМ_дарьиналександр</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-27T11:03:36.391116+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-27</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-28 11:06:05)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:15.813256+00:00</t>
+          <t>2025-11-28T03:01:48.940560+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:18.505254+00:00</t>
+          <t>2025-11-28T03:01:51.243024+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:18.505287+00:00</t>
+          <t>2025-11-28T03:01:51.243055+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:18.505307+00:00</t>
+          <t>2025-11-28T03:01:51.243073+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:21.358081+00:00</t>
+          <t>2025-11-28T03:01:53.488595+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:24.168007+00:00</t>
+          <t>2025-11-28T03:01:55.760451+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:26.589564+00:00</t>
+          <t>2025-11-28T03:01:58.155169+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:30.008443+00:00</t>
+          <t>2025-11-28T03:02:00.919121+00:00</t>
         </is>
       </c>
     </row>
@@ -966,12 +966,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Ожгихин Алексей</t>
+          <t>Обидин Андрей</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>58</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -981,12 +981,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>23021</t>
+          <t>21310</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1369_ЛАД_ожгихиналексей</t>
+          <t>1369_ЛАД_обидинандрей</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1001,49 +1001,49 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:35.012012+00:00</t>
+          <t>2025-11-28T03:02:05.528010+00:00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ЛОК</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>lokomotiv</t>
+          <t>lada</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Сергеев Андрей</t>
+          <t>Ожгихин Алексей</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>15416</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1369_ЛОК_сергеевандрей</t>
+          <t>1369_ЛАД_ожгихиналексей</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1053,54 +1053,54 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
+          <t>https://www.khl.ru/clubs/lada/team/</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:37.948007+00:00</t>
+          <t>2025-11-28T03:02:05.528038+00:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ММГ</t>
+          <t>ЛОК</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>metallurg_mg</t>
+          <t>lokomotiv</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Козлов Андрей Е</t>
+          <t>Сергеев Андрей</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>40899</t>
+          <t>15416</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1369_ММГ_козловандрейе</t>
+          <t>1369_ЛОК_сергеевандрей</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1110,39 +1110,39 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
+          <t>https://www.khl.ru/clubs/lokomotiv/team/</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:40.266757+00:00</t>
+          <t>2025-11-28T03:02:08.557962+00:00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Квочко Илья</t>
+          <t>Козлов Андрей Е</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>39445</t>
+          <t>40899</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1369_СЕВ_квочкоилья</t>
+          <t>1369_ММГ_козловандрейе</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1167,39 +1167,39 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:45.572430+00:00</t>
+          <t>2025-11-28T03:02:10.844916+00:00</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Фомин Макар</t>
+          <t>Хлыстов Никита</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1209,12 +1209,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>42087</t>
+          <t>17881</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_СЕВ_фоминмакар</t>
+          <t>1369_НХК_хлыстовникита</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1224,12 +1224,12 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:45.572462+00:00</t>
+          <t>2025-11-28T03:02:13.533025+00:00</t>
         </is>
       </c>
     </row>
@@ -1251,12 +1251,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Квочко Илья</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1266,12 +1266,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>39445</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СЕВ_квочкоилья</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1286,34 +1286,34 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:45.572487+00:00</t>
+          <t>2025-11-28T03:02:15.836049+00:00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Аланов Егор</t>
+          <t>Фомин Макар</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1323,12 +1323,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>26698</t>
+          <t>42087</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_СИБ_алановегор</t>
+          <t>1369_СЕВ_фоминмакар</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1338,54 +1338,54 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:48.217316+00:00</t>
+          <t>2025-11-28T03:02:15.836090+00:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>sibir</t>
+          <t>severstal</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Приски Чейз Эванс</t>
+          <t>Цицюра Владислав</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>45392</t>
+          <t>23840</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_СИБ_прискичейзэванс</t>
+          <t>1369_СЕВ_цицюравладислав</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1395,12 +1395,12 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/sibir/team/</t>
+          <t>https://www.khl.ru/clubs/severstal/team/</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:48.217351+00:00</t>
+          <t>2025-11-28T03:02:15.836114+00:00</t>
         </is>
       </c>
     </row>
@@ -1422,27 +1422,27 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Пьянов Валентин</t>
+          <t>Аланов Егор</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>16195</t>
+          <t>26698</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1369_СИБ_пьяноввалентин</t>
+          <t>1369_СИБ_алановегор</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:48.217372+00:00</t>
+          <t>2025-11-28T03:02:18.165672+00:00</t>
         </is>
       </c>
     </row>
@@ -1479,27 +1479,27 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Широков Сергей</t>
+          <t>Приски Чейз Эванс</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>45392</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1369_СИБ_широковсергей</t>
+          <t>1369_СИБ_прискичейзэванс</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1514,49 +1514,49 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:48.217391+00:00</t>
+          <t>2025-11-28T03:02:18.165703+00:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Зайцев Никита И</t>
+          <t>Пьянов Валентин</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>16024</t>
+          <t>16195</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1369_СКА_зайцевникитаи</t>
+          <t>1369_СИБ_пьяноввалентин</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1566,39 +1566,39 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:50.538544+00:00</t>
+          <t>2025-11-28T03:02:18.165721+00:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>СИБ</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ska</t>
+          <t>sibir</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Короткий Матвей</t>
+          <t>Широков Сергей</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>41566</t>
+          <t>524</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1369_СКА_короткийматвей</t>
+          <t>1369_СИБ_широковсергей</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1623,54 +1623,54 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/ska/team/</t>
+          <t>https://www.khl.ru/clubs/sibir/team/</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:50.538576+00:00</t>
+          <t>2025-11-28T03:02:18.165738+00:00</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Венгрыжановский Денис</t>
+          <t>Зайцев Никита И</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>31892</t>
+          <t>16024</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1369_СОЧ_венгрыжановскийденис</t>
+          <t>1369_СКА_зайцевникитаи</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1680,39 +1680,39 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:52.826512+00:00</t>
+          <t>2025-11-28T03:02:20.962480+00:00</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>СОЧ</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>hc_sochi</t>
+          <t>ska</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Гуськов Матвей</t>
+          <t>Короткий Матвей</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1722,12 +1722,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>29136</t>
+          <t>41566</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1369_СОЧ_гуськовматвей</t>
+          <t>1369_СКА_короткийматвей</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1737,12 +1737,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
+          <t>https://www.khl.ru/clubs/ska/team/</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:52.826543+00:00</t>
+          <t>2025-11-28T03:02:20.962514+00:00</t>
         </is>
       </c>
     </row>
@@ -1764,27 +1764,27 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Сушко Илья</t>
+          <t>Венгрыжановский Денис</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>22691</t>
+          <t>31892</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1369_СОЧ_сушкоилья</t>
+          <t>1369_СОЧ_венгрыжановскийденис</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:52.826562+00:00</t>
+          <t>2025-11-28T03:02:23.318938+00:00</t>
         </is>
       </c>
     </row>
@@ -1821,27 +1821,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Хёфенмайер Ноэль</t>
+          <t>Гуськов Матвей</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>44847</t>
+          <t>29136</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1369_СОЧ_хефенмайерноэль</t>
+          <t>1369_СОЧ_гуськовматвей</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1856,34 +1856,34 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:52.826581+00:00</t>
+          <t>2025-11-28T03:02:23.318971+00:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>СПР</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>spartak</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Вишневский Дмитрий</t>
+          <t>Сушко Илья</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>15299</t>
+          <t>22691</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1369_СПР_вишневскийдмитрий</t>
+          <t>1369_СОЧ_сушкоилья</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1908,54 +1908,54 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/spartak/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:55.587073+00:00</t>
+          <t>2025-11-28T03:02:23.318987+00:00</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>СЮЛ</t>
+          <t>СОЧ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>salavat_yulaev</t>
+          <t>hc_sochi</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Хворов Николай</t>
+          <t>Хёфенмайер Ноэль</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>39828</t>
+          <t>44847</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1369_СЮЛ_хворовниколай</t>
+          <t>1369_СОЧ_хефенмайерноэль</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1965,39 +1965,39 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
+          <t>https://www.khl.ru/clubs/hc_sochi/team/</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-27T07:02:58.365887+00:00</t>
+          <t>2025-11-28T03:02:23.319004+00:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СПР</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>spartak</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Науменков Михаил</t>
+          <t>Вишневский Дмитрий</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>55</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2007,12 +2007,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>16400</t>
+          <t>15299</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1369_ТОР_науменковмихаил</t>
+          <t>1369_СПР_вишневскийдмитрий</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2022,39 +2022,39 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/spartak/team/</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-27T07:03:01.416339+00:00</t>
+          <t>2025-11-28T03:02:25.696923+00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ТОР</t>
+          <t>СЮЛ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>torpedo</t>
+          <t>salavat_yulaev</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Рожков Никита А</t>
+          <t>Хворов Николай</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2064,12 +2064,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>27912</t>
+          <t>39828</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1369_ТОР_рожковникитаа</t>
+          <t>1369_СЮЛ_хворовниколай</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2079,54 +2079,54 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/torpedo/team/</t>
+          <t>https://www.khl.ru/clubs/salavat_yulaev/team/</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-27T07:03:01.416374+00:00</t>
+          <t>2025-11-28T03:02:28.046360+00:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ЦСК</t>
+          <t>ТОР</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>cska</t>
+          <t>torpedo</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Моисеев Данила</t>
+          <t>Науменков Михаил</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>23931</t>
+          <t>16400</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1369_ЦСК_моисеевданила</t>
+          <t>1369_ТОР_науменковмихаил</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2136,54 +2136,54 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/cska/team/</t>
+          <t>https://www.khl.ru/clubs/torpedo/team/</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-27T07:03:06.486007+00:00</t>
+          <t>2025-11-28T03:02:30.350463+00:00</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ШДР</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>kunlun</t>
+          <t>cska</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Бишофф Джейк</t>
+          <t>Бучельников Дмитрий</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>72</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>45490</t>
+          <t>39102</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1369_ШДР_бишоффджейк</t>
+          <t>1369_ЦСК_бучельниковдмитрий</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2193,69 +2193,183 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-27T07:03:08.783400+00:00</t>
+          <t>2025-11-28T03:02:36.081590+00:00</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>ЦСК</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>cska</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Моисеев Данила</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>нападающий</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>23931</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>1369_ЦСК_моисеевданила</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/cska/team/</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>2025-11-28T03:02:36.081619+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>ШДР</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B33" t="inlineStr">
         <is>
           <t>Драконы</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>kunlun</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Бишофф Джейк</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>защитник</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>45490</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>1369_ШДР_бишоффджейк</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>https://www.khl.ru/clubs/kunlun/team/</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>2025-11-28T03:02:38.842617+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ШДР</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Драконы</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>kunlun</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
         <is>
           <t>Гроло Жереми</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>75</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>защитник</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="G34" t="inlineStr">
         <is>
           <t>45343</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="H34" t="inlineStr">
         <is>
           <t>1369_ШДР_гроложереми</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>injured_active</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>injured_active</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
         <is>
           <t>https://www.khl.ru/clubs/kunlun/team/</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>2025-11-27T07:03:08.783429+00:00</t>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>2025-11-28T03:02:38.842644+00:00</t>
         </is>
       </c>
     </row>
@@ -2265,6 +2379,99 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>team_abbr</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>team_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>player_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>player_uid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>changed_at</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>changed_day</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ТОР</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Торпедо</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Рожков Никита А</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1369_ТОР_рожковникитаа</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-28T11:02:39.354541+08:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2318,167 +2525,111 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>ЛАД</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Бояркин Никита</t>
+          <t>Обидин Андрей</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1369_БАР_бояркинникита</t>
+          <t>1369_ЛАД_обидинандрей</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>RETURN</t>
+          <t>INJURED_NEW</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-27T11:03:36.391116+08:00</t>
+          <t>2025-11-28T11:02:39.354541+08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>БАР</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Савицкий Кирилл</t>
+          <t>Хлыстов Никита</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1369_БАР_савицкийкирилл</t>
+          <t>1369_НХК_хлыстовникита</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>RETURN</t>
+          <t>INJURED_NEW</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-27T11:03:36.391116+08:00</t>
+          <t>2025-11-28T11:02:39.354541+08:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ДМН</t>
+          <t>ЦСК</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Уэлле Ксавье</t>
+          <t>Бучельников Дмитрий</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1369_ДМН_уэллексавье</t>
+          <t>1369_ЦСК_бучельниковдмитрий</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>RETURN</t>
+          <t>INJURED_NEW</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-11-27T11:03:36.391116+08:00</t>
+          <t>2025-11-28T11:02:39.354541+08:00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>team_abbr</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>team_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>player_name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>player_uid</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>changed_at</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>changed_day</t>
+          <t>2025-11-28</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-28 15:06:34)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-28T03:01:48.940560+00:00</t>
+          <t>2025-11-28T07:01:46.444715+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-28T03:01:51.243024+00:00</t>
+          <t>2025-11-28T07:01:48.828176+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-28T03:01:51.243055+00:00</t>
+          <t>2025-11-28T07:01:48.828209+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-28T03:01:51.243073+00:00</t>
+          <t>2025-11-28T07:01:48.828227+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-28T03:01:53.488595+00:00</t>
+          <t>2025-11-28T07:01:51.584186+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-28T03:01:55.760451+00:00</t>
+          <t>2025-11-28T07:01:54.856430+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-28T03:01:58.155169+00:00</t>
+          <t>2025-11-28T07:01:57.217986+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:00.919121+00:00</t>
+          <t>2025-11-28T07:01:59.486195+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:05.528010+00:00</t>
+          <t>2025-11-28T07:02:04.051106+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:05.528038+00:00</t>
+          <t>2025-11-28T07:02:04.051148+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:08.557962+00:00</t>
+          <t>2025-11-28T07:02:06.532836+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:10.844916+00:00</t>
+          <t>2025-11-28T07:02:08.905927+00:00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:13.533025+00:00</t>
+          <t>2025-11-28T07:02:11.605414+00:00</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:15.836049+00:00</t>
+          <t>2025-11-28T07:02:13.908911+00:00</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:15.836090+00:00</t>
+          <t>2025-11-28T07:02:13.908939+00:00</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:15.836114+00:00</t>
+          <t>2025-11-28T07:02:13.908958+00:00</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:18.165672+00:00</t>
+          <t>2025-11-28T07:02:16.688791+00:00</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:18.165703+00:00</t>
+          <t>2025-11-28T07:02:16.688822+00:00</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:18.165721+00:00</t>
+          <t>2025-11-28T07:02:16.688840+00:00</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:18.165738+00:00</t>
+          <t>2025-11-28T07:02:16.688856+00:00</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:20.962480+00:00</t>
+          <t>2025-11-28T07:02:19.522043+00:00</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:20.962514+00:00</t>
+          <t>2025-11-28T07:02:19.522072+00:00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:23.318938+00:00</t>
+          <t>2025-11-28T07:02:21.886861+00:00</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:23.318971+00:00</t>
+          <t>2025-11-28T07:02:21.886892+00:00</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:23.318987+00:00</t>
+          <t>2025-11-28T07:02:21.886909+00:00</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:23.319004+00:00</t>
+          <t>2025-11-28T07:02:21.886928+00:00</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:25.696923+00:00</t>
+          <t>2025-11-28T07:02:24.181498+00:00</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:28.046360+00:00</t>
+          <t>2025-11-28T07:02:26.432659+00:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:30.350463+00:00</t>
+          <t>2025-11-28T07:02:28.699798+00:00</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:36.081590+00:00</t>
+          <t>2025-11-28T07:02:34.188496+00:00</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:36.081619+00:00</t>
+          <t>2025-11-28T07:02:34.188527+00:00</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:38.842617+00:00</t>
+          <t>2025-11-28T07:02:36.560639+00:00</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2025-11-28T03:02:38.842644+00:00</t>
+          <t>2025-11-28T07:02:36.560674+00:00</t>
         </is>
       </c>
     </row>
@@ -2477,7 +2477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2522,117 +2522,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ЛАД</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Лада</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Обидин Андрей</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1369_ЛАД_обидинандрей</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-28T11:02:39.354541+08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-11-28</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>НХК</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Нефтехимик</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Хлыстов Никита</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1369_НХК_хлыстовникита</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-11-28T11:02:39.354541+08:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-11-28</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ЦСК</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Бучельников Дмитрий</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1369_ЦСК_бучельниковдмитрий</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>INJURED_NEW</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-11-28T11:02:39.354541+08:00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2025-11-28</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-29 11:05:00)
</commit_message>
<xml_diff>
--- a/khl/Injuries_Master_Clubs.xlsx
+++ b/khl/Injuries_Master_Clubs.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-11-28T07:01:46.444715+00:00</t>
+          <t>2025-11-29T03:01:44.128873+00:00</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-11-28T07:01:48.828176+00:00</t>
+          <t>2025-11-29T03:01:46.486325+00:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-11-28T07:01:48.828209+00:00</t>
+          <t>2025-11-29T03:01:46.486357+00:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-11-28T07:01:48.828227+00:00</t>
+          <t>2025-11-29T03:01:46.486404+00:00</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-11-28T07:01:51.584186+00:00</t>
+          <t>2025-11-29T03:01:49.291067+00:00</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-11-28T07:01:54.856430+00:00</t>
+          <t>2025-11-29T03:01:52.246627+00:00</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-11-28T07:01:57.217986+00:00</t>
+          <t>2025-11-29T03:01:55.054289+00:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-11-28T07:01:59.486195+00:00</t>
+          <t>2025-11-29T03:01:57.858109+00:00</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-11-28T07:02:04.051106+00:00</t>
+          <t>2025-11-29T03:02:02.904222+00:00</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-11-28T07:02:04.051148+00:00</t>
+          <t>2025-11-29T03:02:02.904252+00:00</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-11-28T07:02:06.532836+00:00</t>
+          <t>2025-11-29T03:02:05.740750+00:00</t>
         </is>
       </c>
     </row>
@@ -1172,34 +1172,34 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-11-28T07:02:08.905927+00:00</t>
+          <t>2025-11-29T03:02:08.439163+00:00</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>НХК</t>
+          <t>ММГ</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>neftekhimik</t>
+          <t>metallurg_mg</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Хлыстов Никита</t>
+          <t>Сиряцкий Александр</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>74</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1209,12 +1209,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>17881</t>
+          <t>42458</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1369_НХК_хлыстовникита</t>
+          <t>1369_ММГ_сиряцкийалександр</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1224,54 +1224,54 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
+          <t>https://www.khl.ru/clubs/metallurg_mg/team/</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-11-28T07:02:11.605414+00:00</t>
+          <t>2025-11-29T03:02:08.439194+00:00</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>СЕВ</t>
+          <t>НХК</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>severstal</t>
+          <t>neftekhimik</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Квочко Илья</t>
+          <t>Хлыстов Никита</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>39445</t>
+          <t>17881</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1369_СЕВ_квочкоилья</t>
+          <t>1369_НХК_хлыстовникита</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1281,12 +1281,12 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>https://www.khl.ru/clubs/severstal/team/</t>
+          <t>https://www.khl.ru/clubs/neftekhimik/team/</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-11-28T07:02:13.908911+00:00</t>
+          <t>2025-11-29T03:02:11.204790+00:00</t>
         </is>
       </c>
     </row>
@@ -1308,27 +1308,27 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Фомин Макар</t>
+          <t>Квочко Илья</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>защитник</t>
+          <t>нападающий</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>42087</t>
+          <t>39445</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1369_СЕВ_фоминмакар</t>
+          <t>1369_СЕВ_квочкоилья</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-11-28T07:02:13.908939+00:00</t>
+          <t>2025-11-29T03:02:14.048242+00:00</t>
         </is>
       </c>
     </row>
@@ -1365,27 +1365,27 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Цицюра Владислав</t>
+          <t>Фомин Макар</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>нападающий</t>
+          <t>защитник</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>23840</t>
+          <t>42087</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1369_СЕВ_цицюравладислав</t>
+          <t>1369_СЕВ_фоминмакар</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1400,49 +1400,49 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-11-28T07:02:13.908958+00:00</t>
+          <t>2025-11-29T03:02:14.048274+00:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>СИБ</t>
+          <t>СЕВ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Северсталь</t>
         </is>
       </c>
  